<commit_message>
Regression Testing - Admin
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(18-07-2022)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(19-07-2002)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA14F40-5716-4E24-8B67-4E2FB96DB780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EE463B-3216-46FD-969D-C336CBA809FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -932,7 +933,7 @@
   <si>
     <t xml:space="preserve">coyni.admin.tests.CoyniPortalTest,
 testAddSignetAccountInvalidAmount,
--amount,
+-pamount,
 -pdescription,
 -perrMessage
 </t>
@@ -1292,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,7 +1613,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>31</v>
@@ -1884,7 +1885,7 @@
         <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>57</v>
@@ -1914,7 +1915,7 @@
         <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>57</v>
@@ -1944,7 +1945,7 @@
         <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>57</v>
@@ -1974,7 +1975,7 @@
         <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>57</v>
@@ -2004,7 +2005,7 @@
         <v>65</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>57</v>
@@ -2034,7 +2035,7 @@
         <v>67</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>57</v>
@@ -2064,7 +2065,7 @@
         <v>69</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>71</v>
@@ -2188,7 +2189,7 @@
         <v>80</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>71</v>
@@ -2250,7 +2251,7 @@
         <v>85</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>71</v>
@@ -2281,7 +2282,7 @@
         <v>87</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>71</v>
@@ -2312,7 +2313,7 @@
         <v>89</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>90</v>

</xml_diff>

<commit_message>
Added test methods in Profile test
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,18 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(19-07-2002)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\web(21-07-2022)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EE463B-3216-46FD-969D-C336CBA809FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67187429-7BE0-4707-A8C6-361856925717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="176">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -937,6 +936,50 @@
 -pdescription,
 -perrMessage
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">create Api Business </t>
+  </si>
+  <si>
+    <t>testdata-admin.xlsx,profileApiBusiness</t>
+  </si>
+  <si>
+    <t>Api Business</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testAddApiBusiness,
+-pheadingInvitation,
+-pheadingContact,
+-pfirstName,
+-plastName,
+-pemail1,
+-pphoneNumber,
+-pbusiness,
+-pdoller,
+-ppercentage,
+-pecoSystem,
+-pbusinessLimit,
+-pecoSystemLimit</t>
+  </si>
+  <si>
+    <t>Verify Business userList</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testveifyGrid,
+-pfilterType,
+-ptoAmount,
+-pamount,
+-pheading,
+-pexportHeading</t>
+  </si>
+  <si>
+    <t>Verify Business Details</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testveifyApiBusinessDetails</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1041,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1011,6 +1054,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1291,26 +1337,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="B65" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
-    <col min="9" max="9" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.44140625" customWidth="1"/>
+    <col min="9" max="9" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1339,7 +1385,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1365,7 +1411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1391,7 +1437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1417,7 +1463,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1446,7 +1492,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1475,7 +1521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1504,7 +1550,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1530,7 +1576,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="210.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="202.8" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
@@ -1556,7 +1602,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -1582,7 +1628,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
@@ -1608,12 +1654,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>31</v>
@@ -1634,7 +1680,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -1660,7 +1706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -1686,7 +1732,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -1712,7 +1758,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -1738,7 +1784,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -1764,12 +1810,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="255" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>155</v>
@@ -1793,12 +1839,12 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>166</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>155</v>
@@ -1822,12 +1868,12 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>155</v>
@@ -1851,12 +1897,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="270" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>155</v>
@@ -1880,12 +1926,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>57</v>
@@ -1910,12 +1956,12 @@
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>57</v>
@@ -1940,12 +1986,12 @@
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>57</v>
@@ -1970,12 +2016,12 @@
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>57</v>
@@ -2000,12 +2046,12 @@
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>57</v>
@@ -2030,12 +2076,12 @@
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>57</v>
@@ -2060,12 +2106,12 @@
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>71</v>
@@ -2091,7 +2137,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>74</v>
       </c>
@@ -2122,7 +2168,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>76</v>
       </c>
@@ -2153,7 +2199,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>78</v>
       </c>
@@ -2184,12 +2230,12 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>71</v>
@@ -2215,7 +2261,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -2246,12 +2292,12 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>71</v>
@@ -2277,12 +2323,12 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>71</v>
@@ -2308,12 +2354,12 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>90</v>
@@ -2337,7 +2383,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>94</v>
       </c>
@@ -2366,7 +2412,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>97</v>
       </c>
@@ -2395,7 +2441,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>99</v>
       </c>
@@ -2424,7 +2470,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>101</v>
       </c>
@@ -2453,7 +2499,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>103</v>
       </c>
@@ -2482,7 +2528,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>157</v>
       </c>
@@ -2511,7 +2557,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>109</v>
       </c>
@@ -2540,7 +2586,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>111</v>
       </c>
@@ -2569,7 +2615,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>114</v>
       </c>
@@ -2601,7 +2647,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>117</v>
       </c>
@@ -2633,7 +2679,7 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>119</v>
       </c>
@@ -2665,7 +2711,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>121</v>
       </c>
@@ -2697,7 +2743,7 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>123</v>
       </c>
@@ -2729,7 +2775,7 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>125</v>
       </c>
@@ -2761,7 +2807,7 @@
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>127</v>
       </c>
@@ -2793,7 +2839,7 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>111</v>
       </c>
@@ -2822,7 +2868,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>130</v>
       </c>
@@ -2851,7 +2897,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>132</v>
       </c>
@@ -2880,7 +2926,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>134</v>
       </c>
@@ -2909,7 +2955,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>136</v>
       </c>
@@ -2938,7 +2984,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>138</v>
       </c>
@@ -2967,7 +3013,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>140</v>
       </c>
@@ -2996,7 +3042,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>149</v>
       </c>
@@ -3025,7 +3071,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>145</v>
       </c>
@@ -3054,7 +3100,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>148</v>
       </c>
@@ -3083,7 +3129,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>147</v>
       </c>
@@ -3112,7 +3158,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>146</v>
       </c>
@@ -3139,6 +3185,93 @@
       </c>
       <c r="I63" s="2" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I65" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I66" s="8" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and modified methods in PaymentMethodcomponent, ProfileComponenet, ProfileSideBarComponent, UserDetailsComponent and ProfileTest
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\web(21-07-2022)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2022\080822_Web\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67187429-7BE0-4707-A8C6-361856925717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAB60D8-E48C-47D8-832B-7ABA294A86F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="184">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -403,9 +403,6 @@
   </si>
   <si>
     <t>testTransactionListExportsToday</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>testData-admin.xlsx,transaction</t>
@@ -980,6 +977,52 @@
   <si>
     <t>coyni.admin.tests.ProfilesTest,
 testveifyApiBusinessDetails</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Verify Individual SideBar View</t>
+  </si>
+  <si>
+    <t>testdata-admin.xlsx,profiles</t>
+  </si>
+  <si>
+    <t>Individuals</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testIndividualSideBarView,
+-pprofileHeading,
+-psearchText,
+-pexpID,
+-pexpUserName,
+-pexpAccountID</t>
+  </si>
+  <si>
+    <t>Verify Individual User Details View</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testIndividualUserDetailsView,
+-pprofileHeading,
+-psearchText,
+-pexpID,
+-pexpUserHeading,
+-puserName,
+-pexpAccountID,
+-pexpAccountStatus</t>
+  </si>
+  <si>
+    <t>Verify Individual User Details Payment Methods</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testIndividualPaymentMethodView,
+-pprofileHeading,
+-psearchText,
+-pexpID,
+-pexpPaymentMethodHeading</t>
   </si>
 </sst>
 </file>
@@ -1337,26 +1380,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B65" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.44140625" customWidth="1"/>
-    <col min="9" max="9" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.42578125" customWidth="1"/>
+    <col min="9" max="9" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1385,12 +1428,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -1399,10 +1442,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>12</v>
@@ -1411,12 +1454,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -1425,10 +1468,10 @@
         <v>15</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
@@ -1437,12 +1480,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -1451,10 +1494,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>12</v>
@@ -1463,12 +1506,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
@@ -1477,10 +1520,10 @@
         <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>21</v>
@@ -1492,12 +1535,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
@@ -1506,10 +1549,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>25</v>
@@ -1521,12 +1564,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
@@ -1535,10 +1578,10 @@
         <v>11</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>28</v>
@@ -1550,12 +1593,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>31</v>
@@ -1564,24 +1607,24 @@
         <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="202.8" x14ac:dyDescent="0.4">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="210.75" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>31</v>
@@ -1590,24 +1633,24 @@
         <v>15</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>31</v>
@@ -1616,10 +1659,10 @@
         <v>15</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>32</v>
@@ -1628,12 +1671,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>31</v>
@@ -1642,10 +1685,10 @@
         <v>15</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>32</v>
@@ -1654,12 +1697,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>31</v>
@@ -1668,10 +1711,10 @@
         <v>15</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>32</v>
@@ -1680,12 +1723,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>41</v>
@@ -1694,10 +1737,10 @@
         <v>11</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>42</v>
@@ -1706,12 +1749,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>41</v>
@@ -1720,10 +1763,10 @@
         <v>11</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>42</v>
@@ -1732,12 +1775,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>41</v>
@@ -1758,12 +1801,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>41</v>
@@ -1784,12 +1827,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>41</v>
@@ -1810,15 +1853,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
@@ -1836,18 +1879,18 @@
         <v>22</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>15</v>
@@ -1865,18 +1908,18 @@
         <v>22</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
@@ -1894,18 +1937,18 @@
         <v>22</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="270" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>15</v>
@@ -1923,15 +1966,15 @@
         <v>22</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>57</v>
@@ -1940,10 +1983,10 @@
         <v>11</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>53</v>
@@ -1956,12 +1999,12 @@
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>57</v>
@@ -1970,10 +2013,10 @@
         <v>11</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>53</v>
@@ -1986,12 +2029,12 @@
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>57</v>
@@ -2000,10 +2043,10 @@
         <v>11</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>53</v>
@@ -2016,12 +2059,12 @@
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>57</v>
@@ -2030,10 +2073,10 @@
         <v>11</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>53</v>
@@ -2046,12 +2089,12 @@
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>57</v>
@@ -2060,10 +2103,10 @@
         <v>11</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>53</v>
@@ -2076,12 +2119,12 @@
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>57</v>
@@ -2090,10 +2133,10 @@
         <v>11</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>53</v>
@@ -2106,492 +2149,492 @@
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I38" s="2" t="s">
+      <c r="B39" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I41" s="2" t="s">
+      <c r="B42" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>157</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G42" s="1" t="s">
+      <c r="H42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I42" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I42" s="2" t="s">
+    </row>
+    <row r="43" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="B43" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I43" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="B44" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>20</v>
@@ -2600,251 +2643,251 @@
         <v>15</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I44" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H44" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="B45" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I45" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I46" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I48" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I50" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>20</v>
@@ -2853,27 +2896,27 @@
         <v>11</v>
       </c>
       <c r="E52" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="B53" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>20</v>
@@ -2882,27 +2925,27 @@
         <v>15</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I53" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="B54" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>20</v>
@@ -2911,27 +2954,27 @@
         <v>11</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I54" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="B55" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>20</v>
@@ -2940,27 +2983,27 @@
         <v>11</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I55" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="B56" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>20</v>
@@ -2969,27 +3012,27 @@
         <v>11</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I56" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="B57" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>20</v>
@@ -2998,27 +3041,27 @@
         <v>11</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I57" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="B58" s="1" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>20</v>
@@ -3027,251 +3070,367 @@
         <v>11</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I62" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    </row>
+    <row r="63" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I62" s="2" t="s">
+      <c r="B63" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I63" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G64" s="1" t="s">
+      <c r="H64" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I64" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I64" s="2" t="s">
+    </row>
+    <row r="65" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+      <c r="B65" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I65" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65" s="1" t="s">
+    </row>
+    <row r="66" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I65" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="H66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I66" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I66" s="8" t="s">
-        <v>175</v>
+    </row>
+    <row r="67" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I67" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I68" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I69" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I70" s="8" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test methods in Transaction Test and Login Test
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2022\080922-Web\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin Test Data And Test Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6175F17-9769-49C1-BFFD-0387A931178F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CF4684-D926-45B0-99FD-8BB78DEF71AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="202">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1020,6 +1020,108 @@
 -psearchText,
 -pexpID,
 -pexpPaymentMethodHeading</t>
+  </si>
+  <si>
+    <t>test Change Password</t>
+  </si>
+  <si>
+    <t>TokenAccount-ChangePassword</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.LoginTest,
+testAdminLogin,
+-ploginHeading,
+-pemail,
+-ppassword,
+-pauthyHeading,
+-pauthyDescription,
+-pcode</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.HomeTest,
+testUserDetailsChangePasswordWithValid,
+-pcode,
+-pcurrentPassword,
+-pnewPassword,
+-pconfirmPassword</t>
+  </si>
+  <si>
+    <t>test Change Password invalid information</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.HomeTest,
+testUserDetailsChangePasswordInvalidCredentials,
+-pcode,
+-pcurrentPassword,
+-pnewPassword,
+-pconfirmPassword,
+-perrMessage</t>
+  </si>
+  <si>
+    <t>testdata-admin.xlsx,changePassword</t>
+  </si>
+  <si>
+    <t>test upload image</t>
+  </si>
+  <si>
+    <t>testdata-admin.xlsx,userDetails</t>
+  </si>
+  <si>
+    <t>UserDetails-Upload Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.admin.tests.HomeTest,
+uploadImg,
+-paccountProfileHeading,
+-pcropYourImageHeading,
+-pfolderName,
+-pfileName
+</t>
+  </si>
+  <si>
+    <t>testTransactionFiltersList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.admin.tests.TransactionTest,
+testverifyFilters,
+-pfilters
+</t>
+  </si>
+  <si>
+    <t>testTransactionDetailsWithChargeBack</t>
+  </si>
+  <si>
+    <t>testData-admin.xlsx,TransactionDetails</t>
+  </si>
+  <si>
+    <t>ChargeBack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.admin.tests.TransactionTest,
+testgenerateDisputes,
+-pchargeBackHeading,
+-pcaseNumber,
+-pstartDate,
+-pendDate,
+-ptableData,
+-pmessage,
+-pwonHeading,
+-pcontent,
+-pnameOfUser
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin login Page With Invalid Email </t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.LoginTest,
+testAdminLoginWithInvalidEmail,
+-ploginHeading,
+-ploginDescription,
+-pemail,
+-ppassword,
+-ptitle,
+-ptoastMessage</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1096,6 +1198,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1377,26 +1488,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
-    <col min="9" max="9" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.44140625" customWidth="1"/>
+    <col min="9" max="9" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1425,7 +1536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1451,7 +1562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1477,64 +1588,61 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>200</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>70</v>
@@ -1552,18 +1660,18 @@
         <v>129</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>70</v>
@@ -1580,45 +1688,48 @@
       <c r="F7" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="210.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>70</v>
@@ -1639,12 +1750,12 @@
         <v>32</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="210" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="202.8" x14ac:dyDescent="0.4">
+      <c r="A10" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>70</v>
@@ -1659,18 +1770,18 @@
         <v>129</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>70</v>
@@ -1685,18 +1796,18 @@
         <v>129</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>70</v>
@@ -1711,44 +1822,44 @@
         <v>129</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="255" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>70</v>
@@ -1769,12 +1880,12 @@
         <v>42</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>70</v>
@@ -1783,24 +1894,24 @@
         <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>70</v>
@@ -1809,24 +1920,24 @@
         <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
       </c>
       <c r="F16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>70</v>
@@ -1847,18 +1958,18 @@
         <v>42</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="255" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>155</v>
+        <v>41</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
@@ -1870,18 +1981,15 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>166</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>70</v>
@@ -1890,13 +1998,13 @@
         <v>155</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
       </c>
       <c r="F19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>53</v>
@@ -1905,12 +2013,12 @@
         <v>22</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>70</v>
@@ -1919,13 +2027,13 @@
         <v>155</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
       </c>
       <c r="F20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>53</v>
@@ -1934,12 +2042,12 @@
         <v>22</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="270" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>70</v>
@@ -1948,13 +2056,13 @@
         <v>155</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
       </c>
       <c r="F21" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>53</v>
@@ -1963,27 +2071,27 @@
         <v>22</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>129</v>
+        <v>15</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>5</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>53</v>
@@ -1992,13 +2100,12 @@
         <v>22</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>70</v>
@@ -2022,13 +2129,13 @@
         <v>22</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>70</v>
@@ -2052,13 +2159,13 @@
         <v>22</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>70</v>
@@ -2082,13 +2189,13 @@
         <v>22</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>70</v>
@@ -2112,13 +2219,13 @@
         <v>22</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>70</v>
@@ -2142,19 +2249,19 @@
         <v>22</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>11</v>
@@ -2166,20 +2273,19 @@
         <v>129</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>70</v>
@@ -2203,14 +2309,14 @@
         <v>22</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>70</v>
@@ -2234,14 +2340,14 @@
         <v>22</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>70</v>
@@ -2265,14 +2371,14 @@
         <v>22</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>70</v>
@@ -2296,14 +2402,14 @@
         <v>22</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>70</v>
@@ -2321,20 +2427,20 @@
         <v>129</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>70</v>
@@ -2358,14 +2464,14 @@
         <v>22</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>70</v>
@@ -2389,43 +2495,45 @@
         <v>22</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>70</v>
@@ -2443,18 +2551,18 @@
         <v>129</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>92</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>70</v>
@@ -2472,18 +2580,18 @@
         <v>129</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>92</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>70</v>
@@ -2507,12 +2615,12 @@
         <v>92</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>70</v>
@@ -2530,24 +2638,24 @@
         <v>129</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>92</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
@@ -2565,18 +2673,18 @@
         <v>92</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>157</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>11</v>
@@ -2588,18 +2696,18 @@
         <v>129</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>92</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>157</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>70</v>
@@ -2608,13 +2716,13 @@
         <v>106</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>129</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>107</v>
@@ -2623,18 +2731,18 @@
         <v>92</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>15</v>
@@ -2643,30 +2751,30 @@
         <v>129</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>92</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>129</v>
@@ -2675,21 +2783,18 @@
         <v>129</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>92</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-    </row>
-    <row r="46" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>70</v>
@@ -2713,15 +2818,15 @@
         <v>92</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>70</v>
@@ -2745,15 +2850,15 @@
         <v>92</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>70</v>
@@ -2777,15 +2882,15 @@
         <v>92</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>70</v>
@@ -2809,15 +2914,15 @@
         <v>92</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>70</v>
@@ -2841,15 +2946,15 @@
         <v>92</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>70</v>
@@ -2873,21 +2978,21 @@
         <v>92</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -2899,18 +3004,21 @@
         <v>129</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="I52" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+    </row>
+    <row r="53" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>70</v>
@@ -2919,7 +3027,7 @@
         <v>20</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>129</v>
@@ -2934,12 +3042,12 @@
         <v>92</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>70</v>
@@ -2948,7 +3056,7 @@
         <v>20</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>129</v>
@@ -2960,15 +3068,15 @@
         <v>112</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>70</v>
@@ -2992,12 +3100,12 @@
         <v>22</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>70</v>
@@ -3021,12 +3129,12 @@
         <v>22</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>70</v>
@@ -3050,12 +3158,12 @@
         <v>22</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>70</v>
@@ -3079,41 +3187,41 @@
         <v>22</v>
       </c>
       <c r="I58" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I59" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>70</v>
@@ -3137,12 +3245,12 @@
         <v>92</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>70</v>
@@ -3166,12 +3274,12 @@
         <v>92</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>70</v>
@@ -3195,12 +3303,12 @@
         <v>92</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>70</v>
@@ -3224,18 +3332,18 @@
         <v>92</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>11</v>
@@ -3247,18 +3355,18 @@
         <v>129</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>92</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>70</v>
@@ -3281,16 +3389,16 @@
       <c r="H65" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I65" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="I65" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>176</v>
@@ -3311,15 +3419,15 @@
         <v>92</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>176</v>
@@ -3334,18 +3442,18 @@
         <v>129</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>92</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>70</v>
@@ -3369,15 +3477,15 @@
         <v>92</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>176</v>
@@ -3398,10 +3506,10 @@
         <v>92</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>181</v>
       </c>
@@ -3429,6 +3537,196 @@
       <c r="I70" s="8" t="s">
         <v>182</v>
       </c>
+    </row>
+    <row r="71" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I71" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F72" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+    </row>
+    <row r="73" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A73" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F73" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+    </row>
+    <row r="74" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+    </row>
+    <row r="75" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+    </row>
+    <row r="76" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Test test script for Transaction Details and Filters
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin Test Data And Test Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(25-08-2022)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CF4684-D926-45B0-99FD-8BB78DEF71AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560B4510-BBBE-4573-BB66-5F74A8D296D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$76</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="206">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -412,12 +415,6 @@
   </si>
   <si>
     <t>TransactionListExport</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.TransactionTest,
-testExportSelectedTransactionToday,
--pheading,
--pexportHeading</t>
   </si>
   <si>
     <t>testTransactionListExportsYesterday</t>
@@ -1122,6 +1119,28 @@
 -ppassword,
 -ptitle,
 -ptoastMessage</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.TransactionTest,
+testExportSelectedTransactionToday,
+-pheading,
+-pexportHeading
+-pcontent</t>
+  </si>
+  <si>
+    <t>TransactionDetails</t>
+  </si>
+  <si>
+    <t>testFiltersWithClearListOfData</t>
+  </si>
+  <si>
+    <t>Verify Filters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.admin.tests.TransactionTest,
+testverifyApplyFilterAndClearFilters,
+-pfilters
+</t>
   </si>
 </sst>
 </file>
@@ -1202,11 +1221,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1488,26 +1507,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.44140625" customWidth="1"/>
-    <col min="9" max="9" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.42578125" customWidth="1"/>
+    <col min="9" max="9" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1536,7 +1555,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1550,10 +1569,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>12</v>
@@ -1562,7 +1581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1576,10 +1595,10 @@
         <v>15</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
@@ -1588,12 +1607,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -1602,19 +1621,19 @@
         <v>15</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1628,10 +1647,10 @@
         <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
@@ -1640,7 +1659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1654,10 +1673,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>21</v>
@@ -1669,7 +1688,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1683,10 +1702,10 @@
         <v>11</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>25</v>
@@ -1698,7 +1717,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1712,10 +1731,10 @@
         <v>11</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>28</v>
@@ -1727,7 +1746,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1741,19 +1760,19 @@
         <v>15</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="202.8" x14ac:dyDescent="0.4">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="210.75" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -1767,19 +1786,19 @@
         <v>15</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1793,10 +1812,10 @@
         <v>15</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>32</v>
@@ -1805,7 +1824,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -1819,10 +1838,10 @@
         <v>15</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>32</v>
@@ -1831,7 +1850,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -1845,10 +1864,10 @@
         <v>15</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>32</v>
@@ -1857,7 +1876,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -1871,10 +1890,10 @@
         <v>11</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>42</v>
@@ -1883,7 +1902,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -1897,10 +1916,10 @@
         <v>11</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>42</v>
@@ -1909,7 +1928,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1935,7 +1954,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -1961,7 +1980,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
@@ -1987,7 +2006,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>52</v>
       </c>
@@ -1995,7 +2014,7 @@
         <v>70</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>11</v>
@@ -2013,18 +2032,18 @@
         <v>22</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>15</v>
@@ -2042,10 +2061,10 @@
         <v>22</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
@@ -2053,7 +2072,7 @@
         <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>11</v>
@@ -2071,10 +2090,10 @@
         <v>22</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="270" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -2082,7 +2101,7 @@
         <v>70</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>15</v>
@@ -2100,10 +2119,10 @@
         <v>22</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
@@ -2117,13 +2136,13 @@
         <v>11</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>53</v>
+        <v>202</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>22</v>
@@ -2133,7 +2152,7 @@
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -2147,10 +2166,10 @@
         <v>11</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>53</v>
@@ -2163,7 +2182,7 @@
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
@@ -2177,10 +2196,10 @@
         <v>11</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>53</v>
@@ -2193,7 +2212,7 @@
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
@@ -2207,10 +2226,10 @@
         <v>11</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>53</v>
@@ -2223,7 +2242,7 @@
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
@@ -2237,10 +2256,10 @@
         <v>11</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>53</v>
@@ -2253,7 +2272,7 @@
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>67</v>
       </c>
@@ -2267,10 +2286,10 @@
         <v>11</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>53</v>
@@ -2283,7 +2302,7 @@
       </c>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
@@ -2297,10 +2316,10 @@
         <v>11</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>72</v>
@@ -2309,14 +2328,14 @@
         <v>22</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>73</v>
+        <v>201</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>70</v>
@@ -2328,10 +2347,10 @@
         <v>11</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>72</v>
@@ -2340,14 +2359,14 @@
         <v>22</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>70</v>
@@ -2359,10 +2378,10 @@
         <v>11</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>72</v>
@@ -2371,14 +2390,14 @@
         <v>22</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>70</v>
@@ -2390,10 +2409,10 @@
         <v>11</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>72</v>
@@ -2402,14 +2421,14 @@
         <v>22</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>70</v>
@@ -2421,10 +2440,10 @@
         <v>11</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>72</v>
@@ -2433,14 +2452,14 @@
         <v>22</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>70</v>
@@ -2452,26 +2471,26 @@
         <v>11</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>70</v>
@@ -2483,26 +2502,26 @@
         <v>11</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>70</v>
@@ -2514,258 +2533,258 @@
         <v>11</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I39" s="2" t="s">
+      <c r="B40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I42" s="2" t="s">
+      <c r="B43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>157</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G43" s="1" t="s">
+      <c r="H43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I43" s="2" t="s">
+    </row>
+    <row r="44" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="B44" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I44" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>70</v>
@@ -2777,248 +2796,248 @@
         <v>15</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I45" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I45" s="2" t="s">
+    </row>
+    <row r="46" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="B46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I46" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I48" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I50" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I52" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>70</v>
@@ -3030,24 +3049,24 @@
         <v>11</v>
       </c>
       <c r="E53" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>70</v>
@@ -3059,24 +3078,24 @@
         <v>15</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I54" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>70</v>
@@ -3088,24 +3107,24 @@
         <v>11</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I55" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>70</v>
@@ -3117,24 +3136,24 @@
         <v>11</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I56" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>70</v>
@@ -3146,24 +3165,24 @@
         <v>11</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I57" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>70</v>
@@ -3175,24 +3194,24 @@
         <v>11</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I58" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>70</v>
@@ -3204,471 +3223,471 @@
         <v>11</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I63" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+    </row>
+    <row r="64" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I63" s="2" t="s">
+      <c r="B64" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I64" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65" s="1" t="s">
+      <c r="H65" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I66" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I67" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I65" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="H68" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I68" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G69" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I66" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C67" s="1" t="s">
+      <c r="H69" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I69" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G70" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I67" s="8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="H70" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I70" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="1" t="s">
+      <c r="D71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I68" s="8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I69" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+      <c r="H71" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I71" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I70" s="8" t="s">
+    </row>
+    <row r="72" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I71" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A72" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="B72" s="10" t="s">
+      <c r="B72" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E72" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="F72" s="11" t="s">
-        <v>153</v>
+      <c r="E72" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="G72" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H72" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="I72" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>158</v>
+        <v>186</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E73" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="F73" s="11" t="s">
-        <v>154</v>
+      <c r="E73" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="G73" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H73" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="H73" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="I73" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C74" s="9" t="s">
         <v>190</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>191</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E74" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="F74" s="11" t="s">
-        <v>129</v>
+      <c r="E74" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="G74" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I74" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
     </row>
-    <row r="75" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>70</v>
@@ -3680,10 +3699,10 @@
         <v>11</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>72</v>
@@ -3692,43 +3711,75 @@
         <v>22</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C76" s="1" t="s">
+      <c r="D76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
+    <row r="77" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I77" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:I76" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added methods in CheckOut Test
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(25-08-2022)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(06-09-2022)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560B4510-BBBE-4573-BB66-5F74A8D296D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C316EB-27B5-4795-A35F-673EFC0C9E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$78</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="219">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1067,15 +1067,6 @@
     <t>UserDetails-Upload Image</t>
   </si>
   <si>
-    <t xml:space="preserve">coyni.admin.tests.HomeTest,
-uploadImg,
--paccountProfileHeading,
--pcropYourImageHeading,
--pfolderName,
--pfileName
-</t>
-  </si>
-  <si>
     <t>testTransactionFiltersList</t>
   </si>
   <si>
@@ -1141,6 +1132,72 @@
 testverifyApplyFilterAndClearFilters,
 -pfilters
 </t>
+  </si>
+  <si>
+    <t>verify Payout transactionList</t>
+  </si>
+  <si>
+    <t>Commission History</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.CoyniPortalTest,
+testVerifyPayoutTransactionHistory,
+-pheading</t>
+  </si>
+  <si>
+    <t>testApplyFiltersCountWithDB</t>
+  </si>
+  <si>
+    <t>Verify Apply Filters Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.admin.tests.TransactionTest,
+testVerifyFiltersDataInTransaction,
+-pquery
+</t>
+  </si>
+  <si>
+    <t>test remove image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.admin.tests.HomeTest,
+testRemoveUploadedImg,
+-paccountProfileHeading,
+-premoveHeading,
+-pcontent
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.admin.tests.HomeTest,
+uploadImg,
+-paccountProfileHeading,
+-pcropYourImageHeading,
+-pfolderName,
+-pfileName,
+-ptitle,
+-pmessage
+</t>
+  </si>
+  <si>
+    <t>UserDetails-RemoveImage</t>
+  </si>
+  <si>
+    <t>test checkOut Transaction</t>
+  </si>
+  <si>
+    <t>testData-admin.xlsx,checkOut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.checkout.tests.CheckOutTest,
+tesCheckOutTransaction,
+-pdomain,
+-porderId,
+-ppublicKey,
+-psecretKey
+</t>
+  </si>
+  <si>
+    <t>Verify Check Out Transaction</t>
   </si>
 </sst>
 </file>
@@ -1182,12 +1239,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1202,7 +1265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1226,6 +1289,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1507,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M77"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="I77" sqref="I77"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1590,7 @@
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.42578125" customWidth="1"/>
     <col min="9" max="9" width="43.140625" customWidth="1"/>
   </cols>
@@ -1609,7 +1678,7 @@
     </row>
     <row r="4" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>70</v>
@@ -1630,7 +1699,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
@@ -2142,7 +2211,7 @@
         <v>128</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>22</v>
@@ -2328,7 +2397,7 @@
         <v>22</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -3652,7 +3721,7 @@
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>189</v>
       </c>
@@ -3678,53 +3747,55 @@
         <v>184</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
     </row>
-    <row r="75" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>193</v>
+    <row r="75" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>211</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>72</v>
+      <c r="C75" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>22</v>
+        <v>184</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
-    </row>
-    <row r="76" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+    </row>
+    <row r="76" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>196</v>
+        <v>71</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -3736,50 +3807,170 @@
         <v>128</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>197</v>
+        <v>72</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>157</v>
+        <v>70</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I77" s="11" t="s">
-        <v>205</v>
+      <c r="I77" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
+    <row r="78" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I78" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+    </row>
+    <row r="79" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="A79" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C79" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F79" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="G79" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="H79" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I79" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I80" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+    </row>
+    <row r="81" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I81" s="11"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I76" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added test methods in check out transaction and pages and components
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(06-09-2022)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(06-09-2022)[2]\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C316EB-27B5-4795-A35F-673EFC0C9E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5CB7FF-13DF-46FB-8938-1A43A71AE9B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="223">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1188,16 +1188,64 @@
     <t>testData-admin.xlsx,checkOut</t>
   </si>
   <si>
+    <t>Verify Check Out Transaction</t>
+  </si>
+  <si>
+    <t>test checkOut Transaction invalid PopUp</t>
+  </si>
+  <si>
+    <t>coyni.checkout.tests.CheckOutTest,
+tesCheckOutInvalidData,
+-pdomain,
+-porderId,
+-ppublicKey,
+-psecretKey</t>
+  </si>
+  <si>
+    <t>test checkOut Cancel Transaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.checkout.tests.CheckOutTest,
+tesCheckOutCancelTransaction,
+-pdomain,
+-ppublicKey,
+-psecretKey,
+-pemail,
+-ppassword,
+-pheading,
+-pcode,
+-pcancelHeading,
+-pcontent,
+-pcheckOutContent
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">coyni.checkout.tests.CheckOutTest,
 tesCheckOutTransaction,
 -pdomain,
--porderId,
 -ppublicKey,
--psecretKey
+-psecretKey,
+-pemail,
+-ppassword,
+-pheading,
+-pcode,
+-psuccessContent,
+-pinsufficient,
+-pcvv,
+-pamount,
+-pnameOnCard,
+-pcardNumber,
+-pcardType,
+-pcardExpiry,
+-pcvvNumber,
+-paddressLine1,
+-paddressLine2,
+-pcity,
+-pzipCode,
+-pstate,
+-pcountry,
+-ppreamount
 </t>
-  </si>
-  <si>
-    <t>Verify Check Out Transaction</t>
   </si>
 </sst>
 </file>
@@ -1576,10 +1624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3940,7 +3988,7 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="390" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>215</v>
       </c>
@@ -3960,14 +4008,72 @@
         <v>128</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="I81" s="11"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
+    </row>
+    <row r="82" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I82" s="11"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+    </row>
+    <row r="83" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="I83" s="11"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Added test script in System setting and Change the method in disputes
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(13-09-2022)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Code-push\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CF479B-9077-4DA6-93CD-31C34CF191C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CC4B34-4261-437D-B1A7-4F63DCFC40B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$94</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="253">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1332,9 +1332,6 @@
 -pdisputesExportsStatusCaseID</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>testTransactionSearch</t>
   </si>
   <si>
@@ -1344,6 +1341,34 @@
     <t>coyni.admin.tests.TransactionTest,
 testTransactionSearch,
 -pdata</t>
+  </si>
+  <si>
+    <t>verify fee struture status active to sheduled</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.SystemSettingsTest,
+testFeeStructuresActiveToSheduled,
+-pdebitAmnt,
+-pselectDate,
+-psuccess,
+-pmessage</t>
+  </si>
+  <si>
+    <t>verify accountLimits status active to sheduled</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.SystemSettingsTest,
+testAccountLimitsActiveToSheduled,
+-pdebitAmnt,
+-pselectDate,
+-psuccess,
+-pmessage</t>
+  </si>
+  <si>
+    <t>AccountLimit - shedule</t>
   </si>
 </sst>
 </file>
@@ -1723,10 +1748,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:M92"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2761,12 +2786,12 @@
       </c>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>244</v>
+        <v>68</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>55</v>
@@ -2781,13 +2806,13 @@
         <v>126</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J37" s="1"/>
     </row>
@@ -3623,16 +3648,16 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C65" s="1" t="s">
+      <c r="A65" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C65" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E65" s="5" t="s">
@@ -3641,19 +3666,19 @@
       <c r="F65" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G65" s="1" t="s">
+      <c r="G65" s="7" t="s">
         <v>92</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>89</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>93</v>
+        <v>249</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>68</v>
@@ -3671,18 +3696,18 @@
         <v>126</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>89</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>68</v>
@@ -3706,12 +3731,12 @@
         <v>89</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>97</v>
+        <v>153</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>68</v>
@@ -3729,24 +3754,24 @@
         <v>126</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>89</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -3764,18 +3789,18 @@
         <v>89</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -3787,18 +3812,18 @@
         <v>126</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>89</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>68</v>
@@ -3822,18 +3847,18 @@
         <v>89</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>145</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>155</v>
+        <v>248</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>11</v>
@@ -3845,18 +3870,18 @@
         <v>126</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>141</v>
+        <v>252</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>89</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>68</v>
@@ -3880,12 +3905,12 @@
         <v>89</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>68</v>
@@ -3909,18 +3934,18 @@
         <v>89</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="210" hidden="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>11</v>
@@ -3932,24 +3957,24 @@
         <v>126</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>222</v>
+        <v>141</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>89</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -3961,18 +3986,18 @@
         <v>126</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>222</v>
+        <v>141</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I76" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I76" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>68</v>
@@ -3995,13 +4020,13 @@
       <c r="H77" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I77" s="8" t="s">
-        <v>169</v>
+      <c r="I77" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>68</v>
@@ -4019,18 +4044,18 @@
         <v>126</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>89</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>68</v>
@@ -4048,18 +4073,18 @@
         <v>126</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>89</v>
       </c>
       <c r="I79" s="8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>68</v>
@@ -4083,12 +4108,12 @@
         <v>89</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>68</v>
@@ -4112,79 +4137,76 @@
         <v>89</v>
       </c>
       <c r="I81" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="135" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I82" s="8" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="180" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:11" ht="135" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I83" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="180" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C82" s="1" t="s">
+      <c r="B84" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="J82" s="1"/>
-      <c r="K82" s="1"/>
-    </row>
-    <row r="83" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="J83" s="2"/>
-    </row>
-    <row r="84" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>11</v>
@@ -4202,13 +4224,14 @@
         <v>22</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="J84" s="2"/>
-    </row>
-    <row r="85" spans="1:11" ht="195" hidden="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+    </row>
+    <row r="85" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>68</v>
@@ -4232,73 +4255,75 @@
         <v>22</v>
       </c>
       <c r="I85" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J85" s="2"/>
+    </row>
+    <row r="86" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I86" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="J85" s="6" t="s">
+      <c r="J86" s="2"/>
+    </row>
+    <row r="87" spans="1:11" ht="195" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="J87" s="6" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="390" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="88" spans="1:11" ht="390" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I86" s="11"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
-    </row>
-    <row r="87" spans="1:11" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="I87" s="11"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
-    </row>
-    <row r="88" spans="1:11" ht="195" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>68</v>
@@ -4319,15 +4344,15 @@
         <v>211</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I88" s="11"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>68</v>
@@ -4348,21 +4373,21 @@
         <v>211</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I89" s="11"/>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>11</v>
@@ -4374,26 +4399,24 @@
         <v>126</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>227</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="I90" s="11"/>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -4405,20 +4428,18 @@
         <v>126</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>230</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="I91" s="11"/>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
     <row r="92" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>68</v>
@@ -4436,22 +4457,84 @@
         <v>126</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
+    <row r="93" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+    </row>
+    <row r="94" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I92" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
+  <autoFilter ref="A1:I94" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="6">
       <filters>
-        <filter val="Yes"/>
+        <filter val="AccountLimit"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
modified the test methods
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Code-push\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA34D05-8073-4041-A884-228AFF92CDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645483C3-61BE-410B-B4B5-8D79D76484FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1731,11 +1731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +1779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1832,7 +1831,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>188</v>
       </c>
@@ -1858,7 +1857,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1884,7 +1883,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="210.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="210.75" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1936,7 +1935,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>214</v>
       </c>
@@ -1962,7 +1961,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -1988,7 +1987,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="255" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -2014,7 +2013,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -2040,7 +2039,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
@@ -2066,7 +2065,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -2092,7 +2091,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>173</v>
       </c>
@@ -2151,7 +2150,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>177</v>
       </c>
@@ -2184,7 +2183,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>180</v>
       </c>
@@ -2217,7 +2216,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>200</v>
       </c>
@@ -2250,7 +2249,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -2305,7 +2304,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -2334,7 +2333,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -2363,7 +2362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="255" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>50</v>
       </c>
@@ -2392,7 +2391,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>158</v>
       </c>
@@ -2421,7 +2420,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -2450,7 +2449,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="270" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
@@ -2479,7 +2478,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>194</v>
       </c>
@@ -2508,7 +2507,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>108</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>108</v>
       </c>
@@ -2566,7 +2565,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>127</v>
       </c>
@@ -2595,7 +2594,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>129</v>
       </c>
@@ -2624,7 +2623,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>131</v>
       </c>
@@ -2653,7 +2652,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>133</v>
       </c>
@@ -2682,7 +2681,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>135</v>
       </c>
@@ -2711,7 +2710,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>137</v>
       </c>
@@ -2740,7 +2739,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>54</v>
       </c>
@@ -2770,7 +2769,7 @@
       </c>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>239</v>
       </c>
@@ -2800,7 +2799,7 @@
       </c>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>57</v>
       </c>
@@ -2830,7 +2829,7 @@
       </c>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
@@ -2860,7 +2859,7 @@
       </c>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
@@ -2890,7 +2889,7 @@
       </c>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
@@ -2920,7 +2919,7 @@
       </c>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -2950,7 +2949,7 @@
       </c>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
@@ -2981,7 +2980,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>71</v>
       </c>
@@ -3012,7 +3011,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>73</v>
       </c>
@@ -3043,7 +3042,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>75</v>
       </c>
@@ -3074,7 +3073,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>77</v>
       </c>
@@ -3105,7 +3104,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>79</v>
       </c>
@@ -3136,7 +3135,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>82</v>
       </c>
@@ -3167,7 +3166,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>183</v>
       </c>
@@ -3198,7 +3197,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>84</v>
       </c>
@@ -3229,7 +3228,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>191</v>
       </c>
@@ -3260,7 +3259,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>197</v>
       </c>
@@ -3291,7 +3290,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>111</v>
       </c>
@@ -3323,7 +3322,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>114</v>
       </c>
@@ -3355,7 +3354,7 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
     </row>
-    <row r="56" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>116</v>
       </c>
@@ -3387,7 +3386,7 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>118</v>
       </c>
@@ -3419,7 +3418,7 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
     </row>
-    <row r="58" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>120</v>
       </c>
@@ -3451,7 +3450,7 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>122</v>
       </c>
@@ -3483,7 +3482,7 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>124</v>
       </c>
@@ -3515,7 +3514,7 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>230</v>
       </c>
@@ -3544,7 +3543,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>150</v>
       </c>
@@ -3573,7 +3572,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>106</v>
       </c>
@@ -3602,7 +3601,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>86</v>
       </c>
@@ -3631,7 +3630,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>242</v>
       </c>
@@ -3660,7 +3659,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>91</v>
       </c>
@@ -3689,7 +3688,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>94</v>
       </c>
@@ -3718,7 +3717,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>96</v>
       </c>
@@ -3747,7 +3746,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>98</v>
       </c>
@@ -3776,7 +3775,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>100</v>
       </c>
@@ -3805,7 +3804,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>144</v>
       </c>
@@ -3834,7 +3833,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>245</v>
       </c>
@@ -3863,7 +3862,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>142</v>
       </c>
@@ -3892,7 +3891,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>143</v>
       </c>
@@ -4008,7 +4007,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>165</v>
       </c>
@@ -4037,7 +4036,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>169</v>
       </c>
@@ -4066,7 +4065,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>171</v>
       </c>
@@ -4095,7 +4094,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>171</v>
       </c>
@@ -4124,7 +4123,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>185</v>
       </c>
@@ -4155,7 +4154,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>232</v>
       </c>
@@ -4185,7 +4184,7 @@
       </c>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>235</v>
       </c>
@@ -4215,7 +4214,7 @@
       </c>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:11" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>237</v>
       </c>
@@ -4247,7 +4246,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="390" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="390" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>204</v>
       </c>
@@ -4276,7 +4275,7 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" spans="1:11" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>207</v>
       </c>
@@ -4305,7 +4304,7 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="1:11" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>209</v>
       </c>
@@ -4334,7 +4333,7 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>212</v>
       </c>
@@ -4363,7 +4362,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>219</v>
       </c>
@@ -4394,7 +4393,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>223</v>
       </c>
@@ -4425,7 +4424,7 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>226</v>
       </c>
@@ -4457,13 +4456,7 @@
       <c r="K92" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I92" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Profile Api Business"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I92" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Admin Test Script and test data
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ideyaLabs\git\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2022\101222_Web\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A1A142-160C-4952-B3EA-F67D86C93736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E54CDA-AE75-4612-BFA7-1EFBB90B7F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="290">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1597,6 +1597,9 @@
   <si>
     <t>coyni.admin.tests.UnderWritingTest,
 testIdentifivericationSuccesfull</t>
+  </si>
+  <si>
+    <t>testData-admin.xlsx,profilesIndividuals</t>
   </si>
 </sst>
 </file>
@@ -1977,8 +1980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100:XFD100"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4681,7 +4684,7 @@
         <v>68</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>11</v>
@@ -4710,7 +4713,7 @@
         <v>68</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>11</v>
@@ -4739,7 +4742,7 @@
         <v>68</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>11</v>
@@ -4768,7 +4771,7 @@
         <v>68</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>11</v>
@@ -4797,7 +4800,7 @@
         <v>68</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -4826,7 +4829,7 @@
         <v>68</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
@@ -4855,7 +4858,7 @@
         <v>68</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>11</v>
@@ -4884,7 +4887,7 @@
         <v>68</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>11</v>
@@ -4913,7 +4916,7 @@
         <v>68</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>11</v>
@@ -4942,7 +4945,7 @@
         <v>68</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>11</v>
@@ -4971,7 +4974,7 @@
         <v>68</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -5000,7 +5003,7 @@
         <v>68</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>11</v>
@@ -5029,7 +5032,7 @@
         <v>68</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>166</v>
+        <v>289</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
added test data and test Script
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(20-10-2022)RegressionTestData and test Script\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24575901-B5DA-4895-ABA3-F36FEEA48640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA30316-6A66-4123-8AA9-DA83E5A1AC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1423,16 +1423,6 @@
 -pconfirmPassword</t>
   </si>
   <si>
-    <t>coyni.admin.tests.HomeTest,
-testUserDetailsChangePasswordInvalidCredentials,
--pcode,
--p-psecurityKey,
--pcurrentPassword,
--pnewPassword,
--pconfirmPassword,
--perrMessage</t>
-  </si>
-  <si>
     <t>coyni.admin.tests.LoginTest,
 testAdminLogin,
 -ploginHeading,
@@ -1511,6 +1501,16 @@
 -pcode,
 -pmessage,
 -psecurityKey</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.HomeTest,
+testUserDetailsChangePasswordInvalidCredentials,
+-pcode,
+-psecurityKey,
+-pcurrentPassword,
+-pnewPassword,
+-pconfirmPassword,
+-perrMessage</t>
   </si>
 </sst>
 </file>
@@ -1886,11 +1886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,7 +1934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1958,10 +1957,10 @@
         <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1987,7 +1986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>179</v>
       </c>
@@ -2013,7 +2012,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -2039,7 +2038,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="210.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="210.75" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -2065,7 +2064,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -2091,7 +2090,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -2143,7 +2142,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -2169,7 +2168,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -2195,7 +2194,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -2221,7 +2220,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -2247,7 +2246,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>167</v>
       </c>
@@ -2280,7 +2279,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>169</v>
       </c>
@@ -2306,14 +2305,14 @@
         <v>268</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>171</v>
       </c>
@@ -2346,7 +2345,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>191</v>
       </c>
@@ -2379,7 +2378,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2405,7 +2404,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2434,7 +2433,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2463,7 +2462,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -2486,13 +2485,13 @@
         <v>25</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="270" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>47</v>
       </c>
@@ -2515,13 +2514,13 @@
         <v>48</v>
       </c>
       <c r="H22" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>152</v>
       </c>
@@ -2544,13 +2543,13 @@
         <v>48</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -2573,13 +2572,13 @@
         <v>48</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="285" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
@@ -2602,13 +2601,13 @@
         <v>48</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>185</v>
       </c>
@@ -2631,13 +2630,13 @@
         <v>186</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I26" s="11" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>104</v>
       </c>
@@ -2660,13 +2659,13 @@
         <v>105</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>104</v>
       </c>
@@ -2689,13 +2688,13 @@
         <v>105</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>123</v>
       </c>
@@ -2718,13 +2717,13 @@
         <v>105</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>125</v>
       </c>
@@ -2747,13 +2746,13 @@
         <v>105</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>127</v>
       </c>
@@ -2776,13 +2775,13 @@
         <v>105</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>129</v>
       </c>
@@ -2805,13 +2804,13 @@
         <v>105</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>131</v>
       </c>
@@ -2834,13 +2833,13 @@
         <v>105</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>133</v>
       </c>
@@ -2863,13 +2862,13 @@
         <v>105</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>51</v>
       </c>
@@ -2892,14 +2891,14 @@
         <v>196</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>53</v>
       </c>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>218</v>
       </c>
@@ -2922,14 +2921,14 @@
         <v>219</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>220</v>
       </c>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>54</v>
       </c>
@@ -2952,14 +2951,14 @@
         <v>196</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>55</v>
       </c>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>56</v>
       </c>
@@ -2982,14 +2981,14 @@
         <v>196</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>57</v>
       </c>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>58</v>
       </c>
@@ -3012,14 +3011,14 @@
         <v>196</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>59</v>
       </c>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>60</v>
       </c>
@@ -3042,14 +3041,14 @@
         <v>196</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>61</v>
       </c>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>62</v>
       </c>
@@ -3072,14 +3071,14 @@
         <v>196</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>63</v>
       </c>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>67</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>181</v>
@@ -3110,7 +3109,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>68</v>
       </c>
@@ -3133,7 +3132,7 @@
         <v>67</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>69</v>
@@ -3141,7 +3140,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>70</v>
       </c>
@@ -3164,7 +3163,7 @@
         <v>67</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>71</v>
@@ -3172,7 +3171,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>72</v>
       </c>
@@ -3195,7 +3194,7 @@
         <v>67</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>73</v>
@@ -3203,7 +3202,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>74</v>
       </c>
@@ -3226,7 +3225,7 @@
         <v>67</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>75</v>
@@ -3234,7 +3233,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>76</v>
       </c>
@@ -3257,7 +3256,7 @@
         <v>77</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>78</v>
@@ -3265,7 +3264,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>79</v>
       </c>
@@ -3288,7 +3287,7 @@
         <v>77</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>80</v>
@@ -3296,7 +3295,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>174</v>
       </c>
@@ -3319,7 +3318,7 @@
         <v>67</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>175</v>
@@ -3327,7 +3326,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>81</v>
       </c>
@@ -3350,7 +3349,7 @@
         <v>77</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>82</v>
@@ -3358,7 +3357,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>182</v>
       </c>
@@ -3381,7 +3380,7 @@
         <v>183</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I51" s="11" t="s">
         <v>184</v>
@@ -3389,7 +3388,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>188</v>
       </c>
@@ -3412,7 +3411,7 @@
         <v>189</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I52" s="11" t="s">
         <v>190</v>
@@ -3420,7 +3419,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>107</v>
       </c>
@@ -3443,7 +3442,7 @@
         <v>195</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>109</v>
@@ -3452,7 +3451,7 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
     </row>
-    <row r="54" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>110</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>195</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>111</v>
@@ -3484,7 +3483,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>112</v>
       </c>
@@ -3507,7 +3506,7 @@
         <v>195</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>113</v>
@@ -3516,7 +3515,7 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
     </row>
-    <row r="56" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>114</v>
       </c>
@@ -3539,7 +3538,7 @@
         <v>195</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>115</v>
@@ -3548,7 +3547,7 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>116</v>
       </c>
@@ -3571,7 +3570,7 @@
         <v>195</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>117</v>
@@ -3580,7 +3579,7 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
     </row>
-    <row r="58" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>118</v>
       </c>
@@ -3603,7 +3602,7 @@
         <v>195</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>119</v>
@@ -3612,7 +3611,7 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>120</v>
       </c>
@@ -3635,7 +3634,7 @@
         <v>195</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>121</v>
@@ -3644,7 +3643,7 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>209</v>
       </c>
@@ -3667,13 +3666,13 @@
         <v>100</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>146</v>
       </c>
@@ -3696,13 +3695,13 @@
         <v>100</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>102</v>
       </c>
@@ -3725,13 +3724,13 @@
         <v>100</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>83</v>
       </c>
@@ -3754,13 +3753,13 @@
         <v>85</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>221</v>
       </c>
@@ -3783,13 +3782,13 @@
         <v>88</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>87</v>
       </c>
@@ -3812,13 +3811,13 @@
         <v>88</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>90</v>
       </c>
@@ -3841,13 +3840,13 @@
         <v>91</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>92</v>
       </c>
@@ -3870,13 +3869,13 @@
         <v>91</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>94</v>
       </c>
@@ -3899,13 +3898,13 @@
         <v>88</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>96</v>
       </c>
@@ -3928,13 +3927,13 @@
         <v>88</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>140</v>
       </c>
@@ -3957,13 +3956,13 @@
         <v>137</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="141.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>223</v>
       </c>
@@ -3986,13 +3985,13 @@
         <v>225</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>138</v>
       </c>
@@ -4015,13 +4014,13 @@
         <v>137</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>139</v>
       </c>
@@ -4044,13 +4043,13 @@
         <v>137</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>154</v>
       </c>
@@ -4073,13 +4072,13 @@
         <v>197</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>156</v>
       </c>
@@ -4102,13 +4101,13 @@
         <v>197</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I75" s="8" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>157</v>
       </c>
@@ -4131,7 +4130,7 @@
         <v>197</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I76" s="8" t="s">
         <v>158</v>
@@ -4160,7 +4159,7 @@
         <v>161</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I77" s="8" t="s">
         <v>162</v>
@@ -4189,7 +4188,7 @@
         <v>161</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I78" s="8" t="s">
         <v>164</v>
@@ -4218,7 +4217,7 @@
         <v>161</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I79" s="8" t="s">
         <v>166</v>
@@ -4247,13 +4246,13 @@
         <v>161</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I80" s="8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>176</v>
       </c>
@@ -4276,7 +4275,7 @@
         <v>210</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>178</v>
@@ -4284,7 +4283,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>211</v>
       </c>
@@ -4307,14 +4306,14 @@
         <v>210</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>213</v>
       </c>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:11" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>214</v>
       </c>
@@ -4337,14 +4336,14 @@
         <v>210</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>215</v>
       </c>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>216</v>
       </c>
@@ -4367,7 +4366,7 @@
         <v>210</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>215</v>
@@ -4376,7 +4375,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>198</v>
       </c>
@@ -4399,7 +4398,7 @@
         <v>199</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>201</v>
@@ -4407,7 +4406,7 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>202</v>
       </c>
@@ -4430,7 +4429,7 @@
         <v>203</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>204</v>
@@ -4438,7 +4437,7 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" spans="1:11" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>205</v>
       </c>
@@ -4461,7 +4460,7 @@
         <v>206</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>207</v>
@@ -4492,7 +4491,7 @@
         <v>161</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I88" s="8" t="s">
         <v>244</v>
@@ -4521,7 +4520,7 @@
         <v>161</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I89" s="8" t="s">
         <v>245</v>
@@ -4550,7 +4549,7 @@
         <v>161</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I90" s="8" t="s">
         <v>246</v>
@@ -4579,7 +4578,7 @@
         <v>161</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I91" s="8" t="s">
         <v>247</v>
@@ -4608,7 +4607,7 @@
         <v>161</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I92" s="8" t="s">
         <v>248</v>
@@ -4637,7 +4636,7 @@
         <v>161</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I93" s="8" t="s">
         <v>249</v>
@@ -4666,7 +4665,7 @@
         <v>161</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I94" s="8" t="s">
         <v>250</v>
@@ -4695,7 +4694,7 @@
         <v>161</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I95" s="8" t="s">
         <v>251</v>
@@ -4724,7 +4723,7 @@
         <v>161</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I96" s="8" t="s">
         <v>252</v>
@@ -4753,7 +4752,7 @@
         <v>161</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I97" s="8" t="s">
         <v>253</v>
@@ -4782,7 +4781,7 @@
         <v>161</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I98" s="8" t="s">
         <v>254</v>
@@ -4811,7 +4810,7 @@
         <v>161</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I99" s="8" t="s">
         <v>255</v>
@@ -4840,13 +4839,13 @@
         <v>161</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I100" s="8" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="300" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>240</v>
       </c>
@@ -4873,7 +4872,7 @@
       </c>
       <c r="I101" s="8"/>
     </row>
-    <row r="102" spans="1:14" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>242</v>
       </c>
@@ -4896,7 +4895,7 @@
         <v>267</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I102" s="8" t="s">
         <v>258</v>
@@ -4908,7 +4907,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>243</v>
       </c>
@@ -4953,13 +4952,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I103" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Individuals"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I103" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes the elements and changed the report status to Crypto - mobile to coyni web
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\En-Auto-new(11-11-2-2022)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174EFDCF-4255-443F-9E18-AD1522E07C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B92F31-9CBA-476C-879E-BBC91BFB51E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$106</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1337,15 +1337,6 @@
 -pauthyDescription,
 -pcode,
 -psecurityKey</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.HomeTest,
-testUserDetailsChangePasswordWithValid,
--pcode,
--psecurityKey,
--pcurrentPassword,
--pnewPassword,
--pconfirmPassword</t>
   </si>
   <si>
     <t>coyni.admin.tests.LoginTest,
@@ -1635,6 +1626,16 @@
 -ploginDescription,
 -pemail,
 -ppassword,
+-pattribute</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.HomeTest,
+testUserDetailsChangePasswordWithValid,
+-pcode,
+-psecurityKey,
+-pcurrentPassword,
+-pnewPassword,
+-pconfirmPassword,
 -pattribute</t>
   </si>
 </sst>
@@ -2053,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,7 +2110,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -2127,15 +2128,15 @@
         <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -2147,13 +2148,13 @@
         <v>114</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2161,7 +2162,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -2187,7 +2188,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -2205,7 +2206,7 @@
         <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2213,7 +2214,7 @@
         <v>167</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
@@ -2239,7 +2240,7 @@
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
@@ -2265,7 +2266,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
@@ -2291,7 +2292,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
@@ -2317,7 +2318,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
@@ -2343,7 +2344,7 @@
         <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>36</v>
@@ -2369,7 +2370,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>36</v>
@@ -2395,7 +2396,7 @@
         <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>36</v>
@@ -2421,7 +2422,7 @@
         <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>36</v>
@@ -2447,7 +2448,7 @@
         <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>36</v>
@@ -2473,7 +2474,7 @@
         <v>155</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>158</v>
@@ -2494,7 +2495,7 @@
         <v>250</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>251</v>
+        <v>285</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -2506,7 +2507,7 @@
         <v>157</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>158</v>
@@ -2527,7 +2528,7 @@
         <v>250</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -2539,7 +2540,7 @@
         <v>159</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>160</v>
@@ -2572,7 +2573,7 @@
         <v>179</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>160</v>
@@ -2605,7 +2606,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>10</v>
@@ -2631,7 +2632,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
@@ -2660,7 +2661,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -2689,7 +2690,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>18</v>
@@ -2707,7 +2708,7 @@
         <v>25</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>26</v>
@@ -2715,13 +2716,13 @@
     </row>
     <row r="24" spans="1:13" ht="270" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>11</v>
@@ -2733,24 +2734,24 @@
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>14</v>
@@ -2762,24 +2763,24 @@
         <v>2</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>11</v>
@@ -2791,24 +2792,24 @@
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="285" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>14</v>
@@ -2820,13 +2821,13 @@
         <v>135</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="23" customFormat="1" ht="165" x14ac:dyDescent="0.25">
@@ -2834,7 +2835,7 @@
         <v>173</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C28" s="19" t="s">
         <v>18</v>
@@ -2852,7 +2853,7 @@
         <v>174</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I28" s="22" t="s">
         <v>175</v>
@@ -2863,7 +2864,7 @@
         <v>96</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>18</v>
@@ -2881,7 +2882,7 @@
         <v>97</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>98</v>
@@ -2892,7 +2893,7 @@
         <v>115</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>18</v>
@@ -2910,7 +2911,7 @@
         <v>97</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>116</v>
@@ -2921,7 +2922,7 @@
         <v>117</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
@@ -2939,7 +2940,7 @@
         <v>97</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>118</v>
@@ -2950,7 +2951,7 @@
         <v>119</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
@@ -2968,7 +2969,7 @@
         <v>97</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>120</v>
@@ -2979,7 +2980,7 @@
         <v>121</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>18</v>
@@ -2997,7 +2998,7 @@
         <v>97</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>122</v>
@@ -3008,7 +3009,7 @@
         <v>123</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>
@@ -3026,7 +3027,7 @@
         <v>97</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>124</v>
@@ -3037,7 +3038,7 @@
         <v>125</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>18</v>
@@ -3055,7 +3056,7 @@
         <v>97</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>126</v>
@@ -3066,7 +3067,7 @@
         <v>47</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>48</v>
@@ -3084,7 +3085,7 @@
         <v>184</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>49</v>
@@ -3096,7 +3097,7 @@
         <v>206</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>48</v>
@@ -3114,7 +3115,7 @@
         <v>207</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>208</v>
@@ -3126,7 +3127,7 @@
         <v>50</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>48</v>
@@ -3144,7 +3145,7 @@
         <v>184</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>51</v>
@@ -3156,7 +3157,7 @@
         <v>52</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>48</v>
@@ -3174,7 +3175,7 @@
         <v>184</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>53</v>
@@ -3186,7 +3187,7 @@
         <v>54</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>48</v>
@@ -3204,7 +3205,7 @@
         <v>184</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>55</v>
@@ -3216,7 +3217,7 @@
         <v>56</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>48</v>
@@ -3234,7 +3235,7 @@
         <v>184</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>57</v>
@@ -3246,7 +3247,7 @@
         <v>58</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>48</v>
@@ -3264,7 +3265,7 @@
         <v>184</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>59</v>
@@ -3276,7 +3277,7 @@
         <v>60</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>61</v>
@@ -3294,7 +3295,7 @@
         <v>62</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>169</v>
@@ -3307,7 +3308,7 @@
         <v>63</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>61</v>
@@ -3325,7 +3326,7 @@
         <v>62</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>64</v>
@@ -3338,7 +3339,7 @@
         <v>65</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>61</v>
@@ -3356,7 +3357,7 @@
         <v>62</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>66</v>
@@ -3369,7 +3370,7 @@
         <v>67</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>61</v>
@@ -3387,7 +3388,7 @@
         <v>62</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>68</v>
@@ -3400,7 +3401,7 @@
         <v>69</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>61</v>
@@ -3418,7 +3419,7 @@
         <v>62</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>70</v>
@@ -3431,7 +3432,7 @@
         <v>71</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>61</v>
@@ -3449,7 +3450,7 @@
         <v>72</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>73</v>
@@ -3462,7 +3463,7 @@
         <v>74</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>61</v>
@@ -3480,7 +3481,7 @@
         <v>72</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>75</v>
@@ -3493,7 +3494,7 @@
         <v>162</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>61</v>
@@ -3511,7 +3512,7 @@
         <v>62</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>163</v>
@@ -3524,7 +3525,7 @@
         <v>76</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>61</v>
@@ -3542,7 +3543,7 @@
         <v>72</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>77</v>
@@ -3555,7 +3556,7 @@
         <v>170</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>165</v>
@@ -3573,7 +3574,7 @@
         <v>171</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I52" s="11" t="s">
         <v>172</v>
@@ -3586,7 +3587,7 @@
         <v>176</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>165</v>
@@ -3604,7 +3605,7 @@
         <v>177</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I53" s="11" t="s">
         <v>178</v>
@@ -3617,7 +3618,7 @@
         <v>99</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>100</v>
@@ -3635,7 +3636,7 @@
         <v>183</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>101</v>
@@ -3649,7 +3650,7 @@
         <v>102</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>100</v>
@@ -3667,7 +3668,7 @@
         <v>183</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>103</v>
@@ -3681,7 +3682,7 @@
         <v>104</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>100</v>
@@ -3699,7 +3700,7 @@
         <v>183</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>105</v>
@@ -3713,7 +3714,7 @@
         <v>106</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>100</v>
@@ -3731,7 +3732,7 @@
         <v>183</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>107</v>
@@ -3745,7 +3746,7 @@
         <v>108</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>100</v>
@@ -3763,7 +3764,7 @@
         <v>183</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>109</v>
@@ -3777,7 +3778,7 @@
         <v>110</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>100</v>
@@ -3795,7 +3796,7 @@
         <v>183</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>111</v>
@@ -3809,7 +3810,7 @@
         <v>112</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>100</v>
@@ -3827,7 +3828,7 @@
         <v>183</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>113</v>
@@ -3841,7 +3842,7 @@
         <v>197</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>91</v>
@@ -3859,7 +3860,7 @@
         <v>92</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>196</v>
@@ -3870,7 +3871,7 @@
         <v>137</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>91</v>
@@ -3888,7 +3889,7 @@
         <v>92</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>93</v>
@@ -3899,7 +3900,7 @@
         <v>94</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>91</v>
@@ -3917,7 +3918,7 @@
         <v>92</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>95</v>
@@ -3928,7 +3929,7 @@
         <v>78</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>79</v>
@@ -3946,7 +3947,7 @@
         <v>80</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>81</v>
@@ -3957,7 +3958,7 @@
         <v>209</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>79</v>
@@ -3975,7 +3976,7 @@
         <v>83</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>210</v>
@@ -3986,7 +3987,7 @@
         <v>82</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>79</v>
@@ -4004,7 +4005,7 @@
         <v>83</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>84</v>
@@ -4015,7 +4016,7 @@
         <v>85</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>79</v>
@@ -4033,7 +4034,7 @@
         <v>86</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>136</v>
@@ -4044,7 +4045,7 @@
         <v>87</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>79</v>
@@ -4062,7 +4063,7 @@
         <v>86</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>88</v>
@@ -4073,7 +4074,7 @@
         <v>89</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>79</v>
@@ -4091,7 +4092,7 @@
         <v>83</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>90</v>
@@ -4102,7 +4103,7 @@
         <v>132</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>138</v>
@@ -4120,7 +4121,7 @@
         <v>129</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>139</v>
@@ -4131,7 +4132,7 @@
         <v>211</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>79</v>
@@ -4149,7 +4150,7 @@
         <v>213</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>212</v>
@@ -4160,7 +4161,7 @@
         <v>130</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>138</v>
@@ -4178,7 +4179,7 @@
         <v>129</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>141</v>
@@ -4189,7 +4190,7 @@
         <v>131</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>138</v>
@@ -4207,7 +4208,7 @@
         <v>129</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>140</v>
@@ -4218,7 +4219,7 @@
         <v>142</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C74" s="12" t="s">
         <v>148</v>
@@ -4236,7 +4237,7 @@
         <v>185</v>
       </c>
       <c r="H74" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I74" s="16" t="s">
         <v>143</v>
@@ -4247,7 +4248,7 @@
         <v>144</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>148</v>
@@ -4265,7 +4266,7 @@
         <v>185</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I75" s="8" t="s">
         <v>214</v>
@@ -4276,7 +4277,7 @@
         <v>145</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>148</v>
@@ -4294,7 +4295,7 @@
         <v>185</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I76" s="8" t="s">
         <v>146</v>
@@ -4305,7 +4306,7 @@
         <v>147</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>148</v>
@@ -4323,7 +4324,7 @@
         <v>149</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I77" s="8" t="s">
         <v>150</v>
@@ -4334,7 +4335,7 @@
         <v>151</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>148</v>
@@ -4352,7 +4353,7 @@
         <v>149</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I78" s="8" t="s">
         <v>152</v>
@@ -4363,7 +4364,7 @@
         <v>153</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>148</v>
@@ -4381,7 +4382,7 @@
         <v>149</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I79" s="8" t="s">
         <v>154</v>
@@ -4392,7 +4393,7 @@
         <v>153</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>148</v>
@@ -4410,7 +4411,7 @@
         <v>149</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I80" s="8" t="s">
         <v>154</v>
@@ -4421,7 +4422,7 @@
         <v>164</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>165</v>
@@ -4439,7 +4440,7 @@
         <v>198</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>166</v>
@@ -4452,7 +4453,7 @@
         <v>199</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>200</v>
@@ -4470,7 +4471,7 @@
         <v>198</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>201</v>
@@ -4482,7 +4483,7 @@
         <v>202</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>200</v>
@@ -4500,7 +4501,7 @@
         <v>198</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>203</v>
@@ -4512,7 +4513,7 @@
         <v>204</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>200</v>
@@ -4530,7 +4531,7 @@
         <v>198</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>203</v>
@@ -4544,7 +4545,7 @@
         <v>186</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>188</v>
@@ -4562,7 +4563,7 @@
         <v>187</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>189</v>
@@ -4575,7 +4576,7 @@
         <v>190</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>188</v>
@@ -4593,7 +4594,7 @@
         <v>191</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>192</v>
@@ -4606,7 +4607,7 @@
         <v>193</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>188</v>
@@ -4624,7 +4625,7 @@
         <v>194</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>195</v>
@@ -4637,7 +4638,7 @@
         <v>215</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>248</v>
@@ -4655,7 +4656,7 @@
         <v>149</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I88" s="8" t="s">
         <v>229</v>
@@ -4666,7 +4667,7 @@
         <v>216</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>248</v>
@@ -4684,7 +4685,7 @@
         <v>149</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I89" s="8" t="s">
         <v>230</v>
@@ -4695,7 +4696,7 @@
         <v>217</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>248</v>
@@ -4713,7 +4714,7 @@
         <v>149</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I90" s="8" t="s">
         <v>231</v>
@@ -4724,7 +4725,7 @@
         <v>218</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>248</v>
@@ -4742,7 +4743,7 @@
         <v>149</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I91" s="8" t="s">
         <v>232</v>
@@ -4753,7 +4754,7 @@
         <v>219</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>248</v>
@@ -4771,7 +4772,7 @@
         <v>149</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I92" s="8" t="s">
         <v>233</v>
@@ -4782,7 +4783,7 @@
         <v>220</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>248</v>
@@ -4800,7 +4801,7 @@
         <v>149</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I93" s="8" t="s">
         <v>234</v>
@@ -4811,7 +4812,7 @@
         <v>221</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>248</v>
@@ -4829,7 +4830,7 @@
         <v>149</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I94" s="8" t="s">
         <v>235</v>
@@ -4840,7 +4841,7 @@
         <v>222</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>248</v>
@@ -4858,7 +4859,7 @@
         <v>149</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I95" s="8" t="s">
         <v>236</v>
@@ -4869,7 +4870,7 @@
         <v>223</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>248</v>
@@ -4887,7 +4888,7 @@
         <v>149</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I96" s="8" t="s">
         <v>237</v>
@@ -4898,7 +4899,7 @@
         <v>224</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>248</v>
@@ -4916,7 +4917,7 @@
         <v>149</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I97" s="8" t="s">
         <v>238</v>
@@ -4927,7 +4928,7 @@
         <v>225</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>226</v>
@@ -4945,7 +4946,7 @@
         <v>249</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>239</v>
@@ -4956,7 +4957,7 @@
         <v>227</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>226</v>
@@ -4974,7 +4975,7 @@
         <v>249</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I99" s="8" t="s">
         <v>240</v>
@@ -4991,7 +4992,7 @@
         <v>228</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>226</v>
@@ -5032,13 +5033,13 @@
     </row>
     <row r="101" spans="1:14" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>255</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C101" t="s">
         <v>256</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C101" t="s">
-        <v>257</v>
       </c>
       <c r="D101" t="s">
         <v>11</v>
@@ -5050,24 +5051,24 @@
         <v>1</v>
       </c>
       <c r="G101" t="s">
+        <v>257</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="I101" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="H101" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="I101" s="6" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="102" spans="1:14" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C102" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D102" t="s">
         <v>11</v>
@@ -5079,24 +5080,24 @@
         <v>1</v>
       </c>
       <c r="G102" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H102" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I102" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="103" spans="1:14" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C103" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D103" t="s">
         <v>11</v>
@@ -5108,24 +5109,24 @@
         <v>1</v>
       </c>
       <c r="G103" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I103" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" spans="1:14" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D104" s="24" t="s">
         <v>11</v>
@@ -5140,18 +5141,18 @@
         <v>249</v>
       </c>
       <c r="H104" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I104" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="105" spans="1:14" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>226</v>
@@ -5169,24 +5170,24 @@
         <v>249</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I105" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J105" s="6" t="s">
         <v>241</v>
       </c>
       <c r="K105" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="106" spans="1:14" ht="300" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>226</v>
@@ -5226,7 +5227,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I103" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I106" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Verify coyni portal headings
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(17-11-2022)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\automation\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99A6D2E-5D11-41ED-A0DC-862D0F162F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B06FD1A-54FF-4029-88DE-766764DF40A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,13 +105,6 @@
   </si>
   <si>
     <t>Coyni Portal</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.CoyniPortalTest,
-testCoyniPortal,
--pcssProp,
--pexpValue,
--pexpColor</t>
   </si>
   <si>
     <t>verify TopBar</t>
@@ -1647,9 +1640,6 @@
 </t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>coyni.admin.tests.LoginTest,
 testForgotPassword,
 -ploginHeading,
@@ -1666,6 +1656,17 @@
 -psuccessHeading,
 -psuccessDescription,
 -pattribute</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.CoyniPortalTest,
+testCoyniPortal,
+-pcssProp,
+-pexpValue,
+-pexpColor,
+-pheadings</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -2080,8 +2081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,7 +2137,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -2145,24 +2146,24 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -2171,16 +2172,16 @@
         <v>14</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2188,7 +2189,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -2197,10 +2198,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>12</v>
@@ -2214,7 +2215,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -2223,24 +2224,24 @@
         <v>14</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
@@ -2249,24 +2250,24 @@
         <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
@@ -2275,183 +2276,183 @@
         <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="210.75" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>14</v>
@@ -2463,21 +2464,21 @@
         <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -2489,21 +2490,21 @@
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
@@ -2515,18 +2516,18 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>10</v>
@@ -2535,48 +2536,48 @@
         <v>11</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="17" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
@@ -2585,31 +2586,31 @@
     </row>
     <row r="19" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -2618,31 +2619,31 @@
     </row>
     <row r="20" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -2651,31 +2652,31 @@
     </row>
     <row r="21" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -2687,7 +2688,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>10</v>
@@ -2696,16 +2697,16 @@
         <v>11</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="135" x14ac:dyDescent="0.25">
@@ -2713,7 +2714,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>18</v>
@@ -2722,27 +2723,27 @@
         <v>11</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>20</v>
+        <v>289</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
@@ -2751,27 +2752,27 @@
         <v>11</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>18</v>
@@ -2780,30 +2781,30 @@
         <v>11</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="270" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>11</v>
@@ -2815,24 +2816,24 @@
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>14</v>
@@ -2844,24 +2845,24 @@
         <v>2</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>11</v>
@@ -2873,50 +2874,50 @@
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="285" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>134</v>
-      </c>
       <c r="G29" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="23" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C30" s="19" t="s">
         <v>18</v>
@@ -2925,27 +2926,27 @@
         <v>11</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G30" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="I30" s="22" t="s">
         <v>173</v>
-      </c>
-      <c r="H30" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="I30" s="22" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
@@ -2954,27 +2955,27 @@
         <v>14</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
@@ -2983,27 +2984,27 @@
         <v>14</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>18</v>
@@ -3012,27 +3013,27 @@
         <v>11</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>
@@ -3041,27 +3042,27 @@
         <v>11</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>18</v>
@@ -3070,27 +3071,27 @@
         <v>11</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>18</v>
@@ -3099,27 +3100,27 @@
         <v>11</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>18</v>
@@ -3128,599 +3129,599 @@
         <v>11</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I41" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I42" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I44" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="H45" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
     <row r="46" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I46" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
     <row r="47" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
     <row r="48" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I48" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
     <row r="49" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
     <row r="50" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G50" s="1" t="s">
+      <c r="H50" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I50" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
     <row r="51" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
     <row r="52" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I52" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
     <row r="53" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I53" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
     <row r="54" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G54" s="1" t="s">
+      <c r="H54" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I54" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I54" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G55" s="1" t="s">
+      <c r="H55" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I55" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I55" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I56" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
@@ -3728,31 +3729,31 @@
     </row>
     <row r="57" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I57" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
@@ -3760,31 +3761,31 @@
     </row>
     <row r="58" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I58" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
@@ -3792,31 +3793,31 @@
     </row>
     <row r="59" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I59" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
@@ -3824,31 +3825,31 @@
     </row>
     <row r="60" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I60" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
@@ -3856,31 +3857,31 @@
     </row>
     <row r="61" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I61" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
@@ -3888,31 +3889,31 @@
     </row>
     <row r="62" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I62" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
@@ -3920,1384 +3921,1384 @@
     </row>
     <row r="63" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="H63" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G64" s="1" t="s">
+      <c r="H64" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I64" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G66" s="1" t="s">
+      <c r="H66" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I66" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I67" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G68" s="1" t="s">
+      <c r="H68" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I68" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G69" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="H69" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I70" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I71" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I72" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I73" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="17" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F76" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="H76" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="I76" s="16" t="s">
         <v>141</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C76" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="D76" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="F76" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="H76" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="I76" s="16" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I77" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I78" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I78" s="8" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G79" s="1" t="s">
+      <c r="H79" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I79" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I79" s="8" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I80" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I80" s="8" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I81" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I81" s="8" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I82" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I82" s="8" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I83" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
     <row r="84" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I84" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="J84" s="2"/>
     </row>
     <row r="85" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I85" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="J85" s="2"/>
     </row>
     <row r="86" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="J86" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="J86" s="6" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G87" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C87" s="1" t="s">
+      <c r="H87" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I87" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
     <row r="88" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G88" s="1" t="s">
+      <c r="H88" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I88" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
     <row r="89" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G89" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G89" s="1" t="s">
+      <c r="H89" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I89" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I89" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
     <row r="90" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I91" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A92" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I92" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A93" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I93" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I94" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="96" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="300" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="D100" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I101" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="J101" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="J101" s="6" t="s">
+      <c r="K101" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="K101" s="6" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="102" spans="1:14" ht="300" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I102" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="J102" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="J102" s="6" t="s">
+      <c r="K102" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="L102" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="K102" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="L102" s="6" t="s">
+      <c r="M102" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="M102" s="6" t="s">
+      <c r="N102" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="N102" s="6" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="103" spans="1:14" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>253</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C103" t="s">
         <v>254</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G103" t="s">
         <v>255</v>
       </c>
-      <c r="D103" t="s">
-        <v>11</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G103" t="s">
+      <c r="H103" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="I103" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="H103" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="I103" s="6" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="104" spans="1:14" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>257</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C104" t="s">
+        <v>254</v>
+      </c>
+      <c r="D104" t="s">
+        <v>11</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G104" t="s">
+        <v>255</v>
+      </c>
+      <c r="H104" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="I104" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C104" t="s">
-        <v>255</v>
-      </c>
-      <c r="D104" t="s">
-        <v>11</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G104" t="s">
-        <v>256</v>
-      </c>
-      <c r="H104" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="I104" s="6" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="105" spans="1:14" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>259</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C105" t="s">
+        <v>254</v>
+      </c>
+      <c r="D105" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G105" t="s">
+        <v>255</v>
+      </c>
+      <c r="H105" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="I105" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C105" t="s">
-        <v>255</v>
-      </c>
-      <c r="D105" t="s">
-        <v>11</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F105" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G105" t="s">
-        <v>256</v>
-      </c>
-      <c r="H105" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="I105" s="6" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="106" spans="1:14" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D106" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H106" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="I106" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="B106" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D106" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E106" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F106" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="H106" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="I106" s="8" t="s">
-        <v>274</v>
-      </c>
       <c r="J106" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K106" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I107" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J107" s="6"/>
       <c r="K107" s="6"/>
     </row>
     <row r="108" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I108" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J108" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K108" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L108" s="6"/>
       <c r="M108" s="6"/>

</xml_diff>

<commit_message>
added test method in login
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\automation\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\fix-Features in Admin\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEED5B47-7BC6-42EB-AEFA-029112B65BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCED058-8B6D-4AF9-B2A3-3AD8A0771096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1561,9 +1561,6 @@
 </t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Verify Create Account Merchant with valid credentials</t>
   </si>
   <si>
@@ -1615,12 +1612,6 @@
   </si>
   <si>
     <t>verify New Verification CodeSend Upto 5Times</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.LoginTest,
-testNewCodeUpto5Times,
--pemail,
--ppassword</t>
   </si>
   <si>
     <t>testdata-admin.xlsx,SignupPageMerchant</t>
@@ -1666,7 +1657,17 @@
 -pheadings</t>
   </si>
   <si>
-    <t>yes</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.LoginTest,
+testNewCodeUpto5Times,
+-pemail,
+-ppassword,
+-pfiveTimeContent</t>
   </si>
 </sst>
 </file>
@@ -1745,7 +1746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1795,10 +1796,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2081,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,7 +2139,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -2159,11 +2161,11 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>277</v>
+      <c r="A3" s="25" t="s">
+        <v>276</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -2175,13 +2177,13 @@
         <v>113</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2189,7 +2191,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
@@ -2211,11 +2213,11 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -2233,7 +2235,7 @@
         <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2241,7 +2243,7 @@
         <v>165</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
@@ -2264,10 +2266,10 @@
     </row>
     <row r="7" spans="1:9" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
@@ -2285,7 +2287,7 @@
         <v>12</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="240" x14ac:dyDescent="0.25">
@@ -2293,7 +2295,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>27</v>
@@ -2311,7 +2313,7 @@
         <v>28</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="210.75" x14ac:dyDescent="0.3">
@@ -2319,7 +2321,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -2345,7 +2347,7 @@
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>27</v>
@@ -2371,7 +2373,7 @@
         <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
@@ -2397,7 +2399,7 @@
         <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>35</v>
@@ -2423,7 +2425,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>35</v>
@@ -2449,7 +2451,7 @@
         <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>35</v>
@@ -2475,7 +2477,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>35</v>
@@ -2501,7 +2503,7 @@
         <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>35</v>
@@ -2524,10 +2526,10 @@
     </row>
     <row r="17" spans="1:13" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>10</v>
@@ -2548,7 +2550,7 @@
         <v>251</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="17" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -2556,7 +2558,7 @@
         <v>153</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>156</v>
@@ -2577,7 +2579,7 @@
         <v>248</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
@@ -2589,7 +2591,7 @@
         <v>155</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>156</v>
@@ -2622,7 +2624,7 @@
         <v>157</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>158</v>
@@ -2655,7 +2657,7 @@
         <v>177</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>158</v>
@@ -2688,7 +2690,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>10</v>
@@ -2714,7 +2716,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>18</v>
@@ -2735,7 +2737,7 @@
         <v>248</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="135" x14ac:dyDescent="0.25">
@@ -2743,7 +2745,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
@@ -2772,7 +2774,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>18</v>
@@ -2801,7 +2803,7 @@
         <v>266</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>270</v>
@@ -2830,7 +2832,7 @@
         <v>267</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>270</v>
@@ -2859,7 +2861,7 @@
         <v>268</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>270</v>
@@ -2888,7 +2890,7 @@
         <v>269</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>270</v>
@@ -2897,7 +2899,7 @@
         <v>14</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>133</v>
@@ -2917,7 +2919,7 @@
         <v>171</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C30" s="19" t="s">
         <v>18</v>
@@ -2946,7 +2948,7 @@
         <v>95</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>18</v>
@@ -2975,7 +2977,7 @@
         <v>114</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>18</v>
@@ -3004,7 +3006,7 @@
         <v>116</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>18</v>
@@ -3033,7 +3035,7 @@
         <v>118</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>18</v>
@@ -3062,7 +3064,7 @@
         <v>120</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>18</v>
@@ -3091,7 +3093,7 @@
         <v>122</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>18</v>
@@ -3120,7 +3122,7 @@
         <v>124</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>18</v>
@@ -3149,7 +3151,7 @@
         <v>46</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>47</v>
@@ -3179,7 +3181,7 @@
         <v>204</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>47</v>
@@ -3209,7 +3211,7 @@
         <v>49</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>47</v>
@@ -3239,7 +3241,7 @@
         <v>51</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>47</v>
@@ -3269,7 +3271,7 @@
         <v>53</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>47</v>
@@ -3299,7 +3301,7 @@
         <v>55</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>47</v>
@@ -3329,7 +3331,7 @@
         <v>57</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>47</v>
@@ -3359,7 +3361,7 @@
         <v>59</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>60</v>
@@ -3390,7 +3392,7 @@
         <v>62</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>60</v>
@@ -3421,7 +3423,7 @@
         <v>64</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>60</v>
@@ -3452,7 +3454,7 @@
         <v>66</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>60</v>
@@ -3483,7 +3485,7 @@
         <v>68</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>60</v>
@@ -3514,7 +3516,7 @@
         <v>70</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>60</v>
@@ -3545,7 +3547,7 @@
         <v>73</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>60</v>
@@ -3576,7 +3578,7 @@
         <v>160</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>60</v>
@@ -3607,7 +3609,7 @@
         <v>75</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>60</v>
@@ -3638,7 +3640,7 @@
         <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>163</v>
@@ -3669,7 +3671,7 @@
         <v>174</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>163</v>
@@ -3696,11 +3698,11 @@
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="12" t="s">
         <v>98</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>99</v>
@@ -3728,11 +3730,11 @@
       <c r="L56" s="1"/>
     </row>
     <row r="57" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="12" t="s">
         <v>101</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>99</v>
@@ -3760,11 +3762,11 @@
       <c r="L57" s="1"/>
     </row>
     <row r="58" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="12" t="s">
         <v>103</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>99</v>
@@ -3792,11 +3794,11 @@
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="12" t="s">
         <v>105</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>99</v>
@@ -3824,11 +3826,11 @@
       <c r="L59" s="1"/>
     </row>
     <row r="60" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="12" t="s">
         <v>107</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>99</v>
@@ -3856,11 +3858,11 @@
       <c r="L60" s="1"/>
     </row>
     <row r="61" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="12" t="s">
         <v>109</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>99</v>
@@ -3888,11 +3890,11 @@
       <c r="L61" s="1"/>
     </row>
     <row r="62" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="12" t="s">
         <v>111</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>99</v>
@@ -3924,7 +3926,7 @@
         <v>195</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>90</v>
@@ -3953,7 +3955,7 @@
         <v>135</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>90</v>
@@ -3982,7 +3984,7 @@
         <v>93</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>90</v>
@@ -4007,11 +4009,11 @@
       </c>
     </row>
     <row r="66" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="12" t="s">
         <v>77</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>78</v>
@@ -4036,11 +4038,11 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="26" t="s">
         <v>207</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>78</v>
@@ -4065,11 +4067,11 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="12" t="s">
         <v>81</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>78</v>
@@ -4094,11 +4096,11 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="12" t="s">
         <v>84</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>78</v>
@@ -4123,11 +4125,11 @@
       </c>
     </row>
     <row r="70" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="12" t="s">
         <v>86</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>78</v>
@@ -4152,11 +4154,11 @@
       </c>
     </row>
     <row r="71" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="12" t="s">
         <v>88</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>78</v>
@@ -4181,11 +4183,11 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="12" t="s">
         <v>130</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>136</v>
@@ -4210,11 +4212,11 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="26" t="s">
         <v>209</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>78</v>
@@ -4239,11 +4241,11 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="12" t="s">
         <v>128</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>136</v>
@@ -4268,11 +4270,11 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="12" t="s">
         <v>129</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>136</v>
@@ -4301,7 +4303,7 @@
         <v>140</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>146</v>
@@ -4330,7 +4332,7 @@
         <v>142</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>146</v>
@@ -4359,7 +4361,7 @@
         <v>143</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>146</v>
@@ -4388,7 +4390,7 @@
         <v>145</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>146</v>
@@ -4417,7 +4419,7 @@
         <v>149</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>146</v>
@@ -4446,7 +4448,7 @@
         <v>151</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>146</v>
@@ -4475,7 +4477,7 @@
         <v>151</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>146</v>
@@ -4500,11 +4502,11 @@
       </c>
     </row>
     <row r="83" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="12" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>163</v>
@@ -4531,11 +4533,11 @@
       <c r="K83" s="1"/>
     </row>
     <row r="84" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="12" t="s">
         <v>197</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>198</v>
@@ -4561,11 +4563,11 @@
       <c r="J84" s="2"/>
     </row>
     <row r="85" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="12" t="s">
         <v>200</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>198</v>
@@ -4591,11 +4593,11 @@
       <c r="J85" s="2"/>
     </row>
     <row r="86" spans="1:11" ht="165" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="12" t="s">
         <v>202</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>198</v>
@@ -4627,7 +4629,7 @@
         <v>184</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>186</v>
@@ -4658,7 +4660,7 @@
         <v>188</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>186</v>
@@ -4689,7 +4691,7 @@
         <v>191</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>186</v>
@@ -4720,7 +4722,7 @@
         <v>213</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>246</v>
@@ -4749,7 +4751,7 @@
         <v>214</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>246</v>
@@ -4778,7 +4780,7 @@
         <v>215</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>246</v>
@@ -4807,7 +4809,7 @@
         <v>216</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>246</v>
@@ -4836,7 +4838,7 @@
         <v>217</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>246</v>
@@ -4865,7 +4867,7 @@
         <v>218</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>246</v>
@@ -4894,7 +4896,7 @@
         <v>219</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>246</v>
@@ -4923,7 +4925,7 @@
         <v>220</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>246</v>
@@ -4952,7 +4954,7 @@
         <v>221</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>246</v>
@@ -4981,7 +4983,7 @@
         <v>222</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>246</v>
@@ -5006,11 +5008,11 @@
       </c>
     </row>
     <row r="100" spans="1:14" ht="300" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="A100" s="12" t="s">
         <v>223</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>224</v>
@@ -5035,11 +5037,11 @@
       </c>
     </row>
     <row r="101" spans="1:14" ht="165" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="A101" s="12" t="s">
         <v>225</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>224</v>
@@ -5070,11 +5072,11 @@
       </c>
     </row>
     <row r="102" spans="1:14" ht="300" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="A102" s="12" t="s">
         <v>226</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>224</v>
@@ -5118,7 +5120,7 @@
         <v>253</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C103" t="s">
         <v>254</v>
@@ -5147,7 +5149,7 @@
         <v>257</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C104" t="s">
         <v>254</v>
@@ -5176,7 +5178,7 @@
         <v>259</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C105" t="s">
         <v>254</v>
@@ -5201,11 +5203,11 @@
       </c>
     </row>
     <row r="106" spans="1:14" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="25" t="s">
+      <c r="A106" s="27" t="s">
         <v>272</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>224</v>
@@ -5232,18 +5234,18 @@
         <v>239</v>
       </c>
       <c r="K106" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>275</v>
+      <c r="A107" s="12" t="s">
+        <v>274</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -5267,11 +5269,11 @@
       <c r="K107" s="6"/>
     </row>
     <row r="108" spans="1:14" ht="165" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>285</v>
+      <c r="A108" s="12" t="s">
+        <v>283</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>224</v>
@@ -5298,7 +5300,7 @@
         <v>239</v>
       </c>
       <c r="K108" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L108" s="6"/>
       <c r="M108" s="6"/>

</xml_diff>

<commit_message>
bug fixes in admin portal
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebAutomation\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DACB17-12BC-45BA-B0A7-392E281E6B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65EAE0F-84E5-4E19-8408-5D27F5B0CBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="10455" windowHeight="9180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$107</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="292">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1570,9 +1570,6 @@
 -ptoastMessage</t>
   </si>
   <si>
-    <t>Admin Login with invalid Authy</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -1668,6 +1665,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>tes+A28tData-admin.xlsx,AddCogentAccount</t>
+  </si>
+  <si>
+    <t>Admin Login with invalid Authy</t>
   </si>
 </sst>
 </file>
@@ -1714,7 +1717,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1730,6 +1733,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1761,7 +1770,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1807,6 +1816,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2087,10 +2097,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB108"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AB107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2145,7 +2156,7 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2191,9 +2202,9 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>276</v>
+    <row r="3" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>289</v>
@@ -2208,13 +2219,13 @@
         <v>113</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -2237,7 +2248,7 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -2283,7 +2294,7 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
@@ -2306,7 +2317,7 @@
         <v>12</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -2329,7 +2340,7 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>165</v>
       </c>
@@ -2375,15 +2386,15 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>281</v>
+    <row r="7" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>14</v>
@@ -2395,10 +2406,10 @@
         <v>113</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -2421,9 +2432,9 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="240" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
+    <row r="8" spans="1:28" ht="210.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>289</v>
@@ -2444,7 +2455,7 @@
         <v>28</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>286</v>
+        <v>126</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -2467,9 +2478,9 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="210.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>29</v>
+    <row r="9" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>289</v>
@@ -2484,13 +2495,13 @@
         <v>113</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>126</v>
+        <v>31</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
@@ -2513,9 +2524,9 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="210" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>289</v>
@@ -2530,13 +2541,13 @@
         <v>113</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -2559,18 +2570,18 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>113</v>
@@ -2579,10 +2590,10 @@
         <v>113</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -2605,9 +2616,9 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="255" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>289</v>
@@ -2628,7 +2639,7 @@
         <v>36</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -2651,9 +2662,9 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="225" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>289</v>
@@ -2662,19 +2673,19 @@
         <v>35</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>113</v>
+        <v>14</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
+        <v>3</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -2697,9 +2708,9 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="210" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>289</v>
@@ -2708,19 +2719,19 @@
         <v>35</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E14" s="6">
         <v>1</v>
       </c>
       <c r="F14" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>36</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -2743,9 +2754,9 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>289</v>
@@ -2766,7 +2777,7 @@
         <v>36</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -2789,32 +2800,34 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="195" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>283</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="6">
-        <v>1</v>
-      </c>
-      <c r="F16" s="6">
-        <v>1</v>
+      <c r="E16" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I16" s="9"/>
+        <v>251</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>284</v>
+      </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
@@ -2835,38 +2848,38 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
-    <row r="17" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>284</v>
+    <row r="17" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>12</v>
+      <c r="C17" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>154</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
       <c r="N17" s="9"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -2883,12 +2896,12 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:28" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>153</v>
+    <row r="18" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>156</v>
@@ -2900,7 +2913,7 @@
         <v>113</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>154</v>
@@ -2909,7 +2922,7 @@
         <v>248</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>279</v>
+        <v>252</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -2931,15 +2944,15 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>14</v>
@@ -2948,16 +2961,16 @@
         <v>113</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>248</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>252</v>
+        <v>179</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -2979,9 +2992,9 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
     </row>
-    <row r="20" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>289</v>
@@ -2999,13 +3012,13 @@
         <v>113</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>248</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -3027,38 +3040,36 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
     </row>
-    <row r="21" spans="1:28" ht="135" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>177</v>
+    <row r="21" spans="1:28" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>180</v>
+      <c r="C21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -3075,15 +3086,15 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>11</v>
@@ -3095,12 +3106,14 @@
         <v>113</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="8" t="s">
+        <v>286</v>
+      </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
@@ -3121,9 +3134,9 @@
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
     </row>
-    <row r="23" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>289</v>
@@ -3141,13 +3154,13 @@
         <v>113</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>248</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>287</v>
+        <v>22</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -3169,9 +3182,9 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
     </row>
-    <row r="24" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>289</v>
@@ -3188,14 +3201,14 @@
       <c r="F24" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>21</v>
+      <c r="G24" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -3217,33 +3230,33 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
     </row>
-    <row r="25" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>23</v>
+    <row r="25" spans="1:28" ht="270" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>266</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>18</v>
+        <v>270</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>24</v>
+      <c r="E25" s="6">
+        <v>1</v>
+      </c>
+      <c r="F25" s="6">
+        <v>1</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>265</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>25</v>
+        <v>261</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -3265,9 +3278,9 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
     </row>
-    <row r="26" spans="1:28" ht="270" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>266</v>
+    <row r="26" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>267</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>289</v>
@@ -3276,13 +3289,13 @@
         <v>270</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E26" s="6">
         <v>1</v>
       </c>
       <c r="F26" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>265</v>
@@ -3291,7 +3304,7 @@
         <v>249</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -3313,9 +3326,9 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>289</v>
@@ -3324,13 +3337,13 @@
         <v>270</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E27" s="6">
         <v>1</v>
       </c>
       <c r="F27" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>265</v>
@@ -3339,7 +3352,7 @@
         <v>249</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -3361,24 +3374,24 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="6">
-        <v>1</v>
-      </c>
-      <c r="F28" s="6">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>265</v>
@@ -3387,7 +3400,7 @@
         <v>249</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -3409,57 +3422,43 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:28" ht="285" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>269</v>
+    <row r="29" spans="1:28" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>171</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>270</v>
+        <v>18</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>113</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>265</v>
+        <v>172</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>264</v>
+      <c r="I29" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
-      <c r="Z29" s="2"/>
-      <c r="AA29" s="2"/>
-      <c r="AB29" s="2"/>
-    </row>
-    <row r="30" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
-        <v>171</v>
+    </row>
+    <row r="30" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>289</v>
@@ -3468,7 +3467,7 @@
         <v>18</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>113</v>
@@ -3477,23 +3476,37 @@
         <v>113</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>172</v>
+        <v>96</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I30" s="19" t="s">
-        <v>173</v>
+      <c r="I30" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
-    </row>
-    <row r="31" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+    </row>
+    <row r="31" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>289</v>
@@ -3516,8 +3529,8 @@
       <c r="H31" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>97</v>
+      <c r="I31" s="20" t="s">
+        <v>115</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -3539,9 +3552,9 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>289</v>
@@ -3550,7 +3563,7 @@
         <v>18</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>113</v>
@@ -3564,8 +3577,8 @@
       <c r="H32" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I32" s="20" t="s">
-        <v>115</v>
+      <c r="I32" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3587,9 +3600,9 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>289</v>
@@ -3613,7 +3626,7 @@
         <v>249</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -3635,9 +3648,9 @@
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
     </row>
-    <row r="34" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>289</v>
@@ -3661,7 +3674,7 @@
         <v>249</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -3683,9 +3696,9 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>289</v>
@@ -3709,7 +3722,7 @@
         <v>249</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -3731,9 +3744,9 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>289</v>
@@ -3757,7 +3770,7 @@
         <v>249</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -3779,15 +3792,15 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>11</v>
@@ -3799,15 +3812,15 @@
         <v>113</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>96</v>
+        <v>182</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="J37" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="J37" s="6"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
@@ -3827,9 +3840,9 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>46</v>
+        <v>204</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>289</v>
@@ -3847,13 +3860,13 @@
         <v>113</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="H38" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>48</v>
+        <v>206</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="9"/>
@@ -3875,9 +3888,9 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>204</v>
+        <v>49</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>289</v>
@@ -3895,13 +3908,13 @@
         <v>113</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>206</v>
+        <v>50</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="9"/>
@@ -3923,9 +3936,9 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>289</v>
@@ -3949,7 +3962,7 @@
         <v>249</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="9"/>
@@ -3971,9 +3984,9 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>289</v>
@@ -3997,7 +4010,7 @@
         <v>249</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="9"/>
@@ -4021,7 +4034,7 @@
     </row>
     <row r="42" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>289</v>
@@ -4045,7 +4058,7 @@
         <v>249</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J42" s="6"/>
       <c r="K42" s="9"/>
@@ -4067,9 +4080,9 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>289</v>
@@ -4093,7 +4106,7 @@
         <v>249</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J43" s="6"/>
       <c r="K43" s="9"/>
@@ -4115,15 +4128,15 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>11</v>
@@ -4135,16 +4148,16 @@
         <v>113</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>182</v>
+        <v>61</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>58</v>
+        <v>167</v>
       </c>
       <c r="J44" s="6"/>
-      <c r="K44" s="9"/>
+      <c r="K44" s="6"/>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
@@ -4163,9 +4176,9 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>289</v>
@@ -4189,7 +4202,7 @@
         <v>249</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>167</v>
+        <v>63</v>
       </c>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -4211,9 +4224,9 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>289</v>
@@ -4237,7 +4250,7 @@
         <v>249</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -4259,9 +4272,9 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>289</v>
@@ -4285,7 +4298,7 @@
         <v>249</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
@@ -4307,9 +4320,9 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>289</v>
@@ -4333,7 +4346,7 @@
         <v>249</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -4355,9 +4368,9 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>289</v>
@@ -4375,13 +4388,13 @@
         <v>113</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -4403,9 +4416,9 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>289</v>
@@ -4429,7 +4442,7 @@
         <v>249</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -4451,9 +4464,9 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>73</v>
+        <v>160</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>289</v>
@@ -4471,13 +4484,13 @@
         <v>113</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -4499,9 +4512,9 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>160</v>
+        <v>75</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>289</v>
@@ -4519,13 +4532,13 @@
         <v>113</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>161</v>
+        <v>76</v>
       </c>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -4547,15 +4560,15 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>60</v>
+        <v>163</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>11</v>
@@ -4567,13 +4580,13 @@
         <v>113</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>71</v>
+        <v>169</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I53" s="8" t="s">
-        <v>76</v>
+      <c r="I53" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -4595,9 +4608,9 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>168</v>
+    <row r="54" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>174</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>289</v>
@@ -4615,13 +4628,13 @@
         <v>113</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -4645,13 +4658,13 @@
     </row>
     <row r="55" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
-        <v>174</v>
+        <v>98</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>11</v>
@@ -4663,17 +4676,17 @@
         <v>113</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I55" s="19" t="s">
-        <v>176</v>
+        <v>250</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
-      <c r="L55" s="9"/>
+      <c r="L55" s="6"/>
       <c r="M55" s="9"/>
       <c r="N55" s="9"/>
       <c r="O55" s="2"/>
@@ -4693,10 +4706,10 @@
     </row>
     <row r="56" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>99</v>
@@ -4717,7 +4730,7 @@
         <v>250</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -4739,12 +4752,12 @@
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>99</v>
@@ -4765,7 +4778,7 @@
         <v>250</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
@@ -4789,10 +4802,10 @@
     </row>
     <row r="58" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>99</v>
@@ -4813,7 +4826,7 @@
         <v>250</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
@@ -4835,12 +4848,12 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>99</v>
@@ -4861,7 +4874,7 @@
         <v>250</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
@@ -4883,12 +4896,12 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>107</v>
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="25" t="s">
+        <v>109</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>99</v>
@@ -4909,7 +4922,7 @@
         <v>250</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -4933,10 +4946,10 @@
     </row>
     <row r="61" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>99</v>
@@ -4957,7 +4970,7 @@
         <v>250</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -4979,15 +4992,15 @@
       <c r="AA61" s="2"/>
       <c r="AB61" s="2"/>
     </row>
-    <row r="62" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
-        <v>111</v>
+    <row r="62" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>11</v>
@@ -4999,17 +5012,17 @@
         <v>113</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>181</v>
+        <v>91</v>
       </c>
       <c r="H62" s="8" t="s">
         <v>250</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J62" s="6"/>
-      <c r="K62" s="6"/>
-      <c r="L62" s="6"/>
+        <v>194</v>
+      </c>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
       <c r="M62" s="9"/>
       <c r="N62" s="9"/>
       <c r="O62" s="2"/>
@@ -5027,9 +5040,9 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>289</v>
@@ -5053,7 +5066,7 @@
         <v>250</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>194</v>
+        <v>92</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -5075,9 +5088,9 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>135</v>
+    <row r="64" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>289</v>
@@ -5086,13 +5099,13 @@
         <v>90</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>113</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="G64" s="6" t="s">
         <v>91</v>
@@ -5101,7 +5114,7 @@
         <v>250</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -5123,33 +5136,33 @@
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
     </row>
-    <row r="65" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>93</v>
+    <row r="65" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>113</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H65" s="8" t="s">
         <v>250</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -5171,17 +5184,17 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
-        <v>77</v>
+    <row r="66" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="21" t="s">
+        <v>207</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C66" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C66" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E66" s="7" t="s">
@@ -5190,14 +5203,14 @@
       <c r="F66" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G66" s="6" t="s">
-        <v>79</v>
+      <c r="G66" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="H66" s="8" t="s">
         <v>250</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>80</v>
+        <v>208</v>
       </c>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -5219,17 +5232,17 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A67" s="21" t="s">
-        <v>207</v>
+    <row r="67" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C67" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D67" s="18" t="s">
+      <c r="D67" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="7" t="s">
@@ -5238,14 +5251,14 @@
       <c r="F67" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G67" s="18" t="s">
+      <c r="G67" s="6" t="s">
         <v>82</v>
       </c>
       <c r="H67" s="8" t="s">
         <v>250</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>208</v>
+        <v>83</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -5267,12 +5280,12 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>78</v>
@@ -5287,13 +5300,13 @@
         <v>113</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H68" s="8" t="s">
         <v>250</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -5315,12 +5328,12 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>78</v>
@@ -5341,7 +5354,7 @@
         <v>250</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -5363,12 +5376,12 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>78</v>
@@ -5383,13 +5396,13 @@
         <v>113</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H70" s="8" t="s">
         <v>250</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -5411,15 +5424,15 @@
       <c r="AA70" s="2"/>
       <c r="AB70" s="2"/>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>88</v>
+        <v>130</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>11</v>
@@ -5431,13 +5444,13 @@
         <v>113</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="H71" s="8" t="s">
         <v>250</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>89</v>
+        <v>137</v>
       </c>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -5459,15 +5472,15 @@
       <c r="AA71" s="2"/>
       <c r="AB71" s="2"/>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
-        <v>130</v>
+    <row r="72" spans="1:28" s="1" customFormat="1" ht="141.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="21" t="s">
+        <v>209</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>136</v>
+        <v>289</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>78</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>11</v>
@@ -5479,13 +5492,13 @@
         <v>113</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>127</v>
+        <v>211</v>
       </c>
       <c r="H72" s="8" t="s">
         <v>250</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>137</v>
+        <v>210</v>
       </c>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -5507,15 +5520,15 @@
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="21" t="s">
-        <v>209</v>
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>78</v>
+        <v>288</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>11</v>
@@ -5527,13 +5540,13 @@
         <v>113</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>211</v>
+        <v>127</v>
       </c>
       <c r="H73" s="8" t="s">
         <v>250</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -5555,12 +5568,12 @@
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>136</v>
@@ -5581,7 +5594,7 @@
         <v>250</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
@@ -5603,15 +5616,15 @@
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>129</v>
+    <row r="75" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>11</v>
@@ -5623,37 +5636,23 @@
         <v>113</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>127</v>
+        <v>183</v>
       </c>
       <c r="H75" s="8" t="s">
         <v>250</v>
       </c>
       <c r="I75" s="8" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
       <c r="N75" s="9"/>
-      <c r="O75" s="2"/>
-      <c r="P75" s="2"/>
-      <c r="Q75" s="2"/>
-      <c r="R75" s="2"/>
-      <c r="S75" s="2"/>
-      <c r="T75" s="2"/>
-      <c r="U75" s="2"/>
-      <c r="V75" s="2"/>
-      <c r="W75" s="2"/>
-      <c r="X75" s="2"/>
-      <c r="Y75" s="2"/>
-      <c r="Z75" s="2"/>
-      <c r="AA75" s="2"/>
-      <c r="AB75" s="2"/>
-    </row>
-    <row r="76" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>140</v>
+    </row>
+    <row r="76" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>289</v>
@@ -5676,21 +5675,35 @@
       <c r="H76" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="I76" s="8" t="s">
-        <v>141</v>
+      <c r="I76" s="22" t="s">
+        <v>212</v>
       </c>
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
       <c r="N76" s="9"/>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+      <c r="R76" s="2"/>
+      <c r="S76" s="2"/>
+      <c r="T76" s="2"/>
+      <c r="U76" s="2"/>
+      <c r="V76" s="2"/>
+      <c r="W76" s="2"/>
+      <c r="X76" s="2"/>
+      <c r="Y76" s="2"/>
+      <c r="Z76" s="2"/>
+      <c r="AA76" s="2"/>
+      <c r="AB76" s="2"/>
     </row>
     <row r="77" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>146</v>
@@ -5711,7 +5724,7 @@
         <v>250</v>
       </c>
       <c r="I77" s="22" t="s">
-        <v>212</v>
+        <v>144</v>
       </c>
       <c r="J77" s="9"/>
       <c r="K77" s="9"/>
@@ -5733,9 +5746,9 @@
       <c r="AA77" s="2"/>
       <c r="AB77" s="2"/>
     </row>
-    <row r="78" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>289</v>
@@ -5753,13 +5766,13 @@
         <v>113</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="H78" s="8" t="s">
         <v>250</v>
       </c>
       <c r="I78" s="22" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
@@ -5781,9 +5794,9 @@
       <c r="AA78" s="2"/>
       <c r="AB78" s="2"/>
     </row>
-    <row r="79" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>289</v>
@@ -5807,7 +5820,7 @@
         <v>250</v>
       </c>
       <c r="I79" s="22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
@@ -5829,9 +5842,9 @@
       <c r="AA79" s="2"/>
       <c r="AB79" s="2"/>
     </row>
-    <row r="80" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>289</v>
@@ -5855,7 +5868,7 @@
         <v>250</v>
       </c>
       <c r="I80" s="22" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
@@ -5877,15 +5890,15 @@
       <c r="AA80" s="2"/>
       <c r="AB80" s="2"/>
     </row>
-    <row r="81" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>151</v>
+    <row r="81" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A81" s="11" t="s">
+        <v>162</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>11</v>
@@ -5897,16 +5910,16 @@
         <v>113</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
       <c r="H81" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="I81" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="J81" s="9"/>
-      <c r="K81" s="9"/>
+      <c r="I81" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
       <c r="N81" s="9"/>
@@ -5925,15 +5938,15 @@
       <c r="AA81" s="2"/>
       <c r="AB81" s="2"/>
     </row>
-    <row r="82" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>151</v>
+    <row r="82" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
+        <v>197</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>146</v>
+        <v>198</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>11</v>
@@ -5945,15 +5958,15 @@
         <v>113</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
       <c r="H82" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="I82" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="J82" s="9"/>
+      <c r="I82" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="J82" s="8"/>
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
@@ -5973,15 +5986,15 @@
       <c r="AA82" s="2"/>
       <c r="AB82" s="2"/>
     </row>
-    <row r="83" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>163</v>
+        <v>198</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>11</v>
@@ -5999,10 +6012,10 @@
         <v>250</v>
       </c>
       <c r="I83" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="J83" s="6"/>
-      <c r="K83" s="6"/>
+        <v>201</v>
+      </c>
+      <c r="J83" s="8"/>
+      <c r="K83" s="9"/>
       <c r="L83" s="9"/>
       <c r="M83" s="9"/>
       <c r="N83" s="9"/>
@@ -6021,12 +6034,12 @@
       <c r="AA83" s="2"/>
       <c r="AB83" s="2"/>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>198</v>
@@ -6044,12 +6057,14 @@
         <v>196</v>
       </c>
       <c r="H84" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J84" s="8"/>
+        <v>201</v>
+      </c>
+      <c r="J84" s="20" t="s">
+        <v>203</v>
+      </c>
       <c r="K84" s="9"/>
       <c r="L84" s="9"/>
       <c r="M84" s="9"/>
@@ -6069,15 +6084,15 @@
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
-        <v>200</v>
+    <row r="85" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>11</v>
@@ -6089,16 +6104,16 @@
         <v>113</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="H85" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="J85" s="8"/>
-      <c r="K85" s="9"/>
+        <v>187</v>
+      </c>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
       <c r="L85" s="9"/>
       <c r="M85" s="9"/>
       <c r="N85" s="9"/>
@@ -6117,15 +6132,15 @@
       <c r="AA85" s="2"/>
       <c r="AB85" s="2"/>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A86" s="11" t="s">
-        <v>202</v>
+    <row r="86" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>11</v>
@@ -6137,18 +6152,16 @@
         <v>113</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H86" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="J86" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="K86" s="9"/>
+        <v>190</v>
+      </c>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
       <c r="L86" s="9"/>
       <c r="M86" s="9"/>
       <c r="N86" s="9"/>
@@ -6167,9 +6180,9 @@
       <c r="AA86" s="2"/>
       <c r="AB86" s="2"/>
     </row>
-    <row r="87" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>289</v>
@@ -6187,13 +6200,13 @@
         <v>113</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="H87" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
@@ -6216,14 +6229,14 @@
       <c r="AB87" s="2"/>
     </row>
     <row r="88" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>188</v>
+      <c r="A88" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>186</v>
+        <v>246</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>11</v>
@@ -6235,16 +6248,16 @@
         <v>113</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>189</v>
+        <v>147</v>
       </c>
       <c r="H88" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I88" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="J88" s="6"/>
-      <c r="K88" s="6"/>
+      <c r="I88" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="J88" s="9"/>
+      <c r="K88" s="9"/>
       <c r="L88" s="9"/>
       <c r="M88" s="9"/>
       <c r="N88" s="9"/>
@@ -6264,14 +6277,14 @@
       <c r="AB88" s="2"/>
     </row>
     <row r="89" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>191</v>
+      <c r="A89" s="6" t="s">
+        <v>214</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>186</v>
+        <v>246</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>11</v>
@@ -6283,16 +6296,16 @@
         <v>113</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="H89" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I89" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="J89" s="6"/>
-      <c r="K89" s="6"/>
+      <c r="I89" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="J89" s="9"/>
+      <c r="K89" s="9"/>
       <c r="L89" s="9"/>
       <c r="M89" s="9"/>
       <c r="N89" s="9"/>
@@ -6313,10 +6326,10 @@
     </row>
     <row r="90" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>246</v>
@@ -6337,7 +6350,7 @@
         <v>249</v>
       </c>
       <c r="I90" s="22" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J90" s="9"/>
       <c r="K90" s="9"/>
@@ -6361,10 +6374,10 @@
     </row>
     <row r="91" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>246</v>
@@ -6385,7 +6398,7 @@
         <v>249</v>
       </c>
       <c r="I91" s="22" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="J91" s="9"/>
       <c r="K91" s="9"/>
@@ -6407,9 +6420,9 @@
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
     </row>
-    <row r="92" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
-        <v>215</v>
+    <row r="92" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>289</v>
@@ -6433,7 +6446,7 @@
         <v>249</v>
       </c>
       <c r="I92" s="22" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="J92" s="9"/>
       <c r="K92" s="9"/>
@@ -6455,9 +6468,9 @@
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
     </row>
-    <row r="93" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
-        <v>216</v>
+    <row r="93" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="25" t="s">
+        <v>218</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>289</v>
@@ -6481,7 +6494,7 @@
         <v>249</v>
       </c>
       <c r="I93" s="22" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
@@ -6503,12 +6516,12 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
-        <v>217</v>
+    <row r="94" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>246</v>
@@ -6529,7 +6542,7 @@
         <v>249</v>
       </c>
       <c r="I94" s="22" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
@@ -6553,10 +6566,10 @@
     </row>
     <row r="95" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>246</v>
@@ -6577,7 +6590,7 @@
         <v>249</v>
       </c>
       <c r="I95" s="22" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
@@ -6599,12 +6612,12 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
-        <v>219</v>
+    <row r="96" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>246</v>
@@ -6625,7 +6638,7 @@
         <v>249</v>
       </c>
       <c r="I96" s="22" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
@@ -6649,10 +6662,10 @@
     </row>
     <row r="97" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>246</v>
@@ -6673,7 +6686,7 @@
         <v>249</v>
       </c>
       <c r="I97" s="22" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -6695,15 +6708,15 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>221</v>
+    <row r="98" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="11" t="s">
+        <v>223</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>11</v>
@@ -6715,13 +6728,13 @@
         <v>113</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>147</v>
+        <v>247</v>
       </c>
       <c r="H98" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I98" s="22" t="s">
-        <v>235</v>
+      <c r="I98" s="8" t="s">
+        <v>237</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -6743,15 +6756,15 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
-        <v>222</v>
+    <row r="99" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>289</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>11</v>
@@ -6763,16 +6776,20 @@
         <v>113</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>147</v>
+        <v>247</v>
       </c>
       <c r="H99" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I99" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="J99" s="9"/>
-      <c r="K99" s="9"/>
+        <v>238</v>
+      </c>
+      <c r="J99" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="K99" s="20" t="s">
+        <v>240</v>
+      </c>
       <c r="L99" s="9"/>
       <c r="M99" s="9"/>
       <c r="N99" s="9"/>
@@ -6791,12 +6808,12 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>224</v>
@@ -6814,16 +6831,26 @@
         <v>247</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I100" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="J100" s="9"/>
-      <c r="K100" s="9"/>
-      <c r="L100" s="9"/>
-      <c r="M100" s="9"/>
-      <c r="N100" s="9"/>
+      <c r="I100" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="J100" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="K100" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="L100" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="M100" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="N100" s="20" t="s">
+        <v>245</v>
+      </c>
       <c r="O100" s="2"/>
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
@@ -6839,17 +6866,17 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A101" s="11" t="s">
-        <v>225</v>
+    <row r="101" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D101" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D101" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E101" s="7" t="s">
@@ -6858,21 +6885,17 @@
       <c r="F101" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G101" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H101" s="8" t="s">
+      <c r="G101" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="H101" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="I101" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="J101" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="K101" s="20" t="s">
-        <v>240</v>
-      </c>
+      <c r="I101" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="J101" s="9"/>
+      <c r="K101" s="9"/>
       <c r="L101" s="9"/>
       <c r="M101" s="9"/>
       <c r="N101" s="9"/>
@@ -6891,17 +6914,17 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
-      <c r="A102" s="11" t="s">
-        <v>226</v>
+    <row r="102" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>257</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D102" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D102" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E102" s="7" t="s">
@@ -6910,30 +6933,20 @@
       <c r="F102" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G102" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H102" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="I102" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="J102" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="K102" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="L102" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="M102" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="N102" s="20" t="s">
-        <v>245</v>
-      </c>
+      <c r="G102" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="H102" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="I102" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="J102" s="9"/>
+      <c r="K102" s="9"/>
+      <c r="L102" s="9"/>
+      <c r="M102" s="9"/>
+      <c r="N102" s="9"/>
       <c r="O102" s="2"/>
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
@@ -6949,9 +6962,9 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>289</v>
@@ -6975,7 +6988,7 @@
         <v>249</v>
       </c>
       <c r="I103" s="20" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
@@ -6997,17 +7010,17 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
-        <v>257</v>
+    <row r="104" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="23" t="s">
+        <v>272</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C104" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D104" s="9" t="s">
+      <c r="C104" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D104" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E104" s="7" t="s">
@@ -7016,17 +7029,21 @@
       <c r="F104" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G104" s="9" t="s">
-        <v>255</v>
+      <c r="G104" s="6" t="s">
+        <v>247</v>
       </c>
       <c r="H104" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="I104" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="J104" s="9"/>
-      <c r="K104" s="9"/>
+      <c r="I104" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="J104" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="K104" s="20" t="s">
+        <v>275</v>
+      </c>
       <c r="L104" s="9"/>
       <c r="M104" s="9"/>
       <c r="N104" s="9"/>
@@ -7045,17 +7062,17 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>259</v>
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="11" t="s">
+        <v>274</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C105" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D105" s="9" t="s">
+      <c r="C105" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D105" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E105" s="7" t="s">
@@ -7064,17 +7081,17 @@
       <c r="F105" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G105" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="H105" s="20" t="s">
+      <c r="G105" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="H105" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I105" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="J105" s="9"/>
-      <c r="K105" s="9"/>
+      <c r="I105" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="J105" s="20"/>
+      <c r="K105" s="20"/>
       <c r="L105" s="9"/>
       <c r="M105" s="9"/>
       <c r="N105" s="9"/>
@@ -7093,17 +7110,17 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="23" t="s">
-        <v>272</v>
+    <row r="106" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="11" t="s">
+        <v>282</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="D106" s="24" t="s">
+      <c r="D106" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E106" s="7" t="s">
@@ -7115,7 +7132,7 @@
       <c r="G106" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="H106" s="20" t="s">
+      <c r="H106" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I106" s="22" t="s">
@@ -7127,9 +7144,9 @@
       <c r="K106" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="L106" s="9"/>
-      <c r="M106" s="9"/>
-      <c r="N106" s="9"/>
+      <c r="L106" s="20"/>
+      <c r="M106" s="20"/>
+      <c r="N106" s="20"/>
       <c r="O106" s="2"/>
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
@@ -7145,18 +7162,18 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>282</v>
+        <v>10</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>113</v>
@@ -7165,16 +7182,14 @@
         <v>113</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>247</v>
+        <v>12</v>
       </c>
       <c r="H107" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I107" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="J107" s="20"/>
-      <c r="K107" s="20"/>
+        <v>287</v>
+      </c>
+      <c r="I107" s="9"/>
+      <c r="J107" s="9"/>
+      <c r="K107" s="9"/>
       <c r="L107" s="9"/>
       <c r="M107" s="9"/>
       <c r="N107" s="9"/>
@@ -7193,60 +7208,14 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A108" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D108" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E108" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F108" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G108" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H108" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I108" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="J108" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="K108" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="L108" s="20"/>
-      <c r="M108" s="20"/>
-      <c r="N108" s="20"/>
-      <c r="O108" s="2"/>
-      <c r="P108" s="2"/>
-      <c r="Q108" s="2"/>
-      <c r="R108" s="2"/>
-      <c r="S108" s="2"/>
-      <c r="T108" s="2"/>
-      <c r="U108" s="2"/>
-      <c r="V108" s="2"/>
-      <c r="W108" s="2"/>
-      <c r="X108" s="2"/>
-      <c r="Y108" s="2"/>
-      <c r="Z108" s="2"/>
-      <c r="AA108" s="2"/>
-      <c r="AB108" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I108" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I107" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a test Method for profile->merchant
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebAutomation\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(08-02-2023)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65EAE0F-84E5-4E19-8408-5D27F5B0CBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DD1B99-E645-489E-9302-EB0038F5B85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="10455" windowHeight="9180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="307">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1661,9 +1661,6 @@
 -pfiveTimeContent</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -1671,13 +1668,97 @@
   </si>
   <si>
     <t>Admin Login with invalid Authy</t>
+  </si>
+  <si>
+    <t>add Merchant user</t>
+  </si>
+  <si>
+    <t>Profile Merchant</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>add Merchant user with invalid scenarios</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testAddMerchantWithInvalidData,
+-pheading,
+-pheadingContact,
+-pfirstName,
+-plastName,
+-ppartnerName,
+-pcompanyName,
+-perrMessage,
+-pcolour,
+-pelementName</t>
+  </si>
+  <si>
+    <t>add Merchant user with Field Validation</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testAddMerchantWithFieldValidation,
+-pheading,
+-pheadingContact,
+-pfirstName,
+-plastName,
+-ppartnerName,
+-pcompanyName</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testAddMerchantUser,
+-pheading,
+-pheadingContact,
+-pfirstName,
+-plastName,
+-ppartnerName,
+-pcompanyName,
+-pmessage,
+-ptitle</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testEditMerchantInvitation,
+-pheading,
+-pheadingContact</t>
+  </si>
+  <si>
+    <t>Resend Merchant invitation</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testMerchantResendInvitation,
+-pfirstName,
+-plastName</t>
+  </si>
+  <si>
+    <t>Cancel Merchant invitation</t>
+  </si>
+  <si>
+    <t>Verify Edit Merchant Invitation</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testMerchantCancelInvitation,
+-pfirstName,
+-plastName,
+-pheading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1716,6 +1797,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1743,7 +1831,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1766,11 +1854,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1817,6 +1916,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2098,10 +2199,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB107"/>
+  <dimension ref="A1:AB113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,7 +2262,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>
@@ -2204,10 +2305,10 @@
     </row>
     <row r="3" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>10</v>
@@ -2253,7 +2354,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>10</v>
@@ -2299,7 +2400,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
@@ -2345,7 +2446,7 @@
         <v>165</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>10</v>
@@ -2391,7 +2492,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>27</v>
@@ -2437,7 +2538,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>27</v>
@@ -2483,7 +2584,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>27</v>
@@ -2529,7 +2630,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>27</v>
@@ -2575,7 +2676,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>35</v>
@@ -2621,7 +2722,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>35</v>
@@ -2667,7 +2768,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>35</v>
@@ -2713,7 +2814,7 @@
         <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>35</v>
@@ -2759,7 +2860,7 @@
         <v>44</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>35</v>
@@ -2805,7 +2906,7 @@
         <v>283</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>10</v>
@@ -2853,7 +2954,7 @@
         <v>153</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>156</v>
@@ -2901,7 +3002,7 @@
         <v>155</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>156</v>
@@ -2949,7 +3050,7 @@
         <v>157</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>158</v>
@@ -2997,7 +3098,7 @@
         <v>177</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>158</v>
@@ -3045,7 +3146,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>10</v>
@@ -3091,7 +3192,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>18</v>
@@ -3139,7 +3240,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
@@ -3187,7 +3288,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>18</v>
@@ -3235,7 +3336,7 @@
         <v>266</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>270</v>
@@ -3283,7 +3384,7 @@
         <v>267</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>270</v>
@@ -3331,7 +3432,7 @@
         <v>268</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>270</v>
@@ -3379,10 +3480,10 @@
         <v>269</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>289</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>290</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>14</v>
@@ -3427,7 +3528,7 @@
         <v>171</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>18</v>
@@ -3461,7 +3562,7 @@
         <v>95</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>18</v>
@@ -3509,7 +3610,7 @@
         <v>114</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>18</v>
@@ -3557,7 +3658,7 @@
         <v>116</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>18</v>
@@ -3605,7 +3706,7 @@
         <v>118</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>18</v>
@@ -3653,7 +3754,7 @@
         <v>120</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>18</v>
@@ -3701,7 +3802,7 @@
         <v>122</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>18</v>
@@ -3749,7 +3850,7 @@
         <v>124</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>18</v>
@@ -3797,7 +3898,7 @@
         <v>46</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>47</v>
@@ -3845,7 +3946,7 @@
         <v>204</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>47</v>
@@ -3893,7 +3994,7 @@
         <v>49</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>47</v>
@@ -3941,7 +4042,7 @@
         <v>51</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>47</v>
@@ -3989,7 +4090,7 @@
         <v>53</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>47</v>
@@ -4037,7 +4138,7 @@
         <v>55</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>47</v>
@@ -4085,7 +4186,7 @@
         <v>57</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>47</v>
@@ -4133,7 +4234,7 @@
         <v>59</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>60</v>
@@ -4181,7 +4282,7 @@
         <v>62</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>60</v>
@@ -4229,7 +4330,7 @@
         <v>64</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>60</v>
@@ -4277,7 +4378,7 @@
         <v>66</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>60</v>
@@ -4325,7 +4426,7 @@
         <v>68</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>60</v>
@@ -4373,7 +4474,7 @@
         <v>70</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>60</v>
@@ -4421,7 +4522,7 @@
         <v>73</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>60</v>
@@ -4469,7 +4570,7 @@
         <v>160</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>60</v>
@@ -4517,7 +4618,7 @@
         <v>75</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>60</v>
@@ -4565,7 +4666,7 @@
         <v>168</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>163</v>
@@ -4613,7 +4714,7 @@
         <v>174</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>163</v>
@@ -4661,7 +4762,7 @@
         <v>98</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>99</v>
@@ -4709,7 +4810,7 @@
         <v>101</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>99</v>
@@ -4757,7 +4858,7 @@
         <v>103</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>99</v>
@@ -4805,7 +4906,7 @@
         <v>105</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>99</v>
@@ -4853,7 +4954,7 @@
         <v>107</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>99</v>
@@ -4901,7 +5002,7 @@
         <v>109</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>99</v>
@@ -4949,7 +5050,7 @@
         <v>111</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>99</v>
@@ -4997,7 +5098,7 @@
         <v>195</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>90</v>
@@ -5045,7 +5146,7 @@
         <v>135</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>90</v>
@@ -5093,7 +5194,7 @@
         <v>93</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>90</v>
@@ -5141,7 +5242,7 @@
         <v>77</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>78</v>
@@ -5189,7 +5290,7 @@
         <v>207</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C66" s="18" t="s">
         <v>78</v>
@@ -5237,7 +5338,7 @@
         <v>81</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>78</v>
@@ -5285,7 +5386,7 @@
         <v>84</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>78</v>
@@ -5333,7 +5434,7 @@
         <v>86</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>78</v>
@@ -5381,7 +5482,7 @@
         <v>88</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>78</v>
@@ -5429,7 +5530,7 @@
         <v>130</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>136</v>
@@ -5477,7 +5578,7 @@
         <v>209</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>78</v>
@@ -5525,7 +5626,7 @@
         <v>128</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>136</v>
@@ -5573,7 +5674,7 @@
         <v>129</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>136</v>
@@ -5621,7 +5722,7 @@
         <v>140</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>146</v>
@@ -5655,7 +5756,7 @@
         <v>142</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>146</v>
@@ -5703,7 +5804,7 @@
         <v>143</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>146</v>
@@ -5751,7 +5852,7 @@
         <v>145</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>146</v>
@@ -5799,7 +5900,7 @@
         <v>149</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>146</v>
@@ -5847,7 +5948,7 @@
         <v>151</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>146</v>
@@ -5895,7 +5996,7 @@
         <v>162</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>163</v>
@@ -5943,7 +6044,7 @@
         <v>197</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>198</v>
@@ -5991,7 +6092,7 @@
         <v>200</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>198</v>
@@ -6039,7 +6140,7 @@
         <v>202</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>198</v>
@@ -6089,7 +6190,7 @@
         <v>184</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>186</v>
@@ -6137,7 +6238,7 @@
         <v>188</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>186</v>
@@ -6185,7 +6286,7 @@
         <v>191</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>186</v>
@@ -6233,7 +6334,7 @@
         <v>213</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>246</v>
@@ -6281,7 +6382,7 @@
         <v>214</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>246</v>
@@ -6329,7 +6430,7 @@
         <v>215</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>246</v>
@@ -6377,7 +6478,7 @@
         <v>216</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>246</v>
@@ -6425,7 +6526,7 @@
         <v>217</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>246</v>
@@ -6473,7 +6574,7 @@
         <v>218</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>246</v>
@@ -6521,7 +6622,7 @@
         <v>219</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>246</v>
@@ -6569,7 +6670,7 @@
         <v>220</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>246</v>
@@ -6617,7 +6718,7 @@
         <v>221</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>246</v>
@@ -6665,7 +6766,7 @@
         <v>222</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>246</v>
@@ -6713,7 +6814,7 @@
         <v>223</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>224</v>
@@ -6761,7 +6862,7 @@
         <v>225</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>224</v>
@@ -6813,7 +6914,7 @@
         <v>226</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>224</v>
@@ -6871,7 +6972,7 @@
         <v>253</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C101" s="9" t="s">
         <v>254</v>
@@ -6919,7 +7020,7 @@
         <v>257</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C102" s="9" t="s">
         <v>254</v>
@@ -6967,7 +7068,7 @@
         <v>259</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C103" s="9" t="s">
         <v>254</v>
@@ -7015,7 +7116,7 @@
         <v>272</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>224</v>
@@ -7067,7 +7168,7 @@
         <v>274</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>281</v>
@@ -7115,7 +7216,7 @@
         <v>282</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>224</v>
@@ -7167,7 +7268,7 @@
         <v>280</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>10</v>
@@ -7208,6 +7309,180 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
+    <row r="108" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A108" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G108" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H108" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I108" s="22" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="109" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>295</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="G109" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H109" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I109" s="22" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="110" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>298</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G110" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H110" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I110" s="22" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="111" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>305</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G111" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H111" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I111" s="22" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="112" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>302</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G112" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H112" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>304</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G113" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H113" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I113" s="22" t="s">
+        <v>306</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I107" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="1">

</xml_diff>

<commit_message>
Added a test method in profile merchant user details
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(08-02-2023)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DD1B99-E645-489E-9302-EB0038F5B85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF77370D-CC71-4853-87DA-7279387C7FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="313">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1752,6 +1752,37 @@
 -pfirstName,
 -plastName,
 -pheading</t>
+  </si>
+  <si>
+    <t>Merchant Details Filters And Exports</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testProfileMerchantFilterandExports,
+-pheading,
+-pexportHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merchant user  Details </t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testProfileMerchantDetails,
+-psearchText,
+-pexportHeading</t>
+  </si>
+  <si>
+    <t>Merchant user  Details  with Token Account</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testProfileMerchantDetailsWithTokenAccount,
+-pfilterType,
+-ptoAmount,
+-pamount,
+-pheading,
+-pexportHeading,
+-psearchText</t>
   </si>
 </sst>
 </file>
@@ -2199,10 +2230,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB113"/>
+  <dimension ref="A1:AB116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" topLeftCell="B115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I116" sqref="I116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7430,7 +7461,7 @@
         <v>302</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>146</v>
@@ -7459,7 +7490,7 @@
         <v>304</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>146</v>
@@ -7481,6 +7512,93 @@
       </c>
       <c r="I113" s="22" t="s">
         <v>306</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>307</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G114" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H114" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I114" s="22" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>309</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E115" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G115" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H115" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I115" s="22" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>311</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G116" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H116" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I116" s="22" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a test method for profile merchant
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(08-02-2023)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(17-02-2023)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF77370D-CC71-4853-87DA-7279387C7FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C5F0A0-CC30-4F36-8F5C-FA9A4F8B032B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="315">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1782,6 +1782,14 @@
 -pamount,
 -pheading,
 -pexportHeading,
+-psearchText</t>
+  </si>
+  <si>
+    <t>Merchant user  Details  with Payout Transaction</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testProfileMerchantPayoutHistory,
 -psearchText</t>
   </si>
 </sst>
@@ -2230,10 +2238,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB116"/>
+  <dimension ref="A1:AB117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I116" sqref="I116"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7577,7 +7585,7 @@
         <v>311</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>146</v>
@@ -7599,6 +7607,35 @@
       </c>
       <c r="I116" s="22" t="s">
         <v>312</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>313</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E117" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G117" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H117" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I117" s="22" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Global search scripts in HomeTest-Admin_web
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(17-02-2023)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C5F0A0-CC30-4F36-8F5C-FA9A4F8B032B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B14CEC-E9B9-4C4C-A5CB-4382D262B845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$120</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="324">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1791,6 +1791,39 @@
     <t>coyni.admin.tests.ProfilesTest,
 testProfileMerchantPayoutHistory,
 -psearchText</t>
+  </si>
+  <si>
+    <t>testGobalSearchWithLast4digits</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.HomeTest,
+tesGobalSearchWithLastFourDigitsOfDebitCardAndCreditCard,
+-plastFourDigits</t>
+  </si>
+  <si>
+    <t>testGobalSearchWithFirst6digits</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.HomeTest,
+tesGobalSearchWithFirstSixDigitsOfDebitCardAndCreditCard,
+-pfirstSixDigits</t>
+  </si>
+  <si>
+    <t>Gobal Seach with First 6 digits</t>
+  </si>
+  <si>
+    <t>Gobal Seach with last 4 digits</t>
+  </si>
+  <si>
+    <t>testGobalSearchWithBankAccount</t>
+  </si>
+  <si>
+    <t>Gobal Seach with Bank Account</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.HomeTest,
+tesGobalSearchWithBankNumber,
+-pbankAccount</t>
   </si>
 </sst>
 </file>
@@ -2237,11 +2270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB117"/>
+  <dimension ref="A1:AB120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,7 +2328,7 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2342,7 +2374,7 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>290</v>
       </c>
@@ -2388,7 +2420,7 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -2434,7 +2466,7 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
@@ -2480,7 +2512,7 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>165</v>
       </c>
@@ -2526,7 +2558,7 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="240" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -2572,7 +2604,7 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="210.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="210.75" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>29</v>
       </c>
@@ -2618,7 +2650,7 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="210" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
@@ -2664,7 +2696,7 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -2710,7 +2742,7 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="255" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
@@ -2756,7 +2788,7 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="225" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
@@ -2802,7 +2834,7 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="210" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -2848,7 +2880,7 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -2894,7 +2926,7 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="195" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -2940,7 +2972,7 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>283</v>
       </c>
@@ -2988,7 +3020,7 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
-    <row r="17" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>153</v>
       </c>
@@ -3036,7 +3068,7 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>155</v>
       </c>
@@ -3084,7 +3116,7 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>157</v>
       </c>
@@ -3132,7 +3164,7 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
     </row>
-    <row r="20" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>177</v>
       </c>
@@ -3180,7 +3212,7 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
     </row>
-    <row r="21" spans="1:28" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
@@ -3226,7 +3258,7 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -3274,7 +3306,7 @@
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
     </row>
-    <row r="23" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -3322,7 +3354,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
     </row>
-    <row r="24" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -3370,7 +3402,7 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
     </row>
-    <row r="25" spans="1:28" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="270" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>266</v>
       </c>
@@ -3418,7 +3450,7 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
     </row>
-    <row r="26" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>267</v>
       </c>
@@ -3466,7 +3498,7 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>268</v>
       </c>
@@ -3514,7 +3546,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="285" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>269</v>
       </c>
@@ -3562,7 +3594,7 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:28" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>171</v>
       </c>
@@ -3596,7 +3628,7 @@
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
     </row>
-    <row r="30" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>95</v>
       </c>
@@ -3644,7 +3676,7 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>114</v>
       </c>
@@ -3692,7 +3724,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>116</v>
       </c>
@@ -3740,7 +3772,7 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>118</v>
       </c>
@@ -3788,7 +3820,7 @@
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
     </row>
-    <row r="34" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>120</v>
       </c>
@@ -3836,7 +3868,7 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>122</v>
       </c>
@@ -3884,7 +3916,7 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>124</v>
       </c>
@@ -3932,7 +3964,7 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>46</v>
       </c>
@@ -3980,7 +4012,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>204</v>
       </c>
@@ -4028,7 +4060,7 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>49</v>
       </c>
@@ -4076,7 +4108,7 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
@@ -4124,7 +4156,7 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>53</v>
       </c>
@@ -4220,7 +4252,7 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>57</v>
       </c>
@@ -4268,7 +4300,7 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>59</v>
       </c>
@@ -4316,7 +4348,7 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>62</v>
       </c>
@@ -4364,7 +4396,7 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>64</v>
       </c>
@@ -4412,7 +4444,7 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>66</v>
       </c>
@@ -4460,7 +4492,7 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>68</v>
       </c>
@@ -4508,7 +4540,7 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>70</v>
       </c>
@@ -4556,7 +4588,7 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>73</v>
       </c>
@@ -4604,7 +4636,7 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>160</v>
       </c>
@@ -4652,7 +4684,7 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>75</v>
       </c>
@@ -4700,7 +4732,7 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>168</v>
       </c>
@@ -4748,7 +4780,7 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>174</v>
       </c>
@@ -4892,7 +4924,7 @@
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>103</v>
       </c>
@@ -4988,7 +5020,7 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>107</v>
       </c>
@@ -5036,7 +5068,7 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
         <v>109</v>
       </c>
@@ -5180,7 +5212,7 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>135</v>
       </c>
@@ -5228,7 +5260,7 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>93</v>
       </c>
@@ -5276,7 +5308,7 @@
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
     </row>
-    <row r="65" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>77</v>
       </c>
@@ -5324,7 +5356,7 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
         <v>207</v>
       </c>
@@ -5372,7 +5404,7 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>81</v>
       </c>
@@ -5420,7 +5452,7 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>84</v>
       </c>
@@ -5468,7 +5500,7 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>86</v>
       </c>
@@ -5516,7 +5548,7 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>88</v>
       </c>
@@ -5612,7 +5644,7 @@
       <c r="AA71" s="2"/>
       <c r="AB71" s="2"/>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="141.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
         <v>209</v>
       </c>
@@ -5708,7 +5740,7 @@
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>129</v>
       </c>
@@ -5756,7 +5788,7 @@
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
     </row>
-    <row r="75" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>140</v>
       </c>
@@ -5790,7 +5822,7 @@
       <c r="M75" s="9"/>
       <c r="N75" s="9"/>
     </row>
-    <row r="76" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>142</v>
       </c>
@@ -5886,7 +5918,7 @@
       <c r="AA77" s="2"/>
       <c r="AB77" s="2"/>
     </row>
-    <row r="78" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>145</v>
       </c>
@@ -5934,7 +5966,7 @@
       <c r="AA78" s="2"/>
       <c r="AB78" s="2"/>
     </row>
-    <row r="79" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>149</v>
       </c>
@@ -5982,7 +6014,7 @@
       <c r="AA79" s="2"/>
       <c r="AB79" s="2"/>
     </row>
-    <row r="80" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>151</v>
       </c>
@@ -6078,7 +6110,7 @@
       <c r="AA81" s="2"/>
       <c r="AB81" s="2"/>
     </row>
-    <row r="82" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>197</v>
       </c>
@@ -6126,7 +6158,7 @@
       <c r="AA82" s="2"/>
       <c r="AB82" s="2"/>
     </row>
-    <row r="83" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>200</v>
       </c>
@@ -6174,7 +6206,7 @@
       <c r="AA83" s="2"/>
       <c r="AB83" s="2"/>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
         <v>202</v>
       </c>
@@ -6224,12 +6256,12 @@
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
     </row>
-    <row r="85" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>184</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>186</v>
@@ -6272,12 +6304,12 @@
       <c r="AA85" s="2"/>
       <c r="AB85" s="2"/>
     </row>
-    <row r="86" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>186</v>
@@ -6320,12 +6352,12 @@
       <c r="AA86" s="2"/>
       <c r="AB86" s="2"/>
     </row>
-    <row r="87" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>191</v>
+        <v>321</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>186</v>
@@ -6340,13 +6372,13 @@
         <v>113</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>192</v>
+        <v>322</v>
       </c>
       <c r="H87" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>193</v>
+        <v>323</v>
       </c>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
@@ -6369,14 +6401,14 @@
       <c r="AB87" s="2"/>
     </row>
     <row r="88" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
-        <v>213</v>
+      <c r="A88" s="3" t="s">
+        <v>317</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>246</v>
+        <v>186</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>11</v>
@@ -6388,16 +6420,16 @@
         <v>113</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>147</v>
+        <v>319</v>
       </c>
       <c r="H88" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I88" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="J88" s="9"/>
-      <c r="K88" s="9"/>
+      <c r="I88" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
       <c r="L88" s="9"/>
       <c r="M88" s="9"/>
       <c r="N88" s="9"/>
@@ -6417,14 +6449,14 @@
       <c r="AB88" s="2"/>
     </row>
     <row r="89" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
-        <v>214</v>
+      <c r="A89" s="3" t="s">
+        <v>315</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>246</v>
+        <v>186</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>11</v>
@@ -6436,16 +6468,16 @@
         <v>113</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>147</v>
+        <v>320</v>
       </c>
       <c r="H89" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I89" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="J89" s="9"/>
-      <c r="K89" s="9"/>
+      <c r="I89" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="J89" s="6"/>
+      <c r="K89" s="6"/>
       <c r="L89" s="9"/>
       <c r="M89" s="9"/>
       <c r="N89" s="9"/>
@@ -6465,14 +6497,14 @@
       <c r="AB89" s="2"/>
     </row>
     <row r="90" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
-        <v>215</v>
+      <c r="A90" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>246</v>
+        <v>186</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>11</v>
@@ -6484,16 +6516,16 @@
         <v>113</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>147</v>
+        <v>192</v>
       </c>
       <c r="H90" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I90" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="J90" s="9"/>
-      <c r="K90" s="9"/>
+      <c r="I90" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
       <c r="L90" s="9"/>
       <c r="M90" s="9"/>
       <c r="N90" s="9"/>
@@ -6514,7 +6546,7 @@
     </row>
     <row r="91" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>293</v>
@@ -6538,7 +6570,7 @@
         <v>249</v>
       </c>
       <c r="I91" s="22" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="J91" s="9"/>
       <c r="K91" s="9"/>
@@ -6560,12 +6592,12 @@
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
     </row>
-    <row r="92" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
-        <v>217</v>
+    <row r="92" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>214</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>246</v>
@@ -6586,7 +6618,7 @@
         <v>249</v>
       </c>
       <c r="I92" s="22" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J92" s="9"/>
       <c r="K92" s="9"/>
@@ -6608,12 +6640,12 @@
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
     </row>
-    <row r="93" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="25" t="s">
-        <v>218</v>
+    <row r="93" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>246</v>
@@ -6634,7 +6666,7 @@
         <v>249</v>
       </c>
       <c r="I93" s="22" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
@@ -6656,9 +6688,9 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>293</v>
@@ -6682,7 +6714,7 @@
         <v>249</v>
       </c>
       <c r="I94" s="22" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
@@ -6706,10 +6738,10 @@
     </row>
     <row r="95" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>246</v>
@@ -6730,7 +6762,7 @@
         <v>249</v>
       </c>
       <c r="I95" s="22" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
@@ -6752,9 +6784,9 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
-        <v>221</v>
+    <row r="96" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A96" s="25" t="s">
+        <v>218</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>288</v>
@@ -6778,7 +6810,7 @@
         <v>249</v>
       </c>
       <c r="I96" s="22" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
@@ -6800,9 +6832,9 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
-        <v>222</v>
+    <row r="97" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>293</v>
@@ -6826,7 +6858,7 @@
         <v>249</v>
       </c>
       <c r="I97" s="22" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -6848,15 +6880,15 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="11" t="s">
-        <v>223</v>
+    <row r="98" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>11</v>
@@ -6868,13 +6900,13 @@
         <v>113</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>247</v>
+        <v>147</v>
       </c>
       <c r="H98" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I98" s="8" t="s">
-        <v>237</v>
+      <c r="I98" s="22" t="s">
+        <v>234</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -6896,15 +6928,15 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="11" t="s">
-        <v>225</v>
+    <row r="99" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>288</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>11</v>
@@ -6916,20 +6948,16 @@
         <v>113</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>247</v>
+        <v>147</v>
       </c>
       <c r="H99" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I99" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="J99" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="K99" s="20" t="s">
-        <v>240</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="J99" s="9"/>
+      <c r="K99" s="9"/>
       <c r="L99" s="9"/>
       <c r="M99" s="9"/>
       <c r="N99" s="9"/>
@@ -6948,15 +6976,15 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="11" t="s">
-        <v>226</v>
+    <row r="100" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>11</v>
@@ -6968,29 +6996,19 @@
         <v>113</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>247</v>
+        <v>147</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="I100" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="J100" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="K100" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="L100" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="M100" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="N100" s="20" t="s">
-        <v>245</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="J100" s="9"/>
+      <c r="K100" s="9"/>
+      <c r="L100" s="9"/>
+      <c r="M100" s="9"/>
+      <c r="N100" s="9"/>
       <c r="O100" s="2"/>
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
@@ -7006,17 +7024,17 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
-        <v>253</v>
+    <row r="101" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A101" s="11" t="s">
+        <v>223</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C101" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D101" s="9" t="s">
+      <c r="C101" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D101" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E101" s="7" t="s">
@@ -7025,14 +7043,14 @@
       <c r="F101" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G101" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="H101" s="20" t="s">
+      <c r="G101" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="H101" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I101" s="20" t="s">
-        <v>256</v>
+      <c r="I101" s="8" t="s">
+        <v>237</v>
       </c>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
@@ -7054,17 +7072,17 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>257</v>
+    <row r="102" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A102" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C102" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D102" s="9" t="s">
+      <c r="C102" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D102" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E102" s="7" t="s">
@@ -7073,17 +7091,21 @@
       <c r="F102" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G102" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="H102" s="20" t="s">
+      <c r="G102" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="H102" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I102" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="J102" s="9"/>
-      <c r="K102" s="9"/>
+      <c r="I102" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="J102" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="K102" s="20" t="s">
+        <v>240</v>
+      </c>
       <c r="L102" s="9"/>
       <c r="M102" s="9"/>
       <c r="N102" s="9"/>
@@ -7102,17 +7124,17 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>259</v>
+    <row r="103" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A103" s="11" t="s">
+        <v>226</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C103" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D103" s="9" t="s">
+      <c r="C103" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D103" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E103" s="7" t="s">
@@ -7121,20 +7143,30 @@
       <c r="F103" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G103" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="H103" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="I103" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="J103" s="9"/>
-      <c r="K103" s="9"/>
-      <c r="L103" s="9"/>
-      <c r="M103" s="9"/>
-      <c r="N103" s="9"/>
+      <c r="G103" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="H103" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I103" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="J103" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="K103" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="L103" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="M103" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="N103" s="20" t="s">
+        <v>245</v>
+      </c>
       <c r="O103" s="2"/>
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
@@ -7150,17 +7182,17 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="23" t="s">
-        <v>272</v>
+    <row r="104" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C104" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D104" s="24" t="s">
+      <c r="C104" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D104" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E104" s="7" t="s">
@@ -7169,21 +7201,17 @@
       <c r="F104" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G104" s="6" t="s">
-        <v>247</v>
+      <c r="G104" s="9" t="s">
+        <v>255</v>
       </c>
       <c r="H104" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="I104" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="J104" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="K104" s="20" t="s">
-        <v>275</v>
-      </c>
+      <c r="I104" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="J104" s="9"/>
+      <c r="K104" s="9"/>
       <c r="L104" s="9"/>
       <c r="M104" s="9"/>
       <c r="N104" s="9"/>
@@ -7202,17 +7230,17 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="11" t="s">
-        <v>274</v>
+    <row r="105" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>257</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C105" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="D105" s="6" t="s">
+      <c r="C105" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D105" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E105" s="7" t="s">
@@ -7221,17 +7249,17 @@
       <c r="F105" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G105" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H105" s="8" t="s">
+      <c r="G105" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="H105" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="I105" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="J105" s="20"/>
-      <c r="K105" s="20"/>
+      <c r="I105" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="J105" s="9"/>
+      <c r="K105" s="9"/>
       <c r="L105" s="9"/>
       <c r="M105" s="9"/>
       <c r="N105" s="9"/>
@@ -7250,17 +7278,17 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="11" t="s">
-        <v>282</v>
+    <row r="106" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C106" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D106" s="6" t="s">
+      <c r="C106" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D106" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E106" s="7" t="s">
@@ -7269,24 +7297,20 @@
       <c r="F106" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G106" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H106" s="8" t="s">
+      <c r="G106" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="H106" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="I106" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="J106" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="K106" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="L106" s="20"/>
-      <c r="M106" s="20"/>
-      <c r="N106" s="20"/>
+      <c r="I106" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="J106" s="9"/>
+      <c r="K106" s="9"/>
+      <c r="L106" s="9"/>
+      <c r="M106" s="9"/>
+      <c r="N106" s="9"/>
       <c r="O106" s="2"/>
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
@@ -7302,18 +7326,18 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="11" t="s">
-        <v>280</v>
+    <row r="107" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="23" t="s">
+        <v>272</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>288</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D107" s="6" t="s">
-        <v>14</v>
+        <v>224</v>
+      </c>
+      <c r="D107" s="24" t="s">
+        <v>11</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>113</v>
@@ -7322,14 +7346,20 @@
         <v>113</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H107" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="I107" s="9"/>
-      <c r="J107" s="9"/>
-      <c r="K107" s="9"/>
+        <v>247</v>
+      </c>
+      <c r="H107" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="I107" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="J107" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="K107" s="20" t="s">
+        <v>275</v>
+      </c>
       <c r="L107" s="9"/>
       <c r="M107" s="9"/>
       <c r="N107" s="9"/>
@@ -7348,18 +7378,18 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A108" s="27" t="s">
-        <v>291</v>
+    <row r="108" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="11" t="s">
+        <v>274</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>288</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>146</v>
+        <v>281</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E108" s="7" t="s">
         <v>113</v>
@@ -7367,54 +7397,96 @@
       <c r="F108" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G108" s="26" t="s">
-        <v>292</v>
+      <c r="G108" s="6" t="s">
+        <v>247</v>
       </c>
       <c r="H108" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I108" s="22" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="109" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>295</v>
+        <v>271</v>
+      </c>
+      <c r="J108" s="20"/>
+      <c r="K108" s="20"/>
+      <c r="L108" s="9"/>
+      <c r="M108" s="9"/>
+      <c r="N108" s="9"/>
+      <c r="O108" s="2"/>
+      <c r="P108" s="2"/>
+      <c r="Q108" s="2"/>
+      <c r="R108" s="2"/>
+      <c r="S108" s="2"/>
+      <c r="T108" s="2"/>
+      <c r="U108" s="2"/>
+      <c r="V108" s="2"/>
+      <c r="W108" s="2"/>
+      <c r="X108" s="2"/>
+      <c r="Y108" s="2"/>
+      <c r="Z108" s="2"/>
+      <c r="AA108" s="2"/>
+      <c r="AB108" s="2"/>
+    </row>
+    <row r="109" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A109" s="11" t="s">
+        <v>282</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E109" s="7" t="s">
         <v>113</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="G109" s="26" t="s">
-        <v>292</v>
+        <v>113</v>
+      </c>
+      <c r="G109" s="6" t="s">
+        <v>247</v>
       </c>
       <c r="H109" s="8" t="s">
         <v>249</v>
       </c>
       <c r="I109" s="22" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="110" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>298</v>
+        <v>273</v>
+      </c>
+      <c r="J109" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="K109" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="L109" s="20"/>
+      <c r="M109" s="20"/>
+      <c r="N109" s="20"/>
+      <c r="O109" s="2"/>
+      <c r="P109" s="2"/>
+      <c r="Q109" s="2"/>
+      <c r="R109" s="2"/>
+      <c r="S109" s="2"/>
+      <c r="T109" s="2"/>
+      <c r="U109" s="2"/>
+      <c r="V109" s="2"/>
+      <c r="W109" s="2"/>
+      <c r="X109" s="2"/>
+      <c r="Y109" s="2"/>
+      <c r="Z109" s="2"/>
+      <c r="AA109" s="2"/>
+      <c r="AB109" s="2"/>
+    </row>
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="11" t="s">
+        <v>280</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>146</v>
+        <v>10</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>14</v>
@@ -7425,22 +7497,39 @@
       <c r="F110" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G110" s="26" t="s">
-        <v>292</v>
+      <c r="G110" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I110" s="22" t="s">
-        <v>299</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="I110" s="9"/>
+      <c r="J110" s="9"/>
+      <c r="K110" s="9"/>
+      <c r="L110" s="9"/>
+      <c r="M110" s="9"/>
+      <c r="N110" s="9"/>
+      <c r="O110" s="2"/>
+      <c r="P110" s="2"/>
+      <c r="Q110" s="2"/>
+      <c r="R110" s="2"/>
+      <c r="S110" s="2"/>
+      <c r="T110" s="2"/>
+      <c r="U110" s="2"/>
+      <c r="V110" s="2"/>
+      <c r="W110" s="2"/>
+      <c r="X110" s="2"/>
+      <c r="Y110" s="2"/>
+      <c r="Z110" s="2"/>
+      <c r="AA110" s="2"/>
+      <c r="AB110" s="2"/>
     </row>
     <row r="111" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>305</v>
+      <c r="A111" s="27" t="s">
+        <v>291</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>146</v>
@@ -7461,12 +7550,12 @@
         <v>249</v>
       </c>
       <c r="I111" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="112" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>293</v>
@@ -7481,7 +7570,7 @@
         <v>113</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>113</v>
+        <v>296</v>
       </c>
       <c r="G112" s="26" t="s">
         <v>292</v>
@@ -7490,12 +7579,12 @@
         <v>249</v>
       </c>
       <c r="I112" s="22" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>293</v>
@@ -7519,12 +7608,12 @@
         <v>249</v>
       </c>
       <c r="I113" s="22" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>293</v>
@@ -7548,12 +7637,12 @@
         <v>249</v>
       </c>
       <c r="I114" s="22" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>293</v>
@@ -7577,12 +7666,12 @@
         <v>249</v>
       </c>
       <c r="I115" s="22" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>293</v>
@@ -7606,15 +7695,15 @@
         <v>249</v>
       </c>
       <c r="I116" s="22" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>146</v>
@@ -7635,17 +7724,98 @@
         <v>249</v>
       </c>
       <c r="I117" s="22" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>309</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F118" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G118" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H118" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I118" s="22" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>311</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F119" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G119" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H119" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I119" s="22" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>313</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G120" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H120" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="I120" s="22" t="s">
         <v>314</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I107" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I120" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified test methods in Admin
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(17-02-2023)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(02-01-2023)-Admin(2.3)encha\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B14CEC-E9B9-4C4C-A5CB-4382D262B845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07BE90B-41CA-417B-A99C-4BEDB36C4738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$119</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="321">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -445,15 +445,7 @@
 -plabelColumn</t>
   </si>
   <si>
-    <t>verify fee struture view</t>
-  </si>
-  <si>
     <t>feeStructureView</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.SystemSettingsTest,
-testViewPersonalFeeStructure,
--pexpViewHeading</t>
   </si>
   <si>
     <t>verify fee struture Edit</t>
@@ -469,14 +461,6 @@
 testEditMerchantFeeStructure,
 -pexpHeading,
 -pexpEditHeading</t>
-  </si>
-  <si>
-    <t>verify fee struture Merchant view</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.SystemSettingsTest,
-testViewMerchantfeeStructurePage,
--pexpViewHeading</t>
   </si>
   <si>
     <t>testdata-admin.xlsx,BalanceReport</t>
@@ -584,22 +568,6 @@
   <si>
     <t>coyni.admin.tests.AccountingTest,
 testTotalDepositsBankAccount,
--pwithdraw,
--pbatchId,
--pbID,
--pwithdrawId,
--prefrenceId,
--puserId,
--pnameOnBank,
--pheading,
--pexportPrepared</t>
-  </si>
-  <si>
-    <t>testTotalDepositSignetAccount</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.AccountingTest,
-testTotalDepositSignetAccount,
 -pwithdraw,
 -pbatchId,
 -pbID,
@@ -1012,11 +980,6 @@
   </si>
   <si>
     <t>testdata-admin.xlsx,Disputes</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.DisputesTest,
-VerifyFilter,
--pfilterHeadings</t>
   </si>
   <si>
     <t>Verify case num filter won dispaly</t>
@@ -1661,9 +1624,6 @@
 -pfiveTimeContent</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>tes+A28tData-admin.xlsx,AddCogentAccount</t>
   </si>
   <si>
@@ -1824,6 +1784,36 @@
     <t>coyni.admin.tests.HomeTest,
 tesGobalSearchWithBankNumber,
 -pbankAccount</t>
+  </si>
+  <si>
+    <t>Merchant user  Details  with Payout Transaction Switch to window example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.admin.tests.AccountingTest,
+testSwitchToWindow
+</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.DisputesTest,
+VerifyFilter,
+-pfilterHeadings,
+-pstartDate</t>
+  </si>
+  <si>
+    <t>testTotalDepositCogentAccount</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.AccountingTest,
+testTotalDepositCogentAccount,
+-pwithdraw,
+-pbatchId,
+-pbID,
+-pwithdrawId,
+-prefrenceId,
+-puserId,
+-pnameOnBank,
+-pheading,
+-pexportPrepared</t>
   </si>
 </sst>
 </file>
@@ -1877,7 +1867,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1899,6 +1889,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1941,7 +1937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1990,6 +1986,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2270,10 +2268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB120"/>
+  <dimension ref="A1:AB119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,7 +2331,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>
@@ -2342,16 +2340,16 @@
         <v>11</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -2376,10 +2374,10 @@
     </row>
     <row r="3" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>10</v>
@@ -2388,16 +2386,16 @@
         <v>14</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -2425,7 +2423,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>10</v>
@@ -2434,10 +2432,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>12</v>
@@ -2471,7 +2469,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
@@ -2480,16 +2478,16 @@
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -2514,10 +2512,10 @@
     </row>
     <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>10</v>
@@ -2526,16 +2524,16 @@
         <v>14</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -2563,7 +2561,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>27</v>
@@ -2572,16 +2570,16 @@
         <v>14</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -2609,7 +2607,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>27</v>
@@ -2618,16 +2616,16 @@
         <v>14</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -2655,7 +2653,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>27</v>
@@ -2664,10 +2662,10 @@
         <v>14</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>28</v>
@@ -2701,7 +2699,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>27</v>
@@ -2710,10 +2708,10 @@
         <v>14</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>28</v>
@@ -2747,7 +2745,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>35</v>
@@ -2756,10 +2754,10 @@
         <v>11</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>36</v>
@@ -2793,7 +2791,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>35</v>
@@ -2802,10 +2800,10 @@
         <v>11</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>36</v>
@@ -2839,7 +2837,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>35</v>
@@ -2885,7 +2883,7 @@
         <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>35</v>
@@ -2931,7 +2929,7 @@
         <v>44</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>35</v>
@@ -2974,10 +2972,10 @@
     </row>
     <row r="16" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>10</v>
@@ -2986,19 +2984,19 @@
         <v>11</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
@@ -3022,31 +3020,31 @@
     </row>
     <row r="17" spans="1:28" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -3070,31 +3068,31 @@
     </row>
     <row r="18" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -3118,31 +3116,31 @@
     </row>
     <row r="19" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -3166,31 +3164,31 @@
     </row>
     <row r="20" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -3217,7 +3215,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>10</v>
@@ -3226,16 +3224,16 @@
         <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -3263,7 +3261,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>18</v>
@@ -3272,19 +3270,19 @@
         <v>11</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -3311,7 +3309,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
@@ -3320,16 +3318,16 @@
         <v>11</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>21</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>22</v>
@@ -3359,7 +3357,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>18</v>
@@ -3368,16 +3366,16 @@
         <v>11</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>24</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>25</v>
@@ -3404,13 +3402,13 @@
     </row>
     <row r="25" spans="1:28" ht="270" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>11</v>
@@ -3422,13 +3420,13 @@
         <v>1</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -3452,13 +3450,13 @@
     </row>
     <row r="26" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>14</v>
@@ -3470,13 +3468,13 @@
         <v>2</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -3500,13 +3498,13 @@
     </row>
     <row r="27" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>11</v>
@@ -3518,13 +3516,13 @@
         <v>1</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -3548,31 +3546,31 @@
     </row>
     <row r="28" spans="1:28" ht="285" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -3596,10 +3594,10 @@
     </row>
     <row r="29" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>18</v>
@@ -3608,19 +3606,19 @@
         <v>11</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -3630,10 +3628,10 @@
     </row>
     <row r="30" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>18</v>
@@ -3642,19 +3640,19 @@
         <v>14</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -3678,10 +3676,10 @@
     </row>
     <row r="31" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>18</v>
@@ -3690,19 +3688,19 @@
         <v>14</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I31" s="20" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -3726,10 +3724,10 @@
     </row>
     <row r="32" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>18</v>
@@ -3738,19 +3736,19 @@
         <v>11</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3774,10 +3772,10 @@
     </row>
     <row r="33" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>18</v>
@@ -3786,19 +3784,19 @@
         <v>11</v>
       </c>
       <c r="E33" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="I33" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>119</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -3822,10 +3820,10 @@
     </row>
     <row r="34" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>18</v>
@@ -3834,19 +3832,19 @@
         <v>11</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -3870,10 +3868,10 @@
     </row>
     <row r="35" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>18</v>
@@ -3882,19 +3880,19 @@
         <v>11</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -3918,10 +3916,10 @@
     </row>
     <row r="36" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>18</v>
@@ -3930,19 +3928,19 @@
         <v>11</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -3969,7 +3967,7 @@
         <v>46</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>47</v>
@@ -3978,16 +3976,16 @@
         <v>11</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>48</v>
@@ -4014,10 +4012,10 @@
     </row>
     <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>47</v>
@@ -4026,19 +4024,19 @@
         <v>11</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="9"/>
@@ -4065,7 +4063,7 @@
         <v>49</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>47</v>
@@ -4074,16 +4072,16 @@
         <v>11</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>50</v>
@@ -4113,7 +4111,7 @@
         <v>51</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>47</v>
@@ -4122,16 +4120,16 @@
         <v>11</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>52</v>
@@ -4161,7 +4159,7 @@
         <v>53</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>47</v>
@@ -4170,16 +4168,16 @@
         <v>11</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I41" s="8" t="s">
         <v>54</v>
@@ -4209,7 +4207,7 @@
         <v>55</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>47</v>
@@ -4218,16 +4216,16 @@
         <v>11</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>56</v>
@@ -4257,7 +4255,7 @@
         <v>57</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>47</v>
@@ -4266,16 +4264,16 @@
         <v>11</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I43" s="8" t="s">
         <v>58</v>
@@ -4305,7 +4303,7 @@
         <v>59</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>60</v>
@@ -4314,19 +4312,19 @@
         <v>11</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -4353,7 +4351,7 @@
         <v>62</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>60</v>
@@ -4362,16 +4360,16 @@
         <v>11</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>63</v>
@@ -4401,7 +4399,7 @@
         <v>64</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>60</v>
@@ -4410,16 +4408,16 @@
         <v>11</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>65</v>
@@ -4449,7 +4447,7 @@
         <v>66</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>60</v>
@@ -4458,16 +4456,16 @@
         <v>11</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I47" s="8" t="s">
         <v>67</v>
@@ -4497,7 +4495,7 @@
         <v>68</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>60</v>
@@ -4506,16 +4504,16 @@
         <v>11</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>69</v>
@@ -4545,7 +4543,7 @@
         <v>70</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>60</v>
@@ -4554,16 +4552,16 @@
         <v>11</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>72</v>
@@ -4593,7 +4591,7 @@
         <v>73</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>60</v>
@@ -4602,16 +4600,16 @@
         <v>11</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I50" s="8" t="s">
         <v>74</v>
@@ -4638,10 +4636,10 @@
     </row>
     <row r="51" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>60</v>
@@ -4650,19 +4648,19 @@
         <v>11</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -4689,7 +4687,7 @@
         <v>75</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>60</v>
@@ -4698,16 +4696,16 @@
         <v>11</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I52" s="8" t="s">
         <v>76</v>
@@ -4734,31 +4732,31 @@
     </row>
     <row r="53" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C53" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G53" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D53" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>169</v>
-      </c>
       <c r="H53" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -4781,32 +4779,32 @@
       <c r="AB53" s="2"/>
     </row>
     <row r="54" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
-        <v>174</v>
+      <c r="A54" s="29" t="s">
+        <v>168</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -4829,32 +4827,32 @@
       <c r="AB54" s="2"/>
     </row>
     <row r="55" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
-        <v>98</v>
+      <c r="A55" s="29" t="s">
+        <v>94</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -4877,32 +4875,32 @@
       <c r="AB55" s="2"/>
     </row>
     <row r="56" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
-        <v>101</v>
+      <c r="A56" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -4925,32 +4923,32 @@
       <c r="AB56" s="2"/>
     </row>
     <row r="57" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>103</v>
+      <c r="A57" s="29" t="s">
+        <v>99</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
@@ -4973,32 +4971,32 @@
       <c r="AB57" s="2"/>
     </row>
     <row r="58" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
-        <v>105</v>
+      <c r="A58" s="29" t="s">
+        <v>101</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
@@ -5021,32 +5019,32 @@
       <c r="AB58" s="2"/>
     </row>
     <row r="59" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
-        <v>107</v>
+      <c r="A59" s="29" t="s">
+        <v>103</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
@@ -5069,32 +5067,32 @@
       <c r="AB59" s="2"/>
     </row>
     <row r="60" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A60" s="25" t="s">
-        <v>109</v>
+      <c r="A60" s="28" t="s">
+        <v>319</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>110</v>
+        <v>320</v>
       </c>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -5117,32 +5115,32 @@
       <c r="AB60" s="2"/>
     </row>
     <row r="61" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
-        <v>111</v>
+      <c r="A61" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -5166,31 +5164,31 @@
     </row>
     <row r="62" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -5214,31 +5212,31 @@
     </row>
     <row r="63" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -5262,31 +5260,31 @@
     </row>
     <row r="64" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -5309,11 +5307,11 @@
       <c r="AB64" s="2"/>
     </row>
     <row r="65" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="29" t="s">
         <v>77</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>78</v>
@@ -5322,16 +5320,16 @@
         <v>11</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>79</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I65" s="8" t="s">
         <v>80</v>
@@ -5358,10 +5356,10 @@
     </row>
     <row r="66" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C66" s="18" t="s">
         <v>78</v>
@@ -5370,19 +5368,19 @@
         <v>11</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -5405,11 +5403,11 @@
       <c r="AB66" s="2"/>
     </row>
     <row r="67" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
-        <v>81</v>
+      <c r="A67" s="29" t="s">
+        <v>82</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>78</v>
@@ -5418,19 +5416,19 @@
         <v>11</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -5453,11 +5451,11 @@
       <c r="AB67" s="2"/>
     </row>
     <row r="68" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="29" t="s">
         <v>84</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>78</v>
@@ -5466,19 +5464,19 @@
         <v>11</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G68" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H68" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="I68" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="H68" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="I68" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -5500,33 +5498,33 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -5548,33 +5546,33 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>88</v>
+    <row r="70" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="21" t="s">
+        <v>202</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C70" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C70" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>82</v>
+        <v>204</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>89</v>
+        <v>203</v>
       </c>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -5598,31 +5596,31 @@
     </row>
     <row r="71" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C71" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>136</v>
-      </c>
       <c r="D71" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -5644,33 +5642,33 @@
       <c r="AA71" s="2"/>
       <c r="AB71" s="2"/>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="21" t="s">
-        <v>209</v>
+    <row r="72" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="11" t="s">
+        <v>123</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>78</v>
+        <v>286</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>211</v>
+        <v>121</v>
       </c>
       <c r="H72" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>210</v>
+        <v>132</v>
       </c>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -5692,81 +5690,67 @@
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
-        <v>128</v>
+    <row r="73" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>127</v>
+        <v>177</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
       <c r="N73" s="9"/>
-      <c r="O73" s="2"/>
-      <c r="P73" s="2"/>
-      <c r="Q73" s="2"/>
-      <c r="R73" s="2"/>
-      <c r="S73" s="2"/>
-      <c r="T73" s="2"/>
-      <c r="U73" s="2"/>
-      <c r="V73" s="2"/>
-      <c r="W73" s="2"/>
-      <c r="X73" s="2"/>
-      <c r="Y73" s="2"/>
-      <c r="Z73" s="2"/>
-      <c r="AA73" s="2"/>
-      <c r="AB73" s="2"/>
-    </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>129</v>
+    </row>
+    <row r="74" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>127</v>
+        <v>177</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="I74" s="8" t="s">
-        <v>138</v>
+        <v>243</v>
+      </c>
+      <c r="I74" s="22" t="s">
+        <v>205</v>
       </c>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
@@ -5788,67 +5772,81 @@
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
     </row>
-    <row r="75" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
+    <row r="75" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C75" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>146</v>
-      </c>
       <c r="D75" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="I75" s="8" t="s">
-        <v>141</v>
+        <v>243</v>
+      </c>
+      <c r="I75" s="22" t="s">
+        <v>138</v>
       </c>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
       <c r="N75" s="9"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="2"/>
+      <c r="Q75" s="2"/>
+      <c r="R75" s="2"/>
+      <c r="S75" s="2"/>
+      <c r="T75" s="2"/>
+      <c r="U75" s="2"/>
+      <c r="V75" s="2"/>
+      <c r="W75" s="2"/>
+      <c r="X75" s="2"/>
+      <c r="Y75" s="2"/>
+      <c r="Z75" s="2"/>
+      <c r="AA75" s="2"/>
+      <c r="AB75" s="2"/>
     </row>
     <row r="76" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H76" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="I76" s="22" t="s">
         <v>142</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="H76" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="I76" s="22" t="s">
-        <v>212</v>
       </c>
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
@@ -5875,25 +5873,25 @@
         <v>143</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>183</v>
+        <v>141</v>
       </c>
       <c r="H77" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I77" s="22" t="s">
         <v>144</v>
@@ -5923,28 +5921,28 @@
         <v>145</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C78" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H78" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="I78" s="22" t="s">
         <v>146</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G78" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H78" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="I78" s="22" t="s">
-        <v>148</v>
       </c>
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
@@ -5966,36 +5964,36 @@
       <c r="AA78" s="2"/>
       <c r="AB78" s="2"/>
     </row>
-    <row r="79" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>149</v>
+    <row r="79" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A79" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="H79" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="I79" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="J79" s="9"/>
-      <c r="K79" s="9"/>
+        <v>243</v>
+      </c>
+      <c r="I79" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
       <c r="N79" s="9"/>
@@ -6014,35 +6012,35 @@
       <c r="AA79" s="2"/>
       <c r="AB79" s="2"/>
     </row>
-    <row r="80" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>151</v>
+    <row r="80" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A80" s="11" t="s">
+        <v>191</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="I80" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="J80" s="9"/>
+        <v>243</v>
+      </c>
+      <c r="I80" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="J80" s="8"/>
       <c r="K80" s="9"/>
       <c r="L80" s="9"/>
       <c r="M80" s="9"/>
@@ -6062,36 +6060,36 @@
       <c r="AA80" s="2"/>
       <c r="AB80" s="2"/>
     </row>
-    <row r="81" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="H81" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="J81" s="6"/>
-      <c r="K81" s="6"/>
+        <v>194</v>
+      </c>
+      <c r="J81" s="8"/>
+      <c r="K81" s="9"/>
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
       <c r="N81" s="9"/>
@@ -6110,35 +6108,37 @@
       <c r="AA81" s="2"/>
       <c r="AB81" s="2"/>
     </row>
-    <row r="82" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G82" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="H82" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="I82" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="J82" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="H82" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="I82" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J82" s="8"/>
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
@@ -6158,36 +6158,36 @@
       <c r="AA82" s="2"/>
       <c r="AB82" s="2"/>
     </row>
-    <row r="83" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
-        <v>200</v>
+    <row r="83" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="H83" s="8" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="I83" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="J83" s="8"/>
-      <c r="K83" s="9"/>
+        <v>181</v>
+      </c>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
       <c r="L83" s="9"/>
       <c r="M83" s="9"/>
       <c r="N83" s="9"/>
@@ -6206,38 +6206,36 @@
       <c r="AA83" s="2"/>
       <c r="AB83" s="2"/>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
-        <v>202</v>
+    <row r="84" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H84" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="J84" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="K84" s="9"/>
+        <v>184</v>
+      </c>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
       <c r="L84" s="9"/>
       <c r="M84" s="9"/>
       <c r="N84" s="9"/>
@@ -6258,31 +6256,31 @@
     </row>
     <row r="85" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>184</v>
+        <v>313</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>185</v>
+        <v>314</v>
       </c>
       <c r="H85" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>187</v>
+        <v>315</v>
       </c>
       <c r="J85" s="6"/>
       <c r="K85" s="6"/>
@@ -6306,31 +6304,31 @@
     </row>
     <row r="86" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>188</v>
+        <v>309</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>189</v>
+        <v>311</v>
       </c>
       <c r="H86" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>190</v>
+        <v>310</v>
       </c>
       <c r="J86" s="6"/>
       <c r="K86" s="6"/>
@@ -6354,31 +6352,31 @@
     </row>
     <row r="87" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="H87" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
@@ -6402,31 +6400,31 @@
     </row>
     <row r="88" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>317</v>
+        <v>185</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C88" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G88" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="D88" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G88" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="H88" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>318</v>
+        <v>187</v>
       </c>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
@@ -6449,35 +6447,35 @@
       <c r="AB88" s="2"/>
     </row>
     <row r="89" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>315</v>
+      <c r="A89" s="6" t="s">
+        <v>206</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>186</v>
+        <v>239</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>320</v>
+        <v>141</v>
       </c>
       <c r="H89" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I89" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="J89" s="6"/>
-      <c r="K89" s="6"/>
+        <v>242</v>
+      </c>
+      <c r="I89" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="J89" s="9"/>
+      <c r="K89" s="9"/>
       <c r="L89" s="9"/>
       <c r="M89" s="9"/>
       <c r="N89" s="9"/>
@@ -6497,35 +6495,35 @@
       <c r="AB89" s="2"/>
     </row>
     <row r="90" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>191</v>
+      <c r="A90" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>186</v>
+        <v>239</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>192</v>
+        <v>141</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I90" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="J90" s="6"/>
-      <c r="K90" s="6"/>
+        <v>242</v>
+      </c>
+      <c r="I90" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="J90" s="9"/>
+      <c r="K90" s="9"/>
       <c r="L90" s="9"/>
       <c r="M90" s="9"/>
       <c r="N90" s="9"/>
@@ -6546,31 +6544,31 @@
     </row>
     <row r="91" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I91" s="22" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J91" s="9"/>
       <c r="K91" s="9"/>
@@ -6594,31 +6592,31 @@
     </row>
     <row r="92" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I92" s="22" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J92" s="9"/>
       <c r="K92" s="9"/>
@@ -6641,32 +6639,32 @@
       <c r="AB92" s="2"/>
     </row>
     <row r="93" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
-        <v>215</v>
+      <c r="A93" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I93" s="22" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
@@ -6689,32 +6687,32 @@
       <c r="AB93" s="2"/>
     </row>
     <row r="94" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
-        <v>216</v>
+      <c r="A94" s="25" t="s">
+        <v>211</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H94" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I94" s="22" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
@@ -6736,33 +6734,33 @@
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
     </row>
-    <row r="95" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>217</v>
+    <row r="95" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I95" s="22" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
@@ -6785,32 +6783,32 @@
       <c r="AB95" s="2"/>
     </row>
     <row r="96" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A96" s="25" t="s">
-        <v>218</v>
+      <c r="A96" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H96" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I96" s="22" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
@@ -6832,33 +6830,33 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
-        <v>219</v>
+    <row r="97" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I97" s="22" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -6882,31 +6880,31 @@
     </row>
     <row r="98" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H98" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I98" s="22" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -6928,33 +6926,33 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
-        <v>221</v>
+    <row r="99" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
+        <v>216</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>147</v>
+        <v>240</v>
       </c>
       <c r="H99" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I99" s="22" t="s">
-        <v>235</v>
+        <v>242</v>
+      </c>
+      <c r="I99" s="8" t="s">
+        <v>230</v>
       </c>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -6976,36 +6974,40 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
-        <v>222</v>
+    <row r="100" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A100" s="11" t="s">
+        <v>218</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>147</v>
+        <v>240</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I100" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="J100" s="9"/>
-      <c r="K100" s="9"/>
+        <v>231</v>
+      </c>
+      <c r="J100" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="K100" s="20" t="s">
+        <v>233</v>
+      </c>
       <c r="L100" s="9"/>
       <c r="M100" s="9"/>
       <c r="N100" s="9"/>
@@ -7026,37 +7028,47 @@
     </row>
     <row r="101" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I101" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="I101" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="J101" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="K101" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="L101" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="M101" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="J101" s="9"/>
-      <c r="K101" s="9"/>
-      <c r="L101" s="9"/>
-      <c r="M101" s="9"/>
-      <c r="N101" s="9"/>
+      <c r="N101" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="O101" s="2"/>
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
@@ -7072,40 +7084,36 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A102" s="11" t="s">
-        <v>225</v>
+    <row r="102" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D102" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D102" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G102" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H102" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G102" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="H102" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="I102" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="I102" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="J102" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="K102" s="20" t="s">
-        <v>240</v>
-      </c>
+      <c r="J102" s="9"/>
+      <c r="K102" s="9"/>
       <c r="L102" s="9"/>
       <c r="M102" s="9"/>
       <c r="N102" s="9"/>
@@ -7124,49 +7132,39 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
-      <c r="A103" s="11" t="s">
-        <v>226</v>
+    <row r="103" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D103" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D103" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G103" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H103" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="I103" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="J103" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="H103" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="K103" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="L103" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="M103" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="N103" s="20" t="s">
-        <v>245</v>
-      </c>
+      <c r="I103" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="J103" s="9"/>
+      <c r="K103" s="9"/>
+      <c r="L103" s="9"/>
+      <c r="M103" s="9"/>
+      <c r="N103" s="9"/>
       <c r="O103" s="2"/>
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
@@ -7182,33 +7180,33 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G104" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="H104" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="I104" s="20" t="s">
         <v>253</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C104" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D104" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E104" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F104" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G104" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="H104" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="I104" s="20" t="s">
-        <v>256</v>
       </c>
       <c r="J104" s="9"/>
       <c r="K104" s="9"/>
@@ -7230,36 +7228,40 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>257</v>
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="23" t="s">
+        <v>265</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C105" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D105" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D105" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G105" s="9" t="s">
-        <v>255</v>
+        <v>107</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="H105" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="I105" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="J105" s="9"/>
-      <c r="K105" s="9"/>
+        <v>242</v>
+      </c>
+      <c r="I105" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="J105" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="K105" s="20" t="s">
+        <v>268</v>
+      </c>
       <c r="L105" s="9"/>
       <c r="M105" s="9"/>
       <c r="N105" s="9"/>
@@ -7278,36 +7280,36 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>259</v>
+    <row r="106" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="11" t="s">
+        <v>267</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D106" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D106" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G106" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="H106" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="I106" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="J106" s="9"/>
-      <c r="K106" s="9"/>
+        <v>107</v>
+      </c>
+      <c r="G106" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="H106" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="I106" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="J106" s="20"/>
+      <c r="K106" s="20"/>
       <c r="L106" s="9"/>
       <c r="M106" s="9"/>
       <c r="N106" s="9"/>
@@ -7326,43 +7328,43 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="23" t="s">
-        <v>272</v>
+    <row r="107" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A107" s="11" t="s">
+        <v>275</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D107" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="D107" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H107" s="20" t="s">
-        <v>249</v>
+        <v>240</v>
+      </c>
+      <c r="H107" s="8" t="s">
+        <v>242</v>
       </c>
       <c r="I107" s="22" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="J107" s="20" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="K107" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="L107" s="9"/>
-      <c r="M107" s="9"/>
-      <c r="N107" s="9"/>
+        <v>268</v>
+      </c>
+      <c r="L107" s="20"/>
+      <c r="M107" s="20"/>
+      <c r="N107" s="20"/>
       <c r="O107" s="2"/>
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
@@ -7380,34 +7382,32 @@
     </row>
     <row r="108" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>281</v>
+        <v>10</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>247</v>
+        <v>12</v>
       </c>
       <c r="H108" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I108" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="J108" s="20"/>
-      <c r="K108" s="20"/>
+        <v>280</v>
+      </c>
+      <c r="I108" s="9"/>
+      <c r="J108" s="9"/>
+      <c r="K108" s="9"/>
       <c r="L108" s="9"/>
       <c r="M108" s="9"/>
       <c r="N108" s="9"/>
@@ -7426,396 +7426,327 @@
       <c r="AA108" s="2"/>
       <c r="AB108" s="2"/>
     </row>
-    <row r="109" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A109" s="11" t="s">
-        <v>282</v>
+    <row r="109" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A109" s="27" t="s">
+        <v>283</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>224</v>
+        <v>140</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G109" s="6" t="s">
-        <v>247</v>
+        <v>107</v>
+      </c>
+      <c r="G109" s="26" t="s">
+        <v>284</v>
       </c>
       <c r="H109" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I109" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="J109" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="K109" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="L109" s="20"/>
-      <c r="M109" s="20"/>
-      <c r="N109" s="20"/>
-      <c r="O109" s="2"/>
-      <c r="P109" s="2"/>
-      <c r="Q109" s="2"/>
-      <c r="R109" s="2"/>
-      <c r="S109" s="2"/>
-      <c r="T109" s="2"/>
-      <c r="U109" s="2"/>
-      <c r="V109" s="2"/>
-      <c r="W109" s="2"/>
-      <c r="X109" s="2"/>
-      <c r="Y109" s="2"/>
-      <c r="Z109" s="2"/>
-      <c r="AA109" s="2"/>
-      <c r="AB109" s="2"/>
-    </row>
-    <row r="110" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="11" t="s">
-        <v>280</v>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="110" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>287</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G110" s="6" t="s">
-        <v>12</v>
+        <v>288</v>
+      </c>
+      <c r="G110" s="26" t="s">
+        <v>284</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="I110" s="9"/>
-      <c r="J110" s="9"/>
-      <c r="K110" s="9"/>
-      <c r="L110" s="9"/>
-      <c r="M110" s="9"/>
-      <c r="N110" s="9"/>
-      <c r="O110" s="2"/>
-      <c r="P110" s="2"/>
-      <c r="Q110" s="2"/>
-      <c r="R110" s="2"/>
-      <c r="S110" s="2"/>
-      <c r="T110" s="2"/>
-      <c r="U110" s="2"/>
-      <c r="V110" s="2"/>
-      <c r="W110" s="2"/>
-      <c r="X110" s="2"/>
-      <c r="Y110" s="2"/>
-      <c r="Z110" s="2"/>
-      <c r="AA110" s="2"/>
-      <c r="AB110" s="2"/>
+        <v>242</v>
+      </c>
+      <c r="I110" s="22" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="111" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A111" s="27" t="s">
-        <v>291</v>
+      <c r="A111" t="s">
+        <v>290</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F111" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G111" s="26" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H111" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I111" s="22" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="112" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>296</v>
+        <v>107</v>
       </c>
       <c r="G112" s="26" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H112" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I112" s="22" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G113" s="26" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H113" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I113" s="22" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G114" s="26" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H114" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I114" s="22" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G115" s="26" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H115" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I115" s="22" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G116" s="26" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H116" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I116" s="22" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F117" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G117" s="26" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H117" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I117" s="22" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F118" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G118" s="26" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H118" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I118" s="22" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F119" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G119" s="26" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H119" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I119" s="22" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>313</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E120" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F120" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G120" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="H120" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I120" s="22" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I120" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I119" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added test method for agreements privacy policy
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Web(02-01-2023)-Admin(2.3)encha\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(06-03-2023)Agreements\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5811F2E8-F9DC-486F-B907-CA4EB137E42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC0907C-4EAA-4C9D-8C74-8BDEC3B9A48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$122</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="327">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1821,6 +1821,28 @@
   <si>
     <t>coyni.admin.tests.SystemSettingsTest,
 testTermOfServiceAgreements,
+-pAgreementList,
+-pfolderName,
+-pfileName,
+-ptosHeading</t>
+  </si>
+  <si>
+    <t>Verify  Agreements Privacy policy</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.SystemSettingsTest,
+testPrivacyPolicyAgreements,
+-pAgreementList,
+-pfolderName,
+-pfileName,
+-ptosHeading</t>
+  </si>
+  <si>
+    <t>Verify  Agreements Application Acknowledgement</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.SystemSettingsTest,
+testApplicationAcknowledgementAgreements,
 -pAgreementList,
 -pfolderName,
 -pfileName,
@@ -2279,10 +2301,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB120"/>
+  <dimension ref="A1:AB122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="D66" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5370,7 +5392,7 @@
         <v>320</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>78</v>
@@ -5385,7 +5407,7 @@
         <v>106</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>140</v>
+        <v>321</v>
       </c>
       <c r="H66" s="8" t="s">
         <v>241</v>
@@ -5413,17 +5435,17 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="21" t="s">
-        <v>199</v>
+    <row r="67" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>323</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C67" s="18" t="s">
+      <c r="C67" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D67" s="18" t="s">
+      <c r="D67" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="7" t="s">
@@ -5432,14 +5454,14 @@
       <c r="F67" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G67" s="18" t="s">
-        <v>80</v>
+      <c r="G67" s="6" t="s">
+        <v>321</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="I67" s="8" t="s">
-        <v>200</v>
+        <v>241</v>
+      </c>
+      <c r="I67" s="22" t="s">
+        <v>324</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -5461,12 +5483,12 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>81</v>
+        <v>325</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>78</v>
@@ -5481,13 +5503,13 @@
         <v>106</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>82</v>
+        <v>321</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="I68" s="8" t="s">
-        <v>127</v>
+        <v>241</v>
+      </c>
+      <c r="I68" s="22" t="s">
+        <v>326</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -5510,16 +5532,16 @@
       <c r="AB68" s="2"/>
     </row>
     <row r="69" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>83</v>
+      <c r="A69" s="21" t="s">
+        <v>199</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D69" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="7" t="s">
@@ -5528,14 +5550,14 @@
       <c r="F69" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G69" s="6" t="s">
-        <v>82</v>
+      <c r="G69" s="18" t="s">
+        <v>80</v>
       </c>
       <c r="H69" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>84</v>
+        <v>200</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -5557,15 +5579,15 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>123</v>
+    <row r="70" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>11</v>
@@ -5577,13 +5599,13 @@
         <v>106</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="H70" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -5605,14 +5627,14 @@
       <c r="AA70" s="2"/>
       <c r="AB70" s="2"/>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="141.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="21" t="s">
-        <v>201</v>
+    <row r="71" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C71" s="18" t="s">
+      <c r="C71" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D71" s="6" t="s">
@@ -5625,13 +5647,13 @@
         <v>106</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>203</v>
+        <v>82</v>
       </c>
       <c r="H71" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>202</v>
+        <v>84</v>
       </c>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -5655,7 +5677,7 @@
     </row>
     <row r="72" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>284</v>
@@ -5679,7 +5701,7 @@
         <v>242</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -5701,15 +5723,15 @@
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
-        <v>122</v>
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="141.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="21" t="s">
+        <v>201</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C73" s="6" t="s">
-        <v>129</v>
+      <c r="C73" s="18" t="s">
+        <v>78</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>11</v>
@@ -5721,13 +5743,13 @@
         <v>106</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>120</v>
+        <v>203</v>
       </c>
       <c r="H73" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>131</v>
+        <v>202</v>
       </c>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -5749,15 +5771,15 @@
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
     </row>
-    <row r="74" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>133</v>
+    <row r="74" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>11</v>
@@ -5769,29 +5791,43 @@
         <v>106</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>176</v>
+        <v>120</v>
       </c>
       <c r="H74" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
       <c r="N74" s="9"/>
-    </row>
-    <row r="75" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>135</v>
+      <c r="O74" s="2"/>
+      <c r="P74" s="2"/>
+      <c r="Q74" s="2"/>
+      <c r="R74" s="2"/>
+      <c r="S74" s="2"/>
+      <c r="T74" s="2"/>
+      <c r="U74" s="2"/>
+      <c r="V74" s="2"/>
+      <c r="W74" s="2"/>
+      <c r="X74" s="2"/>
+      <c r="Y74" s="2"/>
+      <c r="Z74" s="2"/>
+      <c r="AA74" s="2"/>
+      <c r="AB74" s="2"/>
+    </row>
+    <row r="75" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
+        <v>122</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>11</v>
@@ -5803,13 +5839,13 @@
         <v>106</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>176</v>
+        <v>120</v>
       </c>
       <c r="H75" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="I75" s="22" t="s">
-        <v>204</v>
+      <c r="I75" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
@@ -5831,9 +5867,9 @@
       <c r="AA75" s="2"/>
       <c r="AB75" s="2"/>
     </row>
-    <row r="76" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>136</v>
+    <row r="76" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>284</v>
@@ -5856,32 +5892,18 @@
       <c r="H76" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="I76" s="22" t="s">
-        <v>137</v>
+      <c r="I76" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
       <c r="N76" s="9"/>
-      <c r="O76" s="2"/>
-      <c r="P76" s="2"/>
-      <c r="Q76" s="2"/>
-      <c r="R76" s="2"/>
-      <c r="S76" s="2"/>
-      <c r="T76" s="2"/>
-      <c r="U76" s="2"/>
-      <c r="V76" s="2"/>
-      <c r="W76" s="2"/>
-      <c r="X76" s="2"/>
-      <c r="Y76" s="2"/>
-      <c r="Z76" s="2"/>
-      <c r="AA76" s="2"/>
-      <c r="AB76" s="2"/>
     </row>
     <row r="77" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>284</v>
@@ -5899,13 +5921,13 @@
         <v>106</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="H77" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I77" s="22" t="s">
-        <v>141</v>
+        <v>204</v>
       </c>
       <c r="J77" s="9"/>
       <c r="K77" s="9"/>
@@ -5929,7 +5951,7 @@
     </row>
     <row r="78" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>284</v>
@@ -5947,13 +5969,13 @@
         <v>106</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="H78" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I78" s="22" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
@@ -5977,7 +5999,7 @@
     </row>
     <row r="79" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>284</v>
@@ -6001,7 +6023,7 @@
         <v>242</v>
       </c>
       <c r="I79" s="22" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
@@ -6023,15 +6045,15 @@
       <c r="AA79" s="2"/>
       <c r="AB79" s="2"/>
     </row>
-    <row r="80" spans="1:28" s="1" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
-        <v>155</v>
+    <row r="80" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>11</v>
@@ -6043,16 +6065,16 @@
         <v>106</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="H80" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="I80" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="J80" s="6"/>
-      <c r="K80" s="6"/>
+      <c r="I80" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
       <c r="L80" s="9"/>
       <c r="M80" s="9"/>
       <c r="N80" s="9"/>
@@ -6071,15 +6093,15 @@
       <c r="AA80" s="2"/>
       <c r="AB80" s="2"/>
     </row>
-    <row r="81" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
-        <v>190</v>
+    <row r="81" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>11</v>
@@ -6091,15 +6113,15 @@
         <v>106</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="H81" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="I81" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="J81" s="8"/>
+      <c r="I81" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="J81" s="9"/>
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
@@ -6119,15 +6141,15 @@
       <c r="AA81" s="2"/>
       <c r="AB81" s="2"/>
     </row>
-    <row r="82" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" s="1" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>11</v>
@@ -6145,10 +6167,10 @@
         <v>242</v>
       </c>
       <c r="I82" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="J82" s="8"/>
-      <c r="K82" s="9"/>
+        <v>157</v>
+      </c>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
       <c r="N82" s="9"/>
@@ -6167,9 +6189,9 @@
       <c r="AA82" s="2"/>
       <c r="AB82" s="2"/>
     </row>
-    <row r="83" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>284</v>
@@ -6190,14 +6212,12 @@
         <v>189</v>
       </c>
       <c r="H83" s="8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I83" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="J83" s="20" t="s">
-        <v>195</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="J83" s="8"/>
       <c r="K83" s="9"/>
       <c r="L83" s="9"/>
       <c r="M83" s="9"/>
@@ -6217,15 +6237,15 @@
       <c r="AA83" s="2"/>
       <c r="AB83" s="2"/>
     </row>
-    <row r="84" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>177</v>
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
+        <v>192</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>11</v>
@@ -6237,16 +6257,16 @@
         <v>106</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="H84" s="8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="J84" s="6"/>
-      <c r="K84" s="6"/>
+        <v>193</v>
+      </c>
+      <c r="J84" s="8"/>
+      <c r="K84" s="9"/>
       <c r="L84" s="9"/>
       <c r="M84" s="9"/>
       <c r="N84" s="9"/>
@@ -6265,15 +6285,15 @@
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
     </row>
-    <row r="85" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>181</v>
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
+        <v>194</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>11</v>
@@ -6285,16 +6305,18 @@
         <v>106</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="H85" s="8" t="s">
         <v>241</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="J85" s="6"/>
-      <c r="K85" s="6"/>
+        <v>193</v>
+      </c>
+      <c r="J85" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="K85" s="9"/>
       <c r="L85" s="9"/>
       <c r="M85" s="9"/>
       <c r="N85" s="9"/>
@@ -6315,7 +6337,7 @@
     </row>
     <row r="86" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>312</v>
+        <v>177</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>284</v>
@@ -6333,13 +6355,13 @@
         <v>106</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>313</v>
+        <v>178</v>
       </c>
       <c r="H86" s="8" t="s">
         <v>241</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>314</v>
+        <v>180</v>
       </c>
       <c r="J86" s="6"/>
       <c r="K86" s="6"/>
@@ -6363,7 +6385,7 @@
     </row>
     <row r="87" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>308</v>
+        <v>181</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>284</v>
@@ -6381,13 +6403,13 @@
         <v>106</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>310</v>
+        <v>182</v>
       </c>
       <c r="H87" s="8" t="s">
         <v>241</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>309</v>
+        <v>183</v>
       </c>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
@@ -6411,7 +6433,7 @@
     </row>
     <row r="88" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>284</v>
@@ -6429,13 +6451,13 @@
         <v>106</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="H88" s="8" t="s">
         <v>241</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
@@ -6459,7 +6481,7 @@
     </row>
     <row r="89" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>184</v>
+        <v>308</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>284</v>
@@ -6477,13 +6499,13 @@
         <v>106</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>185</v>
+        <v>310</v>
       </c>
       <c r="H89" s="8" t="s">
         <v>241</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>186</v>
+        <v>309</v>
       </c>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
@@ -6506,14 +6528,14 @@
       <c r="AB89" s="2"/>
     </row>
     <row r="90" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
-        <v>205</v>
+      <c r="A90" s="3" t="s">
+        <v>306</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>238</v>
+        <v>179</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>11</v>
@@ -6525,16 +6547,16 @@
         <v>106</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>140</v>
+        <v>311</v>
       </c>
       <c r="H90" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="I90" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="J90" s="9"/>
-      <c r="K90" s="9"/>
+      <c r="I90" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
       <c r="L90" s="9"/>
       <c r="M90" s="9"/>
       <c r="N90" s="9"/>
@@ -6554,14 +6576,14 @@
       <c r="AB90" s="2"/>
     </row>
     <row r="91" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
-        <v>206</v>
+      <c r="A91" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>238</v>
+        <v>179</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>11</v>
@@ -6573,16 +6595,16 @@
         <v>106</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>140</v>
+        <v>185</v>
       </c>
       <c r="H91" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="I91" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="J91" s="9"/>
-      <c r="K91" s="9"/>
+      <c r="I91" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
       <c r="L91" s="9"/>
       <c r="M91" s="9"/>
       <c r="N91" s="9"/>
@@ -6603,7 +6625,7 @@
     </row>
     <row r="92" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>284</v>
@@ -6627,7 +6649,7 @@
         <v>241</v>
       </c>
       <c r="I92" s="22" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J92" s="9"/>
       <c r="K92" s="9"/>
@@ -6651,7 +6673,7 @@
     </row>
     <row r="93" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>284</v>
@@ -6675,7 +6697,7 @@
         <v>241</v>
       </c>
       <c r="I93" s="22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
@@ -6698,8 +6720,8 @@
       <c r="AB93" s="2"/>
     </row>
     <row r="94" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
-        <v>209</v>
+      <c r="A94" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>284</v>
@@ -6723,7 +6745,7 @@
         <v>241</v>
       </c>
       <c r="I94" s="22" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
@@ -6746,8 +6768,8 @@
       <c r="AB94" s="2"/>
     </row>
     <row r="95" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="25" t="s">
-        <v>210</v>
+      <c r="A95" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>284</v>
@@ -6771,7 +6793,7 @@
         <v>241</v>
       </c>
       <c r="I95" s="22" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
@@ -6793,9 +6815,9 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
-        <v>211</v>
+    <row r="96" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>284</v>
@@ -6819,7 +6841,7 @@
         <v>241</v>
       </c>
       <c r="I96" s="22" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
@@ -6842,8 +6864,8 @@
       <c r="AB96" s="2"/>
     </row>
     <row r="97" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
-        <v>212</v>
+      <c r="A97" s="25" t="s">
+        <v>210</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>284</v>
@@ -6867,7 +6889,7 @@
         <v>241</v>
       </c>
       <c r="I97" s="22" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -6889,9 +6911,9 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>213</v>
+    <row r="98" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>211</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>284</v>
@@ -6915,7 +6937,7 @@
         <v>241</v>
       </c>
       <c r="I98" s="22" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -6939,7 +6961,7 @@
     </row>
     <row r="99" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>284</v>
@@ -6963,7 +6985,7 @@
         <v>241</v>
       </c>
       <c r="I99" s="22" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -6985,15 +7007,15 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="11" t="s">
-        <v>215</v>
+    <row r="100" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>11</v>
@@ -7005,13 +7027,13 @@
         <v>106</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>239</v>
+        <v>140</v>
       </c>
       <c r="H100" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="I100" s="8" t="s">
-        <v>229</v>
+      <c r="I100" s="22" t="s">
+        <v>227</v>
       </c>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
@@ -7033,15 +7055,15 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="11" t="s">
-        <v>217</v>
+    <row r="101" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>11</v>
@@ -7053,20 +7075,16 @@
         <v>106</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>239</v>
+        <v>140</v>
       </c>
       <c r="H101" s="8" t="s">
         <v>241</v>
       </c>
       <c r="I101" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="J101" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="K101" s="20" t="s">
-        <v>232</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="J101" s="9"/>
+      <c r="K101" s="9"/>
       <c r="L101" s="9"/>
       <c r="M101" s="9"/>
       <c r="N101" s="9"/>
@@ -7087,7 +7105,7 @@
     </row>
     <row r="102" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>284</v>
@@ -7108,26 +7126,16 @@
         <v>239</v>
       </c>
       <c r="H102" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="I102" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="I102" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="J102" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="K102" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="L102" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="M102" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="N102" s="20" t="s">
-        <v>237</v>
-      </c>
+      <c r="J102" s="9"/>
+      <c r="K102" s="9"/>
+      <c r="L102" s="9"/>
+      <c r="M102" s="9"/>
+      <c r="N102" s="9"/>
       <c r="O102" s="2"/>
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
@@ -7143,17 +7151,17 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>245</v>
+    <row r="103" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="11" t="s">
+        <v>217</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C103" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D103" s="9" t="s">
+      <c r="C103" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D103" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E103" s="7" t="s">
@@ -7162,17 +7170,21 @@
       <c r="F103" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G103" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="H103" s="20" t="s">
+      <c r="G103" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H103" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="I103" s="20" t="s">
-        <v>248</v>
-      </c>
-      <c r="J103" s="9"/>
-      <c r="K103" s="9"/>
+      <c r="I103" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="J103" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="K103" s="20" t="s">
+        <v>232</v>
+      </c>
       <c r="L103" s="9"/>
       <c r="M103" s="9"/>
       <c r="N103" s="9"/>
@@ -7191,17 +7203,17 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
-        <v>249</v>
+    <row r="104" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
+        <v>218</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C104" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D104" s="9" t="s">
+      <c r="C104" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D104" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E104" s="7" t="s">
@@ -7210,20 +7222,30 @@
       <c r="F104" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G104" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="H104" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="I104" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="J104" s="9"/>
-      <c r="K104" s="9"/>
-      <c r="L104" s="9"/>
-      <c r="M104" s="9"/>
-      <c r="N104" s="9"/>
+      <c r="G104" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H104" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="I104" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="J104" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="K104" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="L104" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="M104" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="N104" s="20" t="s">
+        <v>237</v>
+      </c>
       <c r="O104" s="2"/>
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
@@ -7239,9 +7261,9 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>284</v>
@@ -7265,7 +7287,7 @@
         <v>241</v>
       </c>
       <c r="I105" s="20" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="J105" s="9"/>
       <c r="K105" s="9"/>
@@ -7287,17 +7309,17 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="23" t="s">
-        <v>264</v>
+    <row r="106" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>249</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C106" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D106" s="24" t="s">
+      <c r="C106" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D106" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E106" s="7" t="s">
@@ -7306,21 +7328,17 @@
       <c r="F106" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G106" s="6" t="s">
-        <v>239</v>
+      <c r="G106" s="9" t="s">
+        <v>247</v>
       </c>
       <c r="H106" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="I106" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="J106" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="K106" s="20" t="s">
-        <v>267</v>
-      </c>
+      <c r="I106" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="J106" s="9"/>
+      <c r="K106" s="9"/>
       <c r="L106" s="9"/>
       <c r="M106" s="9"/>
       <c r="N106" s="9"/>
@@ -7339,17 +7357,17 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="11" t="s">
-        <v>266</v>
+    <row r="107" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>251</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C107" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D107" s="6" t="s">
+      <c r="C107" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D107" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E107" s="7" t="s">
@@ -7358,17 +7376,17 @@
       <c r="F107" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G107" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="H107" s="8" t="s">
+      <c r="G107" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="H107" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="I107" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="J107" s="20"/>
-      <c r="K107" s="20"/>
+      <c r="I107" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="J107" s="9"/>
+      <c r="K107" s="9"/>
       <c r="L107" s="9"/>
       <c r="M107" s="9"/>
       <c r="N107" s="9"/>
@@ -7387,9 +7405,9 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="11" t="s">
-        <v>274</v>
+    <row r="108" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="23" t="s">
+        <v>264</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>284</v>
@@ -7397,7 +7415,7 @@
       <c r="C108" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="D108" s="6" t="s">
+      <c r="D108" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E108" s="7" t="s">
@@ -7409,7 +7427,7 @@
       <c r="G108" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="H108" s="8" t="s">
+      <c r="H108" s="20" t="s">
         <v>241</v>
       </c>
       <c r="I108" s="22" t="s">
@@ -7421,9 +7439,9 @@
       <c r="K108" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="L108" s="20"/>
-      <c r="M108" s="20"/>
-      <c r="N108" s="20"/>
+      <c r="L108" s="9"/>
+      <c r="M108" s="9"/>
+      <c r="N108" s="9"/>
       <c r="O108" s="2"/>
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
@@ -7441,16 +7459,16 @@
     </row>
     <row r="109" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>10</v>
+        <v>273</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E109" s="7" t="s">
         <v>106</v>
@@ -7459,14 +7477,16 @@
         <v>106</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>12</v>
+        <v>239</v>
       </c>
       <c r="H109" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="I109" s="9"/>
-      <c r="J109" s="9"/>
-      <c r="K109" s="9"/>
+        <v>241</v>
+      </c>
+      <c r="I109" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="J109" s="20"/>
+      <c r="K109" s="20"/>
       <c r="L109" s="9"/>
       <c r="M109" s="9"/>
       <c r="N109" s="9"/>
@@ -7485,18 +7505,18 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="27" t="s">
-        <v>282</v>
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="11" t="s">
+        <v>274</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>139</v>
+        <v>216</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E110" s="7" t="s">
         <v>106</v>
@@ -7504,25 +7524,48 @@
       <c r="F110" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G110" s="26" t="s">
-        <v>283</v>
+      <c r="G110" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="H110" s="8" t="s">
         <v>241</v>
       </c>
       <c r="I110" s="22" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="111" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>286</v>
+        <v>265</v>
+      </c>
+      <c r="J110" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="K110" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="L110" s="20"/>
+      <c r="M110" s="20"/>
+      <c r="N110" s="20"/>
+      <c r="O110" s="2"/>
+      <c r="P110" s="2"/>
+      <c r="Q110" s="2"/>
+      <c r="R110" s="2"/>
+      <c r="S110" s="2"/>
+      <c r="T110" s="2"/>
+      <c r="U110" s="2"/>
+      <c r="V110" s="2"/>
+      <c r="W110" s="2"/>
+      <c r="X110" s="2"/>
+      <c r="Y110" s="2"/>
+      <c r="Z110" s="2"/>
+      <c r="AA110" s="2"/>
+      <c r="AB110" s="2"/>
+    </row>
+    <row r="111" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="11" t="s">
+        <v>272</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>14</v>
@@ -7531,21 +7574,38 @@
         <v>106</v>
       </c>
       <c r="F111" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="G111" s="26" t="s">
-        <v>283</v>
+        <v>106</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="H111" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="I111" s="22" t="s">
-        <v>288</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="I111" s="9"/>
+      <c r="J111" s="9"/>
+      <c r="K111" s="9"/>
+      <c r="L111" s="9"/>
+      <c r="M111" s="9"/>
+      <c r="N111" s="9"/>
+      <c r="O111" s="2"/>
+      <c r="P111" s="2"/>
+      <c r="Q111" s="2"/>
+      <c r="R111" s="2"/>
+      <c r="S111" s="2"/>
+      <c r="T111" s="2"/>
+      <c r="U111" s="2"/>
+      <c r="V111" s="2"/>
+      <c r="W111" s="2"/>
+      <c r="X111" s="2"/>
+      <c r="Y111" s="2"/>
+      <c r="Z111" s="2"/>
+      <c r="AA111" s="2"/>
+      <c r="AB111" s="2"/>
     </row>
     <row r="112" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>289</v>
+      <c r="A112" s="27" t="s">
+        <v>282</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>284</v>
@@ -7569,12 +7629,12 @@
         <v>241</v>
       </c>
       <c r="I112" s="22" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>284</v>
@@ -7589,7 +7649,7 @@
         <v>106</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>106</v>
+        <v>287</v>
       </c>
       <c r="G113" s="26" t="s">
         <v>283</v>
@@ -7598,12 +7658,12 @@
         <v>241</v>
       </c>
       <c r="I113" s="22" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>284</v>
@@ -7627,12 +7687,12 @@
         <v>241</v>
       </c>
       <c r="I114" s="22" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>284</v>
@@ -7656,12 +7716,12 @@
         <v>241</v>
       </c>
       <c r="I115" s="22" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>284</v>
@@ -7685,12 +7745,12 @@
         <v>241</v>
       </c>
       <c r="I116" s="22" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>284</v>
@@ -7714,12 +7774,12 @@
         <v>241</v>
       </c>
       <c r="I117" s="22" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>284</v>
@@ -7743,12 +7803,12 @@
         <v>241</v>
       </c>
       <c r="I118" s="22" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>284</v>
@@ -7772,12 +7832,12 @@
         <v>241</v>
       </c>
       <c r="I119" s="22" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>284</v>
@@ -7801,11 +7861,69 @@
         <v>241</v>
       </c>
       <c r="I120" s="22" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>304</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F121" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G121" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="H121" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="I121" s="22" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>315</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F122" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G122" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="H122" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="I122" s="22" t="s">
         <v>316</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I120" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:I122" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="Yes"/>

</xml_diff>

<commit_message>
Modified System settings(Account limits, Fee)
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(06-03-2023)Agreements\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC0907C-4EAA-4C9D-8C74-8BDEC3B9A48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB980E1-EBC5-47BA-A162-ED0051A799AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$123</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="329">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -448,16 +448,7 @@
     <t>verify fee struture Edit</t>
   </si>
   <si>
-    <t>feeStructureEdit</t>
-  </si>
-  <si>
     <t>verify fee struture Merchant Edit</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.SystemSettingsTest,
-testEditMerchantFeeStructure,
--pexpHeading,
--pexpEditHeading</t>
   </si>
   <si>
     <t>testdata-admin.xlsx,BalanceReport</t>
@@ -685,11 +676,6 @@
     <t>4</t>
   </si>
   <si>
-    <t>coyni.admin.tests.SystemSettingsTest,
-testEditPersonalFeeStructure,
--pexpEditHeading</t>
-  </si>
-  <si>
     <t>VerifyBalanceReport</t>
   </si>
   <si>
@@ -705,11 +691,6 @@
     <t>coyni.admin.tests.SystemSettingsTest,
 testEditPersonalAccountLimit,
 -pexpEditHeading</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.SystemSettingsTest,
-testViewPersonalAccountLimits,
--pexpViewHeading</t>
   </si>
   <si>
     <t xml:space="preserve">create Api Business </t>
@@ -1847,6 +1828,50 @@
 -pfolderName,
 -pfileName,
 -ptosHeading</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.SystemSettingsTest,
+testEditPersonalFeeStructure,
+-pAgreementList,
+-pexpEditHeading,
+-pamount,
+-ppercentage,
+-ptosHeading</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.SystemSettingsTest,
+testEditMerchantFeeStructure,
+-pAgreementList,
+-pexpEditHeading,
+-pamount,
+-ppercentage,
+-ptosHeading</t>
+  </si>
+  <si>
+    <t>SystemSettings -AccountLimit</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.SystemSettingsTest,
+testViewPersonalAccountLimits,
+-pexpViewHeading,
+-pamount,
+-ppercentage,
+-ptosHeading,
+-psuccess,
+-pmessage</t>
+  </si>
+  <si>
+    <t>verify Merchant AccountLimit view</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.SystemSettingsTest,
+testViewMerchantAccountLimits,
+-pexpViewHeading,
+-pamount,
+-ppercentage,
+-ptosHeading,
+-psuccess,
+-pmessage</t>
   </si>
 </sst>
 </file>
@@ -1970,7 +1995,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2020,6 +2045,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2301,10 +2327,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB122"/>
+  <dimension ref="A1:AB123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D66" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView tabSelected="1" topLeftCell="B73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2364,7 +2390,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>
@@ -2373,16 +2399,16 @@
         <v>11</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -2407,10 +2433,10 @@
     </row>
     <row r="3" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>10</v>
@@ -2419,16 +2445,16 @@
         <v>14</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -2456,7 +2482,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>10</v>
@@ -2465,10 +2491,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>12</v>
@@ -2502,7 +2528,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
@@ -2511,16 +2537,16 @@
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -2545,10 +2571,10 @@
     </row>
     <row r="6" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>10</v>
@@ -2557,16 +2583,16 @@
         <v>14</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -2594,7 +2620,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>27</v>
@@ -2603,16 +2629,16 @@
         <v>14</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -2640,7 +2666,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>27</v>
@@ -2649,16 +2675,16 @@
         <v>14</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -2686,7 +2712,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>27</v>
@@ -2695,10 +2721,10 @@
         <v>14</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>28</v>
@@ -2732,7 +2758,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>27</v>
@@ -2741,10 +2767,10 @@
         <v>14</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>28</v>
@@ -2778,7 +2804,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>35</v>
@@ -2787,10 +2813,10 @@
         <v>11</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>36</v>
@@ -2824,7 +2850,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>35</v>
@@ -2833,10 +2859,10 @@
         <v>11</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>36</v>
@@ -2870,7 +2896,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>35</v>
@@ -2916,7 +2942,7 @@
         <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>35</v>
@@ -2962,7 +2988,7 @@
         <v>44</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>35</v>
@@ -3005,10 +3031,10 @@
     </row>
     <row r="16" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>10</v>
@@ -3017,19 +3043,19 @@
         <v>11</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
@@ -3053,31 +3079,31 @@
     </row>
     <row r="17" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -3101,31 +3127,31 @@
     </row>
     <row r="18" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H18" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>244</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -3149,31 +3175,31 @@
     </row>
     <row r="19" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -3197,31 +3223,31 @@
     </row>
     <row r="20" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -3248,7 +3274,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>10</v>
@@ -3257,16 +3283,16 @@
         <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -3294,7 +3320,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>18</v>
@@ -3303,19 +3329,19 @@
         <v>11</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -3342,7 +3368,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
@@ -3351,16 +3377,16 @@
         <v>11</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>21</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>22</v>
@@ -3390,7 +3416,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>18</v>
@@ -3399,16 +3425,16 @@
         <v>11</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>24</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>25</v>
@@ -3435,13 +3461,13 @@
     </row>
     <row r="25" spans="1:28" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>262</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>11</v>
@@ -3453,13 +3479,13 @@
         <v>1</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -3483,13 +3509,13 @@
     </row>
     <row r="26" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>14</v>
@@ -3501,13 +3527,13 @@
         <v>2</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -3531,13 +3557,13 @@
     </row>
     <row r="27" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>11</v>
@@ -3549,13 +3575,13 @@
         <v>1</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -3579,31 +3605,31 @@
     </row>
     <row r="28" spans="1:28" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -3627,10 +3653,10 @@
     </row>
     <row r="29" spans="1:28" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>18</v>
@@ -3639,19 +3665,19 @@
         <v>11</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -3661,10 +3687,10 @@
     </row>
     <row r="30" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>18</v>
@@ -3673,19 +3699,19 @@
         <v>14</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -3709,10 +3735,10 @@
     </row>
     <row r="31" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>18</v>
@@ -3721,19 +3747,19 @@
         <v>14</v>
       </c>
       <c r="E31" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I31" s="20" t="s">
         <v>106</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="I31" s="20" t="s">
-        <v>108</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -3757,10 +3783,10 @@
     </row>
     <row r="32" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>18</v>
@@ -3769,19 +3795,19 @@
         <v>11</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3805,10 +3831,10 @@
     </row>
     <row r="33" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>18</v>
@@ -3817,19 +3843,19 @@
         <v>11</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -3853,10 +3879,10 @@
     </row>
     <row r="34" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>18</v>
@@ -3865,19 +3891,19 @@
         <v>11</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -3901,10 +3927,10 @@
     </row>
     <row r="35" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>18</v>
@@ -3913,19 +3939,19 @@
         <v>11</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -3949,10 +3975,10 @@
     </row>
     <row r="36" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>18</v>
@@ -3961,19 +3987,19 @@
         <v>11</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -4000,7 +4026,7 @@
         <v>46</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>47</v>
@@ -4009,16 +4035,16 @@
         <v>11</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>48</v>
@@ -4045,10 +4071,10 @@
     </row>
     <row r="38" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>47</v>
@@ -4057,19 +4083,19 @@
         <v>11</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="9"/>
@@ -4096,7 +4122,7 @@
         <v>49</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>47</v>
@@ -4105,16 +4131,16 @@
         <v>11</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>50</v>
@@ -4144,7 +4170,7 @@
         <v>51</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>47</v>
@@ -4153,16 +4179,16 @@
         <v>11</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>52</v>
@@ -4192,7 +4218,7 @@
         <v>53</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>47</v>
@@ -4201,16 +4227,16 @@
         <v>11</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I41" s="8" t="s">
         <v>54</v>
@@ -4240,7 +4266,7 @@
         <v>55</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>47</v>
@@ -4249,16 +4275,16 @@
         <v>11</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>56</v>
@@ -4288,7 +4314,7 @@
         <v>57</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>47</v>
@@ -4297,16 +4323,16 @@
         <v>11</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I43" s="8" t="s">
         <v>58</v>
@@ -4336,7 +4362,7 @@
         <v>59</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>60</v>
@@ -4345,19 +4371,19 @@
         <v>11</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -4384,7 +4410,7 @@
         <v>62</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>60</v>
@@ -4393,16 +4419,16 @@
         <v>11</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>63</v>
@@ -4432,7 +4458,7 @@
         <v>64</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>60</v>
@@ -4441,16 +4467,16 @@
         <v>11</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>65</v>
@@ -4480,7 +4506,7 @@
         <v>66</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>60</v>
@@ -4489,16 +4515,16 @@
         <v>11</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I47" s="8" t="s">
         <v>67</v>
@@ -4528,7 +4554,7 @@
         <v>68</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>60</v>
@@ -4537,16 +4563,16 @@
         <v>11</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>69</v>
@@ -4576,7 +4602,7 @@
         <v>70</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>60</v>
@@ -4585,16 +4611,16 @@
         <v>11</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>72</v>
@@ -4624,7 +4650,7 @@
         <v>73</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>60</v>
@@ -4633,16 +4659,16 @@
         <v>11</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I50" s="8" t="s">
         <v>74</v>
@@ -4669,10 +4695,10 @@
     </row>
     <row r="51" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>60</v>
@@ -4681,19 +4707,19 @@
         <v>11</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -4720,7 +4746,7 @@
         <v>75</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>60</v>
@@ -4729,16 +4755,16 @@
         <v>11</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I52" s="8" t="s">
         <v>76</v>
@@ -4765,31 +4791,31 @@
     </row>
     <row r="53" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -4813,31 +4839,31 @@
     </row>
     <row r="54" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -4861,31 +4887,31 @@
     </row>
     <row r="55" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="I55" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="I55" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -4909,31 +4935,31 @@
     </row>
     <row r="56" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -4957,31 +4983,31 @@
     </row>
     <row r="57" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
@@ -5005,31 +5031,31 @@
     </row>
     <row r="58" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
@@ -5053,31 +5079,31 @@
     </row>
     <row r="59" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
@@ -5101,31 +5127,31 @@
     </row>
     <row r="60" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="28" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -5149,31 +5175,31 @@
     </row>
     <row r="61" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -5197,31 +5223,31 @@
     </row>
     <row r="62" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -5245,31 +5271,31 @@
     </row>
     <row r="63" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C63" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H63" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="I63" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H63" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="I63" s="8" t="s">
-        <v>87</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -5293,31 +5319,31 @@
     </row>
     <row r="64" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -5344,7 +5370,7 @@
         <v>77</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>78</v>
@@ -5353,16 +5379,16 @@
         <v>11</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I65" s="8" t="s">
         <v>79</v>
@@ -5387,12 +5413,12 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>78</v>
@@ -5401,19 +5427,19 @@
         <v>11</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I66" s="22" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -5435,12 +5461,12 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>78</v>
@@ -5449,19 +5475,19 @@
         <v>11</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I67" s="22" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -5483,12 +5509,12 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>78</v>
@@ -5497,19 +5523,19 @@
         <v>11</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I68" s="22" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -5533,10 +5559,10 @@
     </row>
     <row r="69" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>78</v>
@@ -5545,19 +5571,19 @@
         <v>11</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G69" s="18" t="s">
         <v>80</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -5584,28 +5610,28 @@
         <v>81</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C70" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C70" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>82</v>
+        <v>317</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>127</v>
+        <v>323</v>
       </c>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -5629,10 +5655,10 @@
     </row>
     <row r="71" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>78</v>
@@ -5641,19 +5667,19 @@
         <v>11</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>82</v>
+        <v>317</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>84</v>
+        <v>324</v>
       </c>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -5675,33 +5701,33 @@
       <c r="AA71" s="2"/>
       <c r="AB71" s="2"/>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H72" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -5723,12 +5749,12 @@
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="141.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C73" s="18" t="s">
         <v>78</v>
@@ -5737,19 +5763,19 @@
         <v>11</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -5771,33 +5797,33 @@
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>121</v>
+    <row r="74" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>120</v>
+        <v>325</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>132</v>
+        <v>326</v>
       </c>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
@@ -5819,33 +5845,33 @@
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>122</v>
+    <row r="75" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="29" t="s">
+        <v>327</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>120</v>
+        <v>325</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I75" s="8" t="s">
-        <v>131</v>
+        <v>328</v>
       </c>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
@@ -5867,115 +5893,115 @@
       <c r="AA75" s="2"/>
       <c r="AB75" s="2"/>
     </row>
-    <row r="76" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>133</v>
+    <row r="76" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="H76" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
       <c r="N76" s="9"/>
-    </row>
-    <row r="77" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+      <c r="R76" s="2"/>
+      <c r="S76" s="2"/>
+      <c r="T76" s="2"/>
+      <c r="U76" s="2"/>
+      <c r="V76" s="2"/>
+      <c r="W76" s="2"/>
+      <c r="X76" s="2"/>
+      <c r="Y76" s="2"/>
+      <c r="Z76" s="2"/>
+      <c r="AA76" s="2"/>
+      <c r="AB76" s="2"/>
+    </row>
+    <row r="77" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C77" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>139</v>
-      </c>
       <c r="D77" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H77" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="I77" s="22" t="s">
-        <v>204</v>
+        <v>238</v>
+      </c>
+      <c r="I77" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="J77" s="9"/>
       <c r="K77" s="9"/>
       <c r="L77" s="9"/>
       <c r="M77" s="9"/>
       <c r="N77" s="9"/>
-      <c r="O77" s="2"/>
-      <c r="P77" s="2"/>
-      <c r="Q77" s="2"/>
-      <c r="R77" s="2"/>
-      <c r="S77" s="2"/>
-      <c r="T77" s="2"/>
-      <c r="U77" s="2"/>
-      <c r="V77" s="2"/>
-      <c r="W77" s="2"/>
-      <c r="X77" s="2"/>
-      <c r="Y77" s="2"/>
-      <c r="Z77" s="2"/>
-      <c r="AA77" s="2"/>
-      <c r="AB77" s="2"/>
     </row>
     <row r="78" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H78" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I78" s="22" t="s">
-        <v>137</v>
+        <v>200</v>
       </c>
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
@@ -5999,31 +6025,31 @@
     </row>
     <row r="79" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="H79" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I79" s="22" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
@@ -6047,31 +6073,31 @@
     </row>
     <row r="80" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I80" s="22" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
@@ -6095,31 +6121,31 @@
     </row>
     <row r="81" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C81" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H81" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="I81" s="22" t="s">
         <v>139</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G81" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="H81" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="I81" s="22" t="s">
-        <v>145</v>
       </c>
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
@@ -6141,36 +6167,36 @@
       <c r="AA81" s="2"/>
       <c r="AB81" s="2"/>
     </row>
-    <row r="82" spans="1:28" s="1" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
-        <v>155</v>
+    <row r="82" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>189</v>
+        <v>136</v>
       </c>
       <c r="H82" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="I82" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="J82" s="6"/>
-      <c r="K82" s="6"/>
+        <v>238</v>
+      </c>
+      <c r="I82" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
       <c r="N82" s="9"/>
@@ -6189,36 +6215,36 @@
       <c r="AA82" s="2"/>
       <c r="AB82" s="2"/>
     </row>
-    <row r="83" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" s="1" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H83" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I83" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="J83" s="8"/>
-      <c r="K83" s="9"/>
+        <v>153</v>
+      </c>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
       <c r="L83" s="9"/>
       <c r="M83" s="9"/>
       <c r="N83" s="9"/>
@@ -6239,31 +6265,31 @@
     </row>
     <row r="84" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H84" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>193</v>
+        <v>313</v>
       </c>
       <c r="J84" s="8"/>
       <c r="K84" s="9"/>
@@ -6285,37 +6311,35 @@
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G85" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="H85" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="I85" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="H85" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="I85" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="J85" s="20" t="s">
-        <v>195</v>
-      </c>
+      <c r="J85" s="8"/>
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
       <c r="M85" s="9"/>
@@ -6335,36 +6359,38 @@
       <c r="AA85" s="2"/>
       <c r="AB85" s="2"/>
     </row>
-    <row r="86" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>177</v>
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="11" t="s">
+        <v>190</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="H86" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="J86" s="6"/>
-      <c r="K86" s="6"/>
+        <v>189</v>
+      </c>
+      <c r="J86" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="K86" s="9"/>
       <c r="L86" s="9"/>
       <c r="M86" s="9"/>
       <c r="N86" s="9"/>
@@ -6385,31 +6411,31 @@
     </row>
     <row r="87" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="H87" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
@@ -6433,31 +6459,31 @@
     </row>
     <row r="88" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>312</v>
+        <v>177</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C88" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I88" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G88" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="H88" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="I88" s="8" t="s">
-        <v>314</v>
       </c>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
@@ -6484,28 +6510,28 @@
         <v>308</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G89" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="H89" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I89" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="H89" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="I89" s="8" t="s">
-        <v>309</v>
       </c>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
@@ -6529,31 +6555,31 @@
     </row>
     <row r="90" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G90" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G90" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="H90" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J90" s="6"/>
       <c r="K90" s="6"/>
@@ -6577,31 +6603,31 @@
     </row>
     <row r="91" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>184</v>
+        <v>302</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>185</v>
+        <v>307</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I91" s="8" t="s">
-        <v>186</v>
+        <v>303</v>
       </c>
       <c r="J91" s="6"/>
       <c r="K91" s="6"/>
@@ -6624,35 +6650,35 @@
       <c r="AB91" s="2"/>
     </row>
     <row r="92" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
-        <v>205</v>
+      <c r="A92" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>238</v>
+        <v>175</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="I92" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="J92" s="9"/>
-      <c r="K92" s="9"/>
+        <v>237</v>
+      </c>
+      <c r="I92" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
       <c r="L92" s="9"/>
       <c r="M92" s="9"/>
       <c r="N92" s="9"/>
@@ -6673,31 +6699,31 @@
     </row>
     <row r="93" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I93" s="22" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
@@ -6721,31 +6747,31 @@
     </row>
     <row r="94" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H94" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I94" s="22" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
@@ -6769,31 +6795,31 @@
     </row>
     <row r="95" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I95" s="22" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
@@ -6816,32 +6842,32 @@
       <c r="AB95" s="2"/>
     </row>
     <row r="96" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
-        <v>209</v>
+      <c r="A96" s="6" t="s">
+        <v>204</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H96" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I96" s="22" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
@@ -6864,32 +6890,32 @@
       <c r="AB96" s="2"/>
     </row>
     <row r="97" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="25" t="s">
-        <v>210</v>
+      <c r="A97" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I97" s="22" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -6911,33 +6937,33 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
-        <v>211</v>
+    <row r="98" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="25" t="s">
+        <v>206</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H98" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I98" s="22" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -6959,33 +6985,33 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
-        <v>212</v>
+    <row r="99" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H99" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I99" s="22" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -7009,31 +7035,31 @@
     </row>
     <row r="100" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I100" s="22" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
@@ -7057,31 +7083,31 @@
     </row>
     <row r="101" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I101" s="22" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
@@ -7103,33 +7129,33 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="11" t="s">
-        <v>215</v>
+    <row r="102" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>239</v>
+        <v>136</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="I102" s="8" t="s">
-        <v>229</v>
+        <v>237</v>
+      </c>
+      <c r="I102" s="22" t="s">
+        <v>224</v>
       </c>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
@@ -7151,40 +7177,36 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H103" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="I103" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="J103" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="K103" s="20" t="s">
-        <v>232</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="I103" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J103" s="9"/>
+      <c r="K103" s="9"/>
       <c r="L103" s="9"/>
       <c r="M103" s="9"/>
       <c r="N103" s="9"/>
@@ -7203,49 +7225,43 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H104" s="8" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="I104" s="22" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="J104" s="20" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="K104" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="L104" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="M104" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="N104" s="20" t="s">
-        <v>237</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="L104" s="9"/>
+      <c r="M104" s="9"/>
+      <c r="N104" s="9"/>
       <c r="O104" s="2"/>
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
@@ -7261,39 +7277,49 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>245</v>
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="11" t="s">
+        <v>214</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C105" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D105" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D105" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G105" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="H105" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="I105" s="20" t="s">
-        <v>248</v>
-      </c>
-      <c r="J105" s="9"/>
-      <c r="K105" s="9"/>
-      <c r="L105" s="9"/>
-      <c r="M105" s="9"/>
-      <c r="N105" s="9"/>
+        <v>104</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H105" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="I105" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="J105" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="K105" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="L105" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="M105" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="N105" s="20" t="s">
+        <v>233</v>
+      </c>
       <c r="O105" s="2"/>
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
@@ -7309,33 +7335,33 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H106" s="20" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I106" s="20" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
@@ -7357,33 +7383,33 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C107" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G107" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="H107" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="I107" s="20" t="s">
         <v>246</v>
-      </c>
-      <c r="D107" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E107" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F107" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G107" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="H107" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="I107" s="20" t="s">
-        <v>252</v>
       </c>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
@@ -7405,40 +7431,36 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="23" t="s">
-        <v>264</v>
+    <row r="108" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>247</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D108" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D108" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G108" s="6" t="s">
-        <v>239</v>
+        <v>104</v>
+      </c>
+      <c r="G108" s="9" t="s">
+        <v>243</v>
       </c>
       <c r="H108" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="I108" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="J108" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="K108" s="20" t="s">
-        <v>267</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="I108" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="J108" s="9"/>
+      <c r="K108" s="9"/>
       <c r="L108" s="9"/>
       <c r="M108" s="9"/>
       <c r="N108" s="9"/>
@@ -7457,36 +7479,40 @@
       <c r="AA108" s="2"/>
       <c r="AB108" s="2"/>
     </row>
-    <row r="109" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="11" t="s">
-        <v>266</v>
+    <row r="109" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="23" t="s">
+        <v>260</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D109" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D109" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="H109" s="8" t="s">
-        <v>241</v>
+        <v>235</v>
+      </c>
+      <c r="H109" s="20" t="s">
+        <v>237</v>
       </c>
       <c r="I109" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="J109" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="K109" s="20" t="s">
         <v>263</v>
       </c>
-      <c r="J109" s="20"/>
-      <c r="K109" s="20"/>
       <c r="L109" s="9"/>
       <c r="M109" s="9"/>
       <c r="N109" s="9"/>
@@ -7505,43 +7531,39 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>216</v>
+        <v>269</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I110" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="J110" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="K110" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="L110" s="20"/>
-      <c r="M110" s="20"/>
-      <c r="N110" s="20"/>
+        <v>259</v>
+      </c>
+      <c r="J110" s="20"/>
+      <c r="K110" s="20"/>
+      <c r="L110" s="9"/>
+      <c r="M110" s="9"/>
+      <c r="N110" s="9"/>
       <c r="O110" s="2"/>
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
@@ -7557,37 +7579,43 @@
       <c r="AA110" s="2"/>
       <c r="AB110" s="2"/>
     </row>
-    <row r="111" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>10</v>
+        <v>212</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F111" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="H111" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="I111" s="9"/>
-      <c r="J111" s="9"/>
-      <c r="K111" s="9"/>
-      <c r="L111" s="9"/>
-      <c r="M111" s="9"/>
-      <c r="N111" s="9"/>
+        <v>237</v>
+      </c>
+      <c r="I111" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="J111" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="K111" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="L111" s="20"/>
+      <c r="M111" s="20"/>
+      <c r="N111" s="20"/>
       <c r="O111" s="2"/>
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
@@ -7603,330 +7631,377 @@
       <c r="AA111" s="2"/>
       <c r="AB111" s="2"/>
     </row>
-    <row r="112" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="27" t="s">
-        <v>282</v>
+    <row r="112" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="11" t="s">
+        <v>268</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G112" s="26" t="s">
-        <v>283</v>
+        <v>104</v>
+      </c>
+      <c r="G112" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="H112" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="I112" s="22" t="s">
-        <v>291</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="I112" s="9"/>
+      <c r="J112" s="9"/>
+      <c r="K112" s="9"/>
+      <c r="L112" s="9"/>
+      <c r="M112" s="9"/>
+      <c r="N112" s="9"/>
+      <c r="O112" s="2"/>
+      <c r="P112" s="2"/>
+      <c r="Q112" s="2"/>
+      <c r="R112" s="2"/>
+      <c r="S112" s="2"/>
+      <c r="T112" s="2"/>
+      <c r="U112" s="2"/>
+      <c r="V112" s="2"/>
+      <c r="W112" s="2"/>
+      <c r="X112" s="2"/>
+      <c r="Y112" s="2"/>
+      <c r="Z112" s="2"/>
+      <c r="AA112" s="2"/>
+      <c r="AB112" s="2"/>
     </row>
     <row r="113" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>286</v>
+      <c r="A113" s="27" t="s">
+        <v>278</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F113" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G113" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="H113" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I113" s="22" t="s">
         <v>287</v>
-      </c>
-      <c r="G113" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="H113" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="I113" s="22" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>106</v>
+        <v>283</v>
       </c>
       <c r="G114" s="26" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H114" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I114" s="22" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G115" s="26" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H115" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I115" s="22" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G116" s="26" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H116" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I116" s="22" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F117" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G117" s="26" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H117" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I117" s="22" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F118" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G118" s="26" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H118" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I118" s="22" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F119" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G119" s="26" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H119" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I119" s="22" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G120" s="26" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I120" s="22" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G121" s="26" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H121" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I121" s="22" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F122" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G122" s="26" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H122" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I122" s="22" t="s">
-        <v>316</v>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>311</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G123" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="H123" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I123" s="22" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I122" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
+  <autoFilter ref="A1:I123" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="6">
       <filters>
-        <filter val="Yes"/>
+        <filter val="AccountLimit"/>
+        <filter val="AccountLimit - shedule"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added test methods for feature controls
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(06-03-2023)Agreements\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB980E1-EBC5-47BA-A162-ED0051A799AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46111202-E4F7-452B-8E73-9B98ECDD6942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$125</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="335">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1872,6 +1872,36 @@
 -ptosHeading,
 -psuccess,
 -pmessage</t>
+  </si>
+  <si>
+    <t>testdata-admin.xlsx,featureControl</t>
+  </si>
+  <si>
+    <t>SystemSettings -FeatureControl</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.SystemSettingsTest,
+testFeatureControl,
+-pexpActivityHeading,
+-pexpHeading,
+-pexpDescription,
+-psuccess,
+-pmessage</t>
+  </si>
+  <si>
+    <t>VerifyFeatureControlEnable</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.SystemSettingsTest,
+testFeatureControlEnable,
+-pexpActivityHeading,
+-pexpHeading,
+-pexpDescription,
+-psuccess,
+-pmessage</t>
+  </si>
+  <si>
+    <t>VerifyFeatureControlDisable</t>
   </si>
 </sst>
 </file>
@@ -2326,11 +2356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB123"/>
+  <dimension ref="A1:AB125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,7 +2414,7 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2431,7 +2460,7 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>277</v>
       </c>
@@ -2477,7 +2506,7 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -2523,7 +2552,7 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
@@ -2569,7 +2598,7 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>154</v>
       </c>
@@ -2615,7 +2644,7 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="240" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -2661,7 +2690,7 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="210.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="210.75" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>29</v>
       </c>
@@ -2707,7 +2736,7 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="210" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
@@ -2753,7 +2782,7 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -2799,7 +2828,7 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="255" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
@@ -2845,7 +2874,7 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="225" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
@@ -2891,7 +2920,7 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="210" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -2937,7 +2966,7 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -2983,7 +3012,7 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="195" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -3029,7 +3058,7 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>271</v>
       </c>
@@ -3077,7 +3106,7 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
-    <row r="17" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>142</v>
       </c>
@@ -3125,7 +3154,7 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>144</v>
       </c>
@@ -3173,7 +3202,7 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>146</v>
       </c>
@@ -3221,7 +3250,7 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
     </row>
-    <row r="20" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>166</v>
       </c>
@@ -3269,7 +3298,7 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
     </row>
-    <row r="21" spans="1:28" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
@@ -3315,7 +3344,7 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -3363,7 +3392,7 @@
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
     </row>
-    <row r="23" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -3411,7 +3440,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
     </row>
-    <row r="24" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -3459,7 +3488,7 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
     </row>
-    <row r="25" spans="1:28" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="270" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>254</v>
       </c>
@@ -3507,7 +3536,7 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
     </row>
-    <row r="26" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>255</v>
       </c>
@@ -3555,7 +3584,7 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>256</v>
       </c>
@@ -3603,7 +3632,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="285" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>257</v>
       </c>
@@ -3651,7 +3680,7 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:28" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>160</v>
       </c>
@@ -3685,7 +3714,7 @@
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
     </row>
-    <row r="30" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>88</v>
       </c>
@@ -3733,7 +3762,7 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>105</v>
       </c>
@@ -3781,7 +3810,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>107</v>
       </c>
@@ -3829,7 +3858,7 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>109</v>
       </c>
@@ -3877,7 +3906,7 @@
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
     </row>
-    <row r="34" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>111</v>
       </c>
@@ -3925,7 +3954,7 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>113</v>
       </c>
@@ -3973,7 +4002,7 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>115</v>
       </c>
@@ -4021,7 +4050,7 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>46</v>
       </c>
@@ -4069,7 +4098,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>192</v>
       </c>
@@ -4117,7 +4146,7 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>49</v>
       </c>
@@ -4165,7 +4194,7 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
@@ -4213,7 +4242,7 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>53</v>
       </c>
@@ -4261,7 +4290,7 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>55</v>
       </c>
@@ -4309,7 +4338,7 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>57</v>
       </c>
@@ -4357,7 +4386,7 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>59</v>
       </c>
@@ -4405,7 +4434,7 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>62</v>
       </c>
@@ -4453,7 +4482,7 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>64</v>
       </c>
@@ -4501,7 +4530,7 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>66</v>
       </c>
@@ -4549,7 +4578,7 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>68</v>
       </c>
@@ -4597,7 +4626,7 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>70</v>
       </c>
@@ -4645,7 +4674,7 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>73</v>
       </c>
@@ -4693,7 +4722,7 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>149</v>
       </c>
@@ -4741,7 +4770,7 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>75</v>
       </c>
@@ -4789,7 +4818,7 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>157</v>
       </c>
@@ -4837,7 +4866,7 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>163</v>
       </c>
@@ -4885,7 +4914,7 @@
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
     </row>
-    <row r="55" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>91</v>
       </c>
@@ -4933,7 +4962,7 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>94</v>
       </c>
@@ -4981,7 +5010,7 @@
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>96</v>
       </c>
@@ -5029,7 +5058,7 @@
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
     </row>
-    <row r="58" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>98</v>
       </c>
@@ -5077,7 +5106,7 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>100</v>
       </c>
@@ -5125,7 +5154,7 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="28" t="s">
         <v>314</v>
       </c>
@@ -5173,7 +5202,7 @@
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>102</v>
       </c>
@@ -5221,7 +5250,7 @@
       <c r="AA61" s="2"/>
       <c r="AB61" s="2"/>
     </row>
-    <row r="62" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>184</v>
       </c>
@@ -5269,7 +5298,7 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>125</v>
       </c>
@@ -5317,7 +5346,7 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>86</v>
       </c>
@@ -5365,7 +5394,7 @@
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
     </row>
-    <row r="65" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>77</v>
       </c>
@@ -5413,7 +5442,7 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>316</v>
       </c>
@@ -5461,7 +5490,7 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>319</v>
       </c>
@@ -5509,7 +5538,7 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>321</v>
       </c>
@@ -5557,9 +5586,9 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="21" t="s">
-        <v>195</v>
+    <row r="69" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>280</v>
@@ -5567,7 +5596,7 @@
       <c r="C69" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D69" s="18" t="s">
+      <c r="D69" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="7" t="s">
@@ -5576,14 +5605,14 @@
       <c r="F69" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G69" s="18" t="s">
-        <v>80</v>
+      <c r="G69" s="6" t="s">
+        <v>317</v>
       </c>
       <c r="H69" s="8" t="s">
         <v>238</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>196</v>
+        <v>323</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -5605,14 +5634,14 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C70" s="18" t="s">
+      <c r="C70" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D70" s="6" t="s">
@@ -5631,7 +5660,7 @@
         <v>238</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -5653,15 +5682,15 @@
       <c r="AA70" s="2"/>
       <c r="AB70" s="2"/>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>82</v>
+    <row r="71" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="29" t="s">
+        <v>119</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>11</v>
@@ -5673,13 +5702,13 @@
         <v>104</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="H71" s="8" t="s">
         <v>238</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -5702,8 +5731,8 @@
       <c r="AB71" s="2"/>
     </row>
     <row r="72" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
-        <v>121</v>
+      <c r="A72" s="29" t="s">
+        <v>327</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>280</v>
@@ -5721,13 +5750,13 @@
         <v>104</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>118</v>
+        <v>325</v>
       </c>
       <c r="H72" s="8" t="s">
         <v>238</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>127</v>
+        <v>328</v>
       </c>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -5749,15 +5778,15 @@
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="21" t="s">
-        <v>197</v>
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>334</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>78</v>
+        <v>281</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>329</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>11</v>
@@ -5769,13 +5798,13 @@
         <v>104</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>199</v>
+        <v>330</v>
       </c>
       <c r="H73" s="8" t="s">
         <v>238</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>198</v>
+        <v>331</v>
       </c>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -5798,14 +5827,14 @@
       <c r="AB73" s="2"/>
     </row>
     <row r="74" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="29" t="s">
-        <v>119</v>
+      <c r="A74" t="s">
+        <v>332</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>126</v>
+        <v>329</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>11</v>
@@ -5817,13 +5846,13 @@
         <v>104</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="H74" s="8" t="s">
         <v>238</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
@@ -5845,17 +5874,17 @@
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="29" t="s">
-        <v>327</v>
+    <row r="75" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A75" s="21" t="s">
+        <v>195</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D75" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D75" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E75" s="7" t="s">
@@ -5864,14 +5893,14 @@
       <c r="F75" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G75" s="6" t="s">
-        <v>325</v>
+      <c r="G75" s="18" t="s">
+        <v>80</v>
       </c>
       <c r="H75" s="8" t="s">
         <v>238</v>
       </c>
       <c r="I75" s="8" t="s">
-        <v>328</v>
+        <v>196</v>
       </c>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
@@ -5895,7 +5924,7 @@
     </row>
     <row r="76" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>280</v>
@@ -5919,7 +5948,7 @@
         <v>238</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
@@ -5941,15 +5970,15 @@
       <c r="AA76" s="2"/>
       <c r="AB76" s="2"/>
     </row>
-    <row r="77" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
-        <v>129</v>
+    <row r="77" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C77" s="6" t="s">
-        <v>135</v>
+      <c r="C77" s="18" t="s">
+        <v>78</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>11</v>
@@ -5961,29 +5990,43 @@
         <v>104</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>172</v>
+        <v>199</v>
       </c>
       <c r="H77" s="8" t="s">
         <v>238</v>
       </c>
       <c r="I77" s="8" t="s">
-        <v>130</v>
+        <v>198</v>
       </c>
       <c r="J77" s="9"/>
       <c r="K77" s="9"/>
       <c r="L77" s="9"/>
       <c r="M77" s="9"/>
       <c r="N77" s="9"/>
-    </row>
-    <row r="78" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>131</v>
+      <c r="O77" s="2"/>
+      <c r="P77" s="2"/>
+      <c r="Q77" s="2"/>
+      <c r="R77" s="2"/>
+      <c r="S77" s="2"/>
+      <c r="T77" s="2"/>
+      <c r="U77" s="2"/>
+      <c r="V77" s="2"/>
+      <c r="W77" s="2"/>
+      <c r="X77" s="2"/>
+      <c r="Y77" s="2"/>
+      <c r="Z77" s="2"/>
+      <c r="AA77" s="2"/>
+      <c r="AB77" s="2"/>
+    </row>
+    <row r="78" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>11</v>
@@ -5995,13 +6038,13 @@
         <v>104</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>172</v>
+        <v>118</v>
       </c>
       <c r="H78" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="I78" s="22" t="s">
-        <v>200</v>
+      <c r="I78" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
@@ -6023,9 +6066,9 @@
       <c r="AA78" s="2"/>
       <c r="AB78" s="2"/>
     </row>
-    <row r="79" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>132</v>
+    <row r="79" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>280</v>
@@ -6048,32 +6091,18 @@
       <c r="H79" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="I79" s="22" t="s">
-        <v>133</v>
+      <c r="I79" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
       <c r="N79" s="9"/>
-      <c r="O79" s="2"/>
-      <c r="P79" s="2"/>
-      <c r="Q79" s="2"/>
-      <c r="R79" s="2"/>
-      <c r="S79" s="2"/>
-      <c r="T79" s="2"/>
-      <c r="U79" s="2"/>
-      <c r="V79" s="2"/>
-      <c r="W79" s="2"/>
-      <c r="X79" s="2"/>
-      <c r="Y79" s="2"/>
-      <c r="Z79" s="2"/>
-      <c r="AA79" s="2"/>
-      <c r="AB79" s="2"/>
-    </row>
-    <row r="80" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>280</v>
@@ -6091,13 +6120,13 @@
         <v>104</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="H80" s="8" t="s">
         <v>238</v>
       </c>
       <c r="I80" s="22" t="s">
-        <v>137</v>
+        <v>200</v>
       </c>
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
@@ -6119,9 +6148,9 @@
       <c r="AA80" s="2"/>
       <c r="AB80" s="2"/>
     </row>
-    <row r="81" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>280</v>
@@ -6139,13 +6168,13 @@
         <v>104</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="H81" s="8" t="s">
         <v>238</v>
       </c>
       <c r="I81" s="22" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
@@ -6167,9 +6196,9 @@
       <c r="AA81" s="2"/>
       <c r="AB81" s="2"/>
     </row>
-    <row r="82" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>280</v>
@@ -6193,7 +6222,7 @@
         <v>238</v>
       </c>
       <c r="I82" s="22" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J82" s="9"/>
       <c r="K82" s="9"/>
@@ -6215,15 +6244,15 @@
       <c r="AA82" s="2"/>
       <c r="AB82" s="2"/>
     </row>
-    <row r="83" spans="1:28" s="1" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
-        <v>151</v>
+    <row r="83" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>11</v>
@@ -6235,16 +6264,16 @@
         <v>104</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="H83" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="I83" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J83" s="6"/>
-      <c r="K83" s="6"/>
+      <c r="I83" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="J83" s="9"/>
+      <c r="K83" s="9"/>
       <c r="L83" s="9"/>
       <c r="M83" s="9"/>
       <c r="N83" s="9"/>
@@ -6263,15 +6292,15 @@
       <c r="AA83" s="2"/>
       <c r="AB83" s="2"/>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
-        <v>186</v>
+    <row r="84" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>187</v>
+        <v>135</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>11</v>
@@ -6283,15 +6312,15 @@
         <v>104</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="H84" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="I84" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="J84" s="8"/>
+      <c r="I84" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="J84" s="9"/>
       <c r="K84" s="9"/>
       <c r="L84" s="9"/>
       <c r="M84" s="9"/>
@@ -6311,15 +6340,15 @@
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>11</v>
@@ -6337,10 +6366,10 @@
         <v>238</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="J85" s="8"/>
-      <c r="K85" s="9"/>
+        <v>153</v>
+      </c>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
       <c r="L85" s="9"/>
       <c r="M85" s="9"/>
       <c r="N85" s="9"/>
@@ -6359,9 +6388,9 @@
       <c r="AA85" s="2"/>
       <c r="AB85" s="2"/>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>280</v>
@@ -6382,14 +6411,12 @@
         <v>185</v>
       </c>
       <c r="H86" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="J86" s="20" t="s">
-        <v>191</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="J86" s="8"/>
       <c r="K86" s="9"/>
       <c r="L86" s="9"/>
       <c r="M86" s="9"/>
@@ -6409,15 +6436,15 @@
       <c r="AA86" s="2"/>
       <c r="AB86" s="2"/>
     </row>
-    <row r="87" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
-        <v>173</v>
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
+        <v>188</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>11</v>
@@ -6429,16 +6456,16 @@
         <v>104</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="H87" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="J87" s="6"/>
-      <c r="K87" s="6"/>
+        <v>189</v>
+      </c>
+      <c r="J87" s="8"/>
+      <c r="K87" s="9"/>
       <c r="L87" s="9"/>
       <c r="M87" s="9"/>
       <c r="N87" s="9"/>
@@ -6457,15 +6484,15 @@
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
     </row>
-    <row r="88" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>177</v>
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A88" s="11" t="s">
+        <v>190</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>11</v>
@@ -6477,16 +6504,18 @@
         <v>104</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="H88" s="8" t="s">
         <v>237</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="J88" s="6"/>
-      <c r="K88" s="6"/>
+        <v>189</v>
+      </c>
+      <c r="J88" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="K88" s="9"/>
       <c r="L88" s="9"/>
       <c r="M88" s="9"/>
       <c r="N88" s="9"/>
@@ -6505,9 +6534,9 @@
       <c r="AA88" s="2"/>
       <c r="AB88" s="2"/>
     </row>
-    <row r="89" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>308</v>
+        <v>173</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>280</v>
@@ -6525,13 +6554,13 @@
         <v>104</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>309</v>
+        <v>174</v>
       </c>
       <c r="H89" s="8" t="s">
         <v>237</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>310</v>
+        <v>176</v>
       </c>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
@@ -6553,9 +6582,9 @@
       <c r="AA89" s="2"/>
       <c r="AB89" s="2"/>
     </row>
-    <row r="90" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>304</v>
+        <v>177</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>280</v>
@@ -6573,13 +6602,13 @@
         <v>104</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>306</v>
+        <v>178</v>
       </c>
       <c r="H90" s="8" t="s">
         <v>237</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>305</v>
+        <v>179</v>
       </c>
       <c r="J90" s="6"/>
       <c r="K90" s="6"/>
@@ -6601,9 +6630,9 @@
       <c r="AA90" s="2"/>
       <c r="AB90" s="2"/>
     </row>
-    <row r="91" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>280</v>
@@ -6621,13 +6650,13 @@
         <v>104</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H91" s="8" t="s">
         <v>237</v>
       </c>
       <c r="I91" s="8" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="J91" s="6"/>
       <c r="K91" s="6"/>
@@ -6649,9 +6678,9 @@
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
     </row>
-    <row r="92" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>180</v>
+        <v>304</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>280</v>
@@ -6669,13 +6698,13 @@
         <v>104</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>181</v>
+        <v>306</v>
       </c>
       <c r="H92" s="8" t="s">
         <v>237</v>
       </c>
       <c r="I92" s="8" t="s">
-        <v>182</v>
+        <v>305</v>
       </c>
       <c r="J92" s="6"/>
       <c r="K92" s="6"/>
@@ -6697,15 +6726,15 @@
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
     </row>
-    <row r="93" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
-        <v>201</v>
+    <row r="93" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>234</v>
+        <v>175</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>11</v>
@@ -6717,16 +6746,16 @@
         <v>104</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>136</v>
+        <v>307</v>
       </c>
       <c r="H93" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="I93" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="J93" s="9"/>
-      <c r="K93" s="9"/>
+      <c r="I93" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
       <c r="L93" s="9"/>
       <c r="M93" s="9"/>
       <c r="N93" s="9"/>
@@ -6745,15 +6774,15 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
-        <v>202</v>
+    <row r="94" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>234</v>
+        <v>175</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>11</v>
@@ -6765,16 +6794,16 @@
         <v>104</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>136</v>
+        <v>181</v>
       </c>
       <c r="H94" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="I94" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="J94" s="9"/>
-      <c r="K94" s="9"/>
+      <c r="I94" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
       <c r="L94" s="9"/>
       <c r="M94" s="9"/>
       <c r="N94" s="9"/>
@@ -6793,9 +6822,9 @@
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
     </row>
-    <row r="95" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>280</v>
@@ -6819,7 +6848,7 @@
         <v>237</v>
       </c>
       <c r="I95" s="22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
@@ -6841,9 +6870,9 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>280</v>
@@ -6867,7 +6896,7 @@
         <v>237</v>
       </c>
       <c r="I96" s="22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
@@ -6889,9 +6918,9 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
-        <v>205</v>
+    <row r="97" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>280</v>
@@ -6915,7 +6944,7 @@
         <v>237</v>
       </c>
       <c r="I97" s="22" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -6937,9 +6966,9 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="25" t="s">
-        <v>206</v>
+    <row r="98" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>204</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>280</v>
@@ -6963,7 +6992,7 @@
         <v>237</v>
       </c>
       <c r="I98" s="22" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -6985,9 +7014,9 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
-        <v>207</v>
+    <row r="99" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>280</v>
@@ -7011,7 +7040,7 @@
         <v>237</v>
       </c>
       <c r="I99" s="22" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -7033,9 +7062,9 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
-        <v>208</v>
+    <row r="100" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A100" s="25" t="s">
+        <v>206</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>280</v>
@@ -7059,7 +7088,7 @@
         <v>237</v>
       </c>
       <c r="I100" s="22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
@@ -7081,9 +7110,9 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
-        <v>209</v>
+    <row r="101" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>280</v>
@@ -7107,7 +7136,7 @@
         <v>237</v>
       </c>
       <c r="I101" s="22" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
@@ -7129,9 +7158,9 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>280</v>
@@ -7155,7 +7184,7 @@
         <v>237</v>
       </c>
       <c r="I102" s="22" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
@@ -7177,15 +7206,15 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="11" t="s">
-        <v>211</v>
+    <row r="103" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>11</v>
@@ -7197,13 +7226,13 @@
         <v>104</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>235</v>
+        <v>136</v>
       </c>
       <c r="H103" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="I103" s="8" t="s">
-        <v>225</v>
+      <c r="I103" s="22" t="s">
+        <v>223</v>
       </c>
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
@@ -7225,15 +7254,15 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="11" t="s">
-        <v>213</v>
+    <row r="104" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>11</v>
@@ -7245,20 +7274,16 @@
         <v>104</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>235</v>
+        <v>136</v>
       </c>
       <c r="H104" s="8" t="s">
         <v>237</v>
       </c>
       <c r="I104" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="J104" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="K104" s="20" t="s">
-        <v>228</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="J104" s="9"/>
+      <c r="K104" s="9"/>
       <c r="L104" s="9"/>
       <c r="M104" s="9"/>
       <c r="N104" s="9"/>
@@ -7277,9 +7302,9 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>280</v>
@@ -7300,26 +7325,16 @@
         <v>235</v>
       </c>
       <c r="H105" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I105" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="I105" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="J105" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="K105" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="L105" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="M105" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="N105" s="20" t="s">
-        <v>233</v>
-      </c>
+      <c r="J105" s="9"/>
+      <c r="K105" s="9"/>
+      <c r="L105" s="9"/>
+      <c r="M105" s="9"/>
+      <c r="N105" s="9"/>
       <c r="O105" s="2"/>
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
@@ -7335,17 +7350,17 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>241</v>
+    <row r="106" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A106" s="11" t="s">
+        <v>213</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C106" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="D106" s="9" t="s">
+      <c r="C106" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D106" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E106" s="7" t="s">
@@ -7354,17 +7369,21 @@
       <c r="F106" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G106" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="H106" s="20" t="s">
+      <c r="G106" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H106" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="I106" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="J106" s="9"/>
-      <c r="K106" s="9"/>
+      <c r="I106" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="J106" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="K106" s="20" t="s">
+        <v>228</v>
+      </c>
       <c r="L106" s="9"/>
       <c r="M106" s="9"/>
       <c r="N106" s="9"/>
@@ -7383,17 +7402,17 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>245</v>
+    <row r="107" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A107" s="11" t="s">
+        <v>214</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C107" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="D107" s="9" t="s">
+      <c r="C107" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D107" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E107" s="7" t="s">
@@ -7402,20 +7421,30 @@
       <c r="F107" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G107" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="H107" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="I107" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="J107" s="9"/>
-      <c r="K107" s="9"/>
-      <c r="L107" s="9"/>
-      <c r="M107" s="9"/>
-      <c r="N107" s="9"/>
+      <c r="G107" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H107" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="I107" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="J107" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="K107" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="L107" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="M107" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="N107" s="20" t="s">
+        <v>233</v>
+      </c>
       <c r="O107" s="2"/>
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
@@ -7431,9 +7460,9 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>280</v>
@@ -7457,7 +7486,7 @@
         <v>237</v>
       </c>
       <c r="I108" s="20" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
@@ -7479,17 +7508,17 @@
       <c r="AA108" s="2"/>
       <c r="AB108" s="2"/>
     </row>
-    <row r="109" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="23" t="s">
-        <v>260</v>
+    <row r="109" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>245</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C109" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D109" s="24" t="s">
+      <c r="C109" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D109" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E109" s="7" t="s">
@@ -7498,21 +7527,17 @@
       <c r="F109" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G109" s="6" t="s">
-        <v>235</v>
+      <c r="G109" s="9" t="s">
+        <v>243</v>
       </c>
       <c r="H109" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="I109" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="J109" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="K109" s="20" t="s">
-        <v>263</v>
-      </c>
+      <c r="I109" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="J109" s="9"/>
+      <c r="K109" s="9"/>
       <c r="L109" s="9"/>
       <c r="M109" s="9"/>
       <c r="N109" s="9"/>
@@ -7531,17 +7556,17 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="11" t="s">
-        <v>262</v>
+    <row r="110" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>247</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C110" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="D110" s="6" t="s">
+      <c r="C110" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D110" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E110" s="7" t="s">
@@ -7550,17 +7575,17 @@
       <c r="F110" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G110" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="H110" s="8" t="s">
+      <c r="G110" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="H110" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="I110" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="J110" s="20"/>
-      <c r="K110" s="20"/>
+      <c r="I110" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="J110" s="9"/>
+      <c r="K110" s="9"/>
       <c r="L110" s="9"/>
       <c r="M110" s="9"/>
       <c r="N110" s="9"/>
@@ -7579,9 +7604,9 @@
       <c r="AA110" s="2"/>
       <c r="AB110" s="2"/>
     </row>
-    <row r="111" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="11" t="s">
-        <v>270</v>
+    <row r="111" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="23" t="s">
+        <v>260</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>280</v>
@@ -7589,7 +7614,7 @@
       <c r="C111" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D111" s="6" t="s">
+      <c r="D111" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E111" s="7" t="s">
@@ -7601,7 +7626,7 @@
       <c r="G111" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="H111" s="8" t="s">
+      <c r="H111" s="20" t="s">
         <v>237</v>
       </c>
       <c r="I111" s="22" t="s">
@@ -7613,9 +7638,9 @@
       <c r="K111" s="20" t="s">
         <v>263</v>
       </c>
-      <c r="L111" s="20"/>
-      <c r="M111" s="20"/>
-      <c r="N111" s="20"/>
+      <c r="L111" s="9"/>
+      <c r="M111" s="9"/>
+      <c r="N111" s="9"/>
       <c r="O111" s="2"/>
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
@@ -7631,18 +7656,18 @@
       <c r="AA111" s="2"/>
       <c r="AB111" s="2"/>
     </row>
-    <row r="112" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>10</v>
+        <v>269</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E112" s="7" t="s">
         <v>104</v>
@@ -7651,14 +7676,16 @@
         <v>104</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="H112" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="I112" s="9"/>
-      <c r="J112" s="9"/>
-      <c r="K112" s="9"/>
+        <v>237</v>
+      </c>
+      <c r="I112" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="J112" s="20"/>
+      <c r="K112" s="20"/>
       <c r="L112" s="9"/>
       <c r="M112" s="9"/>
       <c r="N112" s="9"/>
@@ -7677,18 +7704,18 @@
       <c r="AA112" s="2"/>
       <c r="AB112" s="2"/>
     </row>
-    <row r="113" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="27" t="s">
-        <v>278</v>
+    <row r="113" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A113" s="11" t="s">
+        <v>270</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>135</v>
+        <v>212</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E113" s="7" t="s">
         <v>104</v>
@@ -7696,25 +7723,48 @@
       <c r="F113" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G113" s="26" t="s">
-        <v>279</v>
+      <c r="G113" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="H113" s="8" t="s">
         <v>237</v>
       </c>
       <c r="I113" s="22" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>282</v>
+        <v>261</v>
+      </c>
+      <c r="J113" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="K113" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="L113" s="20"/>
+      <c r="M113" s="20"/>
+      <c r="N113" s="20"/>
+      <c r="O113" s="2"/>
+      <c r="P113" s="2"/>
+      <c r="Q113" s="2"/>
+      <c r="R113" s="2"/>
+      <c r="S113" s="2"/>
+      <c r="T113" s="2"/>
+      <c r="U113" s="2"/>
+      <c r="V113" s="2"/>
+      <c r="W113" s="2"/>
+      <c r="X113" s="2"/>
+      <c r="Y113" s="2"/>
+      <c r="Z113" s="2"/>
+      <c r="AA113" s="2"/>
+      <c r="AB113" s="2"/>
+    </row>
+    <row r="114" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="11" t="s">
+        <v>268</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>280</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>135</v>
+        <v>10</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>14</v>
@@ -7723,21 +7773,38 @@
         <v>104</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="G114" s="26" t="s">
-        <v>279</v>
+        <v>104</v>
+      </c>
+      <c r="G114" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="H114" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="I114" s="22" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>285</v>
+        <v>275</v>
+      </c>
+      <c r="I114" s="9"/>
+      <c r="J114" s="9"/>
+      <c r="K114" s="9"/>
+      <c r="L114" s="9"/>
+      <c r="M114" s="9"/>
+      <c r="N114" s="9"/>
+      <c r="O114" s="2"/>
+      <c r="P114" s="2"/>
+      <c r="Q114" s="2"/>
+      <c r="R114" s="2"/>
+      <c r="S114" s="2"/>
+      <c r="T114" s="2"/>
+      <c r="U114" s="2"/>
+      <c r="V114" s="2"/>
+      <c r="W114" s="2"/>
+      <c r="X114" s="2"/>
+      <c r="Y114" s="2"/>
+      <c r="Z114" s="2"/>
+      <c r="AA114" s="2"/>
+      <c r="AB114" s="2"/>
+    </row>
+    <row r="115" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A115" s="27" t="s">
+        <v>278</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>280</v>
@@ -7761,12 +7828,12 @@
         <v>237</v>
       </c>
       <c r="I115" s="22" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="116" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>280</v>
@@ -7781,7 +7848,7 @@
         <v>104</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>104</v>
+        <v>283</v>
       </c>
       <c r="G116" s="26" t="s">
         <v>279</v>
@@ -7790,12 +7857,12 @@
         <v>237</v>
       </c>
       <c r="I116" s="22" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="117" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>280</v>
@@ -7819,12 +7886,12 @@
         <v>237</v>
       </c>
       <c r="I117" s="22" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="118" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>280</v>
@@ -7848,12 +7915,12 @@
         <v>237</v>
       </c>
       <c r="I118" s="22" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="119" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>280</v>
@@ -7877,12 +7944,12 @@
         <v>237</v>
       </c>
       <c r="I119" s="22" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="120" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>280</v>
@@ -7906,12 +7973,12 @@
         <v>237</v>
       </c>
       <c r="I120" s="22" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="121" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>280</v>
@@ -7935,12 +8002,12 @@
         <v>237</v>
       </c>
       <c r="I121" s="22" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="122" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>280</v>
@@ -7964,12 +8031,12 @@
         <v>237</v>
       </c>
       <c r="I122" s="22" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="123" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>280</v>
@@ -7993,18 +8060,69 @@
         <v>237</v>
       </c>
       <c r="I123" s="22" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="124" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>300</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E124" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G124" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="H124" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I124" s="22" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="125" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>311</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G125" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="H125" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I125" s="22" t="s">
         <v>312</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I123" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="AccountLimit"/>
-        <filter val="AccountLimit - shedule"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I125" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added coyni portal - commission account methods
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(06-03-2023)Agreements\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(09-03-2023)Test Data&amp; Script\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21449379-0756-4FB7-A1F7-79013ADF1F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9039767-87C5-4010-927C-CDFC325E6411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -450,14 +450,6 @@
 -pexpSubHeading,
 -pdropDown,
 -pcheckBox</t>
-  </si>
-  <si>
-    <t>verify Token Account Activity</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.CoyniPortalTest,
-testTokenAccountActivity,
--pheading</t>
   </si>
   <si>
     <t>testTotalWithdraw</t>
@@ -1885,6 +1877,15 @@
   </si>
   <si>
     <t>BalanceReport</t>
+  </si>
+  <si>
+    <t>verify Commission Account With Payout history</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.CoyniPortalTest,
+testCommissionAccountPayOut,
+-pheading,
+-psearch</t>
   </si>
 </sst>
 </file>
@@ -1997,7 +1998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2046,7 +2047,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2329,8 +2329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2341,7 +2341,7 @@
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.42578125" customWidth="1"/>
     <col min="9" max="9" width="43.140625" customWidth="1"/>
     <col min="10" max="10" width="38.85546875" customWidth="1"/>
@@ -2390,7 +2390,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>
@@ -2399,16 +2399,16 @@
         <v>11</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -2433,10 +2433,10 @@
     </row>
     <row r="3" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>10</v>
@@ -2445,16 +2445,16 @@
         <v>14</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -2482,7 +2482,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>10</v>
@@ -2491,10 +2491,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>12</v>
@@ -2528,7 +2528,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
@@ -2537,16 +2537,16 @@
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -2571,10 +2571,10 @@
     </row>
     <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>10</v>
@@ -2583,16 +2583,16 @@
         <v>14</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -2620,7 +2620,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>24</v>
@@ -2629,16 +2629,16 @@
         <v>14</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -2666,7 +2666,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>24</v>
@@ -2675,16 +2675,16 @@
         <v>14</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -2712,7 +2712,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>24</v>
@@ -2721,10 +2721,10 @@
         <v>14</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>25</v>
@@ -2758,7 +2758,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>24</v>
@@ -2767,10 +2767,10 @@
         <v>14</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>25</v>
@@ -2804,7 +2804,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>32</v>
@@ -2813,10 +2813,10 @@
         <v>11</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>33</v>
@@ -2850,7 +2850,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>32</v>
@@ -2859,10 +2859,10 @@
         <v>11</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>33</v>
@@ -2896,7 +2896,7 @@
         <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>32</v>
@@ -2942,7 +2942,7 @@
         <v>39</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>32</v>
@@ -2988,7 +2988,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>32</v>
@@ -3031,10 +3031,10 @@
     </row>
     <row r="16" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>10</v>
@@ -3043,19 +3043,19 @@
         <v>11</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
@@ -3079,31 +3079,31 @@
     </row>
     <row r="17" spans="1:28" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>130</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>132</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -3127,31 +3127,31 @@
     </row>
     <row r="18" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -3175,31 +3175,31 @@
     </row>
     <row r="19" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -3223,31 +3223,31 @@
     </row>
     <row r="20" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -3274,7 +3274,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>18</v>
@@ -3283,19 +3283,19 @@
         <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -3322,7 +3322,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>18</v>
@@ -3331,16 +3331,16 @@
         <v>11</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>20</v>
@@ -3370,7 +3370,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
@@ -3379,16 +3379,16 @@
         <v>11</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>22</v>
@@ -3415,13 +3415,13 @@
     </row>
     <row r="24" spans="1:28" ht="270" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>11</v>
@@ -3433,13 +3433,13 @@
         <v>1</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -3463,13 +3463,13 @@
     </row>
     <row r="25" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>14</v>
@@ -3481,13 +3481,13 @@
         <v>2</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -3511,13 +3511,13 @@
     </row>
     <row r="26" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>233</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>11</v>
@@ -3529,13 +3529,13 @@
         <v>1</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -3559,31 +3559,31 @@
     </row>
     <row r="27" spans="1:28" ht="285" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -3607,10 +3607,10 @@
     </row>
     <row r="28" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>18</v>
@@ -3619,19 +3619,19 @@
         <v>11</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -3639,12 +3639,12 @@
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
     </row>
-    <row r="29" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>18</v>
@@ -3653,19 +3653,19 @@
         <v>14</v>
       </c>
       <c r="E29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I29" s="20" t="s">
         <v>96</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -3687,12 +3687,12 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
     </row>
-    <row r="30" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>97</v>
+        <v>332</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>18</v>
@@ -3701,19 +3701,19 @@
         <v>14</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I30" s="20" t="s">
-        <v>98</v>
+        <v>333</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -3737,10 +3737,10 @@
     </row>
     <row r="31" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>18</v>
@@ -3749,19 +3749,19 @@
         <v>11</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -3785,10 +3785,10 @@
     </row>
     <row r="32" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>18</v>
@@ -3797,19 +3797,19 @@
         <v>11</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3833,10 +3833,10 @@
     </row>
     <row r="33" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>18</v>
@@ -3845,19 +3845,19 @@
         <v>11</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -3881,10 +3881,10 @@
     </row>
     <row r="34" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>18</v>
@@ -3893,19 +3893,19 @@
         <v>11</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -3929,10 +3929,10 @@
     </row>
     <row r="35" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>18</v>
@@ -3941,19 +3941,19 @@
         <v>11</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -3980,7 +3980,7 @@
         <v>43</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>44</v>
@@ -3989,16 +3989,16 @@
         <v>11</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>45</v>
@@ -4025,10 +4025,10 @@
     </row>
     <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>44</v>
@@ -4037,19 +4037,19 @@
         <v>11</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="9"/>
@@ -4076,7 +4076,7 @@
         <v>46</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>44</v>
@@ -4085,16 +4085,16 @@
         <v>11</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>47</v>
@@ -4124,7 +4124,7 @@
         <v>48</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>44</v>
@@ -4133,16 +4133,16 @@
         <v>11</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>49</v>
@@ -4172,7 +4172,7 @@
         <v>50</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>44</v>
@@ -4181,16 +4181,16 @@
         <v>11</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>51</v>
@@ -4220,7 +4220,7 @@
         <v>52</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>44</v>
@@ -4229,16 +4229,16 @@
         <v>11</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I41" s="8" t="s">
         <v>53</v>
@@ -4268,7 +4268,7 @@
         <v>54</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>44</v>
@@ -4277,16 +4277,16 @@
         <v>11</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>55</v>
@@ -4316,7 +4316,7 @@
         <v>56</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>57</v>
@@ -4325,19 +4325,19 @@
         <v>11</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
@@ -4364,7 +4364,7 @@
         <v>58</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>57</v>
@@ -4373,16 +4373,16 @@
         <v>11</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>59</v>
@@ -4412,7 +4412,7 @@
         <v>60</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>57</v>
@@ -4421,16 +4421,16 @@
         <v>11</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>61</v>
@@ -4460,7 +4460,7 @@
         <v>62</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>57</v>
@@ -4469,16 +4469,16 @@
         <v>11</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>63</v>
@@ -4508,7 +4508,7 @@
         <v>64</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>57</v>
@@ -4517,16 +4517,16 @@
         <v>11</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I47" s="8" t="s">
         <v>65</v>
@@ -4556,7 +4556,7 @@
         <v>66</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>57</v>
@@ -4565,16 +4565,16 @@
         <v>11</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>67</v>
@@ -4604,7 +4604,7 @@
         <v>68</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>57</v>
@@ -4613,16 +4613,16 @@
         <v>11</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>69</v>
@@ -4649,10 +4649,10 @@
     </row>
     <row r="50" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>57</v>
@@ -4661,19 +4661,19 @@
         <v>11</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -4700,7 +4700,7 @@
         <v>70</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>57</v>
@@ -4709,16 +4709,16 @@
         <v>11</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I51" s="8" t="s">
         <v>71</v>
@@ -4745,31 +4745,31 @@
     </row>
     <row r="52" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -4793,31 +4793,31 @@
     </row>
     <row r="53" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -4841,31 +4841,31 @@
     </row>
     <row r="54" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -4875,31 +4875,31 @@
     </row>
     <row r="55" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I55" s="22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
@@ -4923,31 +4923,31 @@
     </row>
     <row r="56" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I56" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
@@ -4971,31 +4971,31 @@
     </row>
     <row r="57" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I57" s="22" t="s">
         <v>125</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="I57" s="22" t="s">
-        <v>127</v>
       </c>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -5019,31 +5019,31 @@
     </row>
     <row r="58" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -5067,31 +5067,31 @@
     </row>
     <row r="59" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I59" s="22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -5115,31 +5115,31 @@
     </row>
     <row r="60" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -5163,31 +5163,31 @@
     </row>
     <row r="61" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I61" s="22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -5211,31 +5211,31 @@
     </row>
     <row r="62" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -5259,31 +5259,31 @@
     </row>
     <row r="63" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -5307,31 +5307,31 @@
     </row>
     <row r="64" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -5355,31 +5355,31 @@
     </row>
     <row r="65" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I65" s="22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -5403,31 +5403,31 @@
     </row>
     <row r="66" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I66" s="22" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -5451,31 +5451,31 @@
     </row>
     <row r="67" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I67" s="22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -5499,350 +5499,350 @@
     </row>
     <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A68" s="26" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I68" s="22" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I69" s="22" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="70" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I70" s="22" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I71" s="22" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="72" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H72" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I72" s="22" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I73" s="22" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I74" s="22" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="75" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I75" s="22" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="76" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H76" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I76" s="22" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="77" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H77" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I77" s="22" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="78" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H78" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I78" s="22" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="79" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A79" s="28" t="s">
+      <c r="A79" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H79" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I79" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G79" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="H79" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="I79" s="8" t="s">
-        <v>140</v>
       </c>
       <c r="J79" s="6"/>
       <c r="K79" s="6"/>
@@ -5865,32 +5865,32 @@
       <c r="AB79" s="2"/>
     </row>
     <row r="80" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A80" s="28" t="s">
-        <v>165</v>
+      <c r="A80" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J80" s="8"/>
       <c r="K80" s="9"/>
@@ -5913,32 +5913,32 @@
       <c r="AB80" s="2"/>
     </row>
     <row r="81" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A81" s="28" t="s">
-        <v>167</v>
+      <c r="A81" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C81" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H81" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I81" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G81" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="H81" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="I81" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="J81" s="8"/>
       <c r="K81" s="9"/>
@@ -5961,35 +5961,35 @@
       <c r="AB81" s="2"/>
     </row>
     <row r="82" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A82" s="28" t="s">
-        <v>169</v>
+      <c r="A82" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C82" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H82" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I82" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="D82" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="H82" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="I82" s="8" t="s">
+      <c r="J82" s="20" t="s">
         <v>168</v>
-      </c>
-      <c r="J82" s="20" t="s">
-        <v>170</v>
       </c>
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
@@ -6012,31 +6012,31 @@
     </row>
     <row r="83" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="H83" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I83" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="H83" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="I83" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="J83" s="6"/>
       <c r="K83" s="6"/>
@@ -6060,31 +6060,31 @@
     </row>
     <row r="84" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H84" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J84" s="6"/>
       <c r="K84" s="6"/>
@@ -6108,31 +6108,31 @@
     </row>
     <row r="85" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H85" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J85" s="6"/>
       <c r="K85" s="6"/>
@@ -6156,31 +6156,31 @@
     </row>
     <row r="86" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H86" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J86" s="6"/>
       <c r="K86" s="6"/>
@@ -6204,31 +6204,31 @@
     </row>
     <row r="87" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H87" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
@@ -6252,31 +6252,31 @@
     </row>
     <row r="88" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A88" s="27" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
@@ -6300,31 +6300,31 @@
     </row>
     <row r="89" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H89" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
@@ -6348,31 +6348,31 @@
     </row>
     <row r="90" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G90" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C90" s="9" t="s">
+      <c r="H90" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="I90" s="20" t="s">
         <v>218</v>
-      </c>
-      <c r="D90" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G90" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="H90" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="I90" s="20" t="s">
-        <v>220</v>
       </c>
       <c r="J90" s="9"/>
       <c r="K90" s="9"/>
@@ -6396,31 +6396,31 @@
     </row>
     <row r="91" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D91" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H91" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I91" s="20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J91" s="9"/>
       <c r="K91" s="9"/>
@@ -6444,31 +6444,31 @@
     </row>
     <row r="92" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G92" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H92" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I92" s="20" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J92" s="9"/>
       <c r="K92" s="9"/>
@@ -6492,10 +6492,10 @@
     </row>
     <row r="93" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>77</v>
@@ -6504,19 +6504,19 @@
         <v>11</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I93" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
@@ -6540,10 +6540,10 @@
     </row>
     <row r="94" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>77</v>
@@ -6552,16 +6552,16 @@
         <v>11</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H94" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I94" s="8" t="s">
         <v>78</v>
@@ -6591,7 +6591,7 @@
         <v>79</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>77</v>
@@ -6600,16 +6600,16 @@
         <v>14</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I95" s="8" t="s">
         <v>80</v>
@@ -6639,7 +6639,7 @@
         <v>72</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>73</v>
@@ -6648,16 +6648,16 @@
         <v>11</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H96" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I96" s="8" t="s">
         <v>74</v>
@@ -6684,10 +6684,10 @@
     </row>
     <row r="97" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>73</v>
@@ -6696,19 +6696,19 @@
         <v>11</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I97" s="22" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -6732,10 +6732,10 @@
     </row>
     <row r="98" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>73</v>
@@ -6744,19 +6744,19 @@
         <v>11</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H98" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I98" s="22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -6780,10 +6780,10 @@
     </row>
     <row r="99" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>73</v>
@@ -6792,19 +6792,19 @@
         <v>11</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H99" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I99" s="22" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -6831,7 +6831,7 @@
         <v>75</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C100" s="18" t="s">
         <v>73</v>
@@ -6840,19 +6840,19 @@
         <v>11</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
@@ -6879,7 +6879,7 @@
         <v>76</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>73</v>
@@ -6888,19 +6888,19 @@
         <v>11</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I101" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
@@ -6923,32 +6923,32 @@
       <c r="AB101" s="2"/>
     </row>
     <row r="102" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="28" t="s">
-        <v>110</v>
+      <c r="A102" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I102" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
@@ -6971,32 +6971,32 @@
       <c r="AB102" s="2"/>
     </row>
     <row r="103" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="28" t="s">
-        <v>299</v>
+      <c r="A103" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H103" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I103" s="8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
@@ -7020,28 +7020,28 @@
     </row>
     <row r="104" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H104" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I104" s="8" t="s">
         <v>303</v>
@@ -7071,28 +7071,28 @@
         <v>304</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C105" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="H105" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I105" s="8" t="s">
         <v>301</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E105" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F105" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="H105" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="I105" s="8" t="s">
-        <v>305</v>
       </c>
       <c r="J105" s="9"/>
       <c r="K105" s="9"/>
@@ -7116,10 +7116,10 @@
     </row>
     <row r="106" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A106" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C106" s="18" t="s">
         <v>73</v>
@@ -7128,19 +7128,19 @@
         <v>11</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G106" s="18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H106" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
@@ -7164,31 +7164,31 @@
     </row>
     <row r="107" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H107" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I107" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
@@ -7212,10 +7212,10 @@
     </row>
     <row r="108" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C108" s="18" t="s">
         <v>73</v>
@@ -7224,19 +7224,19 @@
         <v>11</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H108" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I108" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
@@ -7260,31 +7260,31 @@
     </row>
     <row r="109" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C109" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G109" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="H109" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I109" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E109" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F109" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G109" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="H109" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="I109" s="8" t="s">
-        <v>119</v>
       </c>
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
@@ -7308,31 +7308,31 @@
     </row>
     <row r="110" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C110" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B110" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C110" s="6" t="s">
-        <v>156</v>
-      </c>
       <c r="D110" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G110" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H110" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I110" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="H110" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="I110" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="J110" s="6"/>
       <c r="K110" s="6"/>
@@ -7356,31 +7356,31 @@
     </row>
     <row r="111" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F111" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H111" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I111" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J111" s="6"/>
       <c r="K111" s="6"/>
@@ -7404,31 +7404,31 @@
     </row>
     <row r="112" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H112" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I112" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J112" s="6"/>
       <c r="K112" s="6"/>
@@ -7452,31 +7452,31 @@
     </row>
     <row r="113" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H113" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I113" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J113" s="6"/>
       <c r="K113" s="6"/>
@@ -7500,31 +7500,31 @@
     </row>
     <row r="114" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H114" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I114" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J114" s="6"/>
       <c r="K114" s="6"/>
@@ -7548,31 +7548,31 @@
     </row>
     <row r="115" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H115" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I115" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J115" s="6"/>
       <c r="K115" s="6"/>
@@ -7596,31 +7596,31 @@
     </row>
     <row r="116" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A116" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G116" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H116" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="H116" s="8" t="s">
-        <v>213</v>
-      </c>
       <c r="I116" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J116" s="9"/>
       <c r="K116" s="9"/>
@@ -7644,37 +7644,37 @@
     </row>
     <row r="117" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A117" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F117" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G117" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H117" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="H117" s="8" t="s">
-        <v>213</v>
-      </c>
       <c r="I117" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="J117" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="K117" s="20" t="s">
         <v>202</v>
-      </c>
-      <c r="J117" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="K117" s="20" t="s">
-        <v>204</v>
       </c>
       <c r="L117" s="9"/>
       <c r="M117" s="9"/>
@@ -7696,46 +7696,46 @@
     </row>
     <row r="118" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F118" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H118" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="I118" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="J118" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="K118" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="I118" s="22" t="s">
+      <c r="L118" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="J118" s="20" t="s">
+      <c r="M118" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="K118" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="L118" s="20" t="s">
+      <c r="N118" s="20" t="s">
         <v>207</v>
-      </c>
-      <c r="M118" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="N118" s="20" t="s">
-        <v>209</v>
       </c>
       <c r="O118" s="2"/>
       <c r="P118" s="2"/>
@@ -7754,37 +7754,37 @@
     </row>
     <row r="119" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="23" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D119" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F119" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G119" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H119" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="H119" s="20" t="s">
-        <v>213</v>
-      </c>
       <c r="I119" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="J119" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="K119" s="20" t="s">
         <v>236</v>
-      </c>
-      <c r="J119" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="K119" s="20" t="s">
-        <v>238</v>
       </c>
       <c r="L119" s="9"/>
       <c r="M119" s="9"/>
@@ -7806,31 +7806,31 @@
     </row>
     <row r="120" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G120" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H120" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="H120" s="8" t="s">
-        <v>213</v>
-      </c>
       <c r="I120" s="22" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J120" s="20"/>
       <c r="K120" s="20"/>
@@ -7854,37 +7854,37 @@
     </row>
     <row r="121" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G121" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H121" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="H121" s="8" t="s">
-        <v>213</v>
-      </c>
       <c r="I121" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="J121" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="K121" s="20" t="s">
         <v>236</v>
-      </c>
-      <c r="J121" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="K121" s="20" t="s">
-        <v>238</v>
       </c>
       <c r="L121" s="20"/>
       <c r="M121" s="20"/>
@@ -7905,11 +7905,11 @@
       <c r="AB121" s="2"/>
     </row>
     <row r="122" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="28" t="s">
-        <v>243</v>
+      <c r="A122" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>10</v>
@@ -7918,16 +7918,16 @@
         <v>14</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F122" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G122" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H122" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I122" s="9"/>
       <c r="J122" s="9"/>

</xml_diff>

<commit_message>
Modified test methods for coyni portal and Commission Account Page
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(09-03-2023)Test Data&amp; Script\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9039767-87C5-4010-927C-CDFC325E6411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF66CC8D-6413-4C35-9818-6222779D8333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$124</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="338">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1884,8 +1884,25 @@
   <si>
     <t>coyni.admin.tests.CoyniPortalTest,
 testCommissionAccountPayOut,
+-pheading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify Commission Account  manual batch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.admin.tests.CoyniPortalTest,
+testCommissionAccountManualBatchNow,
+-pheading
+</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.CoyniPortalTest,
+testCommissionAccountTransactionList,
 -pheading,
--psearch</t>
+-pquery</t>
+  </si>
+  <si>
+    <t>verify CommissionAccountTransactionList</t>
   </si>
 </sst>
 </file>
@@ -2327,10 +2344,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB122"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AB124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,7 +2403,7 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2431,7 +2449,7 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>250</v>
       </c>
@@ -2477,7 +2495,7 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -2523,7 +2541,7 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
@@ -2569,7 +2587,7 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>139</v>
       </c>
@@ -2615,7 +2633,7 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="240" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -2661,7 +2679,7 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="210.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="210.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>26</v>
       </c>
@@ -2707,7 +2725,7 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="210" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -2753,7 +2771,7 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -2799,7 +2817,7 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="255" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
@@ -2845,7 +2863,7 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="225" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
@@ -2891,7 +2909,7 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="210" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
@@ -2937,7 +2955,7 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -2983,7 +3001,7 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="195" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>41</v>
       </c>
@@ -3029,7 +3047,7 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>244</v>
       </c>
@@ -3077,7 +3095,7 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
-    <row r="17" spans="1:28" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>128</v>
       </c>
@@ -3125,7 +3143,7 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>129</v>
       </c>
@@ -3173,7 +3191,7 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>131</v>
       </c>
@@ -3221,7 +3239,7 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
     </row>
-    <row r="20" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>148</v>
       </c>
@@ -3269,7 +3287,7 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
     </row>
-    <row r="21" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -3317,7 +3335,7 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -3365,7 +3383,7 @@
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
     </row>
-    <row r="23" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -3413,7 +3431,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
     </row>
-    <row r="24" spans="1:28" ht="270" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>227</v>
       </c>
@@ -3461,7 +3479,7 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
     </row>
-    <row r="25" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>228</v>
       </c>
@@ -3509,7 +3527,7 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
     </row>
-    <row r="26" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>229</v>
       </c>
@@ -3557,7 +3575,7 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="285" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>230</v>
       </c>
@@ -3605,7 +3623,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>144</v>
       </c>
@@ -3639,12 +3657,12 @@
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
     </row>
-    <row r="29" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>18</v>
@@ -3687,9 +3705,9 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
     </row>
-    <row r="30" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>252</v>
@@ -3713,7 +3731,7 @@
         <v>212</v>
       </c>
       <c r="I30" s="20" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -3735,9 +3753,9 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>97</v>
+        <v>332</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>252</v>
@@ -3746,7 +3764,7 @@
         <v>18</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>94</v>
@@ -3758,10 +3776,10 @@
         <v>328</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>98</v>
+        <v>212</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>333</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -3783,9 +3801,9 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>252</v>
@@ -3809,7 +3827,7 @@
         <v>211</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3831,9 +3849,9 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>252</v>
@@ -3857,7 +3875,7 @@
         <v>211</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -3879,9 +3897,9 @@
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
     </row>
-    <row r="34" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>252</v>
@@ -3905,7 +3923,7 @@
         <v>211</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -3927,9 +3945,9 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>252</v>
@@ -3953,7 +3971,7 @@
         <v>211</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -3975,15 +3993,15 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>11</v>
@@ -3995,15 +4013,15 @@
         <v>94</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J36" s="6"/>
+        <v>106</v>
+      </c>
+      <c r="J36" s="9"/>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
@@ -4025,13 +4043,13 @@
     </row>
     <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>169</v>
+        <v>337</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>11</v>
@@ -4043,15 +4061,15 @@
         <v>94</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="J37" s="6"/>
+        <v>336</v>
+      </c>
+      <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
@@ -4071,9 +4089,9 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>252</v>
@@ -4091,13 +4109,13 @@
         <v>94</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>307</v>
+        <v>329</v>
       </c>
       <c r="H38" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="9"/>
@@ -4119,9 +4137,9 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>48</v>
+        <v>169</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>252</v>
@@ -4139,13 +4157,13 @@
         <v>94</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>49</v>
+        <v>170</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="9"/>
@@ -4167,9 +4185,9 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>252</v>
@@ -4193,7 +4211,7 @@
         <v>211</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="9"/>
@@ -4215,9 +4233,9 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>252</v>
@@ -4241,7 +4259,7 @@
         <v>211</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="9"/>
@@ -4263,9 +4281,9 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>252</v>
@@ -4289,7 +4307,7 @@
         <v>211</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J42" s="6"/>
       <c r="K42" s="9"/>
@@ -4311,15 +4329,15 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>11</v>
@@ -4331,16 +4349,16 @@
         <v>94</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>141</v>
+        <v>53</v>
       </c>
       <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
+      <c r="K43" s="9"/>
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
@@ -4359,15 +4377,15 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>11</v>
@@ -4379,16 +4397,16 @@
         <v>94</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
+      <c r="K44" s="9"/>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
@@ -4407,9 +4425,9 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>252</v>
@@ -4433,7 +4451,7 @@
         <v>211</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -4455,9 +4473,9 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>252</v>
@@ -4481,7 +4499,7 @@
         <v>211</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -4503,9 +4521,9 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>252</v>
@@ -4529,7 +4547,7 @@
         <v>211</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
@@ -4551,9 +4569,9 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>252</v>
@@ -4571,13 +4589,13 @@
         <v>94</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -4599,9 +4617,9 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>252</v>
@@ -4619,13 +4637,13 @@
         <v>94</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -4647,9 +4665,9 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>134</v>
+        <v>66</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>252</v>
@@ -4667,13 +4685,13 @@
         <v>94</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>135</v>
+        <v>67</v>
       </c>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -4695,9 +4713,9 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>252</v>
@@ -4721,7 +4739,7 @@
         <v>211</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -4743,15 +4761,15 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>11</v>
@@ -4763,13 +4781,13 @@
         <v>94</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I52" s="19" t="s">
-        <v>143</v>
+      <c r="I52" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -4791,15 +4809,15 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>146</v>
+        <v>70</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>11</v>
@@ -4811,13 +4829,13 @@
         <v>94</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I53" s="19" t="s">
-        <v>147</v>
+      <c r="I53" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -4839,15 +4857,15 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>118</v>
+    <row r="54" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>11</v>
@@ -4859,29 +4877,43 @@
         <v>94</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I54" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9"/>
+        <v>211</v>
+      </c>
+      <c r="I54" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
       <c r="N54" s="9"/>
-    </row>
-    <row r="55" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+      <c r="V54" s="2"/>
+      <c r="W54" s="2"/>
+      <c r="X54" s="2"/>
+      <c r="Y54" s="2"/>
+      <c r="Z54" s="2"/>
+      <c r="AA54" s="2"/>
+      <c r="AB54" s="2"/>
+    </row>
+    <row r="55" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>11</v>
@@ -4893,16 +4925,16 @@
         <v>94</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I55" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
+        <v>211</v>
+      </c>
+      <c r="I55" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
       <c r="N55" s="9"/>
@@ -4921,9 +4953,9 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>121</v>
+    <row r="56" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>252</v>
@@ -4946,32 +4978,18 @@
       <c r="H56" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="I56" s="22" t="s">
-        <v>122</v>
+      <c r="I56" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
       <c r="N56" s="9"/>
-      <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
-      <c r="Q56" s="2"/>
-      <c r="R56" s="2"/>
-      <c r="S56" s="2"/>
-      <c r="T56" s="2"/>
-      <c r="U56" s="2"/>
-      <c r="V56" s="2"/>
-      <c r="W56" s="2"/>
-      <c r="X56" s="2"/>
-      <c r="Y56" s="2"/>
-      <c r="Z56" s="2"/>
-      <c r="AA56" s="2"/>
-      <c r="AB56" s="2"/>
-    </row>
-    <row r="57" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>252</v>
@@ -4989,13 +5007,13 @@
         <v>94</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H57" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I57" s="22" t="s">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -5017,9 +5035,9 @@
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
     </row>
-    <row r="58" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>252</v>
@@ -5037,13 +5055,13 @@
         <v>94</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H58" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -5065,15 +5083,15 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>178</v>
+    <row r="59" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>208</v>
+        <v>124</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>11</v>
@@ -5085,13 +5103,13 @@
         <v>94</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I59" s="22" t="s">
-        <v>191</v>
+        <v>125</v>
       </c>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -5113,15 +5131,15 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>179</v>
+    <row r="60" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>208</v>
+        <v>124</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>11</v>
@@ -5133,13 +5151,13 @@
         <v>94</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>192</v>
+        <v>127</v>
       </c>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -5161,9 +5179,9 @@
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>252</v>
@@ -5187,7 +5205,7 @@
         <v>211</v>
       </c>
       <c r="I61" s="22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -5209,9 +5227,9 @@
       <c r="AA61" s="2"/>
       <c r="AB61" s="2"/>
     </row>
-    <row r="62" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A62" s="25" t="s">
-        <v>181</v>
+    <row r="62" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>252</v>
@@ -5235,7 +5253,7 @@
         <v>211</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -5257,9 +5275,9 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>252</v>
@@ -5283,7 +5301,7 @@
         <v>211</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -5305,9 +5323,9 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>183</v>
+    <row r="64" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="25" t="s">
+        <v>181</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>252</v>
@@ -5331,7 +5349,7 @@
         <v>211</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -5353,9 +5371,9 @@
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
     </row>
-    <row r="65" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>184</v>
+    <row r="65" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>252</v>
@@ -5379,7 +5397,7 @@
         <v>211</v>
       </c>
       <c r="I65" s="22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -5401,9 +5419,9 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>252</v>
@@ -5427,7 +5445,7 @@
         <v>211</v>
       </c>
       <c r="I66" s="22" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -5449,9 +5467,9 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>252</v>
@@ -5475,7 +5493,7 @@
         <v>211</v>
       </c>
       <c r="I67" s="22" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -5497,18 +5515,18 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A68" s="26" t="s">
-        <v>251</v>
+    <row r="68" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E68" s="7" t="s">
         <v>94</v>
@@ -5517,47 +5535,85 @@
         <v>94</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H68" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I68" s="22" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="69" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>254</v>
+        <v>198</v>
+      </c>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2"/>
+      <c r="S68" s="2"/>
+      <c r="T68" s="2"/>
+      <c r="U68" s="2"/>
+      <c r="V68" s="2"/>
+      <c r="W68" s="2"/>
+      <c r="X68" s="2"/>
+      <c r="Y68" s="2"/>
+      <c r="Z68" s="2"/>
+      <c r="AA68" s="2"/>
+      <c r="AB68" s="2"/>
+    </row>
+    <row r="69" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E69" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>255</v>
+        <v>94</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H69" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I69" s="22" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="70" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>257</v>
+        <v>193</v>
+      </c>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="2"/>
+      <c r="R69" s="2"/>
+      <c r="S69" s="2"/>
+      <c r="T69" s="2"/>
+      <c r="U69" s="2"/>
+      <c r="V69" s="2"/>
+      <c r="W69" s="2"/>
+      <c r="X69" s="2"/>
+      <c r="Y69" s="2"/>
+      <c r="Z69" s="2"/>
+      <c r="AA69" s="2"/>
+      <c r="AB69" s="2"/>
+    </row>
+    <row r="70" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="26" t="s">
+        <v>251</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>252</v>
@@ -5581,12 +5637,12 @@
         <v>211</v>
       </c>
       <c r="I70" s="22" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="71" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>252</v>
@@ -5601,7 +5657,7 @@
         <v>94</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>94</v>
+        <v>255</v>
       </c>
       <c r="G71" s="6" t="s">
         <v>323</v>
@@ -5610,12 +5666,12 @@
         <v>211</v>
       </c>
       <c r="I71" s="22" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="72" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>252</v>
@@ -5639,12 +5695,12 @@
         <v>211</v>
       </c>
       <c r="I72" s="22" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="73" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>252</v>
@@ -5668,12 +5724,12 @@
         <v>211</v>
       </c>
       <c r="I73" s="22" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="74" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>252</v>
@@ -5697,12 +5753,12 @@
         <v>211</v>
       </c>
       <c r="I74" s="22" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="75" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>252</v>
@@ -5726,12 +5782,12 @@
         <v>211</v>
       </c>
       <c r="I75" s="22" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="76" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>252</v>
@@ -5755,12 +5811,12 @@
         <v>211</v>
       </c>
       <c r="I76" s="22" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="77" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>252</v>
@@ -5784,12 +5840,12 @@
         <v>211</v>
       </c>
       <c r="I77" s="22" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="78" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>252</v>
@@ -5813,114 +5869,76 @@
         <v>211</v>
       </c>
       <c r="I78" s="22" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>272</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="H79" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I79" s="22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>281</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="H80" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I80" s="22" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="79" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+    <row r="81" spans="1:28" s="1" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B79" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C79" s="6" t="s">
+      <c r="B81" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G79" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="H79" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I79" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="J79" s="6"/>
-      <c r="K79" s="6"/>
-      <c r="L79" s="9"/>
-      <c r="M79" s="9"/>
-      <c r="N79" s="9"/>
-      <c r="O79" s="2"/>
-      <c r="P79" s="2"/>
-      <c r="Q79" s="2"/>
-      <c r="R79" s="2"/>
-      <c r="S79" s="2"/>
-      <c r="T79" s="2"/>
-      <c r="U79" s="2"/>
-      <c r="V79" s="2"/>
-      <c r="W79" s="2"/>
-      <c r="X79" s="2"/>
-      <c r="Y79" s="2"/>
-      <c r="Z79" s="2"/>
-      <c r="AA79" s="2"/>
-      <c r="AB79" s="2"/>
-    </row>
-    <row r="80" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="H80" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I80" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="J80" s="8"/>
-      <c r="K80" s="9"/>
-      <c r="L80" s="9"/>
-      <c r="M80" s="9"/>
-      <c r="N80" s="9"/>
-      <c r="O80" s="2"/>
-      <c r="P80" s="2"/>
-      <c r="Q80" s="2"/>
-      <c r="R80" s="2"/>
-      <c r="S80" s="2"/>
-      <c r="T80" s="2"/>
-      <c r="U80" s="2"/>
-      <c r="V80" s="2"/>
-      <c r="W80" s="2"/>
-      <c r="X80" s="2"/>
-      <c r="Y80" s="2"/>
-      <c r="Z80" s="2"/>
-      <c r="AA80" s="2"/>
-      <c r="AB80" s="2"/>
-    </row>
-    <row r="81" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>11</v>
@@ -5938,10 +5956,10 @@
         <v>212</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="J81" s="8"/>
-      <c r="K81" s="9"/>
+        <v>138</v>
+      </c>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
       <c r="N81" s="9"/>
@@ -5960,9 +5978,9 @@
       <c r="AA81" s="2"/>
       <c r="AB81" s="2"/>
     </row>
-    <row r="82" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>252</v>
@@ -5983,14 +6001,12 @@
         <v>162</v>
       </c>
       <c r="H82" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I82" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="J82" s="20" t="s">
-        <v>168</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="J82" s="8"/>
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
@@ -6010,15 +6026,15 @@
       <c r="AA82" s="2"/>
       <c r="AB82" s="2"/>
     </row>
-    <row r="83" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>11</v>
@@ -6030,17 +6046,17 @@
         <v>94</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>312</v>
+        <v>162</v>
       </c>
       <c r="H83" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I83" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="J83" s="6"/>
-      <c r="K83" s="6"/>
-      <c r="L83" s="6"/>
+        <v>166</v>
+      </c>
+      <c r="J83" s="8"/>
+      <c r="K83" s="9"/>
+      <c r="L83" s="9"/>
       <c r="M83" s="9"/>
       <c r="N83" s="9"/>
       <c r="O83" s="2"/>
@@ -6058,15 +6074,15 @@
       <c r="AA83" s="2"/>
       <c r="AB83" s="2"/>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>11</v>
@@ -6078,17 +6094,19 @@
         <v>94</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>312</v>
+        <v>162</v>
       </c>
       <c r="H84" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="J84" s="6"/>
-      <c r="K84" s="6"/>
-      <c r="L84" s="6"/>
+        <v>166</v>
+      </c>
+      <c r="J84" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="K84" s="9"/>
+      <c r="L84" s="9"/>
       <c r="M84" s="9"/>
       <c r="N84" s="9"/>
       <c r="O84" s="2"/>
@@ -6106,9 +6124,9 @@
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>252</v>
@@ -6132,7 +6150,7 @@
         <v>212</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J85" s="6"/>
       <c r="K85" s="6"/>
@@ -6154,9 +6172,9 @@
       <c r="AA85" s="2"/>
       <c r="AB85" s="2"/>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>252</v>
@@ -6180,7 +6198,7 @@
         <v>212</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J86" s="6"/>
       <c r="K86" s="6"/>
@@ -6202,9 +6220,9 @@
       <c r="AA86" s="2"/>
       <c r="AB86" s="2"/>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>252</v>
@@ -6222,13 +6240,13 @@
         <v>94</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H87" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
@@ -6250,9 +6268,9 @@
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A88" s="27" t="s">
-        <v>284</v>
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>252</v>
@@ -6270,13 +6288,13 @@
         <v>94</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H88" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>285</v>
+        <v>89</v>
       </c>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
@@ -6298,9 +6316,9 @@
       <c r="AA88" s="2"/>
       <c r="AB88" s="2"/>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>252</v>
@@ -6324,7 +6342,7 @@
         <v>212</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
@@ -6346,17 +6364,17 @@
       <c r="AA89" s="2"/>
       <c r="AB89" s="2"/>
     </row>
-    <row r="90" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
-        <v>215</v>
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="27" t="s">
+        <v>284</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C90" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D90" s="9" t="s">
+      <c r="C90" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D90" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E90" s="7" t="s">
@@ -6365,18 +6383,18 @@
       <c r="F90" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G90" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="H90" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="I90" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="J90" s="9"/>
-      <c r="K90" s="9"/>
-      <c r="L90" s="9"/>
+      <c r="G90" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="H90" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I90" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="6"/>
       <c r="M90" s="9"/>
       <c r="N90" s="9"/>
       <c r="O90" s="2"/>
@@ -6394,17 +6412,17 @@
       <c r="AA90" s="2"/>
       <c r="AB90" s="2"/>
     </row>
-    <row r="91" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
-        <v>219</v>
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C91" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D91" s="9" t="s">
+      <c r="C91" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D91" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E91" s="7" t="s">
@@ -6413,18 +6431,18 @@
       <c r="F91" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G91" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="H91" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="I91" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="J91" s="9"/>
-      <c r="K91" s="9"/>
-      <c r="L91" s="9"/>
+      <c r="G91" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="H91" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I91" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
       <c r="M91" s="9"/>
       <c r="N91" s="9"/>
       <c r="O91" s="2"/>
@@ -6442,9 +6460,9 @@
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
     </row>
-    <row r="92" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>252</v>
@@ -6468,7 +6486,7 @@
         <v>211</v>
       </c>
       <c r="I92" s="20" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="J92" s="9"/>
       <c r="K92" s="9"/>
@@ -6490,17 +6508,17 @@
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
     </row>
-    <row r="93" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>161</v>
+        <v>219</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C93" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D93" s="6" t="s">
+      <c r="C93" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D93" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E93" s="7" t="s">
@@ -6509,14 +6527,14 @@
       <c r="F93" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G93" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="H93" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I93" s="8" t="s">
-        <v>160</v>
+      <c r="G93" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="H93" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="I93" s="20" t="s">
+        <v>220</v>
       </c>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
@@ -6538,17 +6556,17 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>114</v>
+        <v>221</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C94" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D94" s="6" t="s">
+      <c r="C94" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D94" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E94" s="7" t="s">
@@ -6557,14 +6575,14 @@
       <c r="F94" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G94" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="H94" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I94" s="8" t="s">
-        <v>78</v>
+      <c r="G94" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="H94" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="I94" s="20" t="s">
+        <v>222</v>
       </c>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
@@ -6586,9 +6604,9 @@
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
     </row>
-    <row r="95" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>79</v>
+    <row r="95" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>161</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>252</v>
@@ -6597,13 +6615,13 @@
         <v>77</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="G95" s="6" t="s">
         <v>331</v>
@@ -6612,7 +6630,7 @@
         <v>212</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
@@ -6634,15 +6652,15 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
-        <v>72</v>
+    <row r="96" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>11</v>
@@ -6654,13 +6672,13 @@
         <v>94</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>287</v>
+        <v>331</v>
       </c>
       <c r="H96" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
@@ -6682,33 +6700,33 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>286</v>
+        <v>79</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>287</v>
+        <v>331</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I97" s="22" t="s">
-        <v>288</v>
+        <v>212</v>
+      </c>
+      <c r="I97" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -6730,9 +6748,9 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>289</v>
+        <v>72</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>252</v>
@@ -6753,10 +6771,10 @@
         <v>287</v>
       </c>
       <c r="H98" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I98" s="22" t="s">
-        <v>290</v>
+        <v>212</v>
+      </c>
+      <c r="I98" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -6778,9 +6796,9 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>252</v>
@@ -6804,7 +6822,7 @@
         <v>211</v>
       </c>
       <c r="I99" s="22" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -6826,14 +6844,14 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>75</v>
+        <v>289</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C100" s="18" t="s">
+      <c r="C100" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D100" s="6" t="s">
@@ -6849,10 +6867,10 @@
         <v>287</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I100" s="8" t="s">
-        <v>293</v>
+        <v>211</v>
+      </c>
+      <c r="I100" s="22" t="s">
+        <v>290</v>
       </c>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
@@ -6874,9 +6892,9 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>76</v>
+        <v>291</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>252</v>
@@ -6897,10 +6915,10 @@
         <v>287</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I101" s="8" t="s">
-        <v>294</v>
+        <v>211</v>
+      </c>
+      <c r="I101" s="22" t="s">
+        <v>292</v>
       </c>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
@@ -6922,15 +6940,15 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C102" s="6" t="s">
-        <v>115</v>
+      <c r="C102" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>11</v>
@@ -6942,13 +6960,13 @@
         <v>94</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="H102" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I102" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
@@ -6970,15 +6988,15 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>297</v>
+        <v>76</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>11</v>
@@ -6990,13 +7008,13 @@
         <v>94</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="H103" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I103" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
@@ -7018,15 +7036,15 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>302</v>
+    <row r="104" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>299</v>
+        <v>115</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>11</v>
@@ -7038,13 +7056,13 @@
         <v>94</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H104" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I104" s="8" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="J104" s="9"/>
       <c r="K104" s="9"/>
@@ -7066,15 +7084,15 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>304</v>
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>299</v>
+        <v>115</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>11</v>
@@ -7086,13 +7104,13 @@
         <v>94</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H105" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I105" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="J105" s="9"/>
       <c r="K105" s="9"/>
@@ -7114,17 +7132,17 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A106" s="21" t="s">
-        <v>171</v>
+    <row r="106" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>302</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C106" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D106" s="18" t="s">
+      <c r="C106" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D106" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E106" s="7" t="s">
@@ -7133,14 +7151,14 @@
       <c r="F106" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G106" s="18" t="s">
-        <v>314</v>
+      <c r="G106" s="6" t="s">
+        <v>300</v>
       </c>
       <c r="H106" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>172</v>
+        <v>303</v>
       </c>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
@@ -7162,15 +7180,15 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="11" t="s">
-        <v>110</v>
+    <row r="107" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>304</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>115</v>
+        <v>299</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>11</v>
@@ -7182,13 +7200,13 @@
         <v>94</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="H107" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I107" s="8" t="s">
-        <v>116</v>
+        <v>301</v>
       </c>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
@@ -7210,9 +7228,9 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>252</v>
@@ -7220,7 +7238,7 @@
       <c r="C108" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D108" s="6" t="s">
+      <c r="D108" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E108" s="7" t="s">
@@ -7229,14 +7247,14 @@
       <c r="F108" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G108" s="6" t="s">
-        <v>175</v>
+      <c r="G108" s="18" t="s">
+        <v>314</v>
       </c>
       <c r="H108" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I108" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
@@ -7258,9 +7276,9 @@
       <c r="AA108" s="2"/>
       <c r="AB108" s="2"/>
     </row>
-    <row r="109" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>252</v>
@@ -7284,7 +7302,7 @@
         <v>212</v>
       </c>
       <c r="I109" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
@@ -7306,15 +7324,15 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
-        <v>152</v>
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="141.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C110" s="6" t="s">
-        <v>154</v>
+      <c r="C110" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>11</v>
@@ -7326,16 +7344,16 @@
         <v>94</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I110" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="J110" s="6"/>
-      <c r="K110" s="6"/>
+        <v>174</v>
+      </c>
+      <c r="J110" s="9"/>
+      <c r="K110" s="9"/>
       <c r="L110" s="9"/>
       <c r="M110" s="9"/>
       <c r="N110" s="9"/>
@@ -7354,15 +7372,15 @@
       <c r="AA110" s="2"/>
       <c r="AB110" s="2"/>
     </row>
-    <row r="111" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
-        <v>156</v>
+    <row r="111" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>11</v>
@@ -7374,16 +7392,16 @@
         <v>94</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
       <c r="H111" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I111" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="J111" s="6"/>
-      <c r="K111" s="6"/>
+        <v>117</v>
+      </c>
+      <c r="J111" s="9"/>
+      <c r="K111" s="9"/>
       <c r="L111" s="9"/>
       <c r="M111" s="9"/>
       <c r="N111" s="9"/>
@@ -7402,9 +7420,9 @@
       <c r="AA111" s="2"/>
       <c r="AB111" s="2"/>
     </row>
-    <row r="112" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>279</v>
+        <v>152</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>252</v>
@@ -7422,13 +7440,13 @@
         <v>94</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>318</v>
+        <v>153</v>
       </c>
       <c r="H112" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I112" s="8" t="s">
-        <v>280</v>
+        <v>155</v>
       </c>
       <c r="J112" s="6"/>
       <c r="K112" s="6"/>
@@ -7450,9 +7468,9 @@
       <c r="AA112" s="2"/>
       <c r="AB112" s="2"/>
     </row>
-    <row r="113" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>276</v>
+        <v>156</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>252</v>
@@ -7470,13 +7488,13 @@
         <v>94</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H113" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I113" s="8" t="s">
-        <v>277</v>
+        <v>157</v>
       </c>
       <c r="J113" s="6"/>
       <c r="K113" s="6"/>
@@ -7498,9 +7516,9 @@
       <c r="AA113" s="2"/>
       <c r="AB113" s="2"/>
     </row>
-    <row r="114" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>252</v>
@@ -7515,16 +7533,16 @@
         <v>94</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>278</v>
+        <v>94</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H114" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I114" s="8" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="J114" s="6"/>
       <c r="K114" s="6"/>
@@ -7546,9 +7564,9 @@
       <c r="AA114" s="2"/>
       <c r="AB114" s="2"/>
     </row>
-    <row r="115" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>158</v>
+        <v>276</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>252</v>
@@ -7566,13 +7584,13 @@
         <v>94</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H115" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I115" s="8" t="s">
-        <v>159</v>
+        <v>277</v>
       </c>
       <c r="J115" s="6"/>
       <c r="K115" s="6"/>
@@ -7594,15 +7612,15 @@
       <c r="AA115" s="2"/>
       <c r="AB115" s="2"/>
     </row>
-    <row r="116" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
-      <c r="A116" s="11" t="s">
-        <v>186</v>
+    <row r="116" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>274</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>11</v>
@@ -7611,19 +7629,19 @@
         <v>94</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>94</v>
+        <v>278</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>209</v>
+        <v>320</v>
       </c>
       <c r="H116" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I116" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J116" s="9"/>
-      <c r="K116" s="9"/>
+        <v>275</v>
+      </c>
+      <c r="J116" s="6"/>
+      <c r="K116" s="6"/>
       <c r="L116" s="9"/>
       <c r="M116" s="9"/>
       <c r="N116" s="9"/>
@@ -7642,15 +7660,15 @@
       <c r="AA116" s="2"/>
       <c r="AB116" s="2"/>
     </row>
-    <row r="117" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A117" s="11" t="s">
-        <v>188</v>
+    <row r="117" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>11</v>
@@ -7662,20 +7680,16 @@
         <v>94</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>209</v>
+        <v>321</v>
       </c>
       <c r="H117" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I117" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="J117" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K117" s="20" t="s">
-        <v>202</v>
-      </c>
+      <c r="I117" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="J117" s="6"/>
+      <c r="K117" s="6"/>
       <c r="L117" s="9"/>
       <c r="M117" s="9"/>
       <c r="N117" s="9"/>
@@ -7694,9 +7708,9 @@
       <c r="AA117" s="2"/>
       <c r="AB117" s="2"/>
     </row>
-    <row r="118" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>252</v>
@@ -7717,26 +7731,16 @@
         <v>209</v>
       </c>
       <c r="H118" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I118" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="I118" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="J118" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="K118" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="L118" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="M118" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="N118" s="20" t="s">
-        <v>207</v>
-      </c>
+      <c r="J118" s="9"/>
+      <c r="K118" s="9"/>
+      <c r="L118" s="9"/>
+      <c r="M118" s="9"/>
+      <c r="N118" s="9"/>
       <c r="O118" s="2"/>
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
@@ -7752,9 +7756,9 @@
       <c r="AA118" s="2"/>
       <c r="AB118" s="2"/>
     </row>
-    <row r="119" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="23" t="s">
-        <v>233</v>
+    <row r="119" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="11" t="s">
+        <v>188</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>252</v>
@@ -7762,7 +7766,7 @@
       <c r="C119" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D119" s="24" t="s">
+      <c r="D119" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E119" s="7" t="s">
@@ -7774,17 +7778,17 @@
       <c r="G119" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="H119" s="20" t="s">
+      <c r="H119" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I119" s="22" t="s">
-        <v>234</v>
+        <v>200</v>
       </c>
       <c r="J119" s="20" t="s">
         <v>201</v>
       </c>
       <c r="K119" s="20" t="s">
-        <v>236</v>
+        <v>202</v>
       </c>
       <c r="L119" s="9"/>
       <c r="M119" s="9"/>
@@ -7804,15 +7808,15 @@
       <c r="AA119" s="2"/>
       <c r="AB119" s="2"/>
     </row>
-    <row r="120" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
-        <v>235</v>
+        <v>189</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>242</v>
+        <v>187</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>11</v>
@@ -7827,16 +7831,26 @@
         <v>209</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="I120" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="J120" s="20"/>
-      <c r="K120" s="20"/>
-      <c r="L120" s="9"/>
-      <c r="M120" s="9"/>
-      <c r="N120" s="9"/>
+        <v>203</v>
+      </c>
+      <c r="J120" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="K120" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="L120" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="M120" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="N120" s="20" t="s">
+        <v>207</v>
+      </c>
       <c r="O120" s="2"/>
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
@@ -7852,9 +7866,9 @@
       <c r="AA120" s="2"/>
       <c r="AB120" s="2"/>
     </row>
-    <row r="121" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A121" s="11" t="s">
-        <v>243</v>
+    <row r="121" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="23" t="s">
+        <v>233</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>252</v>
@@ -7862,7 +7876,7 @@
       <c r="C121" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D121" s="6" t="s">
+      <c r="D121" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E121" s="7" t="s">
@@ -7874,7 +7888,7 @@
       <c r="G121" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="H121" s="8" t="s">
+      <c r="H121" s="20" t="s">
         <v>211</v>
       </c>
       <c r="I121" s="22" t="s">
@@ -7886,9 +7900,9 @@
       <c r="K121" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="L121" s="20"/>
-      <c r="M121" s="20"/>
-      <c r="N121" s="20"/>
+      <c r="L121" s="9"/>
+      <c r="M121" s="9"/>
+      <c r="N121" s="9"/>
       <c r="O121" s="2"/>
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
@@ -7904,18 +7918,18 @@
       <c r="AA121" s="2"/>
       <c r="AB121" s="2"/>
     </row>
-    <row r="122" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
-        <v>241</v>
+    <row r="122" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>10</v>
+        <v>242</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E122" s="7" t="s">
         <v>94</v>
@@ -7924,14 +7938,16 @@
         <v>94</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="H122" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="I122" s="9"/>
-      <c r="J122" s="9"/>
-      <c r="K122" s="9"/>
+        <v>211</v>
+      </c>
+      <c r="I122" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="J122" s="20"/>
+      <c r="K122" s="20"/>
       <c r="L122" s="9"/>
       <c r="M122" s="9"/>
       <c r="N122" s="9"/>
@@ -7950,8 +7966,112 @@
       <c r="AA122" s="2"/>
       <c r="AB122" s="2"/>
     </row>
+    <row r="123" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G123" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H123" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I123" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="J123" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="K123" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="L123" s="20"/>
+      <c r="M123" s="20"/>
+      <c r="N123" s="20"/>
+      <c r="O123" s="2"/>
+      <c r="P123" s="2"/>
+      <c r="Q123" s="2"/>
+      <c r="R123" s="2"/>
+      <c r="S123" s="2"/>
+      <c r="T123" s="2"/>
+      <c r="U123" s="2"/>
+      <c r="V123" s="2"/>
+      <c r="W123" s="2"/>
+      <c r="X123" s="2"/>
+      <c r="Y123" s="2"/>
+      <c r="Z123" s="2"/>
+      <c r="AA123" s="2"/>
+      <c r="AB123" s="2"/>
+    </row>
+    <row r="124" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E124" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G124" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H124" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="I124" s="9"/>
+      <c r="J124" s="9"/>
+      <c r="K124" s="9"/>
+      <c r="L124" s="9"/>
+      <c r="M124" s="9"/>
+      <c r="N124" s="9"/>
+      <c r="O124" s="2"/>
+      <c r="P124" s="2"/>
+      <c r="Q124" s="2"/>
+      <c r="R124" s="2"/>
+      <c r="S124" s="2"/>
+      <c r="T124" s="2"/>
+      <c r="U124" s="2"/>
+      <c r="V124" s="2"/>
+      <c r="W124" s="2"/>
+      <c r="X124" s="2"/>
+      <c r="Y124" s="2"/>
+      <c r="Z124" s="2"/>
+      <c r="AA124" s="2"/>
+      <c r="AB124" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I122" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I124" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
coyni employee added test method and some components classes
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(09-03-2023)Test Data&amp; Script\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\demo\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF66CC8D-6413-4C35-9818-6222779D8333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226B2D03-A3CF-4FD5-82C8-BEC64AFA8404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$125</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="342">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1903,6 +1903,27 @@
   </si>
   <si>
     <t>verify CommissionAccountTransactionList</t>
+  </si>
+  <si>
+    <t>Verify Create Coyni employee</t>
+  </si>
+  <si>
+    <t>testdata-admin.xlsx,coyniEmployee</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testCreateCoyniEmployee,
+-pprofileHeading,
+-pfirstname,
+-plastname,
+-pphoneNumber,
+-pheading,
+-pverificationCode,
+-pcreatePassword,
+-pconfirmPassword</t>
+  </si>
+  <si>
+    <t>Profile - Coyni Employee</t>
   </si>
 </sst>
 </file>
@@ -2344,32 +2365,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB124"/>
+  <dimension ref="A1:AB125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
-    <col min="9" max="9" width="43.140625" customWidth="1"/>
-    <col min="10" max="10" width="38.85546875" customWidth="1"/>
-    <col min="11" max="11" width="30.28515625" customWidth="1"/>
+    <col min="8" max="8" width="47.44140625" customWidth="1"/>
+    <col min="9" max="9" width="43.109375" customWidth="1"/>
+    <col min="10" max="10" width="38.88671875" customWidth="1"/>
+    <col min="11" max="11" width="30.33203125" customWidth="1"/>
     <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" customWidth="1"/>
-    <col min="14" max="14" width="25.5703125" customWidth="1"/>
+    <col min="13" max="13" width="26.44140625" customWidth="1"/>
+    <col min="14" max="14" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2403,7 +2424,7 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2449,7 +2470,7 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>250</v>
       </c>
@@ -2495,7 +2516,7 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -2541,7 +2562,7 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
@@ -2587,7 +2608,7 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>139</v>
       </c>
@@ -2633,7 +2654,7 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -2679,7 +2700,7 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="210.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="202.8" x14ac:dyDescent="0.4">
       <c r="A8" s="12" t="s">
         <v>26</v>
       </c>
@@ -2725,7 +2746,7 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -2771,7 +2792,7 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -2817,7 +2838,7 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
@@ -2863,7 +2884,7 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="216" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
@@ -2909,7 +2930,7 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
@@ -2955,7 +2976,7 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -3001,7 +3022,7 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>41</v>
       </c>
@@ -3047,7 +3068,7 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>244</v>
       </c>
@@ -3095,7 +3116,7 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
-    <row r="17" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>128</v>
       </c>
@@ -3143,7 +3164,7 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>129</v>
       </c>
@@ -3191,7 +3212,7 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>131</v>
       </c>
@@ -3239,7 +3260,7 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
     </row>
-    <row r="20" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>148</v>
       </c>
@@ -3287,7 +3308,7 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
     </row>
-    <row r="21" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -3335,7 +3356,7 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -3383,7 +3404,7 @@
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
     </row>
-    <row r="23" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -3431,7 +3452,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
     </row>
-    <row r="24" spans="1:28" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>227</v>
       </c>
@@ -3479,7 +3500,7 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
     </row>
-    <row r="25" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>228</v>
       </c>
@@ -3527,7 +3548,7 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
     </row>
-    <row r="26" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>229</v>
       </c>
@@ -3575,7 +3596,7 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>230</v>
       </c>
@@ -3623,7 +3644,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" s="2" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>144</v>
       </c>
@@ -3657,7 +3678,7 @@
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
     </row>
-    <row r="29" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>95</v>
       </c>
@@ -3705,7 +3726,7 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
     </row>
-    <row r="30" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>334</v>
       </c>
@@ -3753,7 +3774,7 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>332</v>
       </c>
@@ -3801,7 +3822,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>97</v>
       </c>
@@ -3849,7 +3870,7 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>99</v>
       </c>
@@ -3897,7 +3918,7 @@
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
     </row>
-    <row r="34" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>101</v>
       </c>
@@ -3945,7 +3966,7 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>103</v>
       </c>
@@ -3993,7 +4014,7 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>105</v>
       </c>
@@ -4041,7 +4062,7 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>337</v>
       </c>
@@ -4089,7 +4110,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>43</v>
       </c>
@@ -4137,7 +4158,7 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>169</v>
       </c>
@@ -4185,7 +4206,7 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>46</v>
       </c>
@@ -4233,7 +4254,7 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>48</v>
       </c>
@@ -4281,7 +4302,7 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>50</v>
       </c>
@@ -4329,7 +4350,7 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>52</v>
       </c>
@@ -4377,7 +4398,7 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>54</v>
       </c>
@@ -4425,7 +4446,7 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>56</v>
       </c>
@@ -4473,7 +4494,7 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>58</v>
       </c>
@@ -4521,7 +4542,7 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>60</v>
       </c>
@@ -4569,7 +4590,7 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>62</v>
       </c>
@@ -4617,7 +4638,7 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>64</v>
       </c>
@@ -4665,7 +4686,7 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>66</v>
       </c>
@@ -4713,7 +4734,7 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>68</v>
       </c>
@@ -4761,7 +4782,7 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>134</v>
       </c>
@@ -4809,7 +4830,7 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>70</v>
       </c>
@@ -4857,7 +4878,7 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>142</v>
       </c>
@@ -4905,7 +4926,7 @@
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
     </row>
-    <row r="55" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>146</v>
       </c>
@@ -4953,7 +4974,7 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" s="2" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>118</v>
       </c>
@@ -4987,7 +5008,7 @@
       <c r="M56" s="9"/>
       <c r="N56" s="9"/>
     </row>
-    <row r="57" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>120</v>
       </c>
@@ -5035,7 +5056,7 @@
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
     </row>
-    <row r="58" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>121</v>
       </c>
@@ -5083,33 +5104,33 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>338</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>124</v>
+        <v>339</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>94</v>
+        <v>14</v>
+      </c>
+      <c r="E59" s="7">
+        <v>1</v>
+      </c>
+      <c r="F59" s="7">
+        <v>1</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I59" s="22" t="s">
-        <v>125</v>
+        <v>340</v>
       </c>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -5131,9 +5152,9 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>252</v>
@@ -5157,7 +5178,7 @@
         <v>212</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -5179,15 +5200,15 @@
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>178</v>
+    <row r="61" spans="1:28" ht="144" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>208</v>
+        <v>124</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>11</v>
@@ -5199,13 +5220,13 @@
         <v>94</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I61" s="22" t="s">
-        <v>191</v>
+        <v>127</v>
       </c>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -5227,9 +5248,9 @@
       <c r="AA61" s="2"/>
       <c r="AB61" s="2"/>
     </row>
-    <row r="62" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>252</v>
@@ -5253,7 +5274,7 @@
         <v>211</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -5275,9 +5296,9 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>252</v>
@@ -5301,7 +5322,7 @@
         <v>211</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -5323,9 +5344,9 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="25" t="s">
-        <v>181</v>
+    <row r="64" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>252</v>
@@ -5349,7 +5370,7 @@
         <v>211</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -5371,9 +5392,9 @@
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
     </row>
-    <row r="65" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>182</v>
+    <row r="65" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A65" s="25" t="s">
+        <v>181</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>252</v>
@@ -5397,7 +5418,7 @@
         <v>211</v>
       </c>
       <c r="I65" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -5419,9 +5440,9 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>183</v>
+    <row r="66" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>252</v>
@@ -5445,7 +5466,7 @@
         <v>211</v>
       </c>
       <c r="I66" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -5467,9 +5488,9 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>252</v>
@@ -5493,7 +5514,7 @@
         <v>211</v>
       </c>
       <c r="I67" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -5515,9 +5536,9 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>252</v>
@@ -5541,7 +5562,7 @@
         <v>211</v>
       </c>
       <c r="I68" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -5563,9 +5584,9 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>252</v>
@@ -5589,7 +5610,7 @@
         <v>211</v>
       </c>
       <c r="I69" s="22" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -5611,18 +5632,18 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="26" t="s">
-        <v>251</v>
+    <row r="70" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E70" s="7" t="s">
         <v>94</v>
@@ -5631,18 +5652,37 @@
         <v>94</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H70" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I70" s="22" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="71" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>254</v>
+        <v>193</v>
+      </c>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
+      <c r="O70" s="2"/>
+      <c r="P70" s="2"/>
+      <c r="Q70" s="2"/>
+      <c r="R70" s="2"/>
+      <c r="S70" s="2"/>
+      <c r="T70" s="2"/>
+      <c r="U70" s="2"/>
+      <c r="V70" s="2"/>
+      <c r="W70" s="2"/>
+      <c r="X70" s="2"/>
+      <c r="Y70" s="2"/>
+      <c r="Z70" s="2"/>
+      <c r="AA70" s="2"/>
+      <c r="AB70" s="2"/>
+    </row>
+    <row r="71" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A71" s="26" t="s">
+        <v>251</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>252</v>
@@ -5657,7 +5697,7 @@
         <v>94</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>255</v>
+        <v>94</v>
       </c>
       <c r="G71" s="6" t="s">
         <v>323</v>
@@ -5666,12 +5706,12 @@
         <v>211</v>
       </c>
       <c r="I71" s="22" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="72" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>252</v>
@@ -5686,7 +5726,7 @@
         <v>94</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>94</v>
+        <v>255</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>323</v>
@@ -5695,12 +5735,12 @@
         <v>211</v>
       </c>
       <c r="I72" s="22" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="73" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>252</v>
@@ -5724,12 +5764,12 @@
         <v>211</v>
       </c>
       <c r="I73" s="22" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="74" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>252</v>
@@ -5753,12 +5793,12 @@
         <v>211</v>
       </c>
       <c r="I74" s="22" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="75" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>252</v>
@@ -5782,12 +5822,12 @@
         <v>211</v>
       </c>
       <c r="I75" s="22" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="76" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>252</v>
@@ -5811,12 +5851,12 @@
         <v>211</v>
       </c>
       <c r="I76" s="22" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="77" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>252</v>
@@ -5840,12 +5880,12 @@
         <v>211</v>
       </c>
       <c r="I77" s="22" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="78" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>252</v>
@@ -5869,12 +5909,12 @@
         <v>211</v>
       </c>
       <c r="I78" s="22" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="79" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>252</v>
@@ -5898,12 +5938,12 @@
         <v>211</v>
       </c>
       <c r="I79" s="22" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="80" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>252</v>
@@ -5927,66 +5967,47 @@
         <v>211</v>
       </c>
       <c r="I80" s="22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>281</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="H81" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I81" s="22" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="81" spans="1:28" s="1" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+    <row r="82" spans="1:28" s="1" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C81" s="6" t="s">
+      <c r="B82" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C82" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G81" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="H81" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I81" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="J81" s="6"/>
-      <c r="K81" s="6"/>
-      <c r="L81" s="9"/>
-      <c r="M81" s="9"/>
-      <c r="N81" s="9"/>
-      <c r="O81" s="2"/>
-      <c r="P81" s="2"/>
-      <c r="Q81" s="2"/>
-      <c r="R81" s="2"/>
-      <c r="S81" s="2"/>
-      <c r="T81" s="2"/>
-      <c r="U81" s="2"/>
-      <c r="V81" s="2"/>
-      <c r="W81" s="2"/>
-      <c r="X81" s="2"/>
-      <c r="Y81" s="2"/>
-      <c r="Z81" s="2"/>
-      <c r="AA81" s="2"/>
-      <c r="AB81" s="2"/>
-    </row>
-    <row r="82" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>11</v>
@@ -6004,10 +6025,10 @@
         <v>212</v>
       </c>
       <c r="I82" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="J82" s="8"/>
-      <c r="K82" s="9"/>
+        <v>138</v>
+      </c>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
       <c r="N82" s="9"/>
@@ -6026,9 +6047,9 @@
       <c r="AA82" s="2"/>
       <c r="AB82" s="2"/>
     </row>
-    <row r="83" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>252</v>
@@ -6052,7 +6073,7 @@
         <v>212</v>
       </c>
       <c r="I83" s="8" t="s">
-        <v>166</v>
+        <v>283</v>
       </c>
       <c r="J83" s="8"/>
       <c r="K83" s="9"/>
@@ -6074,9 +6095,9 @@
       <c r="AA83" s="2"/>
       <c r="AB83" s="2"/>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>252</v>
@@ -6097,14 +6118,12 @@
         <v>162</v>
       </c>
       <c r="H84" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I84" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="J84" s="20" t="s">
-        <v>168</v>
-      </c>
+      <c r="J84" s="8"/>
       <c r="K84" s="9"/>
       <c r="L84" s="9"/>
       <c r="M84" s="9"/>
@@ -6124,15 +6143,15 @@
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>11</v>
@@ -6144,17 +6163,19 @@
         <v>94</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>312</v>
+        <v>162</v>
       </c>
       <c r="H85" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="J85" s="6"/>
-      <c r="K85" s="6"/>
-      <c r="L85" s="6"/>
+        <v>166</v>
+      </c>
+      <c r="J85" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="K85" s="9"/>
+      <c r="L85" s="9"/>
       <c r="M85" s="9"/>
       <c r="N85" s="9"/>
       <c r="O85" s="2"/>
@@ -6172,9 +6193,9 @@
       <c r="AA85" s="2"/>
       <c r="AB85" s="2"/>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>252</v>
@@ -6198,7 +6219,7 @@
         <v>212</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J86" s="6"/>
       <c r="K86" s="6"/>
@@ -6220,9 +6241,9 @@
       <c r="AA86" s="2"/>
       <c r="AB86" s="2"/>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>252</v>
@@ -6246,7 +6267,7 @@
         <v>212</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
@@ -6268,9 +6289,9 @@
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>252</v>
@@ -6294,7 +6315,7 @@
         <v>212</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
@@ -6316,9 +6337,9 @@
       <c r="AA88" s="2"/>
       <c r="AB88" s="2"/>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>252</v>
@@ -6336,13 +6357,13 @@
         <v>94</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H89" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
@@ -6364,9 +6385,9 @@
       <c r="AA89" s="2"/>
       <c r="AB89" s="2"/>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="27" t="s">
-        <v>284</v>
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>252</v>
@@ -6390,7 +6411,7 @@
         <v>212</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>285</v>
+        <v>91</v>
       </c>
       <c r="J90" s="6"/>
       <c r="K90" s="6"/>
@@ -6412,9 +6433,9 @@
       <c r="AA90" s="2"/>
       <c r="AB90" s="2"/>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
-        <v>92</v>
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A91" s="27" t="s">
+        <v>284</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>252</v>
@@ -6438,7 +6459,7 @@
         <v>212</v>
       </c>
       <c r="I91" s="8" t="s">
-        <v>93</v>
+        <v>285</v>
       </c>
       <c r="J91" s="6"/>
       <c r="K91" s="6"/>
@@ -6460,17 +6481,17 @@
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
     </row>
-    <row r="92" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>215</v>
+    <row r="92" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A92" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C92" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D92" s="9" t="s">
+      <c r="C92" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D92" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E92" s="7" t="s">
@@ -6479,18 +6500,18 @@
       <c r="F92" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G92" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="H92" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="I92" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="J92" s="9"/>
-      <c r="K92" s="9"/>
-      <c r="L92" s="9"/>
+      <c r="G92" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="H92" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I92" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="6"/>
       <c r="M92" s="9"/>
       <c r="N92" s="9"/>
       <c r="O92" s="2"/>
@@ -6508,9 +6529,9 @@
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
     </row>
-    <row r="93" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>252</v>
@@ -6534,7 +6555,7 @@
         <v>211</v>
       </c>
       <c r="I93" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
@@ -6556,9 +6577,9 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>252</v>
@@ -6582,7 +6603,7 @@
         <v>211</v>
       </c>
       <c r="I94" s="20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
@@ -6604,17 +6625,17 @@
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
     </row>
-    <row r="95" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>161</v>
+        <v>221</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C95" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D95" s="6" t="s">
+      <c r="C95" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D95" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E95" s="7" t="s">
@@ -6623,14 +6644,14 @@
       <c r="F95" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G95" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="H95" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I95" s="8" t="s">
-        <v>160</v>
+      <c r="G95" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="H95" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="I95" s="20" t="s">
+        <v>222</v>
       </c>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
@@ -6652,9 +6673,9 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>252</v>
@@ -6678,7 +6699,7 @@
         <v>212</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
@@ -6700,9 +6721,9 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
-        <v>79</v>
+    <row r="97" spans="1:28" ht="144" x14ac:dyDescent="0.3">
+      <c r="A97" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>252</v>
@@ -6711,13 +6732,13 @@
         <v>77</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>331</v>
@@ -6726,7 +6747,7 @@
         <v>212</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -6748,33 +6769,33 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>287</v>
+        <v>331</v>
       </c>
       <c r="H98" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -6796,9 +6817,9 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>286</v>
+        <v>72</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>252</v>
@@ -6819,10 +6840,10 @@
         <v>287</v>
       </c>
       <c r="H99" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I99" s="22" t="s">
-        <v>288</v>
+        <v>212</v>
+      </c>
+      <c r="I99" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -6844,9 +6865,9 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>252</v>
@@ -6870,7 +6891,7 @@
         <v>211</v>
       </c>
       <c r="I100" s="22" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
@@ -6892,9 +6913,9 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>252</v>
@@ -6918,7 +6939,7 @@
         <v>211</v>
       </c>
       <c r="I101" s="22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
@@ -6940,14 +6961,14 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>75</v>
+        <v>291</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C102" s="18" t="s">
+      <c r="C102" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D102" s="6" t="s">
@@ -6963,10 +6984,10 @@
         <v>287</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I102" s="8" t="s">
-        <v>293</v>
+        <v>211</v>
+      </c>
+      <c r="I102" s="22" t="s">
+        <v>292</v>
       </c>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
@@ -6988,14 +7009,14 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C103" s="6" t="s">
+      <c r="C103" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D103" s="6" t="s">
@@ -7014,7 +7035,7 @@
         <v>212</v>
       </c>
       <c r="I103" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
@@ -7036,15 +7057,15 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>11</v>
@@ -7056,13 +7077,13 @@
         <v>94</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="H104" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I104" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J104" s="9"/>
       <c r="K104" s="9"/>
@@ -7084,9 +7105,9 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>297</v>
+        <v>108</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>252</v>
@@ -7110,7 +7131,7 @@
         <v>212</v>
       </c>
       <c r="I105" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J105" s="9"/>
       <c r="K105" s="9"/>
@@ -7132,15 +7153,15 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>302</v>
+    <row r="106" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>299</v>
+        <v>115</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>11</v>
@@ -7152,13 +7173,13 @@
         <v>94</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H106" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
@@ -7180,9 +7201,9 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>252</v>
@@ -7206,7 +7227,7 @@
         <v>212</v>
       </c>
       <c r="I107" s="8" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
@@ -7228,17 +7249,17 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="21" t="s">
-        <v>171</v>
+    <row r="108" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>304</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C108" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D108" s="18" t="s">
+      <c r="C108" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D108" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E108" s="7" t="s">
@@ -7247,14 +7268,14 @@
       <c r="F108" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G108" s="18" t="s">
-        <v>314</v>
+      <c r="G108" s="6" t="s">
+        <v>300</v>
       </c>
       <c r="H108" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I108" s="8" t="s">
-        <v>172</v>
+        <v>301</v>
       </c>
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
@@ -7276,17 +7297,17 @@
       <c r="AA108" s="2"/>
       <c r="AB108" s="2"/>
     </row>
-    <row r="109" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="11" t="s">
-        <v>110</v>
+    <row r="109" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+      <c r="A109" s="21" t="s">
+        <v>171</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C109" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D109" s="6" t="s">
+      <c r="C109" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D109" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E109" s="7" t="s">
@@ -7295,14 +7316,14 @@
       <c r="F109" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G109" s="6" t="s">
-        <v>295</v>
+      <c r="G109" s="18" t="s">
+        <v>314</v>
       </c>
       <c r="H109" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I109" s="8" t="s">
-        <v>116</v>
+        <v>172</v>
       </c>
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
@@ -7324,15 +7345,15 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" s="1" customFormat="1" ht="141.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="21" t="s">
-        <v>173</v>
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C110" s="18" t="s">
-        <v>73</v>
+      <c r="C110" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>11</v>
@@ -7344,13 +7365,13 @@
         <v>94</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>175</v>
+        <v>295</v>
       </c>
       <c r="H110" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I110" s="8" t="s">
-        <v>174</v>
+        <v>116</v>
       </c>
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
@@ -7372,15 +7393,15 @@
       <c r="AA110" s="2"/>
       <c r="AB110" s="2"/>
     </row>
-    <row r="111" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="11" t="s">
-        <v>109</v>
+    <row r="111" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C111" s="6" t="s">
-        <v>115</v>
+      <c r="C111" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>11</v>
@@ -7392,13 +7413,13 @@
         <v>94</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>295</v>
+        <v>175</v>
       </c>
       <c r="H111" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I111" s="8" t="s">
-        <v>117</v>
+        <v>174</v>
       </c>
       <c r="J111" s="9"/>
       <c r="K111" s="9"/>
@@ -7420,15 +7441,15 @@
       <c r="AA111" s="2"/>
       <c r="AB111" s="2"/>
     </row>
-    <row r="112" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
-        <v>152</v>
+    <row r="112" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>11</v>
@@ -7440,16 +7461,16 @@
         <v>94</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>153</v>
+        <v>295</v>
       </c>
       <c r="H112" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I112" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="J112" s="6"/>
-      <c r="K112" s="6"/>
+        <v>117</v>
+      </c>
+      <c r="J112" s="9"/>
+      <c r="K112" s="9"/>
       <c r="L112" s="9"/>
       <c r="M112" s="9"/>
       <c r="N112" s="9"/>
@@ -7468,9 +7489,9 @@
       <c r="AA112" s="2"/>
       <c r="AB112" s="2"/>
     </row>
-    <row r="113" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>252</v>
@@ -7488,13 +7509,13 @@
         <v>94</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>317</v>
+        <v>153</v>
       </c>
       <c r="H113" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I113" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J113" s="6"/>
       <c r="K113" s="6"/>
@@ -7516,9 +7537,9 @@
       <c r="AA113" s="2"/>
       <c r="AB113" s="2"/>
     </row>
-    <row r="114" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>279</v>
+        <v>156</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>252</v>
@@ -7536,13 +7557,13 @@
         <v>94</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H114" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I114" s="8" t="s">
-        <v>280</v>
+        <v>157</v>
       </c>
       <c r="J114" s="6"/>
       <c r="K114" s="6"/>
@@ -7564,9 +7585,9 @@
       <c r="AA114" s="2"/>
       <c r="AB114" s="2"/>
     </row>
-    <row r="115" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>252</v>
@@ -7584,13 +7605,13 @@
         <v>94</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H115" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I115" s="8" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="J115" s="6"/>
       <c r="K115" s="6"/>
@@ -7612,9 +7633,9 @@
       <c r="AA115" s="2"/>
       <c r="AB115" s="2"/>
     </row>
-    <row r="116" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>252</v>
@@ -7629,16 +7650,16 @@
         <v>94</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>278</v>
+        <v>94</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H116" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I116" s="8" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="J116" s="6"/>
       <c r="K116" s="6"/>
@@ -7660,9 +7681,9 @@
       <c r="AA116" s="2"/>
       <c r="AB116" s="2"/>
     </row>
-    <row r="117" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>158</v>
+        <v>274</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>252</v>
@@ -7677,16 +7698,16 @@
         <v>94</v>
       </c>
       <c r="F117" s="7" t="s">
-        <v>94</v>
+        <v>278</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H117" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I117" s="8" t="s">
-        <v>159</v>
+        <v>275</v>
       </c>
       <c r="J117" s="6"/>
       <c r="K117" s="6"/>
@@ -7708,15 +7729,15 @@
       <c r="AA117" s="2"/>
       <c r="AB117" s="2"/>
     </row>
-    <row r="118" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="11" t="s">
-        <v>186</v>
+    <row r="118" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A118" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>11</v>
@@ -7728,16 +7749,16 @@
         <v>94</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>209</v>
+        <v>321</v>
       </c>
       <c r="H118" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I118" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J118" s="9"/>
-      <c r="K118" s="9"/>
+        <v>159</v>
+      </c>
+      <c r="J118" s="6"/>
+      <c r="K118" s="6"/>
       <c r="L118" s="9"/>
       <c r="M118" s="9"/>
       <c r="N118" s="9"/>
@@ -7756,9 +7777,9 @@
       <c r="AA118" s="2"/>
       <c r="AB118" s="2"/>
     </row>
-    <row r="119" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28" s="1" customFormat="1" ht="288" x14ac:dyDescent="0.3">
       <c r="A119" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>252</v>
@@ -7781,15 +7802,11 @@
       <c r="H119" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I119" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="J119" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K119" s="20" t="s">
-        <v>202</v>
-      </c>
+      <c r="I119" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="J119" s="9"/>
+      <c r="K119" s="9"/>
       <c r="L119" s="9"/>
       <c r="M119" s="9"/>
       <c r="N119" s="9"/>
@@ -7808,9 +7825,9 @@
       <c r="AA119" s="2"/>
       <c r="AB119" s="2"/>
     </row>
-    <row r="120" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A120" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>252</v>
@@ -7831,26 +7848,20 @@
         <v>209</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="I120" s="22" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J120" s="20" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K120" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="L120" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="M120" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="N120" s="20" t="s">
-        <v>207</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="L120" s="9"/>
+      <c r="M120" s="9"/>
+      <c r="N120" s="9"/>
       <c r="O120" s="2"/>
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
@@ -7866,9 +7877,9 @@
       <c r="AA120" s="2"/>
       <c r="AB120" s="2"/>
     </row>
-    <row r="121" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="23" t="s">
-        <v>233</v>
+    <row r="121" spans="1:28" s="1" customFormat="1" ht="288" x14ac:dyDescent="0.3">
+      <c r="A121" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>252</v>
@@ -7876,7 +7887,7 @@
       <c r="C121" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D121" s="24" t="s">
+      <c r="D121" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E121" s="7" t="s">
@@ -7888,21 +7899,27 @@
       <c r="G121" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="H121" s="20" t="s">
-        <v>211</v>
+      <c r="H121" s="8" t="s">
+        <v>199</v>
       </c>
       <c r="I121" s="22" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="J121" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="K121" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="K121" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="L121" s="9"/>
-      <c r="M121" s="9"/>
-      <c r="N121" s="9"/>
+      <c r="L121" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="M121" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="N121" s="20" t="s">
+        <v>207</v>
+      </c>
       <c r="O121" s="2"/>
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
@@ -7918,17 +7935,17 @@
       <c r="AA121" s="2"/>
       <c r="AB121" s="2"/>
     </row>
-    <row r="122" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="11" t="s">
-        <v>235</v>
+    <row r="122" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="23" t="s">
+        <v>233</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="D122" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D122" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E122" s="7" t="s">
@@ -7940,14 +7957,18 @@
       <c r="G122" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="H122" s="8" t="s">
+      <c r="H122" s="20" t="s">
         <v>211</v>
       </c>
       <c r="I122" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="J122" s="20"/>
-      <c r="K122" s="20"/>
+        <v>234</v>
+      </c>
+      <c r="J122" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="K122" s="20" t="s">
+        <v>236</v>
+      </c>
       <c r="L122" s="9"/>
       <c r="M122" s="9"/>
       <c r="N122" s="9"/>
@@ -7966,15 +7987,15 @@
       <c r="AA122" s="2"/>
       <c r="AB122" s="2"/>
     </row>
-    <row r="123" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="11" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>187</v>
+        <v>242</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>11</v>
@@ -7992,17 +8013,13 @@
         <v>211</v>
       </c>
       <c r="I123" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="J123" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K123" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="L123" s="20"/>
-      <c r="M123" s="20"/>
-      <c r="N123" s="20"/>
+        <v>232</v>
+      </c>
+      <c r="J123" s="20"/>
+      <c r="K123" s="20"/>
+      <c r="L123" s="9"/>
+      <c r="M123" s="9"/>
+      <c r="N123" s="9"/>
       <c r="O123" s="2"/>
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
@@ -8018,18 +8035,18 @@
       <c r="AA123" s="2"/>
       <c r="AB123" s="2"/>
     </row>
-    <row r="124" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
-        <v>241</v>
+    <row r="124" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A124" s="11" t="s">
+        <v>243</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>10</v>
+        <v>187</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>94</v>
@@ -8038,17 +8055,23 @@
         <v>94</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="H124" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="I124" s="9"/>
-      <c r="J124" s="9"/>
-      <c r="K124" s="9"/>
-      <c r="L124" s="9"/>
-      <c r="M124" s="9"/>
-      <c r="N124" s="9"/>
+        <v>211</v>
+      </c>
+      <c r="I124" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="J124" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="K124" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="L124" s="20"/>
+      <c r="M124" s="20"/>
+      <c r="N124" s="20"/>
       <c r="O124" s="2"/>
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
@@ -8064,14 +8087,54 @@
       <c r="AA124" s="2"/>
       <c r="AB124" s="2"/>
     </row>
+    <row r="125" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G125" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H125" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="I125" s="9"/>
+      <c r="J125" s="9"/>
+      <c r="K125" s="9"/>
+      <c r="L125" s="9"/>
+      <c r="M125" s="9"/>
+      <c r="N125" s="9"/>
+      <c r="O125" s="2"/>
+      <c r="P125" s="2"/>
+      <c r="Q125" s="2"/>
+      <c r="R125" s="2"/>
+      <c r="S125" s="2"/>
+      <c r="T125" s="2"/>
+      <c r="U125" s="2"/>
+      <c r="V125" s="2"/>
+      <c r="W125" s="2"/>
+      <c r="X125" s="2"/>
+      <c r="Y125" s="2"/>
+      <c r="Z125" s="2"/>
+      <c r="AA125" s="2"/>
+      <c r="AB125" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I124" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I125" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a new test cases in Login test
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\demo\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Merchant invitation\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226B2D03-A3CF-4FD5-82C8-BEC64AFA8404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE2EA67-061C-4D72-8252-44FAAD58D597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$126</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="344">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1924,6 +1924,24 @@
   </si>
   <si>
     <t>Profile - Coyni Employee</t>
+  </si>
+  <si>
+    <t>Admin login Page With Sms Otp and Navigation</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.LoginTest,
+testAdminLoginWithSmsOtpAndNavigation,
+-ploginHeading,
+-ploginDescription,
+-pemail,
+-ppassword,
+-pattribute,
+-pauthyHeading,
+-pauthyDescription,
+-pcode,
+-pmessage,
+-pheading,
+-psecurityKey</t>
   </si>
 </sst>
 </file>
@@ -2365,32 +2383,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB125"/>
+  <dimension ref="A1:AB126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.44140625" customWidth="1"/>
-    <col min="9" max="9" width="43.109375" customWidth="1"/>
-    <col min="10" max="10" width="38.88671875" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" customWidth="1"/>
+    <col min="8" max="8" width="47.42578125" customWidth="1"/>
+    <col min="9" max="9" width="43.140625" customWidth="1"/>
+    <col min="10" max="10" width="38.85546875" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" customWidth="1"/>
     <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="13" width="26.44140625" customWidth="1"/>
-    <col min="14" max="14" width="25.5546875" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" customWidth="1"/>
+    <col min="14" max="14" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2424,7 +2442,7 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2470,30 +2488,30 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>250</v>
+        <v>342</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>237</v>
+        <v>94</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>238</v>
+        <v>343</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -2516,9 +2534,9 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>250</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>252</v>
@@ -2533,13 +2551,13 @@
         <v>94</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>113</v>
+        <v>237</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>15</v>
+        <v>238</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -2562,9 +2580,9 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>16</v>
+    <row r="5" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>252</v>
@@ -2579,13 +2597,13 @@
         <v>94</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>240</v>
+        <v>15</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
@@ -2608,9 +2626,9 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>139</v>
+    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>252</v>
@@ -2625,13 +2643,13 @@
         <v>94</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>140</v>
+        <v>240</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -2654,15 +2672,15 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>14</v>
@@ -2671,13 +2689,13 @@
         <v>94</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>246</v>
+        <v>140</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -2700,9 +2718,9 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="202.8" x14ac:dyDescent="0.4">
-      <c r="A8" s="12" t="s">
-        <v>26</v>
+    <row r="8" spans="1:28" ht="240" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>252</v>
@@ -2723,7 +2741,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>107</v>
+        <v>246</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -2746,9 +2764,9 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
+    <row r="9" spans="1:28" ht="210.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>252</v>
@@ -2763,13 +2781,13 @@
         <v>94</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
@@ -2792,9 +2810,9 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>252</v>
@@ -2809,13 +2827,13 @@
         <v>94</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -2838,18 +2856,18 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>94</v>
@@ -2858,10 +2876,10 @@
         <v>94</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -2884,9 +2902,9 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="216" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" ht="255" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>252</v>
@@ -2907,7 +2925,7 @@
         <v>33</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -2930,9 +2948,9 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" ht="225" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>252</v>
@@ -2941,19 +2959,19 @@
         <v>32</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -2976,9 +2994,9 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="144" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="210" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>252</v>
@@ -2987,19 +3005,19 @@
         <v>32</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E14" s="6">
         <v>1</v>
       </c>
       <c r="F14" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -3022,9 +3040,9 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>252</v>
@@ -3045,7 +3063,7 @@
         <v>33</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -3068,34 +3086,32 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" ht="195" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>244</v>
+        <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>324</v>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>245</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
@@ -3116,38 +3132,38 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
-    <row r="17" spans="1:28" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>128</v>
+    <row r="17" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>244</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>112</v>
+      <c r="C17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
+        <v>245</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
       <c r="N17" s="9"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -3164,9 +3180,9 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>129</v>
+    <row r="18" spans="1:28" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>128</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>252</v>
@@ -3178,10 +3194,10 @@
         <v>14</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>325</v>
@@ -3190,7 +3206,7 @@
         <v>210</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>214</v>
+        <v>239</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -3212,15 +3228,15 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>14</v>
@@ -3229,16 +3245,16 @@
         <v>94</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>133</v>
+        <v>325</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>150</v>
+        <v>214</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -3260,9 +3276,9 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
     </row>
-    <row r="20" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>252</v>
@@ -3280,13 +3296,13 @@
         <v>94</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -3308,38 +3324,38 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
     </row>
-    <row r="21" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>17</v>
+    <row r="21" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>326</v>
+      <c r="C21" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>151</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
+        <v>149</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
       <c r="N21" s="9"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -3356,9 +3372,9 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>252</v>
@@ -3376,13 +3392,13 @@
         <v>94</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>20</v>
+        <v>247</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -3404,9 +3420,9 @@
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
     </row>
-    <row r="23" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>252</v>
@@ -3423,14 +3439,14 @@
       <c r="F23" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>305</v>
+      <c r="G23" s="6" t="s">
+        <v>306</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -3452,33 +3468,33 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
     </row>
-    <row r="24" spans="1:28" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
-        <v>227</v>
+    <row r="24" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>231</v>
+        <v>18</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="6">
-        <v>1</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>327</v>
+      <c r="E24" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>305</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>223</v>
+        <v>22</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -3500,9 +3516,9 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
     </row>
-    <row r="25" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>228</v>
+    <row r="25" spans="1:28" ht="270" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>227</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>252</v>
@@ -3511,13 +3527,13 @@
         <v>231</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E25" s="6">
         <v>1</v>
       </c>
       <c r="F25" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>327</v>
@@ -3526,7 +3542,7 @@
         <v>211</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -3548,9 +3564,9 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
     </row>
-    <row r="26" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>252</v>
@@ -3559,13 +3575,13 @@
         <v>231</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E26" s="6">
         <v>1</v>
       </c>
       <c r="F26" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>327</v>
@@ -3574,7 +3590,7 @@
         <v>211</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -3596,24 +3612,24 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>113</v>
+        <v>11</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>327</v>
@@ -3622,7 +3638,7 @@
         <v>211</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -3644,43 +3660,57 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" s="2" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
-        <v>144</v>
+    <row r="28" spans="1:28" ht="285" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>18</v>
+        <v>249</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I28" s="19" t="s">
-        <v>145</v>
+      <c r="I28" s="8" t="s">
+        <v>226</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
-    </row>
-    <row r="29" spans="1:28" ht="144" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>95</v>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+    </row>
+    <row r="29" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>252</v>
@@ -3689,7 +3719,7 @@
         <v>18</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>94</v>
@@ -3701,34 +3731,20 @@
         <v>328</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I29" s="20" t="s">
-        <v>96</v>
+        <v>211</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
-      <c r="Z29" s="2"/>
-      <c r="AA29" s="2"/>
-      <c r="AB29" s="2"/>
-    </row>
-    <row r="30" spans="1:28" ht="144" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>334</v>
+        <v>95</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>252</v>
@@ -3752,7 +3768,7 @@
         <v>212</v>
       </c>
       <c r="I30" s="20" t="s">
-        <v>335</v>
+        <v>96</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -3774,9 +3790,9 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="144" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>252</v>
@@ -3800,7 +3816,7 @@
         <v>212</v>
       </c>
       <c r="I31" s="20" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -3822,9 +3838,9 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>97</v>
+        <v>332</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>252</v>
@@ -3833,7 +3849,7 @@
         <v>18</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>94</v>
@@ -3845,10 +3861,10 @@
         <v>328</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>98</v>
+        <v>212</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>333</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3870,9 +3886,9 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>252</v>
@@ -3896,7 +3912,7 @@
         <v>211</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -3918,9 +3934,9 @@
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
     </row>
-    <row r="34" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>252</v>
@@ -3944,7 +3960,7 @@
         <v>211</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -3966,9 +3982,9 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>252</v>
@@ -3992,7 +4008,7 @@
         <v>211</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -4014,9 +4030,9 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>252</v>
@@ -4040,7 +4056,7 @@
         <v>211</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -4062,12 +4078,12 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>337</v>
+        <v>105</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>18</v>
@@ -4088,7 +4104,7 @@
         <v>211</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>336</v>
+        <v>106</v>
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -4110,15 +4126,15 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>43</v>
+        <v>337</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>11</v>
@@ -4130,15 +4146,15 @@
         <v>94</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H38" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J38" s="6"/>
+        <v>336</v>
+      </c>
+      <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
@@ -4158,9 +4174,9 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>169</v>
+        <v>43</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>252</v>
@@ -4178,13 +4194,13 @@
         <v>94</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>170</v>
+        <v>45</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="9"/>
@@ -4206,9 +4222,9 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>46</v>
+        <v>169</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>252</v>
@@ -4226,13 +4242,13 @@
         <v>94</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="H40" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>47</v>
+        <v>170</v>
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="9"/>
@@ -4254,9 +4270,9 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>252</v>
@@ -4280,7 +4296,7 @@
         <v>211</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="9"/>
@@ -4302,9 +4318,9 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>252</v>
@@ -4328,7 +4344,7 @@
         <v>211</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J42" s="6"/>
       <c r="K42" s="9"/>
@@ -4350,9 +4366,9 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>252</v>
@@ -4376,7 +4392,7 @@
         <v>211</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J43" s="6"/>
       <c r="K43" s="9"/>
@@ -4398,9 +4414,9 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>252</v>
@@ -4424,7 +4440,7 @@
         <v>211</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J44" s="6"/>
       <c r="K44" s="9"/>
@@ -4446,15 +4462,15 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>11</v>
@@ -4466,16 +4482,16 @@
         <v>94</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>141</v>
+        <v>55</v>
       </c>
       <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
+      <c r="K45" s="9"/>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
@@ -4494,9 +4510,9 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>252</v>
@@ -4520,7 +4536,7 @@
         <v>211</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
@@ -4542,9 +4558,9 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>252</v>
@@ -4568,7 +4584,7 @@
         <v>211</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
@@ -4590,9 +4606,9 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>252</v>
@@ -4616,7 +4632,7 @@
         <v>211</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -4638,9 +4654,9 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>252</v>
@@ -4664,7 +4680,7 @@
         <v>211</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -4686,9 +4702,9 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>252</v>
@@ -4706,13 +4722,13 @@
         <v>94</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -4734,9 +4750,9 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>252</v>
@@ -4760,7 +4776,7 @@
         <v>211</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -4782,9 +4798,9 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>134</v>
+        <v>68</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>252</v>
@@ -4802,13 +4818,13 @@
         <v>94</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>135</v>
+        <v>69</v>
       </c>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -4830,9 +4846,9 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>70</v>
+        <v>134</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>252</v>
@@ -4850,13 +4866,13 @@
         <v>94</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>71</v>
+        <v>135</v>
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -4878,15 +4894,15 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>142</v>
+        <v>70</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>11</v>
@@ -4898,13 +4914,13 @@
         <v>94</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I54" s="19" t="s">
-        <v>143</v>
+      <c r="I54" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -4926,9 +4942,9 @@
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
     </row>
-    <row r="55" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>252</v>
@@ -4946,13 +4962,13 @@
         <v>94</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H55" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -4974,15 +4990,15 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" spans="1:28" s="2" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="6" t="s">
-        <v>118</v>
+    <row r="56" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>11</v>
@@ -4994,23 +5010,37 @@
         <v>94</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I56" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
+        <v>211</v>
+      </c>
+      <c r="I56" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
       <c r="N56" s="9"/>
-    </row>
-    <row r="57" spans="1:28" ht="144" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>120</v>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+      <c r="V56" s="2"/>
+      <c r="W56" s="2"/>
+      <c r="X56" s="2"/>
+      <c r="Y56" s="2"/>
+      <c r="Z56" s="2"/>
+      <c r="AA56" s="2"/>
+      <c r="AB56" s="2"/>
+    </row>
+    <row r="57" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>252</v>
@@ -5033,32 +5063,18 @@
       <c r="H57" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="I57" s="22" t="s">
-        <v>176</v>
+      <c r="I57" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
-      <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
-      <c r="Q57" s="2"/>
-      <c r="R57" s="2"/>
-      <c r="S57" s="2"/>
-      <c r="T57" s="2"/>
-      <c r="U57" s="2"/>
-      <c r="V57" s="2"/>
-      <c r="W57" s="2"/>
-      <c r="X57" s="2"/>
-      <c r="Y57" s="2"/>
-      <c r="Z57" s="2"/>
-      <c r="AA57" s="2"/>
-      <c r="AB57" s="2"/>
-    </row>
-    <row r="58" spans="1:28" ht="144" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>252</v>
@@ -5082,7 +5098,7 @@
         <v>212</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>122</v>
+        <v>176</v>
       </c>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -5104,33 +5120,33 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>338</v>
+        <v>121</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>339</v>
+        <v>124</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E59" s="7">
-        <v>1</v>
-      </c>
-      <c r="F59" s="7">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>341</v>
+        <v>315</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I59" s="22" t="s">
-        <v>340</v>
+        <v>122</v>
       </c>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -5152,33 +5168,33 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" ht="144" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>123</v>
+        <v>338</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>124</v>
+        <v>339</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>94</v>
+        <v>14</v>
+      </c>
+      <c r="E60" s="7">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7">
+        <v>1</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>125</v>
+        <v>340</v>
       </c>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -5200,9 +5216,9 @@
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" spans="1:28" ht="144" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>252</v>
@@ -5226,7 +5242,7 @@
         <v>212</v>
       </c>
       <c r="I61" s="22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -5248,15 +5264,15 @@
       <c r="AA61" s="2"/>
       <c r="AB61" s="2"/>
     </row>
-    <row r="62" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A62" s="6" t="s">
-        <v>178</v>
+    <row r="62" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>208</v>
+        <v>124</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>11</v>
@@ -5268,13 +5284,13 @@
         <v>94</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>191</v>
+        <v>127</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -5296,9 +5312,9 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>252</v>
@@ -5322,7 +5338,7 @@
         <v>211</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -5344,9 +5360,9 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>252</v>
@@ -5370,7 +5386,7 @@
         <v>211</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -5392,9 +5408,9 @@
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
     </row>
-    <row r="65" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="25" t="s">
-        <v>181</v>
+    <row r="65" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>252</v>
@@ -5418,7 +5434,7 @@
         <v>211</v>
       </c>
       <c r="I65" s="22" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -5440,9 +5456,9 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
-        <v>182</v>
+    <row r="66" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A66" s="25" t="s">
+        <v>181</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>252</v>
@@ -5466,7 +5482,7 @@
         <v>211</v>
       </c>
       <c r="I66" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -5488,9 +5504,9 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>183</v>
+    <row r="67" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>252</v>
@@ -5514,7 +5530,7 @@
         <v>211</v>
       </c>
       <c r="I67" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -5536,9 +5552,9 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>252</v>
@@ -5562,7 +5578,7 @@
         <v>211</v>
       </c>
       <c r="I68" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -5584,9 +5600,9 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>252</v>
@@ -5610,7 +5626,7 @@
         <v>211</v>
       </c>
       <c r="I69" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -5632,9 +5648,9 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>252</v>
@@ -5658,7 +5674,7 @@
         <v>211</v>
       </c>
       <c r="I70" s="22" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -5680,18 +5696,18 @@
       <c r="AA70" s="2"/>
       <c r="AB70" s="2"/>
     </row>
-    <row r="71" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A71" s="26" t="s">
-        <v>251</v>
+    <row r="71" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E71" s="7" t="s">
         <v>94</v>
@@ -5700,24 +5716,43 @@
         <v>94</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H71" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I71" s="22" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="72" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>254</v>
+        <v>193</v>
+      </c>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
+      <c r="O71" s="2"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+      <c r="R71" s="2"/>
+      <c r="S71" s="2"/>
+      <c r="T71" s="2"/>
+      <c r="U71" s="2"/>
+      <c r="V71" s="2"/>
+      <c r="W71" s="2"/>
+      <c r="X71" s="2"/>
+      <c r="Y71" s="2"/>
+      <c r="Z71" s="2"/>
+      <c r="AA71" s="2"/>
+      <c r="AB71" s="2"/>
+    </row>
+    <row r="72" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A72" s="26" t="s">
+        <v>251</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>14</v>
@@ -5726,7 +5761,7 @@
         <v>94</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>255</v>
+        <v>94</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>323</v>
@@ -5735,12 +5770,12 @@
         <v>211</v>
       </c>
       <c r="I72" s="22" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="73" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>252</v>
@@ -5755,7 +5790,7 @@
         <v>94</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>94</v>
+        <v>255</v>
       </c>
       <c r="G73" s="6" t="s">
         <v>323</v>
@@ -5764,12 +5799,12 @@
         <v>211</v>
       </c>
       <c r="I73" s="22" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="74" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>252</v>
@@ -5793,12 +5828,12 @@
         <v>211</v>
       </c>
       <c r="I74" s="22" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="75" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>252</v>
@@ -5822,12 +5857,12 @@
         <v>211</v>
       </c>
       <c r="I75" s="22" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="76" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>252</v>
@@ -5851,12 +5886,12 @@
         <v>211</v>
       </c>
       <c r="I76" s="22" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="77" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>252</v>
@@ -5880,12 +5915,12 @@
         <v>211</v>
       </c>
       <c r="I77" s="22" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="78" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>252</v>
@@ -5909,12 +5944,12 @@
         <v>211</v>
       </c>
       <c r="I78" s="22" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="79" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>252</v>
@@ -5938,12 +5973,12 @@
         <v>211</v>
       </c>
       <c r="I79" s="22" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="80" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>252</v>
@@ -5967,12 +6002,12 @@
         <v>211</v>
       </c>
       <c r="I80" s="22" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="81" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>252</v>
@@ -5996,66 +6031,47 @@
         <v>211</v>
       </c>
       <c r="I81" s="22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>281</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="H82" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I82" s="22" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="82" spans="1:28" s="1" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
+    <row r="83" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B82" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C82" s="6" t="s">
+      <c r="B83" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C83" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="H82" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I82" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="J82" s="6"/>
-      <c r="K82" s="6"/>
-      <c r="L82" s="9"/>
-      <c r="M82" s="9"/>
-      <c r="N82" s="9"/>
-      <c r="O82" s="2"/>
-      <c r="P82" s="2"/>
-      <c r="Q82" s="2"/>
-      <c r="R82" s="2"/>
-      <c r="S82" s="2"/>
-      <c r="T82" s="2"/>
-      <c r="U82" s="2"/>
-      <c r="V82" s="2"/>
-      <c r="W82" s="2"/>
-      <c r="X82" s="2"/>
-      <c r="Y82" s="2"/>
-      <c r="Z82" s="2"/>
-      <c r="AA82" s="2"/>
-      <c r="AB82" s="2"/>
-    </row>
-    <row r="83" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>11</v>
@@ -6073,10 +6089,10 @@
         <v>212</v>
       </c>
       <c r="I83" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="J83" s="8"/>
-      <c r="K83" s="9"/>
+        <v>138</v>
+      </c>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
       <c r="L83" s="9"/>
       <c r="M83" s="9"/>
       <c r="N83" s="9"/>
@@ -6095,9 +6111,9 @@
       <c r="AA83" s="2"/>
       <c r="AB83" s="2"/>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>252</v>
@@ -6121,7 +6137,7 @@
         <v>212</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>166</v>
+        <v>283</v>
       </c>
       <c r="J84" s="8"/>
       <c r="K84" s="9"/>
@@ -6143,9 +6159,9 @@
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>252</v>
@@ -6166,14 +6182,12 @@
         <v>162</v>
       </c>
       <c r="H85" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I85" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="J85" s="20" t="s">
-        <v>168</v>
-      </c>
+      <c r="J85" s="8"/>
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
       <c r="M85" s="9"/>
@@ -6193,15 +6207,15 @@
       <c r="AA85" s="2"/>
       <c r="AB85" s="2"/>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>11</v>
@@ -6213,17 +6227,19 @@
         <v>94</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>312</v>
+        <v>162</v>
       </c>
       <c r="H86" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="J86" s="6"/>
-      <c r="K86" s="6"/>
-      <c r="L86" s="6"/>
+        <v>166</v>
+      </c>
+      <c r="J86" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="K86" s="9"/>
+      <c r="L86" s="9"/>
       <c r="M86" s="9"/>
       <c r="N86" s="9"/>
       <c r="O86" s="2"/>
@@ -6241,9 +6257,9 @@
       <c r="AA86" s="2"/>
       <c r="AB86" s="2"/>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>252</v>
@@ -6267,7 +6283,7 @@
         <v>212</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
@@ -6289,9 +6305,9 @@
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>252</v>
@@ -6315,7 +6331,7 @@
         <v>212</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
@@ -6337,9 +6353,9 @@
       <c r="AA88" s="2"/>
       <c r="AB88" s="2"/>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>252</v>
@@ -6363,7 +6379,7 @@
         <v>212</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
@@ -6385,9 +6401,9 @@
       <c r="AA89" s="2"/>
       <c r="AB89" s="2"/>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>252</v>
@@ -6405,13 +6421,13 @@
         <v>94</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H90" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J90" s="6"/>
       <c r="K90" s="6"/>
@@ -6433,9 +6449,9 @@
       <c r="AA90" s="2"/>
       <c r="AB90" s="2"/>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A91" s="27" t="s">
-        <v>284</v>
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>252</v>
@@ -6459,7 +6475,7 @@
         <v>212</v>
       </c>
       <c r="I91" s="8" t="s">
-        <v>285</v>
+        <v>91</v>
       </c>
       <c r="J91" s="6"/>
       <c r="K91" s="6"/>
@@ -6481,9 +6497,9 @@
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
     </row>
-    <row r="92" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A92" s="3" t="s">
-        <v>92</v>
+    <row r="92" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A92" s="27" t="s">
+        <v>284</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>252</v>
@@ -6507,7 +6523,7 @@
         <v>212</v>
       </c>
       <c r="I92" s="8" t="s">
-        <v>93</v>
+        <v>285</v>
       </c>
       <c r="J92" s="6"/>
       <c r="K92" s="6"/>
@@ -6529,17 +6545,17 @@
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
     </row>
-    <row r="93" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="5" t="s">
-        <v>215</v>
+    <row r="93" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C93" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D93" s="9" t="s">
+      <c r="C93" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D93" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E93" s="7" t="s">
@@ -6548,18 +6564,18 @@
       <c r="F93" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G93" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="H93" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="I93" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="J93" s="9"/>
-      <c r="K93" s="9"/>
-      <c r="L93" s="9"/>
+      <c r="G93" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="H93" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I93" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
       <c r="M93" s="9"/>
       <c r="N93" s="9"/>
       <c r="O93" s="2"/>
@@ -6577,9 +6593,9 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>252</v>
@@ -6603,7 +6619,7 @@
         <v>211</v>
       </c>
       <c r="I94" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
@@ -6625,9 +6641,9 @@
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
     </row>
-    <row r="95" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>252</v>
@@ -6651,7 +6667,7 @@
         <v>211</v>
       </c>
       <c r="I95" s="20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
@@ -6673,17 +6689,17 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" ht="144" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>161</v>
+        <v>221</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C96" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D96" s="6" t="s">
+      <c r="C96" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D96" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E96" s="7" t="s">
@@ -6692,14 +6708,14 @@
       <c r="F96" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G96" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="H96" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I96" s="8" t="s">
-        <v>160</v>
+      <c r="G96" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="H96" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="I96" s="20" t="s">
+        <v>222</v>
       </c>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
@@ -6721,9 +6737,9 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" ht="144" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>252</v>
@@ -6747,7 +6763,7 @@
         <v>212</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -6769,9 +6785,9 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" ht="144" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
-        <v>79</v>
+    <row r="98" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>252</v>
@@ -6780,13 +6796,13 @@
         <v>77</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="G98" s="6" t="s">
         <v>331</v>
@@ -6795,7 +6811,7 @@
         <v>212</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -6817,33 +6833,33 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E99" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>287</v>
+        <v>331</v>
       </c>
       <c r="H99" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -6865,9 +6881,9 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>286</v>
+        <v>72</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>252</v>
@@ -6888,10 +6904,10 @@
         <v>287</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I100" s="22" t="s">
-        <v>288</v>
+        <v>212</v>
+      </c>
+      <c r="I100" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
@@ -6913,9 +6929,9 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>252</v>
@@ -6939,7 +6955,7 @@
         <v>211</v>
       </c>
       <c r="I101" s="22" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
@@ -6961,9 +6977,9 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>252</v>
@@ -6987,7 +7003,7 @@
         <v>211</v>
       </c>
       <c r="I102" s="22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
@@ -7009,14 +7025,14 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>75</v>
+        <v>291</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C103" s="18" t="s">
+      <c r="C103" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D103" s="6" t="s">
@@ -7032,10 +7048,10 @@
         <v>287</v>
       </c>
       <c r="H103" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I103" s="8" t="s">
-        <v>293</v>
+        <v>211</v>
+      </c>
+      <c r="I103" s="22" t="s">
+        <v>292</v>
       </c>
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
@@ -7057,14 +7073,14 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C104" s="6" t="s">
+      <c r="C104" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D104" s="6" t="s">
@@ -7083,7 +7099,7 @@
         <v>212</v>
       </c>
       <c r="I104" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J104" s="9"/>
       <c r="K104" s="9"/>
@@ -7105,15 +7121,15 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>11</v>
@@ -7125,13 +7141,13 @@
         <v>94</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="H105" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I105" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J105" s="9"/>
       <c r="K105" s="9"/>
@@ -7153,9 +7169,9 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>297</v>
+        <v>108</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>252</v>
@@ -7179,7 +7195,7 @@
         <v>212</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
@@ -7201,15 +7217,15 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>302</v>
+    <row r="107" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>299</v>
+        <v>115</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>11</v>
@@ -7221,13 +7237,13 @@
         <v>94</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H107" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I107" s="8" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
@@ -7249,9 +7265,9 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>252</v>
@@ -7275,7 +7291,7 @@
         <v>212</v>
       </c>
       <c r="I108" s="8" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
@@ -7297,17 +7313,17 @@
       <c r="AA108" s="2"/>
       <c r="AB108" s="2"/>
     </row>
-    <row r="109" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
-      <c r="A109" s="21" t="s">
-        <v>171</v>
+    <row r="109" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>304</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C109" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D109" s="18" t="s">
+      <c r="C109" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D109" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E109" s="7" t="s">
@@ -7316,14 +7332,14 @@
       <c r="F109" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G109" s="18" t="s">
-        <v>314</v>
+      <c r="G109" s="6" t="s">
+        <v>300</v>
       </c>
       <c r="H109" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I109" s="8" t="s">
-        <v>172</v>
+        <v>301</v>
       </c>
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
@@ -7345,17 +7361,17 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="11" t="s">
-        <v>110</v>
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A110" s="21" t="s">
+        <v>171</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C110" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D110" s="6" t="s">
+      <c r="C110" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D110" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E110" s="7" t="s">
@@ -7364,14 +7380,14 @@
       <c r="F110" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G110" s="6" t="s">
-        <v>295</v>
+      <c r="G110" s="18" t="s">
+        <v>314</v>
       </c>
       <c r="H110" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I110" s="8" t="s">
-        <v>116</v>
+        <v>172</v>
       </c>
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
@@ -7393,15 +7409,15 @@
       <c r="AA110" s="2"/>
       <c r="AB110" s="2"/>
     </row>
-    <row r="111" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="21" t="s">
-        <v>173</v>
+    <row r="111" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C111" s="18" t="s">
-        <v>73</v>
+      <c r="C111" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>11</v>
@@ -7413,13 +7429,13 @@
         <v>94</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>175</v>
+        <v>295</v>
       </c>
       <c r="H111" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I111" s="8" t="s">
-        <v>174</v>
+        <v>116</v>
       </c>
       <c r="J111" s="9"/>
       <c r="K111" s="9"/>
@@ -7441,15 +7457,15 @@
       <c r="AA111" s="2"/>
       <c r="AB111" s="2"/>
     </row>
-    <row r="112" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="11" t="s">
-        <v>109</v>
+    <row r="112" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C112" s="6" t="s">
-        <v>115</v>
+      <c r="C112" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>11</v>
@@ -7461,13 +7477,13 @@
         <v>94</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>295</v>
+        <v>175</v>
       </c>
       <c r="H112" s="8" t="s">
         <v>212</v>
       </c>
       <c r="I112" s="8" t="s">
-        <v>117</v>
+        <v>174</v>
       </c>
       <c r="J112" s="9"/>
       <c r="K112" s="9"/>
@@ -7489,15 +7505,15 @@
       <c r="AA112" s="2"/>
       <c r="AB112" s="2"/>
     </row>
-    <row r="113" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A113" s="3" t="s">
-        <v>152</v>
+    <row r="113" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>11</v>
@@ -7509,16 +7525,16 @@
         <v>94</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>153</v>
+        <v>295</v>
       </c>
       <c r="H113" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I113" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="J113" s="6"/>
-      <c r="K113" s="6"/>
+        <v>117</v>
+      </c>
+      <c r="J113" s="9"/>
+      <c r="K113" s="9"/>
       <c r="L113" s="9"/>
       <c r="M113" s="9"/>
       <c r="N113" s="9"/>
@@ -7537,9 +7553,9 @@
       <c r="AA113" s="2"/>
       <c r="AB113" s="2"/>
     </row>
-    <row r="114" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>252</v>
@@ -7557,13 +7573,13 @@
         <v>94</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>317</v>
+        <v>153</v>
       </c>
       <c r="H114" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I114" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J114" s="6"/>
       <c r="K114" s="6"/>
@@ -7585,9 +7601,9 @@
       <c r="AA114" s="2"/>
       <c r="AB114" s="2"/>
     </row>
-    <row r="115" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>279</v>
+        <v>156</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>252</v>
@@ -7605,13 +7621,13 @@
         <v>94</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H115" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I115" s="8" t="s">
-        <v>280</v>
+        <v>157</v>
       </c>
       <c r="J115" s="6"/>
       <c r="K115" s="6"/>
@@ -7633,9 +7649,9 @@
       <c r="AA115" s="2"/>
       <c r="AB115" s="2"/>
     </row>
-    <row r="116" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>252</v>
@@ -7653,13 +7669,13 @@
         <v>94</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H116" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I116" s="8" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="J116" s="6"/>
       <c r="K116" s="6"/>
@@ -7681,9 +7697,9 @@
       <c r="AA116" s="2"/>
       <c r="AB116" s="2"/>
     </row>
-    <row r="117" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>252</v>
@@ -7698,16 +7714,16 @@
         <v>94</v>
       </c>
       <c r="F117" s="7" t="s">
-        <v>278</v>
+        <v>94</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H117" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I117" s="8" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="J117" s="6"/>
       <c r="K117" s="6"/>
@@ -7729,9 +7745,9 @@
       <c r="AA117" s="2"/>
       <c r="AB117" s="2"/>
     </row>
-    <row r="118" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>158</v>
+        <v>274</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>252</v>
@@ -7746,16 +7762,16 @@
         <v>94</v>
       </c>
       <c r="F118" s="7" t="s">
-        <v>94</v>
+        <v>278</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H118" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I118" s="8" t="s">
-        <v>159</v>
+        <v>275</v>
       </c>
       <c r="J118" s="6"/>
       <c r="K118" s="6"/>
@@ -7777,15 +7793,15 @@
       <c r="AA118" s="2"/>
       <c r="AB118" s="2"/>
     </row>
-    <row r="119" spans="1:28" s="1" customFormat="1" ht="288" x14ac:dyDescent="0.3">
-      <c r="A119" s="11" t="s">
-        <v>186</v>
+    <row r="119" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>11</v>
@@ -7797,16 +7813,16 @@
         <v>94</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>209</v>
+        <v>321</v>
       </c>
       <c r="H119" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I119" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J119" s="9"/>
-      <c r="K119" s="9"/>
+        <v>159</v>
+      </c>
+      <c r="J119" s="6"/>
+      <c r="K119" s="6"/>
       <c r="L119" s="9"/>
       <c r="M119" s="9"/>
       <c r="N119" s="9"/>
@@ -7825,9 +7841,9 @@
       <c r="AA119" s="2"/>
       <c r="AB119" s="2"/>
     </row>
-    <row r="120" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>252</v>
@@ -7850,15 +7866,11 @@
       <c r="H120" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I120" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="J120" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K120" s="20" t="s">
-        <v>202</v>
-      </c>
+      <c r="I120" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="J120" s="9"/>
+      <c r="K120" s="9"/>
       <c r="L120" s="9"/>
       <c r="M120" s="9"/>
       <c r="N120" s="9"/>
@@ -7877,9 +7889,9 @@
       <c r="AA120" s="2"/>
       <c r="AB120" s="2"/>
     </row>
-    <row r="121" spans="1:28" s="1" customFormat="1" ht="288" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>252</v>
@@ -7900,26 +7912,20 @@
         <v>209</v>
       </c>
       <c r="H121" s="8" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="I121" s="22" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J121" s="20" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K121" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="L121" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="M121" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="N121" s="20" t="s">
-        <v>207</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="L121" s="9"/>
+      <c r="M121" s="9"/>
+      <c r="N121" s="9"/>
       <c r="O121" s="2"/>
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
@@ -7935,9 +7941,9 @@
       <c r="AA121" s="2"/>
       <c r="AB121" s="2"/>
     </row>
-    <row r="122" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="23" t="s">
-        <v>233</v>
+    <row r="122" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A122" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>252</v>
@@ -7945,7 +7951,7 @@
       <c r="C122" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D122" s="24" t="s">
+      <c r="D122" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E122" s="7" t="s">
@@ -7957,21 +7963,27 @@
       <c r="G122" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="H122" s="20" t="s">
-        <v>211</v>
+      <c r="H122" s="8" t="s">
+        <v>199</v>
       </c>
       <c r="I122" s="22" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="J122" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="K122" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="K122" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="L122" s="9"/>
-      <c r="M122" s="9"/>
-      <c r="N122" s="9"/>
+      <c r="L122" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="M122" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="N122" s="20" t="s">
+        <v>207</v>
+      </c>
       <c r="O122" s="2"/>
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
@@ -7987,17 +7999,17 @@
       <c r="AA122" s="2"/>
       <c r="AB122" s="2"/>
     </row>
-    <row r="123" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="11" t="s">
-        <v>235</v>
+    <row r="123" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="23" t="s">
+        <v>233</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="D123" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D123" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E123" s="7" t="s">
@@ -8009,14 +8021,18 @@
       <c r="G123" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="H123" s="8" t="s">
+      <c r="H123" s="20" t="s">
         <v>211</v>
       </c>
       <c r="I123" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="J123" s="20"/>
-      <c r="K123" s="20"/>
+        <v>234</v>
+      </c>
+      <c r="J123" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="K123" s="20" t="s">
+        <v>236</v>
+      </c>
       <c r="L123" s="9"/>
       <c r="M123" s="9"/>
       <c r="N123" s="9"/>
@@ -8035,15 +8051,15 @@
       <c r="AA123" s="2"/>
       <c r="AB123" s="2"/>
     </row>
-    <row r="124" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>187</v>
+        <v>242</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>11</v>
@@ -8061,17 +8077,13 @@
         <v>211</v>
       </c>
       <c r="I124" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="J124" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K124" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="L124" s="20"/>
-      <c r="M124" s="20"/>
-      <c r="N124" s="20"/>
+        <v>232</v>
+      </c>
+      <c r="J124" s="20"/>
+      <c r="K124" s="20"/>
+      <c r="L124" s="9"/>
+      <c r="M124" s="9"/>
+      <c r="N124" s="9"/>
       <c r="O124" s="2"/>
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
@@ -8087,18 +8099,18 @@
       <c r="AA124" s="2"/>
       <c r="AB124" s="2"/>
     </row>
-    <row r="125" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="3" t="s">
-        <v>241</v>
+    <row r="125" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A125" s="11" t="s">
+        <v>243</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>10</v>
+        <v>187</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E125" s="7" t="s">
         <v>94</v>
@@ -8107,17 +8119,23 @@
         <v>94</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="H125" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="I125" s="9"/>
-      <c r="J125" s="9"/>
-      <c r="K125" s="9"/>
-      <c r="L125" s="9"/>
-      <c r="M125" s="9"/>
-      <c r="N125" s="9"/>
+        <v>211</v>
+      </c>
+      <c r="I125" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="J125" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="K125" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="L125" s="20"/>
+      <c r="M125" s="20"/>
+      <c r="N125" s="20"/>
       <c r="O125" s="2"/>
       <c r="P125" s="2"/>
       <c r="Q125" s="2"/>
@@ -8133,8 +8151,54 @@
       <c r="AA125" s="2"/>
       <c r="AB125" s="2"/>
     </row>
+    <row r="126" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E126" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F126" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G126" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H126" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="I126" s="9"/>
+      <c r="J126" s="9"/>
+      <c r="K126" s="9"/>
+      <c r="L126" s="9"/>
+      <c r="M126" s="9"/>
+      <c r="N126" s="9"/>
+      <c r="O126" s="2"/>
+      <c r="P126" s="2"/>
+      <c r="Q126" s="2"/>
+      <c r="R126" s="2"/>
+      <c r="S126" s="2"/>
+      <c r="T126" s="2"/>
+      <c r="U126" s="2"/>
+      <c r="V126" s="2"/>
+      <c r="W126" s="2"/>
+      <c r="X126" s="2"/>
+      <c r="Y126" s="2"/>
+      <c r="Z126" s="2"/>
+      <c r="AA126" s="2"/>
+      <c r="AB126" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I125" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I126" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified test methods in login coyni portal and user details
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Merchant invitation\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(16-03-2023)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE2EA67-061C-4D72-8252-44FAAD58D597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C83C45-30FE-4340-B941-92685EA07D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$129</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="351">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -835,9 +835,6 @@
   </si>
   <si>
     <t>testGobalSearch</t>
-  </si>
-  <si>
-    <t>Gobal Seach</t>
   </si>
   <si>
     <t>testData-admin.xlsx,gobalSearch</t>
@@ -1647,9 +1644,6 @@
 -pfirstSixDigits</t>
   </si>
   <si>
-    <t>Gobal Seach with last 4 digits</t>
-  </si>
-  <si>
     <t>testGobalSearchWithBankAccount</t>
   </si>
   <si>
@@ -1832,21 +1826,6 @@
   </si>
   <si>
     <t>Profile - Individuals</t>
-  </si>
-  <si>
-    <t>Gobal Seach - profile details</t>
-  </si>
-  <si>
-    <t>Gobal Seach - Bank Account</t>
-  </si>
-  <si>
-    <t>Gobal Seach - First 6 digits</t>
-  </si>
-  <si>
-    <t>Gobal Seach - last 4 digits</t>
-  </si>
-  <si>
-    <t>Gobal Seach - Reference Id</t>
   </si>
   <si>
     <t>Profiles - Individuals</t>
@@ -1942,6 +1921,54 @@
 -pmessage,
 -pheading,
 -psecurityKey</t>
+  </si>
+  <si>
+    <t>Global Seach</t>
+  </si>
+  <si>
+    <t>Global Seach - profile details</t>
+  </si>
+  <si>
+    <t>Global Seach - Bank Account</t>
+  </si>
+  <si>
+    <t>Global Seach - First 6 digits</t>
+  </si>
+  <si>
+    <t>Global Seach - last 4 digits</t>
+  </si>
+  <si>
+    <t>Global Seach - Reference Id</t>
+  </si>
+  <si>
+    <t>testGobalSearchWithUnderWritingID</t>
+  </si>
+  <si>
+    <t>Global Seach - UnderWriting Id</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.HomeTest,
+tesGobalSearchUnderWritingCaseId,
+-pcaseId</t>
+  </si>
+  <si>
+    <t>verify Token Account Activity</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.CoyniPortalTest,
+testTokenAccountActivity,
+-pheading</t>
+  </si>
+  <si>
+    <t>verify Token Account - Transaction</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.CoyniPortalTest,
+testTokenAccountTransactionList,
+-pheading</t>
+  </si>
+  <si>
+    <t>System Settings - Agreements</t>
   </si>
 </sst>
 </file>
@@ -2054,7 +2081,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2103,6 +2130,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2383,11 +2411,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB126"/>
+  <dimension ref="A1:AB129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2397,7 +2425,7 @@
     <col min="3" max="3" width="43.140625" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.42578125" customWidth="1"/>
     <col min="9" max="9" width="43.140625" customWidth="1"/>
@@ -2447,7 +2475,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>
@@ -2465,7 +2493,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -2490,10 +2518,10 @@
     </row>
     <row r="3" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>10</v>
@@ -2511,7 +2539,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -2536,10 +2564,10 @@
     </row>
     <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>10</v>
@@ -2551,13 +2579,13 @@
         <v>94</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -2585,7 +2613,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
@@ -2631,7 +2659,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>10</v>
@@ -2649,7 +2677,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -2677,7 +2705,7 @@
         <v>139</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>10</v>
@@ -2723,7 +2751,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>24</v>
@@ -2741,7 +2769,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -2769,7 +2797,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>24</v>
@@ -2815,7 +2843,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>24</v>
@@ -2861,7 +2889,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>24</v>
@@ -2907,7 +2935,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>32</v>
@@ -2953,7 +2981,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>32</v>
@@ -2999,7 +3027,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>32</v>
@@ -3045,7 +3073,7 @@
         <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>32</v>
@@ -3091,7 +3119,7 @@
         <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>32</v>
@@ -3134,10 +3162,10 @@
     </row>
     <row r="17" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>10</v>
@@ -3152,13 +3180,13 @@
         <v>94</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
@@ -3185,7 +3213,7 @@
         <v>128</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>130</v>
@@ -3200,13 +3228,13 @@
         <v>112</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -3233,7 +3261,7 @@
         <v>129</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>130</v>
@@ -3248,13 +3276,13 @@
         <v>113</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -3281,7 +3309,7 @@
         <v>131</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>132</v>
@@ -3299,7 +3327,7 @@
         <v>133</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>150</v>
@@ -3329,7 +3357,7 @@
         <v>148</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>132</v>
@@ -3347,7 +3375,7 @@
         <v>151</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>149</v>
@@ -3377,7 +3405,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>18</v>
@@ -3392,13 +3420,13 @@
         <v>94</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -3425,7 +3453,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
@@ -3440,10 +3468,10 @@
         <v>94</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>20</v>
@@ -3473,7 +3501,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>18</v>
@@ -3488,10 +3516,10 @@
         <v>94</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>22</v>
@@ -3516,33 +3544,33 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
     </row>
-    <row r="25" spans="1:28" ht="270" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>227</v>
+    <row r="25" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>346</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>231</v>
+        <v>18</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="6">
-        <v>1</v>
-      </c>
-      <c r="F25" s="6">
-        <v>1</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>327</v>
+      <c r="E25" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>303</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>223</v>
+        <v>347</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -3565,32 +3593,32 @@
       <c r="AB25" s="2"/>
     </row>
     <row r="26" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>228</v>
+      <c r="A26" s="28" t="s">
+        <v>348</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>231</v>
+        <v>18</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="6">
-        <v>1</v>
-      </c>
-      <c r="F26" s="6">
-        <v>2</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>327</v>
+        <v>11</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>303</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>224</v>
+        <v>349</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -3612,15 +3640,15 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>229</v>
+    <row r="27" spans="1:28" ht="270" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>226</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>11</v>
@@ -3632,13 +3660,13 @@
         <v>1</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -3660,33 +3688,33 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" ht="285" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>230</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>249</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>113</v>
+      <c r="E28" s="6">
+        <v>1</v>
+      </c>
+      <c r="F28" s="6">
+        <v>2</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -3708,49 +3736,63 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
-        <v>144</v>
+    <row r="29" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>18</v>
+        <v>230</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>94</v>
+      <c r="E29" s="6">
+        <v>1</v>
+      </c>
+      <c r="F29" s="6">
+        <v>1</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I29" s="19" t="s">
-        <v>145</v>
+        <v>210</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>224</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
-    </row>
-    <row r="30" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
+    </row>
+    <row r="30" spans="1:28" ht="285" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>95</v>
+        <v>229</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>18</v>
+        <v>248</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>14</v>
@@ -3759,16 +3801,16 @@
         <v>94</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I30" s="20" t="s">
-        <v>96</v>
+        <v>210</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>225</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -3790,18 +3832,18 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>334</v>
+    <row r="31" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>94</v>
@@ -3810,40 +3852,26 @@
         <v>94</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I31" s="20" t="s">
-        <v>335</v>
+        <v>210</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-      <c r="Z31" s="2"/>
-      <c r="AA31" s="2"/>
-      <c r="AB31" s="2"/>
     </row>
     <row r="32" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>332</v>
+        <v>95</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>18</v>
@@ -3858,13 +3886,13 @@
         <v>94</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I32" s="20" t="s">
-        <v>333</v>
+        <v>96</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3886,18 +3914,18 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>97</v>
+        <v>327</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>94</v>
@@ -3906,13 +3934,13 @@
         <v>94</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="H33" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I33" s="8" t="s">
-        <v>98</v>
+      <c r="I33" s="20" t="s">
+        <v>328</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -3934,18 +3962,18 @@
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
     </row>
-    <row r="34" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>99</v>
+        <v>325</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>94</v>
@@ -3954,13 +3982,13 @@
         <v>94</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I34" s="8" t="s">
-        <v>100</v>
+      <c r="I34" s="20" t="s">
+        <v>326</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -3984,10 +4012,10 @@
     </row>
     <row r="35" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>18</v>
@@ -4002,13 +4030,13 @@
         <v>94</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -4032,10 +4060,10 @@
     </row>
     <row r="36" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>18</v>
@@ -4050,13 +4078,13 @@
         <v>94</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -4080,10 +4108,10 @@
     </row>
     <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>18</v>
@@ -4098,13 +4126,13 @@
         <v>94</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
@@ -4128,10 +4156,10 @@
     </row>
     <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>337</v>
+        <v>103</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>18</v>
@@ -4146,13 +4174,13 @@
         <v>94</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>336</v>
+        <v>104</v>
       </c>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
@@ -4176,13 +4204,13 @@
     </row>
     <row r="39" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>11</v>
@@ -4194,15 +4222,15 @@
         <v>94</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J39" s="6"/>
+        <v>106</v>
+      </c>
+      <c r="J39" s="9"/>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
@@ -4224,13 +4252,13 @@
     </row>
     <row r="40" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>169</v>
+        <v>330</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>11</v>
@@ -4242,15 +4270,15 @@
         <v>94</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="J40" s="6"/>
+        <v>329</v>
+      </c>
+      <c r="J40" s="9"/>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
@@ -4272,10 +4300,10 @@
     </row>
     <row r="41" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>44</v>
@@ -4290,13 +4318,13 @@
         <v>94</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="9"/>
@@ -4320,10 +4348,10 @@
     </row>
     <row r="42" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>48</v>
+        <v>168</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>44</v>
@@ -4338,13 +4366,13 @@
         <v>94</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>49</v>
+        <v>169</v>
       </c>
       <c r="J42" s="6"/>
       <c r="K42" s="9"/>
@@ -4368,10 +4396,10 @@
     </row>
     <row r="43" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>44</v>
@@ -4386,13 +4414,13 @@
         <v>94</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J43" s="6"/>
       <c r="K43" s="9"/>
@@ -4416,10 +4444,10 @@
     </row>
     <row r="44" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>44</v>
@@ -4434,13 +4462,13 @@
         <v>94</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J44" s="6"/>
       <c r="K44" s="9"/>
@@ -4464,10 +4492,10 @@
     </row>
     <row r="45" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>44</v>
@@ -4482,13 +4510,13 @@
         <v>94</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J45" s="6"/>
       <c r="K45" s="9"/>
@@ -4512,13 +4540,13 @@
     </row>
     <row r="46" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>11</v>
@@ -4530,16 +4558,16 @@
         <v>94</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>141</v>
+        <v>53</v>
       </c>
       <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
+      <c r="K46" s="9"/>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
       <c r="N46" s="9"/>
@@ -4560,13 +4588,13 @@
     </row>
     <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>11</v>
@@ -4578,16 +4606,16 @@
         <v>94</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
+      <c r="K47" s="9"/>
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
       <c r="N47" s="9"/>
@@ -4608,10 +4636,10 @@
     </row>
     <row r="48" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>57</v>
@@ -4626,13 +4654,13 @@
         <v>94</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
@@ -4656,10 +4684,10 @@
     </row>
     <row r="49" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>57</v>
@@ -4674,13 +4702,13 @@
         <v>94</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -4704,10 +4732,10 @@
     </row>
     <row r="50" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>57</v>
@@ -4722,13 +4750,13 @@
         <v>94</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -4752,10 +4780,10 @@
     </row>
     <row r="51" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>57</v>
@@ -4770,13 +4798,13 @@
         <v>94</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -4800,10 +4828,10 @@
     </row>
     <row r="52" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>57</v>
@@ -4818,13 +4846,13 @@
         <v>94</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -4848,10 +4876,10 @@
     </row>
     <row r="53" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>134</v>
+        <v>66</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>57</v>
@@ -4866,13 +4894,13 @@
         <v>94</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>135</v>
+        <v>67</v>
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
@@ -4896,10 +4924,10 @@
     </row>
     <row r="54" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>57</v>
@@ -4914,13 +4942,13 @@
         <v>94</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -4944,13 +4972,13 @@
     </row>
     <row r="55" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>11</v>
@@ -4962,13 +4990,13 @@
         <v>94</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I55" s="19" t="s">
-        <v>143</v>
+        <v>210</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -4990,15 +5018,15 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>146</v>
+        <v>70</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>11</v>
@@ -5010,13 +5038,13 @@
         <v>94</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I56" s="19" t="s">
-        <v>147</v>
+        <v>210</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -5038,15 +5066,15 @@
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>118</v>
+    <row r="57" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>11</v>
@@ -5058,29 +5086,43 @@
         <v>94</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I57" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
+        <v>210</v>
+      </c>
+      <c r="I57" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
-    </row>
-    <row r="58" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
+      <c r="U57" s="2"/>
+      <c r="V57" s="2"/>
+      <c r="W57" s="2"/>
+      <c r="X57" s="2"/>
+      <c r="Y57" s="2"/>
+      <c r="Z57" s="2"/>
+      <c r="AA57" s="2"/>
+      <c r="AB57" s="2"/>
+    </row>
+    <row r="58" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>11</v>
@@ -5092,16 +5134,16 @@
         <v>94</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I58" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
+        <v>210</v>
+      </c>
+      <c r="I58" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
       <c r="L58" s="9"/>
       <c r="M58" s="9"/>
       <c r="N58" s="9"/>
@@ -5120,12 +5162,12 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>121</v>
+    <row r="59" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>124</v>
@@ -5140,61 +5182,47 @@
         <v>94</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I59" s="22" t="s">
-        <v>122</v>
+        <v>211</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
       <c r="N59" s="9"/>
-      <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-      <c r="R59" s="2"/>
-      <c r="S59" s="2"/>
-      <c r="T59" s="2"/>
-      <c r="U59" s="2"/>
-      <c r="V59" s="2"/>
-      <c r="W59" s="2"/>
-      <c r="X59" s="2"/>
-      <c r="Y59" s="2"/>
-      <c r="Z59" s="2"/>
-      <c r="AA59" s="2"/>
-      <c r="AB59" s="2"/>
-    </row>
-    <row r="60" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>338</v>
+        <v>120</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>339</v>
+        <v>124</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E60" s="7">
-        <v>1</v>
-      </c>
-      <c r="F60" s="7">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>341</v>
+        <v>313</v>
       </c>
       <c r="H60" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>340</v>
+        <v>175</v>
       </c>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -5218,10 +5246,10 @@
     </row>
     <row r="61" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>124</v>
@@ -5236,13 +5264,13 @@
         <v>94</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I61" s="22" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -5264,33 +5292,33 @@
       <c r="AA61" s="2"/>
       <c r="AB61" s="2"/>
     </row>
-    <row r="62" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>126</v>
+        <v>331</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>124</v>
+        <v>332</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>94</v>
+        <v>14</v>
+      </c>
+      <c r="E62" s="7">
+        <v>1</v>
+      </c>
+      <c r="F62" s="7">
+        <v>1</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>127</v>
+        <v>333</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -5312,15 +5340,15 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
-        <v>178</v>
+    <row r="63" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>208</v>
+        <v>124</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>11</v>
@@ -5332,13 +5360,13 @@
         <v>94</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="H63" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>191</v>
+        <v>125</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -5360,15 +5388,15 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
-        <v>179</v>
+    <row r="64" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>208</v>
+        <v>124</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>11</v>
@@ -5380,13 +5408,13 @@
         <v>94</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="H64" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>192</v>
+        <v>127</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -5413,10 +5441,10 @@
         <v>177</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>11</v>
@@ -5428,10 +5456,10 @@
         <v>94</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I65" s="22" t="s">
         <v>190</v>
@@ -5457,14 +5485,14 @@
       <c r="AB65" s="2"/>
     </row>
     <row r="66" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A66" s="25" t="s">
-        <v>181</v>
+      <c r="A66" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>11</v>
@@ -5476,13 +5504,13 @@
         <v>94</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I66" s="22" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -5504,15 +5532,15 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>11</v>
@@ -5524,13 +5552,13 @@
         <v>94</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I67" s="22" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -5553,14 +5581,14 @@
       <c r="AB67" s="2"/>
     </row>
     <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>183</v>
+      <c r="A68" s="25" t="s">
+        <v>180</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>11</v>
@@ -5572,13 +5600,13 @@
         <v>94</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I68" s="22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -5600,15 +5628,15 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>184</v>
+    <row r="69" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>181</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>11</v>
@@ -5620,13 +5648,13 @@
         <v>94</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I69" s="22" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -5650,13 +5678,13 @@
     </row>
     <row r="70" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>11</v>
@@ -5668,13 +5696,13 @@
         <v>94</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I70" s="22" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -5698,13 +5726,13 @@
     </row>
     <row r="71" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>11</v>
@@ -5716,13 +5744,13 @@
         <v>94</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I71" s="22" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -5745,17 +5773,17 @@
       <c r="AB71" s="2"/>
     </row>
     <row r="72" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A72" s="26" t="s">
-        <v>251</v>
+      <c r="A72" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E72" s="7" t="s">
         <v>94</v>
@@ -5764,53 +5792,91 @@
         <v>94</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="H72" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I72" s="22" t="s">
-        <v>259</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
+      <c r="O72" s="2"/>
+      <c r="P72" s="2"/>
+      <c r="Q72" s="2"/>
+      <c r="R72" s="2"/>
+      <c r="S72" s="2"/>
+      <c r="T72" s="2"/>
+      <c r="U72" s="2"/>
+      <c r="V72" s="2"/>
+      <c r="W72" s="2"/>
+      <c r="X72" s="2"/>
+      <c r="Y72" s="2"/>
+      <c r="Z72" s="2"/>
+      <c r="AA72" s="2"/>
+      <c r="AB72" s="2"/>
     </row>
     <row r="73" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>254</v>
+      <c r="A73" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E73" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>255</v>
+        <v>94</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I73" s="22" t="s">
-        <v>256</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
+      <c r="O73" s="2"/>
+      <c r="P73" s="2"/>
+      <c r="Q73" s="2"/>
+      <c r="R73" s="2"/>
+      <c r="S73" s="2"/>
+      <c r="T73" s="2"/>
+      <c r="U73" s="2"/>
+      <c r="V73" s="2"/>
+      <c r="W73" s="2"/>
+      <c r="X73" s="2"/>
+      <c r="Y73" s="2"/>
+      <c r="Z73" s="2"/>
+      <c r="AA73" s="2"/>
+      <c r="AB73" s="2"/>
     </row>
     <row r="74" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>257</v>
+      <c r="A74" s="26" t="s">
+        <v>250</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>14</v>
@@ -5822,10 +5888,10 @@
         <v>94</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I74" s="22" t="s">
         <v>258</v>
@@ -5833,10 +5899,10 @@
     </row>
     <row r="75" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>124</v>
@@ -5848,24 +5914,24 @@
         <v>94</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>94</v>
+        <v>254</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I75" s="22" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="76" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>124</v>
@@ -5880,13 +5946,13 @@
         <v>94</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H76" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I76" s="22" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:28" ht="165" x14ac:dyDescent="0.25">
@@ -5894,7 +5960,7 @@
         <v>263</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>124</v>
@@ -5909,21 +5975,21 @@
         <v>94</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H77" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I77" s="22" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="78" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>124</v>
@@ -5938,21 +6004,21 @@
         <v>94</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H78" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I78" s="22" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="79" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>124</v>
@@ -5967,21 +6033,21 @@
         <v>94</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H79" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I79" s="22" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="80" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>124</v>
@@ -5996,21 +6062,21 @@
         <v>94</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I80" s="22" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="81" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>124</v>
@@ -6025,21 +6091,21 @@
         <v>94</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H81" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I81" s="22" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="82" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>124</v>
@@ -6054,141 +6120,103 @@
         <v>94</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H82" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I82" s="22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>271</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="H83" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I83" s="22" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>279</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="H84" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I84" s="22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H85" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I82" s="22" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="83" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="H83" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I83" s="8" t="s">
+      <c r="I85" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="J83" s="6"/>
-      <c r="K83" s="6"/>
-      <c r="L83" s="9"/>
-      <c r="M83" s="9"/>
-      <c r="N83" s="9"/>
-      <c r="O83" s="2"/>
-      <c r="P83" s="2"/>
-      <c r="Q83" s="2"/>
-      <c r="R83" s="2"/>
-      <c r="S83" s="2"/>
-      <c r="T83" s="2"/>
-      <c r="U83" s="2"/>
-      <c r="V83" s="2"/>
-      <c r="W83" s="2"/>
-      <c r="X83" s="2"/>
-      <c r="Y83" s="2"/>
-      <c r="Z83" s="2"/>
-      <c r="AA83" s="2"/>
-      <c r="AB83" s="2"/>
-    </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="H84" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I84" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="J84" s="8"/>
-      <c r="K84" s="9"/>
-      <c r="L84" s="9"/>
-      <c r="M84" s="9"/>
-      <c r="N84" s="9"/>
-      <c r="O84" s="2"/>
-      <c r="P84" s="2"/>
-      <c r="Q84" s="2"/>
-      <c r="R84" s="2"/>
-      <c r="S84" s="2"/>
-      <c r="T84" s="2"/>
-      <c r="U84" s="2"/>
-      <c r="V84" s="2"/>
-      <c r="W84" s="2"/>
-      <c r="X84" s="2"/>
-      <c r="Y84" s="2"/>
-      <c r="Z84" s="2"/>
-      <c r="AA84" s="2"/>
-      <c r="AB84" s="2"/>
-    </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G85" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="H85" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I85" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="J85" s="8"/>
-      <c r="K85" s="9"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
       <c r="L85" s="9"/>
       <c r="M85" s="9"/>
       <c r="N85" s="9"/>
@@ -6207,15 +6235,15 @@
       <c r="AA85" s="2"/>
       <c r="AB85" s="2"/>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>11</v>
@@ -6227,17 +6255,15 @@
         <v>94</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H86" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="J86" s="20" t="s">
-        <v>168</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="J86" s="8"/>
       <c r="K86" s="9"/>
       <c r="L86" s="9"/>
       <c r="M86" s="9"/>
@@ -6257,15 +6283,15 @@
       <c r="AA86" s="2"/>
       <c r="AB86" s="2"/>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>11</v>
@@ -6277,17 +6303,17 @@
         <v>94</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>312</v>
+        <v>161</v>
       </c>
       <c r="H87" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="J87" s="6"/>
-      <c r="K87" s="6"/>
-      <c r="L87" s="6"/>
+        <v>165</v>
+      </c>
+      <c r="J87" s="8"/>
+      <c r="K87" s="9"/>
+      <c r="L87" s="9"/>
       <c r="M87" s="9"/>
       <c r="N87" s="9"/>
       <c r="O87" s="2"/>
@@ -6307,13 +6333,13 @@
     </row>
     <row r="88" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>11</v>
@@ -6325,17 +6351,19 @@
         <v>94</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>312</v>
+        <v>161</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="J88" s="6"/>
-      <c r="K88" s="6"/>
-      <c r="L88" s="6"/>
+        <v>165</v>
+      </c>
+      <c r="J88" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="K88" s="9"/>
+      <c r="L88" s="9"/>
       <c r="M88" s="9"/>
       <c r="N88" s="9"/>
       <c r="O88" s="2"/>
@@ -6355,10 +6383,10 @@
     </row>
     <row r="89" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>82</v>
@@ -6373,13 +6401,13 @@
         <v>94</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H89" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
@@ -6403,10 +6431,10 @@
     </row>
     <row r="90" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>82</v>
@@ -6421,13 +6449,13 @@
         <v>94</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J90" s="6"/>
       <c r="K90" s="6"/>
@@ -6451,10 +6479,10 @@
     </row>
     <row r="91" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>82</v>
@@ -6469,13 +6497,13 @@
         <v>94</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I91" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J91" s="6"/>
       <c r="K91" s="6"/>
@@ -6498,11 +6526,11 @@
       <c r="AB91" s="2"/>
     </row>
     <row r="92" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A92" s="27" t="s">
-        <v>284</v>
+      <c r="A92" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>82</v>
@@ -6517,13 +6545,13 @@
         <v>94</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I92" s="8" t="s">
-        <v>285</v>
+        <v>89</v>
       </c>
       <c r="J92" s="6"/>
       <c r="K92" s="6"/>
@@ -6547,10 +6575,10 @@
     </row>
     <row r="93" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>82</v>
@@ -6565,13 +6593,13 @@
         <v>94</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I93" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J93" s="6"/>
       <c r="K93" s="6"/>
@@ -6593,17 +6621,17 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>215</v>
+    <row r="94" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A94" s="27" t="s">
+        <v>282</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D94" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D94" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E94" s="7" t="s">
@@ -6612,18 +6640,18 @@
       <c r="F94" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G94" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="H94" s="20" t="s">
+      <c r="G94" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="H94" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I94" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="J94" s="9"/>
-      <c r="K94" s="9"/>
-      <c r="L94" s="9"/>
+      <c r="I94" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
       <c r="M94" s="9"/>
       <c r="N94" s="9"/>
       <c r="O94" s="2"/>
@@ -6641,17 +6669,17 @@
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
     </row>
-    <row r="95" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>219</v>
+    <row r="95" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D95" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D95" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E95" s="7" t="s">
@@ -6660,18 +6688,18 @@
       <c r="F95" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G95" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="H95" s="20" t="s">
+      <c r="G95" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="H95" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I95" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="J95" s="9"/>
-      <c r="K95" s="9"/>
-      <c r="L95" s="9"/>
+      <c r="I95" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="6"/>
       <c r="M95" s="9"/>
       <c r="N95" s="9"/>
       <c r="O95" s="2"/>
@@ -6689,33 +6717,33 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C96" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G96" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="D96" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G96" s="9" t="s">
+      <c r="H96" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="I96" s="20" t="s">
         <v>217</v>
-      </c>
-      <c r="H96" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="I96" s="20" t="s">
-        <v>222</v>
       </c>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
@@ -6737,17 +6765,17 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>161</v>
+        <v>218</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D97" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D97" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E97" s="7" t="s">
@@ -6756,14 +6784,14 @@
       <c r="F97" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G97" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="H97" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I97" s="8" t="s">
-        <v>160</v>
+      <c r="G97" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="H97" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="I97" s="20" t="s">
+        <v>219</v>
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
@@ -6785,17 +6813,17 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>114</v>
+        <v>220</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D98" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D98" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E98" s="7" t="s">
@@ -6804,14 +6832,14 @@
       <c r="F98" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G98" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="H98" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I98" s="8" t="s">
-        <v>78</v>
+      <c r="G98" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="H98" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="I98" s="20" t="s">
+        <v>221</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
@@ -6834,32 +6862,32 @@
       <c r="AB98" s="2"/>
     </row>
     <row r="99" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
-        <v>79</v>
+      <c r="A99" s="5" t="s">
+        <v>160</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>77</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E99" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="H99" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>80</v>
+        <v>159</v>
       </c>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -6881,15 +6909,15 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
-        <v>72</v>
+    <row r="100" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>11</v>
@@ -6901,13 +6929,13 @@
         <v>94</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>287</v>
+        <v>324</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
@@ -6929,33 +6957,33 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>286</v>
+        <v>79</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E101" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>287</v>
+        <v>324</v>
       </c>
       <c r="H101" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I101" s="22" t="s">
-        <v>288</v>
+      <c r="I101" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
@@ -6977,12 +7005,12 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>289</v>
+        <v>72</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>73</v>
@@ -6997,13 +7025,13 @@
         <v>94</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H102" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I102" s="22" t="s">
-        <v>290</v>
+      <c r="I102" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
@@ -7027,10 +7055,10 @@
     </row>
     <row r="103" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>73</v>
@@ -7045,13 +7073,13 @@
         <v>94</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>287</v>
+        <v>350</v>
       </c>
       <c r="H103" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I103" s="22" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
@@ -7073,14 +7101,14 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>75</v>
+        <v>287</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C104" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C104" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D104" s="6" t="s">
@@ -7093,13 +7121,13 @@
         <v>94</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>287</v>
+        <v>350</v>
       </c>
       <c r="H104" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I104" s="8" t="s">
-        <v>293</v>
+        <v>210</v>
+      </c>
+      <c r="I104" s="22" t="s">
+        <v>288</v>
       </c>
       <c r="J104" s="9"/>
       <c r="K104" s="9"/>
@@ -7121,12 +7149,12 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>76</v>
+        <v>289</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>73</v>
@@ -7141,13 +7169,13 @@
         <v>94</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>287</v>
+        <v>350</v>
       </c>
       <c r="H105" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="I105" s="8" t="s">
-        <v>294</v>
+        <v>210</v>
+      </c>
+      <c r="I105" s="22" t="s">
+        <v>290</v>
       </c>
       <c r="J105" s="9"/>
       <c r="K105" s="9"/>
@@ -7169,15 +7197,15 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>115</v>
+        <v>251</v>
+      </c>
+      <c r="C106" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>11</v>
@@ -7189,13 +7217,13 @@
         <v>94</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="H106" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
@@ -7217,15 +7245,15 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>297</v>
+        <v>76</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>11</v>
@@ -7237,13 +7265,13 @@
         <v>94</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="H107" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I107" s="8" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
@@ -7266,14 +7294,14 @@
       <c r="AB107" s="2"/>
     </row>
     <row r="108" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>302</v>
+      <c r="A108" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>299</v>
+        <v>115</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>11</v>
@@ -7285,13 +7313,13 @@
         <v>94</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="H108" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I108" s="8" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
@@ -7314,14 +7342,14 @@
       <c r="AB108" s="2"/>
     </row>
     <row r="109" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>304</v>
+      <c r="A109" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>299</v>
+        <v>115</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>11</v>
@@ -7333,13 +7361,13 @@
         <v>94</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="H109" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I109" s="8" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
@@ -7361,17 +7389,17 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A110" s="21" t="s">
-        <v>171</v>
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>300</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C110" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D110" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="D110" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E110" s="7" t="s">
@@ -7380,14 +7408,14 @@
       <c r="F110" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G110" s="18" t="s">
-        <v>314</v>
+      <c r="G110" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I110" s="8" t="s">
-        <v>172</v>
+        <v>301</v>
       </c>
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
@@ -7410,14 +7438,14 @@
       <c r="AB110" s="2"/>
     </row>
     <row r="111" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="11" t="s">
-        <v>110</v>
+      <c r="A111" t="s">
+        <v>302</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>115</v>
+        <v>297</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>11</v>
@@ -7429,13 +7457,13 @@
         <v>94</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="H111" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I111" s="8" t="s">
-        <v>116</v>
+        <v>299</v>
       </c>
       <c r="J111" s="9"/>
       <c r="K111" s="9"/>
@@ -7457,17 +7485,17 @@
       <c r="AA111" s="2"/>
       <c r="AB111" s="2"/>
     </row>
-    <row r="112" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A112" s="21" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C112" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D112" s="6" t="s">
+      <c r="D112" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E112" s="7" t="s">
@@ -7476,14 +7504,14 @@
       <c r="F112" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G112" s="6" t="s">
-        <v>175</v>
+      <c r="G112" s="18" t="s">
+        <v>312</v>
       </c>
       <c r="H112" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I112" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J112" s="9"/>
       <c r="K112" s="9"/>
@@ -7507,10 +7535,10 @@
     </row>
     <row r="113" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>115</v>
@@ -7525,13 +7553,13 @@
         <v>94</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H113" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I113" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J113" s="9"/>
       <c r="K113" s="9"/>
@@ -7553,15 +7581,15 @@
       <c r="AA113" s="2"/>
       <c r="AB113" s="2"/>
     </row>
-    <row r="114" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
-        <v>152</v>
+    <row r="114" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="21" t="s">
+        <v>172</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>154</v>
+        <v>251</v>
+      </c>
+      <c r="C114" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>11</v>
@@ -7573,16 +7601,16 @@
         <v>94</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="H114" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I114" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="J114" s="6"/>
-      <c r="K114" s="6"/>
+        <v>173</v>
+      </c>
+      <c r="J114" s="9"/>
+      <c r="K114" s="9"/>
       <c r="L114" s="9"/>
       <c r="M114" s="9"/>
       <c r="N114" s="9"/>
@@ -7601,15 +7629,15 @@
       <c r="AA114" s="2"/>
       <c r="AB114" s="2"/>
     </row>
-    <row r="115" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
-        <v>156</v>
+    <row r="115" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>11</v>
@@ -7621,16 +7649,16 @@
         <v>94</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="H115" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I115" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="J115" s="6"/>
-      <c r="K115" s="6"/>
+        <v>117</v>
+      </c>
+      <c r="J115" s="9"/>
+      <c r="K115" s="9"/>
       <c r="L115" s="9"/>
       <c r="M115" s="9"/>
       <c r="N115" s="9"/>
@@ -7651,31 +7679,31 @@
     </row>
     <row r="116" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>279</v>
+        <v>152</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C116" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G116" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="H116" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I116" s="8" t="s">
         <v>154</v>
-      </c>
-      <c r="D116" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E116" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F116" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G116" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="H116" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I116" s="8" t="s">
-        <v>280</v>
       </c>
       <c r="J116" s="6"/>
       <c r="K116" s="6"/>
@@ -7699,13 +7727,13 @@
     </row>
     <row r="117" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>276</v>
+        <v>155</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>11</v>
@@ -7717,13 +7745,13 @@
         <v>94</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>319</v>
+        <v>338</v>
       </c>
       <c r="H117" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I117" s="8" t="s">
-        <v>277</v>
+        <v>156</v>
       </c>
       <c r="J117" s="6"/>
       <c r="K117" s="6"/>
@@ -7747,13 +7775,13 @@
     </row>
     <row r="118" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>11</v>
@@ -7762,16 +7790,16 @@
         <v>94</v>
       </c>
       <c r="F118" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G118" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="H118" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I118" s="8" t="s">
         <v>278</v>
-      </c>
-      <c r="G118" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="H118" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I118" s="8" t="s">
-        <v>275</v>
       </c>
       <c r="J118" s="6"/>
       <c r="K118" s="6"/>
@@ -7795,13 +7823,13 @@
     </row>
     <row r="119" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>158</v>
+        <v>275</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>11</v>
@@ -7813,13 +7841,13 @@
         <v>94</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>321</v>
+        <v>340</v>
       </c>
       <c r="H119" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I119" s="8" t="s">
-        <v>159</v>
+        <v>276</v>
       </c>
       <c r="J119" s="6"/>
       <c r="K119" s="6"/>
@@ -7841,15 +7869,15 @@
       <c r="AA119" s="2"/>
       <c r="AB119" s="2"/>
     </row>
-    <row r="120" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
-      <c r="A120" s="11" t="s">
-        <v>186</v>
+    <row r="120" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>273</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>11</v>
@@ -7861,16 +7889,16 @@
         <v>94</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>209</v>
+        <v>341</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I120" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J120" s="9"/>
-      <c r="K120" s="9"/>
+        <v>274</v>
+      </c>
+      <c r="J120" s="6"/>
+      <c r="K120" s="6"/>
       <c r="L120" s="9"/>
       <c r="M120" s="9"/>
       <c r="N120" s="9"/>
@@ -7889,15 +7917,15 @@
       <c r="AA120" s="2"/>
       <c r="AB120" s="2"/>
     </row>
-    <row r="121" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A121" s="11" t="s">
-        <v>188</v>
+    <row r="121" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>343</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>11</v>
@@ -7909,20 +7937,16 @@
         <v>94</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>209</v>
+        <v>344</v>
       </c>
       <c r="H121" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="I121" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="J121" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K121" s="20" t="s">
-        <v>202</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="I121" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="J121" s="6"/>
+      <c r="K121" s="6"/>
       <c r="L121" s="9"/>
       <c r="M121" s="9"/>
       <c r="N121" s="9"/>
@@ -7941,15 +7965,15 @@
       <c r="AA121" s="2"/>
       <c r="AB121" s="2"/>
     </row>
-    <row r="122" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
-      <c r="A122" s="11" t="s">
-        <v>189</v>
+    <row r="122" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>11</v>
@@ -7961,29 +7985,19 @@
         <v>94</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>209</v>
+        <v>342</v>
       </c>
       <c r="H122" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="I122" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="J122" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="K122" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="L122" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="M122" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="N122" s="20" t="s">
-        <v>207</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="I122" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="J122" s="6"/>
+      <c r="K122" s="6"/>
+      <c r="L122" s="9"/>
+      <c r="M122" s="9"/>
+      <c r="N122" s="9"/>
       <c r="O122" s="2"/>
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
@@ -7999,17 +8013,17 @@
       <c r="AA122" s="2"/>
       <c r="AB122" s="2"/>
     </row>
-    <row r="123" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="23" t="s">
-        <v>233</v>
+    <row r="123" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A123" s="11" t="s">
+        <v>185</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D123" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="D123" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E123" s="7" t="s">
@@ -8019,20 +8033,16 @@
         <v>94</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="H123" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="I123" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="J123" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="K123" s="20" t="s">
-        <v>236</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="H123" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I123" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="J123" s="9"/>
+      <c r="K123" s="9"/>
       <c r="L123" s="9"/>
       <c r="M123" s="9"/>
       <c r="N123" s="9"/>
@@ -8051,15 +8061,15 @@
       <c r="AA123" s="2"/>
       <c r="AB123" s="2"/>
     </row>
-    <row r="124" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>242</v>
+        <v>186</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>11</v>
@@ -8071,16 +8081,20 @@
         <v>94</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H124" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I124" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="J124" s="20"/>
-      <c r="K124" s="20"/>
+        <v>199</v>
+      </c>
+      <c r="J124" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="K124" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="L124" s="9"/>
       <c r="M124" s="9"/>
       <c r="N124" s="9"/>
@@ -8099,15 +8113,15 @@
       <c r="AA124" s="2"/>
       <c r="AB124" s="2"/>
     </row>
-    <row r="125" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
-        <v>243</v>
+        <v>188</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>11</v>
@@ -8119,23 +8133,29 @@
         <v>94</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H125" s="8" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="I125" s="22" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="J125" s="20" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="K125" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="L125" s="20"/>
-      <c r="M125" s="20"/>
-      <c r="N125" s="20"/>
+        <v>200</v>
+      </c>
+      <c r="L125" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="M125" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="N125" s="20" t="s">
+        <v>206</v>
+      </c>
       <c r="O125" s="2"/>
       <c r="P125" s="2"/>
       <c r="Q125" s="2"/>
@@ -8151,18 +8171,18 @@
       <c r="AA125" s="2"/>
       <c r="AB125" s="2"/>
     </row>
-    <row r="126" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
-        <v>241</v>
+    <row r="126" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="23" t="s">
+        <v>232</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D126" s="6" t="s">
-        <v>14</v>
+        <v>186</v>
+      </c>
+      <c r="D126" s="24" t="s">
+        <v>11</v>
       </c>
       <c r="E126" s="7" t="s">
         <v>94</v>
@@ -8171,14 +8191,20 @@
         <v>94</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H126" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="I126" s="9"/>
-      <c r="J126" s="9"/>
-      <c r="K126" s="9"/>
+        <v>208</v>
+      </c>
+      <c r="H126" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="I126" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="J126" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="K126" s="20" t="s">
+        <v>235</v>
+      </c>
       <c r="L126" s="9"/>
       <c r="M126" s="9"/>
       <c r="N126" s="9"/>
@@ -8197,8 +8223,154 @@
       <c r="AA126" s="2"/>
       <c r="AB126" s="2"/>
     </row>
+    <row r="127" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E127" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F127" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G127" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="H127" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I127" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="J127" s="20"/>
+      <c r="K127" s="20"/>
+      <c r="L127" s="9"/>
+      <c r="M127" s="9"/>
+      <c r="N127" s="9"/>
+      <c r="O127" s="2"/>
+      <c r="P127" s="2"/>
+      <c r="Q127" s="2"/>
+      <c r="R127" s="2"/>
+      <c r="S127" s="2"/>
+      <c r="T127" s="2"/>
+      <c r="U127" s="2"/>
+      <c r="V127" s="2"/>
+      <c r="W127" s="2"/>
+      <c r="X127" s="2"/>
+      <c r="Y127" s="2"/>
+      <c r="Z127" s="2"/>
+      <c r="AA127" s="2"/>
+      <c r="AB127" s="2"/>
+    </row>
+    <row r="128" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A128" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D128" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E128" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F128" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G128" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="H128" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I128" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="J128" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="K128" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="L128" s="20"/>
+      <c r="M128" s="20"/>
+      <c r="N128" s="20"/>
+      <c r="O128" s="2"/>
+      <c r="P128" s="2"/>
+      <c r="Q128" s="2"/>
+      <c r="R128" s="2"/>
+      <c r="S128" s="2"/>
+      <c r="T128" s="2"/>
+      <c r="U128" s="2"/>
+      <c r="V128" s="2"/>
+      <c r="W128" s="2"/>
+      <c r="X128" s="2"/>
+      <c r="Y128" s="2"/>
+      <c r="Z128" s="2"/>
+      <c r="AA128" s="2"/>
+      <c r="AB128" s="2"/>
+    </row>
+    <row r="129" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E129" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F129" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G129" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H129" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="I129" s="9"/>
+      <c r="J129" s="9"/>
+      <c r="K129" s="9"/>
+      <c r="L129" s="9"/>
+      <c r="M129" s="9"/>
+      <c r="N129" s="9"/>
+      <c r="O129" s="2"/>
+      <c r="P129" s="2"/>
+      <c r="Q129" s="2"/>
+      <c r="R129" s="2"/>
+      <c r="S129" s="2"/>
+      <c r="T129" s="2"/>
+      <c r="U129" s="2"/>
+      <c r="V129" s="2"/>
+      <c r="W129" s="2"/>
+      <c r="X129" s="2"/>
+      <c r="Y129" s="2"/>
+      <c r="Z129" s="2"/>
+      <c r="AA129" s="2"/>
+      <c r="AB129" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I126" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I129" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
modifications done in create coyni employee Test case
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Admin_Automation_new_09_03_2023\Admin_17_03_2023\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705C1BB3-A58C-4624-AF42-B30D0F04BB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87138BFF-5508-444F-9D44-A786C5F30D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1876,18 +1876,6 @@
     <t>testdata-admin.xlsx,coyniEmployee</t>
   </si>
   <si>
-    <t>coyni.admin.tests.ProfilesTest,
-testCreateCoyniEmployee,
--pprofileHeading,
--pfirstname,
--plastname,
--pphoneNumber,
--pheading,
--pverificationCode,
--pcreatePassword,
--pconfirmPassword</t>
-  </si>
-  <si>
     <t>Profile - Coyni Employee</t>
   </si>
   <si>
@@ -2011,6 +1999,22 @@
 -perrMessage,
 -pcolour,
 -potpColor</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.ProfilesTest,
+testCreateCoyniEmployee,
+-pprofileHeading,
+-pfirstname,
+-plastname,
+-pphoneNumber,
+-pheading,
+-pverificationCode,
+-pcreatePassword,
+-pconfirmPassword,
+-pDepartment,
+-ppermissionRole,
+-pfilter1,
+-pfilter2</t>
   </si>
 </sst>
 </file>
@@ -2469,29 +2473,29 @@
   <dimension ref="A1:AB131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
-    <col min="9" max="9" width="43.140625" customWidth="1"/>
-    <col min="10" max="10" width="38.85546875" customWidth="1"/>
-    <col min="11" max="11" width="30.28515625" customWidth="1"/>
+    <col min="8" max="8" width="47.44140625" customWidth="1"/>
+    <col min="9" max="9" width="43.109375" customWidth="1"/>
+    <col min="10" max="10" width="38.88671875" customWidth="1"/>
+    <col min="11" max="11" width="30.33203125" customWidth="1"/>
     <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" customWidth="1"/>
-    <col min="14" max="14" width="25.5703125" customWidth="1"/>
+    <col min="13" max="13" width="26.44140625" customWidth="1"/>
+    <col min="14" max="14" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2525,7 +2529,7 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2571,9 +2575,9 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>249</v>
@@ -2594,7 +2598,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -2617,7 +2621,7 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>247</v>
       </c>
@@ -2640,7 +2644,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I4" s="32"/>
       <c r="J4" s="9"/>
@@ -2663,7 +2667,7 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -2709,7 +2713,7 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
@@ -2755,7 +2759,7 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>138</v>
       </c>
@@ -2801,7 +2805,7 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="240" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -2847,7 +2851,7 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="210.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="202.8" x14ac:dyDescent="0.4">
       <c r="A9" s="12" t="s">
         <v>26</v>
       </c>
@@ -2893,12 +2897,12 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="210" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>24</v>
@@ -2910,7 +2914,7 @@
         <v>94</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>25</v>
@@ -2939,9 +2943,9 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="180" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>249</v>
@@ -2962,7 +2966,7 @@
         <v>25</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -2985,7 +2989,7 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -3031,7 +3035,7 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="255" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -3077,7 +3081,7 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="225" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="216" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -3123,7 +3127,7 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="210" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -3169,9 +3173,9 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="240" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>249</v>
@@ -3192,7 +3196,7 @@
         <v>33</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -3215,7 +3219,7 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
-    <row r="17" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -3261,7 +3265,7 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:28" ht="195" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -3307,7 +3311,7 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>241</v>
       </c>
@@ -3355,7 +3359,7 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
     </row>
-    <row r="20" spans="1:28" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>127</v>
       </c>
@@ -3403,7 +3407,7 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
     </row>
-    <row r="21" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>128</v>
       </c>
@@ -3451,7 +3455,7 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
@@ -3499,7 +3503,7 @@
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
     </row>
-    <row r="23" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>147</v>
       </c>
@@ -3547,7 +3551,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
     </row>
-    <row r="24" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
@@ -3595,7 +3599,7 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
     </row>
-    <row r="25" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
@@ -3643,7 +3647,7 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
     </row>
-    <row r="26" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
@@ -3691,9 +3695,9 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A27" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>249</v>
@@ -3717,7 +3721,7 @@
         <v>209</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -3739,12 +3743,12 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>18</v>
@@ -3765,7 +3769,7 @@
         <v>209</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -3787,7 +3791,7 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:28" ht="270" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>225</v>
       </c>
@@ -3835,7 +3839,7 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
     </row>
-    <row r="30" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>226</v>
       </c>
@@ -3883,7 +3887,7 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>227</v>
       </c>
@@ -3931,7 +3935,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:28" ht="285" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>228</v>
       </c>
@@ -3979,7 +3983,7 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" s="2" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>143</v>
       </c>
@@ -4013,7 +4017,7 @@
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
     </row>
-    <row r="34" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
@@ -4061,7 +4065,7 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>325</v>
       </c>
@@ -4109,7 +4113,7 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>323</v>
       </c>
@@ -4157,7 +4161,7 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>97</v>
       </c>
@@ -4205,7 +4209,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>99</v>
       </c>
@@ -4253,7 +4257,7 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>101</v>
       </c>
@@ -4301,7 +4305,7 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>103</v>
       </c>
@@ -4349,7 +4353,7 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>105</v>
       </c>
@@ -4397,7 +4401,7 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>328</v>
       </c>
@@ -4445,7 +4449,7 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
@@ -4493,7 +4497,7 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>167</v>
       </c>
@@ -4541,7 +4545,7 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
@@ -4589,7 +4593,7 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>48</v>
       </c>
@@ -4637,7 +4641,7 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
@@ -4685,7 +4689,7 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>52</v>
       </c>
@@ -4733,7 +4737,7 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
@@ -4781,7 +4785,7 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
@@ -4829,7 +4833,7 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>58</v>
       </c>
@@ -4877,7 +4881,7 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>60</v>
       </c>
@@ -4925,7 +4929,7 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>62</v>
       </c>
@@ -4973,7 +4977,7 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>64</v>
       </c>
@@ -5021,7 +5025,7 @@
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
     </row>
-    <row r="55" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>66</v>
       </c>
@@ -5069,7 +5073,7 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>68</v>
       </c>
@@ -5117,7 +5121,7 @@
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>133</v>
       </c>
@@ -5165,7 +5169,7 @@
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
     </row>
-    <row r="58" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>70</v>
       </c>
@@ -5213,7 +5217,7 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>141</v>
       </c>
@@ -5261,7 +5265,7 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>145</v>
       </c>
@@ -5309,7 +5313,7 @@
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" s="2" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>117</v>
       </c>
@@ -5343,7 +5347,7 @@
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
     </row>
-    <row r="62" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>119</v>
       </c>
@@ -5391,7 +5395,7 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>120</v>
       </c>
@@ -5439,12 +5443,12 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" ht="214.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>329</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>330</v>
@@ -5459,13 +5463,13 @@
         <v>1</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H64" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -5487,7 +5491,7 @@
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
     </row>
-    <row r="65" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>122</v>
       </c>
@@ -5535,7 +5539,7 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>125</v>
       </c>
@@ -5583,7 +5587,7 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>176</v>
       </c>
@@ -5631,7 +5635,7 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>177</v>
       </c>
@@ -5679,7 +5683,7 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>175</v>
       </c>
@@ -5727,7 +5731,7 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A70" s="25" t="s">
         <v>179</v>
       </c>
@@ -5775,7 +5779,7 @@
       <c r="AA70" s="2"/>
       <c r="AB70" s="2"/>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>180</v>
       </c>
@@ -5823,7 +5827,7 @@
       <c r="AA71" s="2"/>
       <c r="AB71" s="2"/>
     </row>
-    <row r="72" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>181</v>
       </c>
@@ -5871,7 +5875,7 @@
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
     </row>
-    <row r="73" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>182</v>
       </c>
@@ -5919,7 +5923,7 @@
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
     </row>
-    <row r="74" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>183</v>
       </c>
@@ -5967,7 +5971,7 @@
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
     </row>
-    <row r="75" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>178</v>
       </c>
@@ -6015,7 +6019,7 @@
       <c r="AA75" s="2"/>
       <c r="AB75" s="2"/>
     </row>
-    <row r="76" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A76" s="26" t="s">
         <v>248</v>
       </c>
@@ -6044,7 +6048,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>251</v>
       </c>
@@ -6073,7 +6077,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>254</v>
       </c>
@@ -6102,7 +6106,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>261</v>
       </c>
@@ -6131,7 +6135,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>258</v>
       </c>
@@ -6160,7 +6164,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>260</v>
       </c>
@@ -6189,7 +6193,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>263</v>
       </c>
@@ -6218,7 +6222,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>265</v>
       </c>
@@ -6247,7 +6251,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>267</v>
       </c>
@@ -6276,7 +6280,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>269</v>
       </c>
@@ -6305,7 +6309,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>277</v>
       </c>
@@ -6334,7 +6338,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>135</v>
       </c>
@@ -6382,7 +6386,7 @@
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>161</v>
       </c>
@@ -6430,7 +6434,7 @@
       <c r="AA88" s="2"/>
       <c r="AB88" s="2"/>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>163</v>
       </c>
@@ -6478,7 +6482,7 @@
       <c r="AA89" s="2"/>
       <c r="AB89" s="2"/>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>165</v>
       </c>
@@ -6528,7 +6532,7 @@
       <c r="AA90" s="2"/>
       <c r="AB90" s="2"/>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>81</v>
       </c>
@@ -6576,7 +6580,7 @@
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
     </row>
-    <row r="92" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>84</v>
       </c>
@@ -6624,7 +6628,7 @@
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
     </row>
-    <row r="93" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>86</v>
       </c>
@@ -6672,7 +6676,7 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>88</v>
       </c>
@@ -6720,7 +6724,7 @@
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
     </row>
-    <row r="95" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>90</v>
       </c>
@@ -6768,7 +6772,7 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A96" s="27" t="s">
         <v>280</v>
       </c>
@@ -6816,7 +6820,7 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>92</v>
       </c>
@@ -6864,7 +6868,7 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>213</v>
       </c>
@@ -6912,7 +6916,7 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>217</v>
       </c>
@@ -6960,7 +6964,7 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>219</v>
       </c>
@@ -7008,7 +7012,7 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>159</v>
       </c>
@@ -7056,7 +7060,7 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>113</v>
       </c>
@@ -7104,7 +7108,7 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>79</v>
       </c>
@@ -7152,7 +7156,7 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>72</v>
       </c>
@@ -7200,7 +7204,7 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>282</v>
       </c>
@@ -7220,7 +7224,7 @@
         <v>94</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H105" s="8" t="s">
         <v>209</v>
@@ -7248,7 +7252,7 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>285</v>
       </c>
@@ -7268,7 +7272,7 @@
         <v>94</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H106" s="8" t="s">
         <v>209</v>
@@ -7296,7 +7300,7 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>287</v>
       </c>
@@ -7316,7 +7320,7 @@
         <v>94</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H107" s="8" t="s">
         <v>209</v>
@@ -7344,7 +7348,7 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>75</v>
       </c>
@@ -7392,7 +7396,7 @@
       <c r="AA108" s="2"/>
       <c r="AB108" s="2"/>
     </row>
-    <row r="109" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>76</v>
       </c>
@@ -7440,7 +7444,7 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>108</v>
       </c>
@@ -7488,7 +7492,7 @@
       <c r="AA110" s="2"/>
       <c r="AB110" s="2"/>
     </row>
-    <row r="111" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>293</v>
       </c>
@@ -7536,7 +7540,7 @@
       <c r="AA111" s="2"/>
       <c r="AB111" s="2"/>
     </row>
-    <row r="112" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>298</v>
       </c>
@@ -7584,7 +7588,7 @@
       <c r="AA112" s="2"/>
       <c r="AB112" s="2"/>
     </row>
-    <row r="113" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>300</v>
       </c>
@@ -7632,7 +7636,7 @@
       <c r="AA113" s="2"/>
       <c r="AB113" s="2"/>
     </row>
-    <row r="114" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A114" s="21" t="s">
         <v>169</v>
       </c>
@@ -7680,7 +7684,7 @@
       <c r="AA114" s="2"/>
       <c r="AB114" s="2"/>
     </row>
-    <row r="115" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="11" t="s">
         <v>110</v>
       </c>
@@ -7728,7 +7732,7 @@
       <c r="AA115" s="2"/>
       <c r="AB115" s="2"/>
     </row>
-    <row r="116" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:28" s="1" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="21" t="s">
         <v>171</v>
       </c>
@@ -7776,7 +7780,7 @@
       <c r="AA116" s="2"/>
       <c r="AB116" s="2"/>
     </row>
-    <row r="117" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="11" t="s">
         <v>109</v>
       </c>
@@ -7824,7 +7828,7 @@
       <c r="AA117" s="2"/>
       <c r="AB117" s="2"/>
     </row>
-    <row r="118" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>151</v>
       </c>
@@ -7844,7 +7848,7 @@
         <v>94</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H118" s="8" t="s">
         <v>209</v>
@@ -7872,7 +7876,7 @@
       <c r="AA118" s="2"/>
       <c r="AB118" s="2"/>
     </row>
-    <row r="119" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>154</v>
       </c>
@@ -7892,7 +7896,7 @@
         <v>94</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H119" s="8" t="s">
         <v>209</v>
@@ -7920,7 +7924,7 @@
       <c r="AA119" s="2"/>
       <c r="AB119" s="2"/>
     </row>
-    <row r="120" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>275</v>
       </c>
@@ -7940,7 +7944,7 @@
         <v>94</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H120" s="8" t="s">
         <v>209</v>
@@ -7968,7 +7972,7 @@
       <c r="AA120" s="2"/>
       <c r="AB120" s="2"/>
     </row>
-    <row r="121" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>273</v>
       </c>
@@ -7988,7 +7992,7 @@
         <v>94</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H121" s="8" t="s">
         <v>209</v>
@@ -8016,7 +8020,7 @@
       <c r="AA121" s="2"/>
       <c r="AB121" s="2"/>
     </row>
-    <row r="122" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>271</v>
       </c>
@@ -8036,7 +8040,7 @@
         <v>94</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H122" s="8" t="s">
         <v>209</v>
@@ -8064,9 +8068,9 @@
       <c r="AA122" s="2"/>
       <c r="AB122" s="2"/>
     </row>
-    <row r="123" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>249</v>
@@ -8084,13 +8088,13 @@
         <v>94</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H123" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I123" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J123" s="6"/>
       <c r="K123" s="6"/>
@@ -8112,7 +8116,7 @@
       <c r="AA123" s="2"/>
       <c r="AB123" s="2"/>
     </row>
-    <row r="124" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>156</v>
       </c>
@@ -8132,7 +8136,7 @@
         <v>94</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H124" s="8" t="s">
         <v>209</v>
@@ -8160,7 +8164,7 @@
       <c r="AA124" s="2"/>
       <c r="AB124" s="2"/>
     </row>
-    <row r="125" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:28" s="1" customFormat="1" ht="288" x14ac:dyDescent="0.3">
       <c r="A125" s="11" t="s">
         <v>184</v>
       </c>
@@ -8208,7 +8212,7 @@
       <c r="AA125" s="2"/>
       <c r="AB125" s="2"/>
     </row>
-    <row r="126" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A126" s="11" t="s">
         <v>186</v>
       </c>
@@ -8260,7 +8264,7 @@
       <c r="AA126" s="2"/>
       <c r="AB126" s="2"/>
     </row>
-    <row r="127" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:28" s="1" customFormat="1" ht="288" x14ac:dyDescent="0.3">
       <c r="A127" s="11" t="s">
         <v>187</v>
       </c>
@@ -8318,7 +8322,7 @@
       <c r="AA127" s="2"/>
       <c r="AB127" s="2"/>
     </row>
-    <row r="128" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="23" t="s">
         <v>231</v>
       </c>
@@ -8370,7 +8374,7 @@
       <c r="AA128" s="2"/>
       <c r="AB128" s="2"/>
     </row>
-    <row r="129" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="11" t="s">
         <v>233</v>
       </c>
@@ -8418,7 +8422,7 @@
       <c r="AA129" s="2"/>
       <c r="AB129" s="2"/>
     </row>
-    <row r="130" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A130" s="11" t="s">
         <v>240</v>
       </c>
@@ -8470,7 +8474,7 @@
       <c r="AA130" s="2"/>
       <c r="AB130" s="2"/>
     </row>
-    <row r="131" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>238</v>
       </c>

</xml_diff>

<commit_message>
Added DB validation in Disputes Test
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(17-03-2023)Coyni portal\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DD3AD5-D2F8-4E53-84F1-A21211138618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFDAA80-EF0B-4E54-AA4D-3D7A2E928842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$132</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="357">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2015,6 +2015,16 @@
 -ppermissionRole,
 -pfilter1,
 -pfilter2</t>
+  </si>
+  <si>
+    <t>Verify Disputes Pending count</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.DisputesTest,
+verifyDisputesTransactionsCountWithDB,
+-pquery,
+-pquery2,
+-pquery3</t>
   </si>
 </sst>
 </file>
@@ -2133,7 +2143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2190,6 +2200,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2471,11 +2482,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB131"/>
+  <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3984,7 +3995,7 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>143</v>
       </c>
@@ -4018,7 +4029,7 @@
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
     </row>
-    <row r="34" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
@@ -4066,7 +4077,7 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>325</v>
       </c>
@@ -4119,7 +4130,7 @@
         <v>323</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>18</v>
@@ -4162,7 +4173,7 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>97</v>
       </c>
@@ -4210,7 +4221,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>99</v>
       </c>
@@ -4258,7 +4269,7 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>101</v>
       </c>
@@ -4306,7 +4317,7 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>103</v>
       </c>
@@ -4354,7 +4365,7 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>105</v>
       </c>
@@ -4402,7 +4413,7 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>328</v>
       </c>
@@ -6533,15 +6544,15 @@
       <c r="AA90" s="2"/>
       <c r="AB90" s="2"/>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>81</v>
+        <v>355</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>11</v>
@@ -6553,17 +6564,17 @@
         <v>94</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>308</v>
+        <v>160</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I91" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="J91" s="6"/>
-      <c r="K91" s="6"/>
-      <c r="L91" s="6"/>
+        <v>209</v>
+      </c>
+      <c r="I91" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="J91" s="34"/>
+      <c r="K91" s="9"/>
+      <c r="L91" s="9"/>
       <c r="M91" s="9"/>
       <c r="N91" s="9"/>
       <c r="O91" s="2"/>
@@ -6583,7 +6594,7 @@
     </row>
     <row r="92" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>249</v>
@@ -6607,7 +6618,7 @@
         <v>210</v>
       </c>
       <c r="I92" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J92" s="6"/>
       <c r="K92" s="6"/>
@@ -6631,7 +6642,7 @@
     </row>
     <row r="93" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>249</v>
@@ -6655,7 +6666,7 @@
         <v>210</v>
       </c>
       <c r="I93" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J93" s="6"/>
       <c r="K93" s="6"/>
@@ -6679,7 +6690,7 @@
     </row>
     <row r="94" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>249</v>
@@ -6703,7 +6714,7 @@
         <v>210</v>
       </c>
       <c r="I94" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J94" s="6"/>
       <c r="K94" s="6"/>
@@ -6727,7 +6738,7 @@
     </row>
     <row r="95" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>249</v>
@@ -6745,13 +6756,13 @@
         <v>94</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H95" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J95" s="6"/>
       <c r="K95" s="6"/>
@@ -6774,8 +6785,8 @@
       <c r="AB95" s="2"/>
     </row>
     <row r="96" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="27" t="s">
-        <v>280</v>
+      <c r="A96" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>249</v>
@@ -6799,7 +6810,7 @@
         <v>210</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>281</v>
+        <v>91</v>
       </c>
       <c r="J96" s="6"/>
       <c r="K96" s="6"/>
@@ -6822,8 +6833,8 @@
       <c r="AB96" s="2"/>
     </row>
     <row r="97" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
-        <v>92</v>
+      <c r="A97" s="27" t="s">
+        <v>280</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>249</v>
@@ -6847,7 +6858,7 @@
         <v>210</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>93</v>
+        <v>281</v>
       </c>
       <c r="J97" s="6"/>
       <c r="K97" s="6"/>
@@ -6869,17 +6880,17 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>213</v>
+    <row r="98" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C98" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="D98" s="9" t="s">
+      <c r="C98" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D98" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E98" s="7" t="s">
@@ -6888,18 +6899,18 @@
       <c r="F98" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G98" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="H98" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="I98" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="J98" s="9"/>
-      <c r="K98" s="9"/>
-      <c r="L98" s="9"/>
+      <c r="G98" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="H98" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I98" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="6"/>
       <c r="M98" s="9"/>
       <c r="N98" s="9"/>
       <c r="O98" s="2"/>
@@ -6917,9 +6928,9 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>249</v>
@@ -6943,7 +6954,7 @@
         <v>209</v>
       </c>
       <c r="I99" s="20" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -6965,9 +6976,9 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>249</v>
@@ -6991,7 +7002,7 @@
         <v>209</v>
       </c>
       <c r="I100" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
@@ -7013,17 +7024,17 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>159</v>
+        <v>219</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C101" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D101" s="6" t="s">
+      <c r="C101" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D101" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E101" s="7" t="s">
@@ -7032,14 +7043,14 @@
       <c r="F101" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G101" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="H101" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I101" s="8" t="s">
-        <v>158</v>
+      <c r="G101" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="H101" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="I101" s="20" t="s">
+        <v>220</v>
       </c>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
@@ -7063,7 +7074,7 @@
     </row>
     <row r="102" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>249</v>
@@ -7087,7 +7098,7 @@
         <v>210</v>
       </c>
       <c r="I102" s="8" t="s">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
@@ -7110,8 +7121,8 @@
       <c r="AB102" s="2"/>
     </row>
     <row r="103" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
-        <v>79</v>
+      <c r="A103" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>249</v>
@@ -7120,13 +7131,13 @@
         <v>77</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="G103" s="6" t="s">
         <v>322</v>
@@ -7135,7 +7146,7 @@
         <v>210</v>
       </c>
       <c r="I103" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
@@ -7157,33 +7168,33 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>283</v>
+        <v>322</v>
       </c>
       <c r="H104" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I104" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="J104" s="9"/>
       <c r="K104" s="9"/>
@@ -7205,9 +7216,9 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>282</v>
+        <v>72</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>249</v>
@@ -7225,13 +7236,13 @@
         <v>94</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>347</v>
+        <v>283</v>
       </c>
       <c r="H105" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I105" s="22" t="s">
-        <v>284</v>
+        <v>210</v>
+      </c>
+      <c r="I105" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="J105" s="9"/>
       <c r="K105" s="9"/>
@@ -7255,7 +7266,7 @@
     </row>
     <row r="106" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>249</v>
@@ -7279,7 +7290,7 @@
         <v>209</v>
       </c>
       <c r="I106" s="22" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
@@ -7303,7 +7314,7 @@
     </row>
     <row r="107" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>249</v>
@@ -7327,7 +7338,7 @@
         <v>209</v>
       </c>
       <c r="I107" s="22" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
@@ -7349,14 +7360,14 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>75</v>
+        <v>287</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C108" s="18" t="s">
+      <c r="C108" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D108" s="6" t="s">
@@ -7369,13 +7380,13 @@
         <v>94</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>283</v>
+        <v>347</v>
       </c>
       <c r="H108" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I108" s="8" t="s">
-        <v>289</v>
+        <v>209</v>
+      </c>
+      <c r="I108" s="22" t="s">
+        <v>288</v>
       </c>
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
@@ -7399,12 +7410,12 @@
     </row>
     <row r="109" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C109" s="6" t="s">
+      <c r="C109" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D109" s="6" t="s">
@@ -7423,7 +7434,7 @@
         <v>210</v>
       </c>
       <c r="I109" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
@@ -7445,15 +7456,15 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>11</v>
@@ -7465,13 +7476,13 @@
         <v>94</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="H110" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I110" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
@@ -7495,7 +7506,7 @@
     </row>
     <row r="111" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>293</v>
+        <v>108</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>249</v>
@@ -7519,7 +7530,7 @@
         <v>210</v>
       </c>
       <c r="I111" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J111" s="9"/>
       <c r="K111" s="9"/>
@@ -7542,14 +7553,14 @@
       <c r="AB111" s="2"/>
     </row>
     <row r="112" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>298</v>
+      <c r="A112" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>295</v>
+        <v>114</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>11</v>
@@ -7561,13 +7572,13 @@
         <v>94</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="H112" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I112" s="8" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="J112" s="9"/>
       <c r="K112" s="9"/>
@@ -7591,7 +7602,7 @@
     </row>
     <row r="113" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>249</v>
@@ -7615,7 +7626,7 @@
         <v>210</v>
       </c>
       <c r="I113" s="8" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="J113" s="9"/>
       <c r="K113" s="9"/>
@@ -7637,17 +7648,17 @@
       <c r="AA113" s="2"/>
       <c r="AB113" s="2"/>
     </row>
-    <row r="114" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="21" t="s">
-        <v>169</v>
+    <row r="114" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>300</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C114" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D114" s="18" t="s">
+      <c r="C114" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D114" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E114" s="7" t="s">
@@ -7656,14 +7667,14 @@
       <c r="F114" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G114" s="18" t="s">
-        <v>310</v>
+      <c r="G114" s="6" t="s">
+        <v>296</v>
       </c>
       <c r="H114" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I114" s="8" t="s">
-        <v>170</v>
+        <v>297</v>
       </c>
       <c r="J114" s="9"/>
       <c r="K114" s="9"/>
@@ -7685,17 +7696,17 @@
       <c r="AA114" s="2"/>
       <c r="AB114" s="2"/>
     </row>
-    <row r="115" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="11" t="s">
-        <v>110</v>
+    <row r="115" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="21" t="s">
+        <v>169</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C115" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D115" s="6" t="s">
+      <c r="C115" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D115" s="18" t="s">
         <v>11</v>
       </c>
       <c r="E115" s="7" t="s">
@@ -7704,14 +7715,14 @@
       <c r="F115" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G115" s="6" t="s">
-        <v>291</v>
+      <c r="G115" s="18" t="s">
+        <v>310</v>
       </c>
       <c r="H115" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I115" s="8" t="s">
-        <v>115</v>
+        <v>170</v>
       </c>
       <c r="J115" s="9"/>
       <c r="K115" s="9"/>
@@ -7733,15 +7744,15 @@
       <c r="AA115" s="2"/>
       <c r="AB115" s="2"/>
     </row>
-    <row r="116" spans="1:28" s="1" customFormat="1" ht="141.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="21" t="s">
-        <v>171</v>
+    <row r="116" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C116" s="18" t="s">
-        <v>73</v>
+      <c r="C116" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>11</v>
@@ -7753,13 +7764,13 @@
         <v>94</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>173</v>
+        <v>291</v>
       </c>
       <c r="H116" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I116" s="8" t="s">
-        <v>172</v>
+        <v>115</v>
       </c>
       <c r="J116" s="9"/>
       <c r="K116" s="9"/>
@@ -7781,15 +7792,15 @@
       <c r="AA116" s="2"/>
       <c r="AB116" s="2"/>
     </row>
-    <row r="117" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="11" t="s">
-        <v>109</v>
+    <row r="117" spans="1:28" s="1" customFormat="1" ht="141.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="21" t="s">
+        <v>171</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C117" s="6" t="s">
-        <v>114</v>
+      <c r="C117" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>11</v>
@@ -7801,13 +7812,13 @@
         <v>94</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>291</v>
+        <v>173</v>
       </c>
       <c r="H117" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I117" s="8" t="s">
-        <v>116</v>
+        <v>172</v>
       </c>
       <c r="J117" s="9"/>
       <c r="K117" s="9"/>
@@ -7829,15 +7840,15 @@
       <c r="AA117" s="2"/>
       <c r="AB117" s="2"/>
     </row>
-    <row r="118" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
-        <v>151</v>
+    <row r="118" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>11</v>
@@ -7849,16 +7860,16 @@
         <v>94</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>334</v>
+        <v>291</v>
       </c>
       <c r="H118" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I118" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J118" s="6"/>
-      <c r="K118" s="6"/>
+        <v>116</v>
+      </c>
+      <c r="J118" s="9"/>
+      <c r="K118" s="9"/>
       <c r="L118" s="9"/>
       <c r="M118" s="9"/>
       <c r="N118" s="9"/>
@@ -7879,7 +7890,7 @@
     </row>
     <row r="119" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>249</v>
@@ -7897,13 +7908,13 @@
         <v>94</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H119" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I119" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J119" s="6"/>
       <c r="K119" s="6"/>
@@ -7927,7 +7938,7 @@
     </row>
     <row r="120" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>275</v>
+        <v>154</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>249</v>
@@ -7945,13 +7956,13 @@
         <v>94</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H120" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I120" s="8" t="s">
-        <v>276</v>
+        <v>155</v>
       </c>
       <c r="J120" s="6"/>
       <c r="K120" s="6"/>
@@ -7975,7 +7986,7 @@
     </row>
     <row r="121" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>249</v>
@@ -7993,13 +8004,13 @@
         <v>94</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H121" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I121" s="8" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="J121" s="6"/>
       <c r="K121" s="6"/>
@@ -8023,7 +8034,7 @@
     </row>
     <row r="122" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>249</v>
@@ -8041,13 +8052,13 @@
         <v>94</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H122" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I122" s="8" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="J122" s="6"/>
       <c r="K122" s="6"/>
@@ -8071,7 +8082,7 @@
     </row>
     <row r="123" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>340</v>
+        <v>271</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>249</v>
@@ -8089,13 +8100,13 @@
         <v>94</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="H123" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I123" s="8" t="s">
-        <v>342</v>
+        <v>272</v>
       </c>
       <c r="J123" s="6"/>
       <c r="K123" s="6"/>
@@ -8119,7 +8130,7 @@
     </row>
     <row r="124" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>156</v>
+        <v>340</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>249</v>
@@ -8137,13 +8148,13 @@
         <v>94</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="H124" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I124" s="8" t="s">
-        <v>157</v>
+        <v>342</v>
       </c>
       <c r="J124" s="6"/>
       <c r="K124" s="6"/>
@@ -8165,15 +8176,15 @@
       <c r="AA124" s="2"/>
       <c r="AB124" s="2"/>
     </row>
-    <row r="125" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="11" t="s">
-        <v>184</v>
+    <row r="125" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>11</v>
@@ -8185,16 +8196,16 @@
         <v>94</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>207</v>
+        <v>339</v>
       </c>
       <c r="H125" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I125" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="J125" s="9"/>
-      <c r="K125" s="9"/>
+        <v>157</v>
+      </c>
+      <c r="J125" s="6"/>
+      <c r="K125" s="6"/>
       <c r="L125" s="9"/>
       <c r="M125" s="9"/>
       <c r="N125" s="9"/>
@@ -8213,9 +8224,9 @@
       <c r="AA125" s="2"/>
       <c r="AB125" s="2"/>
     </row>
-    <row r="126" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>249</v>
@@ -8238,15 +8249,11 @@
       <c r="H126" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="I126" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="J126" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="K126" s="20" t="s">
-        <v>200</v>
-      </c>
+      <c r="I126" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="J126" s="9"/>
+      <c r="K126" s="9"/>
       <c r="L126" s="9"/>
       <c r="M126" s="9"/>
       <c r="N126" s="9"/>
@@ -8265,9 +8272,9 @@
       <c r="AA126" s="2"/>
       <c r="AB126" s="2"/>
     </row>
-    <row r="127" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>249</v>
@@ -8288,26 +8295,20 @@
         <v>207</v>
       </c>
       <c r="H127" s="8" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="I127" s="22" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J127" s="20" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K127" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="L127" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="M127" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="N127" s="20" t="s">
-        <v>205</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="L127" s="9"/>
+      <c r="M127" s="9"/>
+      <c r="N127" s="9"/>
       <c r="O127" s="2"/>
       <c r="P127" s="2"/>
       <c r="Q127" s="2"/>
@@ -8323,9 +8324,9 @@
       <c r="AA127" s="2"/>
       <c r="AB127" s="2"/>
     </row>
-    <row r="128" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="23" t="s">
-        <v>231</v>
+    <row r="128" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="11" t="s">
+        <v>187</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>249</v>
@@ -8333,7 +8334,7 @@
       <c r="C128" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D128" s="24" t="s">
+      <c r="D128" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E128" s="7" t="s">
@@ -8345,21 +8346,27 @@
       <c r="G128" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="H128" s="20" t="s">
-        <v>209</v>
+      <c r="H128" s="8" t="s">
+        <v>197</v>
       </c>
       <c r="I128" s="22" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="J128" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="K128" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="K128" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="L128" s="9"/>
-      <c r="M128" s="9"/>
-      <c r="N128" s="9"/>
+      <c r="L128" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="M128" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="N128" s="20" t="s">
+        <v>205</v>
+      </c>
       <c r="O128" s="2"/>
       <c r="P128" s="2"/>
       <c r="Q128" s="2"/>
@@ -8375,17 +8382,17 @@
       <c r="AA128" s="2"/>
       <c r="AB128" s="2"/>
     </row>
-    <row r="129" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="11" t="s">
-        <v>233</v>
+    <row r="129" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="23" t="s">
+        <v>231</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="D129" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D129" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E129" s="7" t="s">
@@ -8397,14 +8404,18 @@
       <c r="G129" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="H129" s="8" t="s">
+      <c r="H129" s="20" t="s">
         <v>209</v>
       </c>
       <c r="I129" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="J129" s="20"/>
-      <c r="K129" s="20"/>
+        <v>232</v>
+      </c>
+      <c r="J129" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="K129" s="20" t="s">
+        <v>234</v>
+      </c>
       <c r="L129" s="9"/>
       <c r="M129" s="9"/>
       <c r="N129" s="9"/>
@@ -8423,15 +8434,15 @@
       <c r="AA129" s="2"/>
       <c r="AB129" s="2"/>
     </row>
-    <row r="130" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>185</v>
+        <v>239</v>
       </c>
       <c r="D130" s="6" t="s">
         <v>11</v>
@@ -8449,17 +8460,13 @@
         <v>209</v>
       </c>
       <c r="I130" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="J130" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="K130" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="L130" s="20"/>
-      <c r="M130" s="20"/>
-      <c r="N130" s="20"/>
+        <v>230</v>
+      </c>
+      <c r="J130" s="20"/>
+      <c r="K130" s="20"/>
+      <c r="L130" s="9"/>
+      <c r="M130" s="9"/>
+      <c r="N130" s="9"/>
       <c r="O130" s="2"/>
       <c r="P130" s="2"/>
       <c r="Q130" s="2"/>
@@ -8475,18 +8482,18 @@
       <c r="AA130" s="2"/>
       <c r="AB130" s="2"/>
     </row>
-    <row r="131" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
-        <v>238</v>
+    <row r="131" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>10</v>
+        <v>185</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E131" s="7" t="s">
         <v>94</v>
@@ -8495,17 +8502,23 @@
         <v>94</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>12</v>
+        <v>207</v>
       </c>
       <c r="H131" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="I131" s="9"/>
-      <c r="J131" s="9"/>
-      <c r="K131" s="9"/>
-      <c r="L131" s="9"/>
-      <c r="M131" s="9"/>
-      <c r="N131" s="9"/>
+        <v>209</v>
+      </c>
+      <c r="I131" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="J131" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="K131" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="L131" s="20"/>
+      <c r="M131" s="20"/>
+      <c r="N131" s="20"/>
       <c r="O131" s="2"/>
       <c r="P131" s="2"/>
       <c r="Q131" s="2"/>
@@ -8521,11 +8534,57 @@
       <c r="AA131" s="2"/>
       <c r="AB131" s="2"/>
     </row>
+    <row r="132" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E132" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F132" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G132" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H132" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="I132" s="9"/>
+      <c r="J132" s="9"/>
+      <c r="K132" s="9"/>
+      <c r="L132" s="9"/>
+      <c r="M132" s="9"/>
+      <c r="N132" s="9"/>
+      <c r="O132" s="2"/>
+      <c r="P132" s="2"/>
+      <c r="Q132" s="2"/>
+      <c r="R132" s="2"/>
+      <c r="S132" s="2"/>
+      <c r="T132" s="2"/>
+      <c r="U132" s="2"/>
+      <c r="V132" s="2"/>
+      <c r="W132" s="2"/>
+      <c r="X132" s="2"/>
+      <c r="Y132" s="2"/>
+      <c r="Z132" s="2"/>
+      <c r="AA132" s="2"/>
+      <c r="AB132" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I131" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
+  <autoFilter ref="A1:I132" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
       <filters>
-        <filter val="Coyni Portal - Commission Account"/>
+        <filter val="Yes"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
modified test method in Different tests
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(17-03-2023)Coyni portal\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(24-03-2023)Home\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFDAA80-EF0B-4E54-AA4D-3D7A2E928842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE895160-6AAD-4B07-A28E-BA4F7A2A8BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1646,12 +1646,6 @@
 </t>
   </si>
   <si>
-    <t>coyni.admin.tests.DisputesTest,
-VerifyFilter,
--pfilterHeadings,
--pstartDate</t>
-  </si>
-  <si>
     <t>testTotalDepositCogentAccount</t>
   </si>
   <si>
@@ -2025,6 +2019,11 @@
 -pquery,
 -pquery2,
 -pquery3</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.DisputesTest,
+VerifyFilter,
+-pfilterHeadings</t>
   </si>
 </sst>
 </file>
@@ -2143,7 +2142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2200,7 +2199,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2484,9 +2482,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I91" sqref="I91"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2589,7 +2587,7 @@
     </row>
     <row r="3" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>249</v>
@@ -2610,7 +2608,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -2656,7 +2654,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I4" s="32"/>
       <c r="J4" s="9"/>
@@ -2926,7 +2924,7 @@
         <v>94</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>25</v>
@@ -2957,7 +2955,7 @@
     </row>
     <row r="11" spans="1:28" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>249</v>
@@ -2978,7 +2976,7 @@
         <v>25</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -3187,7 +3185,7 @@
     </row>
     <row r="16" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>249</v>
@@ -3208,7 +3206,7 @@
         <v>33</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -3343,7 +3341,7 @@
         <v>94</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>211</v>
@@ -3391,7 +3389,7 @@
         <v>111</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>208</v>
@@ -3439,7 +3437,7 @@
         <v>112</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>208</v>
@@ -3583,7 +3581,7 @@
         <v>94</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>208</v>
@@ -3631,7 +3629,7 @@
         <v>94</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>208</v>
@@ -3679,7 +3677,7 @@
         <v>94</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>209</v>
@@ -3709,7 +3707,7 @@
     </row>
     <row r="27" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>249</v>
@@ -3727,13 +3725,13 @@
         <v>94</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -3757,7 +3755,7 @@
     </row>
     <row r="28" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>249</v>
@@ -3775,13 +3773,13 @@
         <v>94</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -3823,7 +3821,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>209</v>
@@ -3871,7 +3869,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>209</v>
@@ -3919,7 +3917,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H31" s="8" t="s">
         <v>209</v>
@@ -3967,7 +3965,7 @@
         <v>112</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>209</v>
@@ -4015,7 +4013,7 @@
         <v>94</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H33" s="8" t="s">
         <v>209</v>
@@ -4049,7 +4047,7 @@
         <v>94</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>210</v>
@@ -4079,7 +4077,7 @@
     </row>
     <row r="35" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>249</v>
@@ -4097,13 +4095,13 @@
         <v>94</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H35" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -4125,9 +4123,9 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>249</v>
@@ -4145,13 +4143,13 @@
         <v>94</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I36" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -4193,7 +4191,7 @@
         <v>94</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>209</v>
@@ -4241,7 +4239,7 @@
         <v>94</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H38" s="8" t="s">
         <v>209</v>
@@ -4289,7 +4287,7 @@
         <v>94</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>209</v>
@@ -4337,7 +4335,7 @@
         <v>94</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H40" s="8" t="s">
         <v>209</v>
@@ -4385,7 +4383,7 @@
         <v>94</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H41" s="8" t="s">
         <v>209</v>
@@ -4415,7 +4413,7 @@
     </row>
     <row r="42" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>249</v>
@@ -4433,13 +4431,13 @@
         <v>94</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H42" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
@@ -4481,7 +4479,7 @@
         <v>94</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>209</v>
@@ -4529,7 +4527,7 @@
         <v>94</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>209</v>
@@ -4577,7 +4575,7 @@
         <v>94</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>209</v>
@@ -4625,7 +4623,7 @@
         <v>94</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>209</v>
@@ -4673,7 +4671,7 @@
         <v>94</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H47" s="8" t="s">
         <v>209</v>
@@ -4721,7 +4719,7 @@
         <v>94</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>209</v>
@@ -4769,7 +4767,7 @@
         <v>94</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>209</v>
@@ -4817,7 +4815,7 @@
         <v>94</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>209</v>
@@ -4865,7 +4863,7 @@
         <v>94</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>209</v>
@@ -4913,7 +4911,7 @@
         <v>94</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>209</v>
@@ -4961,7 +4959,7 @@
         <v>94</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>209</v>
@@ -5009,7 +5007,7 @@
         <v>94</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>209</v>
@@ -5057,7 +5055,7 @@
         <v>94</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H55" s="8" t="s">
         <v>209</v>
@@ -5105,7 +5103,7 @@
         <v>94</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H56" s="8" t="s">
         <v>209</v>
@@ -5153,7 +5151,7 @@
         <v>94</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H57" s="8" t="s">
         <v>209</v>
@@ -5201,7 +5199,7 @@
         <v>94</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H58" s="8" t="s">
         <v>209</v>
@@ -5249,7 +5247,7 @@
         <v>94</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H59" s="8" t="s">
         <v>209</v>
@@ -5297,7 +5295,7 @@
         <v>94</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H60" s="8" t="s">
         <v>209</v>
@@ -5345,7 +5343,7 @@
         <v>94</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H61" s="8" t="s">
         <v>210</v>
@@ -5379,7 +5377,7 @@
         <v>94</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H62" s="8" t="s">
         <v>210</v>
@@ -5427,7 +5425,7 @@
         <v>94</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H63" s="8" t="s">
         <v>210</v>
@@ -5457,13 +5455,13 @@
     </row>
     <row r="64" spans="1:28" ht="214.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C64" s="6" t="s">
         <v>329</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>330</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>14</v>
@@ -5475,13 +5473,13 @@
         <v>1</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H64" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -5523,7 +5521,7 @@
         <v>94</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H65" s="8" t="s">
         <v>210</v>
@@ -5571,7 +5569,7 @@
         <v>94</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H66" s="8" t="s">
         <v>210</v>
@@ -5619,7 +5617,7 @@
         <v>94</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H67" s="8" t="s">
         <v>209</v>
@@ -5667,7 +5665,7 @@
         <v>94</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H68" s="8" t="s">
         <v>209</v>
@@ -5715,7 +5713,7 @@
         <v>94</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H69" s="8" t="s">
         <v>209</v>
@@ -5763,7 +5761,7 @@
         <v>94</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H70" s="8" t="s">
         <v>209</v>
@@ -5811,7 +5809,7 @@
         <v>94</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H71" s="8" t="s">
         <v>209</v>
@@ -5859,7 +5857,7 @@
         <v>94</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H72" s="8" t="s">
         <v>209</v>
@@ -5907,7 +5905,7 @@
         <v>94</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H73" s="8" t="s">
         <v>209</v>
@@ -5955,7 +5953,7 @@
         <v>94</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H74" s="8" t="s">
         <v>209</v>
@@ -6003,7 +6001,7 @@
         <v>94</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H75" s="8" t="s">
         <v>209</v>
@@ -6051,7 +6049,7 @@
         <v>94</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H76" s="8" t="s">
         <v>209</v>
@@ -6080,7 +6078,7 @@
         <v>252</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H77" s="8" t="s">
         <v>209</v>
@@ -6109,7 +6107,7 @@
         <v>94</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H78" s="8" t="s">
         <v>209</v>
@@ -6138,7 +6136,7 @@
         <v>94</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H79" s="8" t="s">
         <v>209</v>
@@ -6167,7 +6165,7 @@
         <v>94</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H80" s="8" t="s">
         <v>209</v>
@@ -6196,7 +6194,7 @@
         <v>94</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H81" s="8" t="s">
         <v>209</v>
@@ -6225,7 +6223,7 @@
         <v>94</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H82" s="8" t="s">
         <v>209</v>
@@ -6254,7 +6252,7 @@
         <v>94</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H83" s="8" t="s">
         <v>209</v>
@@ -6283,7 +6281,7 @@
         <v>94</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H84" s="8" t="s">
         <v>209</v>
@@ -6312,7 +6310,7 @@
         <v>94</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H85" s="8" t="s">
         <v>209</v>
@@ -6341,7 +6339,7 @@
         <v>94</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H86" s="8" t="s">
         <v>209</v>
@@ -6350,7 +6348,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>135</v>
       </c>
@@ -6398,12 +6396,12 @@
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>161</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>162</v>
@@ -6424,7 +6422,7 @@
         <v>210</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>279</v>
+        <v>356</v>
       </c>
       <c r="J88" s="8"/>
       <c r="K88" s="9"/>
@@ -6446,7 +6444,7 @@
       <c r="AA88" s="2"/>
       <c r="AB88" s="2"/>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>163</v>
       </c>
@@ -6494,7 +6492,7 @@
       <c r="AA89" s="2"/>
       <c r="AB89" s="2"/>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>165</v>
       </c>
@@ -6546,10 +6544,10 @@
     </row>
     <row r="91" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>162</v>
@@ -6570,9 +6568,9 @@
         <v>209</v>
       </c>
       <c r="I91" s="20" t="s">
-        <v>356</v>
-      </c>
-      <c r="J91" s="34"/>
+        <v>355</v>
+      </c>
+      <c r="J91"/>
       <c r="K91" s="9"/>
       <c r="L91" s="9"/>
       <c r="M91" s="9"/>
@@ -6612,7 +6610,7 @@
         <v>94</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H92" s="8" t="s">
         <v>210</v>
@@ -6660,7 +6658,7 @@
         <v>94</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H93" s="8" t="s">
         <v>210</v>
@@ -6708,7 +6706,7 @@
         <v>94</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H94" s="8" t="s">
         <v>210</v>
@@ -6756,7 +6754,7 @@
         <v>94</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H95" s="8" t="s">
         <v>210</v>
@@ -6804,7 +6802,7 @@
         <v>94</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H96" s="8" t="s">
         <v>210</v>
@@ -6834,7 +6832,7 @@
     </row>
     <row r="97" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>249</v>
@@ -6852,13 +6850,13 @@
         <v>94</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H97" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J97" s="6"/>
       <c r="K97" s="6"/>
@@ -6900,7 +6898,7 @@
         <v>94</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H98" s="8" t="s">
         <v>210</v>
@@ -7092,7 +7090,7 @@
         <v>94</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H102" s="8" t="s">
         <v>210</v>
@@ -7140,7 +7138,7 @@
         <v>94</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H103" s="8" t="s">
         <v>210</v>
@@ -7188,7 +7186,7 @@
         <v>112</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H104" s="8" t="s">
         <v>210</v>
@@ -7236,7 +7234,7 @@
         <v>94</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H105" s="8" t="s">
         <v>210</v>
@@ -7266,7 +7264,7 @@
     </row>
     <row r="106" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>249</v>
@@ -7284,13 +7282,13 @@
         <v>94</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H106" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I106" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
@@ -7314,7 +7312,7 @@
     </row>
     <row r="107" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>249</v>
@@ -7332,13 +7330,13 @@
         <v>94</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H107" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I107" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
@@ -7362,7 +7360,7 @@
     </row>
     <row r="108" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>249</v>
@@ -7380,13 +7378,13 @@
         <v>94</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H108" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I108" s="22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
@@ -7428,13 +7426,13 @@
         <v>94</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H109" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I109" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
@@ -7476,13 +7474,13 @@
         <v>94</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H110" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I110" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
@@ -7524,13 +7522,13 @@
         <v>94</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H111" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I111" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J111" s="9"/>
       <c r="K111" s="9"/>
@@ -7554,7 +7552,7 @@
     </row>
     <row r="112" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>249</v>
@@ -7572,13 +7570,13 @@
         <v>94</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H112" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I112" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J112" s="9"/>
       <c r="K112" s="9"/>
@@ -7602,31 +7600,31 @@
     </row>
     <row r="113" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C113" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G113" s="6" t="s">
         <v>295</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E113" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F113" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G113" s="6" t="s">
-        <v>296</v>
       </c>
       <c r="H113" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I113" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J113" s="9"/>
       <c r="K113" s="9"/>
@@ -7650,31 +7648,31 @@
     </row>
     <row r="114" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C114" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G114" s="6" t="s">
         <v>295</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E114" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F114" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G114" s="6" t="s">
-        <v>296</v>
       </c>
       <c r="H114" s="8" t="s">
         <v>210</v>
       </c>
       <c r="I114" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J114" s="9"/>
       <c r="K114" s="9"/>
@@ -7716,7 +7714,7 @@
         <v>94</v>
       </c>
       <c r="G115" s="18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H115" s="8" t="s">
         <v>210</v>
@@ -7764,7 +7762,7 @@
         <v>94</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H116" s="8" t="s">
         <v>210</v>
@@ -7860,7 +7858,7 @@
         <v>94</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H118" s="8" t="s">
         <v>210</v>
@@ -7908,7 +7906,7 @@
         <v>94</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H119" s="8" t="s">
         <v>209</v>
@@ -7956,7 +7954,7 @@
         <v>94</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H120" s="8" t="s">
         <v>209</v>
@@ -8004,7 +8002,7 @@
         <v>94</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H121" s="8" t="s">
         <v>209</v>
@@ -8052,7 +8050,7 @@
         <v>94</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H122" s="8" t="s">
         <v>209</v>
@@ -8100,7 +8098,7 @@
         <v>94</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H123" s="8" t="s">
         <v>209</v>
@@ -8130,7 +8128,7 @@
     </row>
     <row r="124" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>249</v>
@@ -8148,13 +8146,13 @@
         <v>94</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H124" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I124" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J124" s="6"/>
       <c r="K124" s="6"/>
@@ -8196,7 +8194,7 @@
         <v>94</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H125" s="8" t="s">
         <v>209</v>
@@ -8582,9 +8580,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I132" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
+    <filterColumn colId="6">
       <filters>
-        <filter val="Yes"/>
+        <filter val="Disputes-ChargeBack"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Modified test script for regression
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(24-03-2023)Home\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE895160-6AAD-4B07-A28E-BA4F7A2A8BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB5674D-B257-49E6-9E5B-8BBBA9F5CB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$132</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$130</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="350">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -900,31 +900,6 @@
     <t>coyni.admin.tests.TransactionTest,
 testTransactionSearch,
 -pdata</t>
-  </si>
-  <si>
-    <t>verify fee struture status active to sheduled</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.SystemSettingsTest,
-testFeeStructuresActiveToSheduled,
--pdebitAmnt,
--pselectDate,
--psuccess,
--pmessage</t>
-  </si>
-  <si>
-    <t>verify accountLimits status active to sheduled</t>
-  </si>
-  <si>
-    <t>coyni.admin.tests.SystemSettingsTest,
-testAccountLimitsActiveToSheduled,
--pdebitAmnt,
--pselectDate,
--psuccess,
--pmessage</t>
-  </si>
-  <si>
-    <t>AccountLimit - shedule</t>
   </si>
   <si>
     <t>coyni.admin.tests.ProfilesTest,
@@ -1500,9 +1475,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>add Merchant user with invalid scenarios</t>
   </si>
   <si>
@@ -1797,9 +1769,6 @@
   </si>
   <si>
     <t>Accounting - TotalDeposit</t>
-  </si>
-  <si>
-    <t>SystemSettings -feeStructureView</t>
   </si>
   <si>
     <t>Profile - Api Business</t>
@@ -2142,7 +2111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2178,7 +2147,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2479,12 +2447,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB132"/>
+  <dimension ref="A1:AB130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I88" sqref="I88"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,12 +2506,12 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>10</v>
@@ -2562,7 +2529,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -2585,12 +2552,12 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>10</v>
@@ -2608,7 +2575,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -2631,32 +2598,32 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>247</v>
+    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>242</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C4" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>235</v>
-      </c>
-      <c r="G4" s="29" t="s">
+      <c r="E4" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="31" t="s">
-        <v>347</v>
-      </c>
-      <c r="I4" s="32"/>
+      <c r="H4" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="I4" s="31"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -2677,12 +2644,12 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
@@ -2723,12 +2690,12 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>10</v>
@@ -2746,7 +2713,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -2769,12 +2736,12 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>10</v>
@@ -2815,12 +2782,12 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="240" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>24</v>
@@ -2838,7 +2805,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -2861,12 +2828,12 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="210.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="210.75" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>24</v>
@@ -2907,29 +2874,29 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+    <row r="10" spans="1:28" ht="210" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C10" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="C10" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>348</v>
-      </c>
-      <c r="G10" s="29" t="s">
+      <c r="E10" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>341</v>
+      </c>
+      <c r="G10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="30" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="9"/>
@@ -2953,30 +2920,30 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="180" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
-        <v>349</v>
+    <row r="11" spans="1:28" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>342</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C11" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>235</v>
-      </c>
-      <c r="G11" s="29" t="s">
+      <c r="E11" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G11" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="31" t="s">
-        <v>350</v>
+      <c r="H11" s="30" t="s">
+        <v>343</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -2999,12 +2966,12 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>24</v>
@@ -3045,12 +3012,12 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="255" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>32</v>
@@ -3091,12 +3058,12 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>32</v>
@@ -3137,12 +3104,12 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="210" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>32</v>
@@ -3183,30 +3150,30 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
-        <v>351</v>
+    <row r="16" spans="1:28" ht="240" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>344</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C16" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="28">
         <v>1</v>
       </c>
-      <c r="F16" s="30" t="s">
-        <v>235</v>
-      </c>
-      <c r="G16" s="29" t="s">
+      <c r="F16" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G16" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="31" t="s">
-        <v>352</v>
+      <c r="H16" s="30" t="s">
+        <v>345</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -3229,12 +3196,12 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
-    <row r="17" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>32</v>
@@ -3275,12 +3242,12 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:28" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="195" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>32</v>
@@ -3321,12 +3288,12 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>10</v>
@@ -3341,13 +3308,13 @@
         <v>94</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
@@ -3369,12 +3336,12 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
     </row>
-    <row r="20" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>127</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>129</v>
@@ -3389,13 +3356,13 @@
         <v>111</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -3417,12 +3384,12 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
     </row>
-    <row r="21" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>128</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>129</v>
@@ -3437,13 +3404,13 @@
         <v>112</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
@@ -3465,12 +3432,12 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>131</v>
@@ -3488,7 +3455,7 @@
         <v>132</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>149</v>
@@ -3513,12 +3480,12 @@
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
     </row>
-    <row r="23" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>147</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>131</v>
@@ -3536,7 +3503,7 @@
         <v>150</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>148</v>
@@ -3561,12 +3528,12 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
     </row>
-    <row r="24" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>18</v>
@@ -3581,13 +3548,13 @@
         <v>94</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -3609,12 +3576,12 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
     </row>
-    <row r="25" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>18</v>
@@ -3629,10 +3596,10 @@
         <v>94</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>20</v>
@@ -3657,12 +3624,12 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
     </row>
-    <row r="26" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>18</v>
@@ -3677,10 +3644,10 @@
         <v>94</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>22</v>
@@ -3705,12 +3672,12 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>342</v>
+    <row r="27" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>335</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>18</v>
@@ -3725,13 +3692,13 @@
         <v>94</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -3753,12 +3720,12 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>344</v>
+    <row r="28" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>337</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>18</v>
@@ -3773,13 +3740,13 @@
         <v>94</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -3801,15 +3768,15 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:28" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="270" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>11</v>
@@ -3821,13 +3788,13 @@
         <v>1</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -3849,15 +3816,15 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
     </row>
-    <row r="30" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>14</v>
@@ -3869,13 +3836,13 @@
         <v>2</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -3897,15 +3864,15 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>11</v>
@@ -3917,13 +3884,13 @@
         <v>1</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -3945,15 +3912,15 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:28" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="285" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>14</v>
@@ -3965,13 +3932,13 @@
         <v>112</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3993,12 +3960,12 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>143</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>18</v>
@@ -4013,10 +3980,10 @@
         <v>94</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I33" s="19" t="s">
         <v>144</v>
@@ -4027,12 +3994,12 @@
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
     </row>
-    <row r="34" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>18</v>
@@ -4047,10 +4014,10 @@
         <v>94</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I34" s="20" t="s">
         <v>96</v>
@@ -4075,12 +4042,12 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>18</v>
@@ -4095,13 +4062,13 @@
         <v>94</v>
       </c>
       <c r="G35" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="I35" s="20" t="s">
         <v>318</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I35" s="20" t="s">
-        <v>325</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -4123,12 +4090,12 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>18</v>
@@ -4143,13 +4110,13 @@
         <v>94</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I36" s="20" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -4171,12 +4138,12 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>18</v>
@@ -4191,10 +4158,10 @@
         <v>94</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>98</v>
@@ -4219,12 +4186,12 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>18</v>
@@ -4239,10 +4206,10 @@
         <v>94</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>100</v>
@@ -4267,12 +4234,12 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>18</v>
@@ -4287,10 +4254,10 @@
         <v>94</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>102</v>
@@ -4315,12 +4282,12 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>18</v>
@@ -4335,10 +4302,10 @@
         <v>94</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>104</v>
@@ -4363,12 +4330,12 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>18</v>
@@ -4383,10 +4350,10 @@
         <v>94</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I41" s="8" t="s">
         <v>106</v>
@@ -4411,12 +4378,12 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>327</v>
+    <row r="42" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A42" s="26" t="s">
+        <v>320</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>18</v>
@@ -4431,13 +4398,13 @@
         <v>94</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
@@ -4459,12 +4426,12 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>44</v>
@@ -4479,10 +4446,10 @@
         <v>94</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I43" s="8" t="s">
         <v>45</v>
@@ -4507,12 +4474,12 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>44</v>
@@ -4527,10 +4494,10 @@
         <v>94</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>168</v>
@@ -4555,12 +4522,12 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>44</v>
@@ -4575,10 +4542,10 @@
         <v>94</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>47</v>
@@ -4603,12 +4570,12 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>44</v>
@@ -4623,10 +4590,10 @@
         <v>94</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>49</v>
@@ -4651,12 +4618,12 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>44</v>
@@ -4671,10 +4638,10 @@
         <v>94</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I47" s="8" t="s">
         <v>51</v>
@@ -4699,12 +4666,12 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>44</v>
@@ -4719,10 +4686,10 @@
         <v>94</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>53</v>
@@ -4747,12 +4714,12 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>44</v>
@@ -4767,10 +4734,10 @@
         <v>94</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>55</v>
@@ -4795,12 +4762,12 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>57</v>
@@ -4815,10 +4782,10 @@
         <v>94</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I50" s="8" t="s">
         <v>140</v>
@@ -4843,12 +4810,12 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>57</v>
@@ -4863,10 +4830,10 @@
         <v>94</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I51" s="8" t="s">
         <v>59</v>
@@ -4891,12 +4858,12 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>57</v>
@@ -4911,10 +4878,10 @@
         <v>94</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I52" s="8" t="s">
         <v>61</v>
@@ -4939,12 +4906,12 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>57</v>
@@ -4959,10 +4926,10 @@
         <v>94</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I53" s="8" t="s">
         <v>63</v>
@@ -4987,12 +4954,12 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>57</v>
@@ -5007,10 +4974,10 @@
         <v>94</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>65</v>
@@ -5035,12 +5002,12 @@
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
     </row>
-    <row r="55" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>57</v>
@@ -5055,10 +5022,10 @@
         <v>94</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I55" s="8" t="s">
         <v>67</v>
@@ -5083,12 +5050,12 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>57</v>
@@ -5103,10 +5070,10 @@
         <v>94</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I56" s="8" t="s">
         <v>69</v>
@@ -5131,12 +5098,12 @@
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>133</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>57</v>
@@ -5151,10 +5118,10 @@
         <v>94</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I57" s="8" t="s">
         <v>134</v>
@@ -5179,12 +5146,12 @@
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
     </row>
-    <row r="58" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>57</v>
@@ -5199,10 +5166,10 @@
         <v>94</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I58" s="8" t="s">
         <v>71</v>
@@ -5227,12 +5194,12 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>136</v>
@@ -5247,10 +5214,10 @@
         <v>94</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I59" s="19" t="s">
         <v>142</v>
@@ -5275,12 +5242,12 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>136</v>
@@ -5295,10 +5262,10 @@
         <v>94</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I60" s="19" t="s">
         <v>146</v>
@@ -5323,12 +5290,12 @@
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>117</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>123</v>
@@ -5343,10 +5310,10 @@
         <v>94</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I61" s="8" t="s">
         <v>118</v>
@@ -5357,12 +5324,12 @@
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
     </row>
-    <row r="62" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>123</v>
@@ -5377,13 +5344,13 @@
         <v>94</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I62" s="22" t="s">
-        <v>174</v>
+        <v>205</v>
+      </c>
+      <c r="I62" s="21" t="s">
+        <v>169</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -5405,12 +5372,12 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>123</v>
@@ -5425,12 +5392,12 @@
         <v>94</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I63" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="I63" s="21" t="s">
         <v>121</v>
       </c>
       <c r="J63" s="9"/>
@@ -5453,15 +5420,15 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="214.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" ht="214.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>14</v>
@@ -5473,13 +5440,13 @@
         <v>1</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I64" s="22" t="s">
-        <v>353</v>
+        <v>204</v>
+      </c>
+      <c r="I64" s="21" t="s">
+        <v>346</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -5501,12 +5468,12 @@
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
     </row>
-    <row r="65" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>123</v>
@@ -5521,12 +5488,12 @@
         <v>94</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I65" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="I65" s="21" t="s">
         <v>124</v>
       </c>
       <c r="J65" s="9"/>
@@ -5549,12 +5516,12 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>123</v>
@@ -5569,12 +5536,12 @@
         <v>94</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I66" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="I66" s="21" t="s">
         <v>126</v>
       </c>
       <c r="J66" s="9"/>
@@ -5597,15 +5564,15 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>11</v>
@@ -5617,13 +5584,13 @@
         <v>94</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I67" s="22" t="s">
-        <v>189</v>
+        <v>204</v>
+      </c>
+      <c r="I67" s="21" t="s">
+        <v>184</v>
       </c>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -5645,15 +5612,15 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>11</v>
@@ -5665,13 +5632,13 @@
         <v>94</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I68" s="22" t="s">
-        <v>190</v>
+        <v>204</v>
+      </c>
+      <c r="I68" s="21" t="s">
+        <v>185</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -5693,15 +5660,15 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>11</v>
@@ -5713,13 +5680,13 @@
         <v>94</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I69" s="22" t="s">
-        <v>188</v>
+        <v>204</v>
+      </c>
+      <c r="I69" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -5741,15 +5708,15 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="25" t="s">
-        <v>179</v>
+    <row r="70" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A70" s="24" t="s">
+        <v>174</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>11</v>
@@ -5761,13 +5728,13 @@
         <v>94</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I70" s="22" t="s">
-        <v>192</v>
+        <v>204</v>
+      </c>
+      <c r="I70" s="21" t="s">
+        <v>187</v>
       </c>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -5789,15 +5756,15 @@
       <c r="AA70" s="2"/>
       <c r="AB70" s="2"/>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>11</v>
@@ -5809,13 +5776,13 @@
         <v>94</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I71" s="22" t="s">
-        <v>193</v>
+        <v>204</v>
+      </c>
+      <c r="I71" s="21" t="s">
+        <v>188</v>
       </c>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
@@ -5837,15 +5804,15 @@
       <c r="AA71" s="2"/>
       <c r="AB71" s="2"/>
     </row>
-    <row r="72" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>11</v>
@@ -5857,13 +5824,13 @@
         <v>94</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="H72" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I72" s="22" t="s">
-        <v>194</v>
+        <v>204</v>
+      </c>
+      <c r="I72" s="21" t="s">
+        <v>189</v>
       </c>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
@@ -5885,15 +5852,15 @@
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
     </row>
-    <row r="73" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>11</v>
@@ -5905,13 +5872,13 @@
         <v>94</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I73" s="22" t="s">
-        <v>195</v>
+        <v>204</v>
+      </c>
+      <c r="I73" s="21" t="s">
+        <v>190</v>
       </c>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -5933,15 +5900,15 @@
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
     </row>
-    <row r="74" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>11</v>
@@ -5953,13 +5920,13 @@
         <v>94</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I74" s="22" t="s">
-        <v>196</v>
+        <v>204</v>
+      </c>
+      <c r="I74" s="21" t="s">
+        <v>191</v>
       </c>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
@@ -5981,15 +5948,15 @@
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
     </row>
-    <row r="75" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>11</v>
@@ -6001,13 +5968,13 @@
         <v>94</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I75" s="22" t="s">
-        <v>191</v>
+        <v>204</v>
+      </c>
+      <c r="I75" s="21" t="s">
+        <v>186</v>
       </c>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
@@ -6029,15 +5996,15 @@
       <c r="AA75" s="2"/>
       <c r="AB75" s="2"/>
     </row>
-    <row r="76" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="26" t="s">
-        <v>248</v>
+    <row r="76" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A76" s="25" t="s">
+        <v>243</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>14</v>
@@ -6049,21 +6016,21 @@
         <v>94</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H76" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I76" s="22" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="77" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I76" s="21" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>123</v>
@@ -6075,24 +6042,24 @@
         <v>94</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H77" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I77" s="22" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="78" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I77" s="21" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>123</v>
@@ -6107,21 +6074,21 @@
         <v>94</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H78" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I78" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="I78" s="21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="79" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>261</v>
-      </c>
       <c r="B79" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>123</v>
@@ -6136,21 +6103,21 @@
         <v>94</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H79" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I79" s="22" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="80" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I79" s="21" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>123</v>
@@ -6165,21 +6132,21 @@
         <v>94</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I80" s="22" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="81" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I80" s="21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>123</v>
@@ -6194,21 +6161,21 @@
         <v>94</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H81" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I81" s="22" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="82" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I81" s="21" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>123</v>
@@ -6223,21 +6190,21 @@
         <v>94</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H82" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I82" s="22" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="83" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I82" s="21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>123</v>
@@ -6252,21 +6219,21 @@
         <v>94</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H83" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I83" s="22" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="84" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I83" s="21" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>123</v>
@@ -6281,21 +6248,21 @@
         <v>94</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H84" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I84" s="22" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="85" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I84" s="21" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>123</v>
@@ -6310,21 +6277,21 @@
         <v>94</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H85" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I85" s="22" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="86" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="I85" s="21" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>123</v>
@@ -6339,13 +6306,13 @@
         <v>94</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="H86" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I86" s="22" t="s">
-        <v>278</v>
+        <v>204</v>
+      </c>
+      <c r="I86" s="21" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="87" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
@@ -6353,7 +6320,7 @@
         <v>135</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>136</v>
@@ -6371,7 +6338,7 @@
         <v>160</v>
       </c>
       <c r="H87" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I87" s="8" t="s">
         <v>137</v>
@@ -6401,7 +6368,7 @@
         <v>161</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>162</v>
@@ -6419,10 +6386,10 @@
         <v>160</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="J88" s="8"/>
       <c r="K88" s="9"/>
@@ -6449,7 +6416,7 @@
         <v>163</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>162</v>
@@ -6467,7 +6434,7 @@
         <v>160</v>
       </c>
       <c r="H89" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I89" s="8" t="s">
         <v>164</v>
@@ -6497,7 +6464,7 @@
         <v>165</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>162</v>
@@ -6515,7 +6482,7 @@
         <v>160</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I90" s="8" t="s">
         <v>164</v>
@@ -6544,10 +6511,10 @@
     </row>
     <row r="91" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>162</v>
@@ -6565,10 +6532,10 @@
         <v>160</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I91" s="20" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="J91"/>
       <c r="K91" s="9"/>
@@ -6590,12 +6557,12 @@
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
     </row>
-    <row r="92" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>82</v>
@@ -6610,10 +6577,10 @@
         <v>94</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I92" s="8" t="s">
         <v>83</v>
@@ -6638,12 +6605,12 @@
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
     </row>
-    <row r="93" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>82</v>
@@ -6658,10 +6625,10 @@
         <v>94</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I93" s="8" t="s">
         <v>85</v>
@@ -6686,12 +6653,12 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>82</v>
@@ -6706,10 +6673,10 @@
         <v>94</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="H94" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I94" s="8" t="s">
         <v>87</v>
@@ -6734,12 +6701,12 @@
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
     </row>
-    <row r="95" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>82</v>
@@ -6754,10 +6721,10 @@
         <v>94</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I95" s="8" t="s">
         <v>89</v>
@@ -6782,12 +6749,12 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>82</v>
@@ -6802,10 +6769,10 @@
         <v>94</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="H96" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I96" s="8" t="s">
         <v>91</v>
@@ -6830,12 +6797,12 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="27" t="s">
-        <v>279</v>
+    <row r="97" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A97" s="26" t="s">
+        <v>273</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>82</v>
@@ -6850,13 +6817,13 @@
         <v>94</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="J97" s="6"/>
       <c r="K97" s="6"/>
@@ -6878,12 +6845,12 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>82</v>
@@ -6898,10 +6865,10 @@
         <v>94</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="H98" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I98" s="8" t="s">
         <v>93</v>
@@ -6926,15 +6893,15 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D99" s="9" t="s">
         <v>11</v>
@@ -6946,13 +6913,13 @@
         <v>94</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H99" s="20" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I99" s="20" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
@@ -6974,15 +6941,15 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>11</v>
@@ -6994,13 +6961,13 @@
         <v>94</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H100" s="20" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I100" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
@@ -7022,15 +6989,15 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>11</v>
@@ -7042,13 +7009,13 @@
         <v>94</v>
       </c>
       <c r="G101" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="H101" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="I101" s="20" t="s">
         <v>215</v>
-      </c>
-      <c r="H101" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="I101" s="20" t="s">
-        <v>220</v>
       </c>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
@@ -7070,12 +7037,12 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>159</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>77</v>
@@ -7090,10 +7057,10 @@
         <v>94</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I102" s="8" t="s">
         <v>158</v>
@@ -7118,12 +7085,12 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>113</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>77</v>
@@ -7138,10 +7105,10 @@
         <v>94</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="H103" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I103" s="8" t="s">
         <v>78</v>
@@ -7166,12 +7133,12 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>77</v>
@@ -7180,16 +7147,16 @@
         <v>14</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="F104" s="7" t="s">
         <v>112</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="H104" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I104" s="8" t="s">
         <v>80</v>
@@ -7214,12 +7181,12 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>73</v>
@@ -7234,10 +7201,10 @@
         <v>94</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="H105" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I105" s="8" t="s">
         <v>74</v>
@@ -7262,12 +7229,12 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>73</v>
@@ -7282,13 +7249,13 @@
         <v>94</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="H106" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I106" s="22" t="s">
-        <v>283</v>
+        <v>204</v>
+      </c>
+      <c r="I106" s="21" t="s">
+        <v>277</v>
       </c>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
@@ -7310,12 +7277,12 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>73</v>
@@ -7330,13 +7297,13 @@
         <v>94</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="H107" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I107" s="22" t="s">
-        <v>285</v>
+        <v>204</v>
+      </c>
+      <c r="I107" s="21" t="s">
+        <v>279</v>
       </c>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
@@ -7358,12 +7325,12 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>73</v>
@@ -7378,13 +7345,13 @@
         <v>94</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="H108" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I108" s="22" t="s">
-        <v>287</v>
+        <v>204</v>
+      </c>
+      <c r="I108" s="21" t="s">
+        <v>281</v>
       </c>
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
@@ -7406,12 +7373,12 @@
       <c r="AA108" s="2"/>
       <c r="AB108" s="2"/>
     </row>
-    <row r="109" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C109" s="18" t="s">
         <v>73</v>
@@ -7426,13 +7393,13 @@
         <v>94</v>
       </c>
       <c r="G109" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="H109" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="I109" s="8" t="s">
         <v>282</v>
-      </c>
-      <c r="H109" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I109" s="8" t="s">
-        <v>288</v>
       </c>
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
@@ -7454,12 +7421,12 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>73</v>
@@ -7474,13 +7441,13 @@
         <v>94</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I110" s="8" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
@@ -7502,12 +7469,12 @@
       <c r="AA110" s="2"/>
       <c r="AB110" s="2"/>
     </row>
-    <row r="111" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>114</v>
@@ -7522,13 +7489,13 @@
         <v>94</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="H111" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I111" s="8" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="J111" s="9"/>
       <c r="K111" s="9"/>
@@ -7550,12 +7517,12 @@
       <c r="AA111" s="2"/>
       <c r="AB111" s="2"/>
     </row>
-    <row r="112" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>114</v>
@@ -7570,13 +7537,13 @@
         <v>94</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="H112" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I112" s="8" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="J112" s="9"/>
       <c r="K112" s="9"/>
@@ -7598,15 +7565,15 @@
       <c r="AA112" s="2"/>
       <c r="AB112" s="2"/>
     </row>
-    <row r="113" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>11</v>
@@ -7618,13 +7585,13 @@
         <v>94</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="H113" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I113" s="8" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="J113" s="9"/>
       <c r="K113" s="9"/>
@@ -7646,15 +7613,15 @@
       <c r="AA113" s="2"/>
       <c r="AB113" s="2"/>
     </row>
-    <row r="114" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>11</v>
@@ -7666,13 +7633,13 @@
         <v>94</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="H114" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I114" s="8" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="J114" s="9"/>
       <c r="K114" s="9"/>
@@ -7694,17 +7661,17 @@
       <c r="AA114" s="2"/>
       <c r="AB114" s="2"/>
     </row>
-    <row r="115" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="21" t="s">
-        <v>169</v>
+    <row r="115" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C115" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D115" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D115" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E115" s="7" t="s">
@@ -7713,14 +7680,14 @@
       <c r="F115" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G115" s="18" t="s">
-        <v>309</v>
+      <c r="G115" s="6" t="s">
+        <v>284</v>
       </c>
       <c r="H115" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I115" s="8" t="s">
-        <v>170</v>
+        <v>115</v>
       </c>
       <c r="J115" s="9"/>
       <c r="K115" s="9"/>
@@ -7742,12 +7709,12 @@
       <c r="AA115" s="2"/>
       <c r="AB115" s="2"/>
     </row>
-    <row r="116" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>114</v>
@@ -7762,13 +7729,13 @@
         <v>94</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="H116" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I116" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J116" s="9"/>
       <c r="K116" s="9"/>
@@ -7790,15 +7757,15 @@
       <c r="AA116" s="2"/>
       <c r="AB116" s="2"/>
     </row>
-    <row r="117" spans="1:28" s="1" customFormat="1" ht="141.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="21" t="s">
-        <v>171</v>
+    <row r="117" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C117" s="18" t="s">
-        <v>73</v>
+        <v>244</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>11</v>
@@ -7810,16 +7777,16 @@
         <v>94</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>173</v>
+        <v>326</v>
       </c>
       <c r="H117" s="8" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="I117" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="J117" s="9"/>
-      <c r="K117" s="9"/>
+        <v>153</v>
+      </c>
+      <c r="J117" s="6"/>
+      <c r="K117" s="6"/>
       <c r="L117" s="9"/>
       <c r="M117" s="9"/>
       <c r="N117" s="9"/>
@@ -7838,15 +7805,15 @@
       <c r="AA117" s="2"/>
       <c r="AB117" s="2"/>
     </row>
-    <row r="118" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="11" t="s">
-        <v>109</v>
+    <row r="118" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>11</v>
@@ -7858,16 +7825,16 @@
         <v>94</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>290</v>
+        <v>327</v>
       </c>
       <c r="H118" s="8" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="I118" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="J118" s="9"/>
-      <c r="K118" s="9"/>
+        <v>155</v>
+      </c>
+      <c r="J118" s="6"/>
+      <c r="K118" s="6"/>
       <c r="L118" s="9"/>
       <c r="M118" s="9"/>
       <c r="N118" s="9"/>
@@ -7886,12 +7853,12 @@
       <c r="AA118" s="2"/>
       <c r="AB118" s="2"/>
     </row>
-    <row r="119" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>151</v>
+        <v>269</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>152</v>
@@ -7906,13 +7873,13 @@
         <v>94</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="H119" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I119" s="8" t="s">
-        <v>153</v>
+        <v>270</v>
       </c>
       <c r="J119" s="6"/>
       <c r="K119" s="6"/>
@@ -7934,12 +7901,12 @@
       <c r="AA119" s="2"/>
       <c r="AB119" s="2"/>
     </row>
-    <row r="120" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>154</v>
+        <v>267</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>152</v>
@@ -7954,13 +7921,13 @@
         <v>94</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I120" s="8" t="s">
-        <v>155</v>
+        <v>268</v>
       </c>
       <c r="J120" s="6"/>
       <c r="K120" s="6"/>
@@ -7982,12 +7949,12 @@
       <c r="AA120" s="2"/>
       <c r="AB120" s="2"/>
     </row>
-    <row r="121" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>152</v>
@@ -8002,13 +7969,13 @@
         <v>94</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="H121" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I121" s="8" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="J121" s="6"/>
       <c r="K121" s="6"/>
@@ -8030,12 +7997,12 @@
       <c r="AA121" s="2"/>
       <c r="AB121" s="2"/>
     </row>
-    <row r="122" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>273</v>
+        <v>332</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>152</v>
@@ -8050,13 +8017,13 @@
         <v>94</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H122" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I122" s="8" t="s">
-        <v>274</v>
+        <v>334</v>
       </c>
       <c r="J122" s="6"/>
       <c r="K122" s="6"/>
@@ -8078,12 +8045,12 @@
       <c r="AA122" s="2"/>
       <c r="AB122" s="2"/>
     </row>
-    <row r="123" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>271</v>
+        <v>156</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>152</v>
@@ -8098,13 +8065,13 @@
         <v>94</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="H123" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I123" s="8" t="s">
-        <v>272</v>
+        <v>157</v>
       </c>
       <c r="J123" s="6"/>
       <c r="K123" s="6"/>
@@ -8126,15 +8093,15 @@
       <c r="AA123" s="2"/>
       <c r="AB123" s="2"/>
     </row>
-    <row r="124" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
-        <v>339</v>
+    <row r="124" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="A124" s="11" t="s">
+        <v>179</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>11</v>
@@ -8146,16 +8113,16 @@
         <v>94</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>340</v>
+        <v>202</v>
       </c>
       <c r="H124" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I124" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="J124" s="6"/>
-      <c r="K124" s="6"/>
+        <v>192</v>
+      </c>
+      <c r="J124" s="9"/>
+      <c r="K124" s="9"/>
       <c r="L124" s="9"/>
       <c r="M124" s="9"/>
       <c r="N124" s="9"/>
@@ -8174,15 +8141,15 @@
       <c r="AA124" s="2"/>
       <c r="AB124" s="2"/>
     </row>
-    <row r="125" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="3" t="s">
-        <v>156</v>
+    <row r="125" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A125" s="11" t="s">
+        <v>181</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="D125" s="6" t="s">
         <v>11</v>
@@ -8194,16 +8161,20 @@
         <v>94</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>338</v>
+        <v>202</v>
       </c>
       <c r="H125" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I125" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="J125" s="6"/>
-      <c r="K125" s="6"/>
+        <v>204</v>
+      </c>
+      <c r="I125" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="J125" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="K125" s="20" t="s">
+        <v>195</v>
+      </c>
       <c r="L125" s="9"/>
       <c r="M125" s="9"/>
       <c r="N125" s="9"/>
@@ -8222,15 +8193,15 @@
       <c r="AA125" s="2"/>
       <c r="AB125" s="2"/>
     </row>
-    <row r="126" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>11</v>
@@ -8242,19 +8213,29 @@
         <v>94</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H126" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I126" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="I126" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="J126" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="J126" s="9"/>
-      <c r="K126" s="9"/>
-      <c r="L126" s="9"/>
-      <c r="M126" s="9"/>
-      <c r="N126" s="9"/>
+      <c r="K126" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="L126" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="M126" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="N126" s="20" t="s">
+        <v>200</v>
+      </c>
       <c r="O126" s="2"/>
       <c r="P126" s="2"/>
       <c r="Q126" s="2"/>
@@ -8270,17 +8251,17 @@
       <c r="AA126" s="2"/>
       <c r="AB126" s="2"/>
     </row>
-    <row r="127" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="11" t="s">
-        <v>186</v>
+    <row r="127" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="22" t="s">
+        <v>226</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D127" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D127" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E127" s="7" t="s">
@@ -8290,19 +8271,19 @@
         <v>94</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="H127" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I127" s="22" t="s">
-        <v>198</v>
+        <v>202</v>
+      </c>
+      <c r="H127" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="I127" s="21" t="s">
+        <v>227</v>
       </c>
       <c r="J127" s="20" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="K127" s="20" t="s">
-        <v>200</v>
+        <v>229</v>
       </c>
       <c r="L127" s="9"/>
       <c r="M127" s="9"/>
@@ -8322,15 +8303,15 @@
       <c r="AA127" s="2"/>
       <c r="AB127" s="2"/>
     </row>
-    <row r="128" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
-        <v>187</v>
+        <v>228</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>185</v>
+        <v>234</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>11</v>
@@ -8342,29 +8323,19 @@
         <v>94</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H128" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="I128" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="J128" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="K128" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="L128" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="M128" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="N128" s="20" t="s">
-        <v>205</v>
-      </c>
+      <c r="I128" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="J128" s="20"/>
+      <c r="K128" s="20"/>
+      <c r="L128" s="9"/>
+      <c r="M128" s="9"/>
+      <c r="N128" s="9"/>
       <c r="O128" s="2"/>
       <c r="P128" s="2"/>
       <c r="Q128" s="2"/>
@@ -8380,17 +8351,17 @@
       <c r="AA128" s="2"/>
       <c r="AB128" s="2"/>
     </row>
-    <row r="129" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="23" t="s">
-        <v>231</v>
+    <row r="129" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A129" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D129" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="D129" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E129" s="7" t="s">
@@ -8400,23 +8371,23 @@
         <v>94</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="H129" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="I129" s="22" t="s">
-        <v>232</v>
+        <v>202</v>
+      </c>
+      <c r="H129" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="I129" s="21" t="s">
+        <v>227</v>
       </c>
       <c r="J129" s="20" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="K129" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="L129" s="9"/>
-      <c r="M129" s="9"/>
-      <c r="N129" s="9"/>
+        <v>229</v>
+      </c>
+      <c r="L129" s="20"/>
+      <c r="M129" s="20"/>
+      <c r="N129" s="20"/>
       <c r="O129" s="2"/>
       <c r="P129" s="2"/>
       <c r="Q129" s="2"/>
@@ -8432,18 +8403,18 @@
       <c r="AA129" s="2"/>
       <c r="AB129" s="2"/>
     </row>
-    <row r="130" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="11" t="s">
+    <row r="130" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
         <v>233</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>239</v>
+        <v>10</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E130" s="7" t="s">
         <v>94</v>
@@ -8452,16 +8423,14 @@
         <v>94</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>207</v>
+        <v>12</v>
       </c>
       <c r="H130" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I130" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="J130" s="20"/>
-      <c r="K130" s="20"/>
+        <v>240</v>
+      </c>
+      <c r="I130" s="9"/>
+      <c r="J130" s="9"/>
+      <c r="K130" s="9"/>
       <c r="L130" s="9"/>
       <c r="M130" s="9"/>
       <c r="N130" s="9"/>
@@ -8480,112 +8449,8 @@
       <c r="AA130" s="2"/>
       <c r="AB130" s="2"/>
     </row>
-    <row r="131" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D131" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E131" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F131" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G131" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="H131" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="I131" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="J131" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="K131" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="L131" s="20"/>
-      <c r="M131" s="20"/>
-      <c r="N131" s="20"/>
-      <c r="O131" s="2"/>
-      <c r="P131" s="2"/>
-      <c r="Q131" s="2"/>
-      <c r="R131" s="2"/>
-      <c r="S131" s="2"/>
-      <c r="T131" s="2"/>
-      <c r="U131" s="2"/>
-      <c r="V131" s="2"/>
-      <c r="W131" s="2"/>
-      <c r="X131" s="2"/>
-      <c r="Y131" s="2"/>
-      <c r="Z131" s="2"/>
-      <c r="AA131" s="2"/>
-      <c r="AB131" s="2"/>
-    </row>
-    <row r="132" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C132" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E132" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F132" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G132" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H132" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="I132" s="9"/>
-      <c r="J132" s="9"/>
-      <c r="K132" s="9"/>
-      <c r="L132" s="9"/>
-      <c r="M132" s="9"/>
-      <c r="N132" s="9"/>
-      <c r="O132" s="2"/>
-      <c r="P132" s="2"/>
-      <c r="Q132" s="2"/>
-      <c r="R132" s="2"/>
-      <c r="S132" s="2"/>
-      <c r="T132" s="2"/>
-      <c r="U132" s="2"/>
-      <c r="V132" s="2"/>
-      <c r="W132" s="2"/>
-      <c r="X132" s="2"/>
-      <c r="Y132" s="2"/>
-      <c r="Z132" s="2"/>
-      <c r="AA132" s="2"/>
-      <c r="AB132" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I132" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Disputes-ChargeBack"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I130" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new method in common function
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoyniSupport\28-03-2023\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(28-03-2023)Sys\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489F40F7-9A99-411E-9298-33AA090C4BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA564408-A9B7-4812-964B-0448654A0979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="373">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2119,6 +2119,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>testData-admin.xlsx,profiles</t>
   </si>
 </sst>
 </file>
@@ -2616,9 +2619,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6171,7 +6174,7 @@
         <v>244</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>201</v>
+        <v>372</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Added test method in system setting test
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(28-03-2023)Sys\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin(30-03-2023)2.3\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA564408-A9B7-4812-964B-0448654A0979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C481E66-3390-49F0-92FE-5C0FF0C7FD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$140</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="372">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2022,9 +2022,6 @@
     <t>testTermOfServiceAgreementsEmptyVersion</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>coyni.admin.tests.SystemSettingsTest,
 testTermOfServiceAgreementsEmptyVersion,
 -perrMessage,
@@ -2085,43 +2082,40 @@
     <t>testEditMerchantFeeStructureReschedulingwithSameDate</t>
   </si>
   <si>
+    <t>testViewPersonalAccountLimitsReschedulingwithSameDate</t>
+  </si>
+  <si>
+    <t>testViewMerchantAccountLimitsReschedulingwithSameDate</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>testData-admin.xlsx,profiles</t>
+  </si>
+  <si>
     <t>coyni.admin.tests.SystemSettingsTest,
-testEditMerchantFeeStructureReschedulingwithSameDate,
--pAgreementList,
+testViewPersonalAccountLimitsReschedulingwithSameDate,
 -pexpEditHeading,
 -pamount,
 -ppercentage,
 -ptosHeading</t>
   </si>
   <si>
-    <t>testViewPersonalAccountLimitsReschedulingwithSameDate</t>
-  </si>
-  <si>
     <t>coyni.admin.tests.SystemSettingsTest,
-testViewPersonalAccountLimitsReschedulingwithSameDate,
--pAgreementList,
+testEditMerchantFeeStructureReschedulingwithSameDate,
 -pexpEditHeading,
 -pamount,
 -ppercentage,
 -ptosHeading</t>
   </si>
   <si>
-    <t>testViewMerchantAccountLimitsReschedulingwithSameDate</t>
-  </si>
-  <si>
     <t>coyni.admin.tests.SystemSettingsTest,
 testViewMerchantAccountLimitsReschedulingwithSameDate,
--pAgreementList,
 -pexpEditHeading,
 -pamount,
 -ppercentage,
 -ptosHeading</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>testData-admin.xlsx,profiles</t>
   </si>
 </sst>
 </file>
@@ -2266,7 +2260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2322,7 +2316,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2617,11 +2610,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB141"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AB140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2676,7 +2670,7 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2722,7 +2716,7 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>324</v>
       </c>
@@ -2768,7 +2762,7 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>242</v>
       </c>
@@ -2814,7 +2808,7 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -2860,7 +2854,7 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
@@ -2906,7 +2900,7 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>138</v>
       </c>
@@ -2952,7 +2946,7 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="240" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -2998,7 +2992,7 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="210.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="210.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>26</v>
       </c>
@@ -3044,7 +3038,7 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="210" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -3090,7 +3084,7 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="180" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>342</v>
       </c>
@@ -3136,7 +3130,7 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -3182,7 +3176,7 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="255" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -3228,7 +3222,7 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="225" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -3274,7 +3268,7 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="210" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -3320,7 +3314,7 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="240" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>344</v>
       </c>
@@ -3366,7 +3360,7 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
-    <row r="17" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -3412,7 +3406,7 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:28" ht="195" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -3458,7 +3452,7 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>236</v>
       </c>
@@ -3506,7 +3500,7 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
     </row>
-    <row r="20" spans="1:28" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>127</v>
       </c>
@@ -3554,7 +3548,7 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
     </row>
-    <row r="21" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>128</v>
       </c>
@@ -3602,7 +3596,7 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
@@ -3650,7 +3644,7 @@
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
     </row>
-    <row r="23" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>147</v>
       </c>
@@ -3698,7 +3692,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
     </row>
-    <row r="24" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
@@ -3746,7 +3740,7 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
     </row>
-    <row r="25" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
@@ -3794,7 +3788,7 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
     </row>
-    <row r="26" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
@@ -3842,7 +3836,7 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>335</v>
       </c>
@@ -3890,7 +3884,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>337</v>
       </c>
@@ -3938,7 +3932,7 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:28" ht="270" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>220</v>
       </c>
@@ -3986,7 +3980,7 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
     </row>
-    <row r="30" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>221</v>
       </c>
@@ -4034,7 +4028,7 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>222</v>
       </c>
@@ -4082,7 +4076,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:28" ht="285" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>223</v>
       </c>
@@ -4130,7 +4124,7 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>143</v>
       </c>
@@ -4164,7 +4158,7 @@
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
     </row>
-    <row r="34" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
@@ -4212,7 +4206,7 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>317</v>
       </c>
@@ -4260,7 +4254,7 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>315</v>
       </c>
@@ -4308,7 +4302,7 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>97</v>
       </c>
@@ -4356,7 +4350,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>99</v>
       </c>
@@ -4404,7 +4398,7 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>101</v>
       </c>
@@ -4452,7 +4446,7 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>103</v>
       </c>
@@ -4500,7 +4494,7 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>105</v>
       </c>
@@ -4548,7 +4542,7 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
         <v>320</v>
       </c>
@@ -4596,7 +4590,7 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
@@ -4644,7 +4638,7 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>167</v>
       </c>
@@ -4692,7 +4686,7 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
@@ -4740,7 +4734,7 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>48</v>
       </c>
@@ -4788,7 +4782,7 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
@@ -4836,7 +4830,7 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>52</v>
       </c>
@@ -4884,7 +4878,7 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
@@ -4932,7 +4926,7 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
@@ -4980,7 +4974,7 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>58</v>
       </c>
@@ -5028,7 +5022,7 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>60</v>
       </c>
@@ -5076,7 +5070,7 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>62</v>
       </c>
@@ -5124,7 +5118,7 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>64</v>
       </c>
@@ -5172,7 +5166,7 @@
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
     </row>
-    <row r="55" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>66</v>
       </c>
@@ -5220,7 +5214,7 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>68</v>
       </c>
@@ -5268,7 +5262,7 @@
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>133</v>
       </c>
@@ -5316,7 +5310,7 @@
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
     </row>
-    <row r="58" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>70</v>
       </c>
@@ -5364,7 +5358,7 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>141</v>
       </c>
@@ -5412,7 +5406,7 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>145</v>
       </c>
@@ -5460,7 +5454,7 @@
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>117</v>
       </c>
@@ -5494,7 +5488,7 @@
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
     </row>
-    <row r="62" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>119</v>
       </c>
@@ -5542,7 +5536,7 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>120</v>
       </c>
@@ -5590,7 +5584,7 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="214.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" ht="214.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>321</v>
       </c>
@@ -5638,7 +5632,7 @@
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
     </row>
-    <row r="65" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>122</v>
       </c>
@@ -5686,7 +5680,7 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>125</v>
       </c>
@@ -5734,7 +5728,7 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>171</v>
       </c>
@@ -5782,7 +5776,7 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>172</v>
       </c>
@@ -5830,7 +5824,7 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>170</v>
       </c>
@@ -5878,7 +5872,7 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
         <v>174</v>
       </c>
@@ -5926,7 +5920,7 @@
       <c r="AA70" s="2"/>
       <c r="AB70" s="2"/>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>175</v>
       </c>
@@ -5974,7 +5968,7 @@
       <c r="AA71" s="2"/>
       <c r="AB71" s="2"/>
     </row>
-    <row r="72" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>176</v>
       </c>
@@ -6022,7 +6016,7 @@
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
     </row>
-    <row r="73" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>177</v>
       </c>
@@ -6070,7 +6064,7 @@
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
     </row>
-    <row r="74" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>178</v>
       </c>
@@ -6118,7 +6112,7 @@
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
     </row>
-    <row r="75" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>173</v>
       </c>
@@ -6166,7 +6160,7 @@
       <c r="AA75" s="2"/>
       <c r="AB75" s="2"/>
     </row>
-    <row r="76" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="25" t="s">
         <v>243</v>
       </c>
@@ -6174,7 +6168,7 @@
         <v>244</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>14</v>
@@ -6195,7 +6189,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>245</v>
       </c>
@@ -6224,7 +6218,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>248</v>
       </c>
@@ -6253,7 +6247,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>255</v>
       </c>
@@ -6282,7 +6276,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>252</v>
       </c>
@@ -6311,7 +6305,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>254</v>
       </c>
@@ -6340,7 +6334,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>257</v>
       </c>
@@ -6369,7 +6363,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>259</v>
       </c>
@@ -6403,7 +6397,7 @@
         <v>261</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>244</v>
+        <v>367</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>123</v>
@@ -6427,7 +6421,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>263</v>
       </c>
@@ -6456,7 +6450,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>271</v>
       </c>
@@ -6490,7 +6484,7 @@
         <v>135</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>244</v>
+        <v>367</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>136</v>
@@ -6533,7 +6527,7 @@
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>161</v>
       </c>
@@ -6581,7 +6575,7 @@
       <c r="AA88" s="2"/>
       <c r="AB88" s="2"/>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>163</v>
       </c>
@@ -6629,7 +6623,7 @@
       <c r="AA89" s="2"/>
       <c r="AB89" s="2"/>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>165</v>
       </c>
@@ -6679,7 +6673,7 @@
       <c r="AA90" s="2"/>
       <c r="AB90" s="2"/>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>347</v>
       </c>
@@ -6727,7 +6721,7 @@
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
     </row>
-    <row r="92" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>81</v>
       </c>
@@ -6775,7 +6769,7 @@
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
     </row>
-    <row r="93" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>84</v>
       </c>
@@ -6823,7 +6817,7 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>86</v>
       </c>
@@ -6871,7 +6865,7 @@
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
     </row>
-    <row r="95" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>88</v>
       </c>
@@ -6919,7 +6913,7 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>90</v>
       </c>
@@ -6967,7 +6961,7 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="26" t="s">
         <v>273</v>
       </c>
@@ -7015,7 +7009,7 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>92</v>
       </c>
@@ -7063,7 +7057,7 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>208</v>
       </c>
@@ -7116,7 +7110,7 @@
         <v>212</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>244</v>
+        <v>367</v>
       </c>
       <c r="C100" s="9" t="s">
         <v>209</v>
@@ -7159,7 +7153,7 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>214</v>
       </c>
@@ -7212,7 +7206,7 @@
         <v>159</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>244</v>
+        <v>367</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>77</v>
@@ -7255,7 +7249,7 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>113</v>
       </c>
@@ -7303,7 +7297,7 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>79</v>
       </c>
@@ -7351,7 +7345,7 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>72</v>
       </c>
@@ -7399,7 +7393,7 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>275</v>
       </c>
@@ -7447,7 +7441,7 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>278</v>
       </c>
@@ -7500,7 +7494,7 @@
         <v>280</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>244</v>
+        <v>367</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>73</v>
@@ -7548,7 +7542,7 @@
         <v>75</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>244</v>
+        <v>367</v>
       </c>
       <c r="C109" s="18" t="s">
         <v>73</v>
@@ -7591,7 +7585,7 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>76</v>
       </c>
@@ -7644,7 +7638,7 @@
         <v>108</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>244</v>
+        <v>367</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>114</v>
@@ -7687,7 +7681,7 @@
       <c r="AA111" s="2"/>
       <c r="AB111" s="2"/>
     </row>
-    <row r="112" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>286</v>
       </c>
@@ -7740,7 +7734,7 @@
         <v>291</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>244</v>
+        <v>367</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>288</v>
@@ -7783,7 +7777,7 @@
       <c r="AA113" s="2"/>
       <c r="AB113" s="2"/>
     </row>
-    <row r="114" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>293</v>
       </c>
@@ -7831,7 +7825,7 @@
       <c r="AA114" s="2"/>
       <c r="AB114" s="2"/>
     </row>
-    <row r="115" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>110</v>
       </c>
@@ -7879,7 +7873,7 @@
       <c r="AA115" s="2"/>
       <c r="AB115" s="2"/>
     </row>
-    <row r="116" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="11" t="s">
         <v>109</v>
       </c>
@@ -7927,7 +7921,7 @@
       <c r="AA116" s="2"/>
       <c r="AB116" s="2"/>
     </row>
-    <row r="117" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>151</v>
       </c>
@@ -7975,7 +7969,7 @@
       <c r="AA117" s="2"/>
       <c r="AB117" s="2"/>
     </row>
-    <row r="118" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>154</v>
       </c>
@@ -8023,7 +8017,7 @@
       <c r="AA118" s="2"/>
       <c r="AB118" s="2"/>
     </row>
-    <row r="119" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>269</v>
       </c>
@@ -8071,7 +8065,7 @@
       <c r="AA119" s="2"/>
       <c r="AB119" s="2"/>
     </row>
-    <row r="120" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>267</v>
       </c>
@@ -8119,7 +8113,7 @@
       <c r="AA120" s="2"/>
       <c r="AB120" s="2"/>
     </row>
-    <row r="121" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>265</v>
       </c>
@@ -8167,7 +8161,7 @@
       <c r="AA121" s="2"/>
       <c r="AB121" s="2"/>
     </row>
-    <row r="122" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>332</v>
       </c>
@@ -8215,7 +8209,7 @@
       <c r="AA122" s="2"/>
       <c r="AB122" s="2"/>
     </row>
-    <row r="123" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>156</v>
       </c>
@@ -8263,7 +8257,7 @@
       <c r="AA123" s="2"/>
       <c r="AB123" s="2"/>
     </row>
-    <row r="124" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
         <v>179</v>
       </c>
@@ -8311,7 +8305,7 @@
       <c r="AA124" s="2"/>
       <c r="AB124" s="2"/>
     </row>
-    <row r="125" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
         <v>181</v>
       </c>
@@ -8363,7 +8357,7 @@
       <c r="AA125" s="2"/>
       <c r="AB125" s="2"/>
     </row>
-    <row r="126" spans="1:28" s="1" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
         <v>182</v>
       </c>
@@ -8421,7 +8415,7 @@
       <c r="AA126" s="2"/>
       <c r="AB126" s="2"/>
     </row>
-    <row r="127" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="22" t="s">
         <v>226</v>
       </c>
@@ -8473,7 +8467,7 @@
       <c r="AA127" s="2"/>
       <c r="AB127" s="2"/>
     </row>
-    <row r="128" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
         <v>228</v>
       </c>
@@ -8521,7 +8515,7 @@
       <c r="AA128" s="2"/>
       <c r="AB128" s="2"/>
     </row>
-    <row r="129" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
         <v>235</v>
       </c>
@@ -8573,84 +8567,67 @@
       <c r="AA129" s="2"/>
       <c r="AB129" s="2"/>
     </row>
-    <row r="130" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
-        <v>233</v>
+    <row r="130" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>350</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C130" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D130" s="6" t="s">
+      <c r="C130" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D130" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E130" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F130" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G130" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H130" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="I130" s="9"/>
-      <c r="J130" s="9"/>
-      <c r="K130" s="9"/>
-      <c r="L130" s="9"/>
-      <c r="M130" s="9"/>
-      <c r="N130" s="9"/>
-      <c r="O130" s="2"/>
-      <c r="P130" s="2"/>
-      <c r="Q130" s="2"/>
-      <c r="R130" s="2"/>
-      <c r="S130" s="2"/>
-      <c r="T130" s="2"/>
-      <c r="U130" s="2"/>
-      <c r="V130" s="2"/>
-      <c r="W130" s="2"/>
-      <c r="X130" s="2"/>
-      <c r="Y130" s="2"/>
-      <c r="Z130" s="2"/>
-      <c r="AA130" s="2"/>
-      <c r="AB130" s="2"/>
+      <c r="E130" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F130" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="G130" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="H130" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="I130" s="36" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="131" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>350</v>
-      </c>
-      <c r="B131" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="C131" s="34" t="s">
+      <c r="A131" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C131" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D131" s="34" t="s">
+      <c r="D131" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E131" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="F131" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="G131" s="34" t="s">
+      <c r="E131" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F131" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G131" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="H131" s="36" t="s">
+      <c r="H131" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="I131" s="37" t="s">
-        <v>351</v>
+      <c r="I131" s="21" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="132" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A132" s="5" t="s">
-        <v>352</v>
+      <c r="A132" s="3" t="s">
+        <v>354</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>244</v>
@@ -8670,19 +8647,19 @@
       <c r="G132" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="H132" s="8" t="s">
+      <c r="H132" s="20" t="s">
         <v>204</v>
       </c>
       <c r="I132" s="21" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="133" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A133" s="3" t="s">
-        <v>354</v>
+      <c r="A133" s="5" t="s">
+        <v>356</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>355</v>
+        <v>244</v>
       </c>
       <c r="C133" s="6" t="s">
         <v>73</v>
@@ -8699,83 +8676,83 @@
       <c r="G133" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="H133" s="20" t="s">
+      <c r="H133" s="8" t="s">
         <v>204</v>
       </c>
       <c r="I133" s="21" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="134" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
-        <v>357</v>
+      <c r="A134" t="s">
+        <v>358</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C134" s="6" t="s">
+      <c r="C134" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="D134" s="6" t="s">
+      <c r="D134" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E134" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F134" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G134" s="6" t="s">
+      <c r="E134" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F134" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="G134" s="33" t="s">
         <v>276</v>
       </c>
-      <c r="H134" s="8" t="s">
+      <c r="H134" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="I134" s="21" t="s">
-        <v>358</v>
+      <c r="I134" s="36" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="135" spans="1:28" ht="165" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>359</v>
-      </c>
-      <c r="B135" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="C135" s="34" t="s">
+      <c r="A135" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C135" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D135" s="34" t="s">
+      <c r="D135" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E135" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="F135" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="G135" s="34" t="s">
+      <c r="E135" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G135" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="H135" s="36" t="s">
+      <c r="H135" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="I135" s="37" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="136" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="I135" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="136" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="C136" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E136" s="7" t="s">
         <v>94</v>
@@ -8787,15 +8764,15 @@
         <v>276</v>
       </c>
       <c r="H136" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="I136" s="21" t="s">
-        <v>362</v>
+        <v>205</v>
+      </c>
+      <c r="I136" s="8" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="137" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>244</v>
@@ -8819,7 +8796,7 @@
         <v>205</v>
       </c>
       <c r="I137" s="8" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
     </row>
     <row r="138" spans="1:28" ht="150" x14ac:dyDescent="0.25">
@@ -8827,10 +8804,10 @@
         <v>365</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C138" s="18" t="s">
-        <v>73</v>
+        <v>367</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="D138" s="6" t="s">
         <v>11</v>
@@ -8842,18 +8819,18 @@
         <v>94</v>
       </c>
       <c r="G138" s="6" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="H138" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="I138" s="8" t="s">
-        <v>366</v>
+      <c r="I138" s="38" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="139" spans="1:28" ht="150" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>244</v>
@@ -8873,25 +8850,25 @@
       <c r="G139" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="H139" s="8" t="s">
+      <c r="H139" s="37" t="s">
         <v>205</v>
       </c>
-      <c r="I139" s="39" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="140" spans="1:28" ht="150" x14ac:dyDescent="0.25">
-      <c r="A140" s="5" t="s">
-        <v>369</v>
+      <c r="I139" s="8" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="140" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>244</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E140" s="7" t="s">
         <v>94</v>
@@ -8900,63 +8877,40 @@
         <v>94</v>
       </c>
       <c r="G140" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="H140" s="38" t="s">
-        <v>205</v>
-      </c>
-      <c r="I140" s="8" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="141" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D141" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E141" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F141" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G141" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H141" s="38" t="s">
+      <c r="H140" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="I141" s="9"/>
-      <c r="J141" s="2"/>
-      <c r="K141" s="2"/>
-      <c r="L141" s="2"/>
-      <c r="M141" s="2"/>
-      <c r="N141" s="2"/>
-      <c r="O141" s="2"/>
-      <c r="P141" s="2"/>
-      <c r="Q141" s="2"/>
-      <c r="R141" s="2"/>
-      <c r="S141" s="2"/>
-      <c r="T141" s="2"/>
-      <c r="U141" s="2"/>
-      <c r="V141" s="2"/>
-      <c r="W141" s="2"/>
-      <c r="X141" s="2"/>
-      <c r="Y141" s="2"/>
-      <c r="Z141" s="2"/>
-      <c r="AA141" s="2"/>
-      <c r="AB141" s="2"/>
+      <c r="I140" s="9"/>
+      <c r="J140" s="2"/>
+      <c r="K140" s="2"/>
+      <c r="L140" s="2"/>
+      <c r="M140" s="2"/>
+      <c r="N140" s="2"/>
+      <c r="O140" s="2"/>
+      <c r="P140" s="2"/>
+      <c r="Q140" s="2"/>
+      <c r="R140" s="2"/>
+      <c r="S140" s="2"/>
+      <c r="T140" s="2"/>
+      <c r="U140" s="2"/>
+      <c r="V140" s="2"/>
+      <c r="W140" s="2"/>
+      <c r="X140" s="2"/>
+      <c r="Y140" s="2"/>
+      <c r="Z140" s="2"/>
+      <c r="AA140" s="2"/>
+      <c r="AB140" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I130" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I140" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a new script for vendors
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin(30-03-2023)2.3\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-web\Admin(17-04-2023)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C481E66-3390-49F0-92FE-5C0FF0C7FD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9844F779-C17C-4153-8680-D8C051DE6597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$140</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$141</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="376">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2116,6 +2116,25 @@
 -pamount,
 -ppercentage,
 -ptosHeading</t>
+  </si>
+  <si>
+    <t>testdata-admin.xlsx,vendors</t>
+  </si>
+  <si>
+    <t>SystemSettings -Vendors</t>
+  </si>
+  <si>
+    <t>coyni.admin.tests.SystemSettingsTest,
+testAddVendor,
+-pheading,
+-pvendorName,
+-pprimaryEmail,
+-pprimaryPhone,
+-pTechnicalEmail,
+-pTechnicalPhone</t>
+  </si>
+  <si>
+    <t>Add Vendors</t>
   </si>
 </sst>
 </file>
@@ -2610,33 +2629,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB140"/>
+  <dimension ref="A1:AB141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I141" sqref="I141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
-    <col min="9" max="9" width="43.140625" customWidth="1"/>
-    <col min="10" max="10" width="38.85546875" customWidth="1"/>
-    <col min="11" max="11" width="30.28515625" customWidth="1"/>
+    <col min="8" max="8" width="47.44140625" customWidth="1"/>
+    <col min="9" max="9" width="43.109375" customWidth="1"/>
+    <col min="10" max="10" width="38.88671875" customWidth="1"/>
+    <col min="11" max="11" width="30.33203125" customWidth="1"/>
     <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" customWidth="1"/>
-    <col min="14" max="14" width="25.5703125" customWidth="1"/>
+    <col min="13" max="13" width="26.44140625" customWidth="1"/>
+    <col min="14" max="14" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2670,7 +2688,7 @@
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2716,7 +2734,7 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>324</v>
       </c>
@@ -2762,7 +2780,7 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
         <v>242</v>
       </c>
@@ -2808,7 +2826,7 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" ht="150.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -2854,7 +2872,7 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
     </row>
-    <row r="6" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
@@ -2900,7 +2918,7 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>138</v>
       </c>
@@ -2946,7 +2964,7 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -2992,7 +3010,7 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" ht="210.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="202.8" x14ac:dyDescent="0.4">
       <c r="A9" s="12" t="s">
         <v>26</v>
       </c>
@@ -3038,7 +3056,7 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -3084,7 +3102,7 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>342</v>
       </c>
@@ -3130,7 +3148,7 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
     </row>
-    <row r="12" spans="1:28" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -3176,7 +3194,7 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13" spans="1:28" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -3222,7 +3240,7 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
     </row>
-    <row r="14" spans="1:28" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="216" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -3268,7 +3286,7 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
     </row>
-    <row r="15" spans="1:28" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -3314,7 +3332,7 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
     </row>
-    <row r="16" spans="1:28" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
         <v>344</v>
       </c>
@@ -3360,7 +3378,7 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
     </row>
-    <row r="17" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -3406,7 +3424,7 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
     </row>
-    <row r="18" spans="1:28" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -3452,7 +3470,7 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
     </row>
-    <row r="19" spans="1:28" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>236</v>
       </c>
@@ -3500,7 +3518,7 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
     </row>
-    <row r="20" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>127</v>
       </c>
@@ -3548,7 +3566,7 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
     </row>
-    <row r="21" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>128</v>
       </c>
@@ -3596,7 +3614,7 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
-    <row r="22" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
@@ -3644,7 +3662,7 @@
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
     </row>
-    <row r="23" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>147</v>
       </c>
@@ -3692,7 +3710,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
     </row>
-    <row r="24" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
@@ -3740,7 +3758,7 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
     </row>
-    <row r="25" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
@@ -3788,7 +3806,7 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
     </row>
-    <row r="26" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
@@ -3836,7 +3854,7 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
         <v>335</v>
       </c>
@@ -3884,7 +3902,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>337</v>
       </c>
@@ -3932,7 +3950,7 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:28" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>220</v>
       </c>
@@ -3980,7 +3998,7 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
     </row>
-    <row r="30" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>221</v>
       </c>
@@ -4028,7 +4046,7 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>222</v>
       </c>
@@ -4076,7 +4094,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:28" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>223</v>
       </c>
@@ -4124,7 +4142,7 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="1:28" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" s="2" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>143</v>
       </c>
@@ -4158,7 +4176,7 @@
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
     </row>
-    <row r="34" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
@@ -4206,7 +4224,7 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>317</v>
       </c>
@@ -4254,7 +4272,7 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>315</v>
       </c>
@@ -4302,7 +4320,7 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>97</v>
       </c>
@@ -4350,7 +4368,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>99</v>
       </c>
@@ -4398,7 +4416,7 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>101</v>
       </c>
@@ -4446,7 +4464,7 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>103</v>
       </c>
@@ -4494,7 +4512,7 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>105</v>
       </c>
@@ -4542,7 +4560,7 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
         <v>320</v>
       </c>
@@ -4590,7 +4608,7 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
@@ -4638,7 +4656,7 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>167</v>
       </c>
@@ -4686,7 +4704,7 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
@@ -4734,7 +4752,7 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>48</v>
       </c>
@@ -4782,7 +4800,7 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
@@ -4830,7 +4848,7 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>52</v>
       </c>
@@ -4878,7 +4896,7 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
@@ -4926,7 +4944,7 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
@@ -4974,7 +4992,7 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>58</v>
       </c>
@@ -5022,7 +5040,7 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>60</v>
       </c>
@@ -5070,7 +5088,7 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>62</v>
       </c>
@@ -5118,7 +5136,7 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>64</v>
       </c>
@@ -5166,7 +5184,7 @@
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
     </row>
-    <row r="55" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>66</v>
       </c>
@@ -5214,7 +5232,7 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>68</v>
       </c>
@@ -5262,7 +5280,7 @@
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>133</v>
       </c>
@@ -5310,7 +5328,7 @@
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
     </row>
-    <row r="58" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>70</v>
       </c>
@@ -5358,7 +5376,7 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>141</v>
       </c>
@@ -5406,7 +5424,7 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>145</v>
       </c>
@@ -5454,7 +5472,7 @@
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" spans="1:28" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" s="2" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>117</v>
       </c>
@@ -5488,7 +5506,7 @@
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
     </row>
-    <row r="62" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>119</v>
       </c>
@@ -5536,7 +5554,7 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>120</v>
       </c>
@@ -5584,7 +5602,7 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" ht="214.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" ht="214.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>321</v>
       </c>
@@ -5632,7 +5650,7 @@
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
     </row>
-    <row r="65" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>122</v>
       </c>
@@ -5680,7 +5698,7 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>125</v>
       </c>
@@ -5728,7 +5746,7 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>171</v>
       </c>
@@ -5776,7 +5794,7 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>172</v>
       </c>
@@ -5824,7 +5842,7 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>170</v>
       </c>
@@ -5872,7 +5890,7 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A70" s="24" t="s">
         <v>174</v>
       </c>
@@ -5920,7 +5938,7 @@
       <c r="AA70" s="2"/>
       <c r="AB70" s="2"/>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>175</v>
       </c>
@@ -5968,7 +5986,7 @@
       <c r="AA71" s="2"/>
       <c r="AB71" s="2"/>
     </row>
-    <row r="72" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>176</v>
       </c>
@@ -6016,7 +6034,7 @@
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
     </row>
-    <row r="73" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>177</v>
       </c>
@@ -6064,7 +6082,7 @@
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
     </row>
-    <row r="74" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>178</v>
       </c>
@@ -6112,7 +6130,7 @@
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
     </row>
-    <row r="75" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>173</v>
       </c>
@@ -6160,7 +6178,7 @@
       <c r="AA75" s="2"/>
       <c r="AB75" s="2"/>
     </row>
-    <row r="76" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A76" s="25" t="s">
         <v>243</v>
       </c>
@@ -6189,7 +6207,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>245</v>
       </c>
@@ -6218,7 +6236,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>248</v>
       </c>
@@ -6247,7 +6265,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>255</v>
       </c>
@@ -6276,7 +6294,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>252</v>
       </c>
@@ -6305,7 +6323,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>254</v>
       </c>
@@ -6334,7 +6352,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>257</v>
       </c>
@@ -6363,7 +6381,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>259</v>
       </c>
@@ -6392,12 +6410,12 @@
         <v>260</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>261</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>367</v>
+        <v>244</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>123</v>
@@ -6421,7 +6439,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>263</v>
       </c>
@@ -6450,7 +6468,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>271</v>
       </c>
@@ -6479,12 +6497,12 @@
         <v>272</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>367</v>
+        <v>244</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>136</v>
@@ -6527,7 +6545,7 @@
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>161</v>
       </c>
@@ -6575,7 +6593,7 @@
       <c r="AA88" s="2"/>
       <c r="AB88" s="2"/>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>163</v>
       </c>
@@ -6623,7 +6641,7 @@
       <c r="AA89" s="2"/>
       <c r="AB89" s="2"/>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>165</v>
       </c>
@@ -6673,7 +6691,7 @@
       <c r="AA90" s="2"/>
       <c r="AB90" s="2"/>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>347</v>
       </c>
@@ -6721,7 +6739,7 @@
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
     </row>
-    <row r="92" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>81</v>
       </c>
@@ -6769,7 +6787,7 @@
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
     </row>
-    <row r="93" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>84</v>
       </c>
@@ -6817,7 +6835,7 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>86</v>
       </c>
@@ -6865,7 +6883,7 @@
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
     </row>
-    <row r="95" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>88</v>
       </c>
@@ -6913,7 +6931,7 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>90</v>
       </c>
@@ -6961,7 +6979,7 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A97" s="26" t="s">
         <v>273</v>
       </c>
@@ -7009,7 +7027,7 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>92</v>
       </c>
@@ -7057,7 +7075,7 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>208</v>
       </c>
@@ -7105,12 +7123,12 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="100" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>212</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>367</v>
+        <v>244</v>
       </c>
       <c r="C100" s="9" t="s">
         <v>209</v>
@@ -7153,7 +7171,7 @@
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
     </row>
-    <row r="101" spans="1:28" ht="175.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>214</v>
       </c>
@@ -7201,12 +7219,12 @@
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
     </row>
-    <row r="102" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>159</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>367</v>
+        <v>244</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>77</v>
@@ -7249,7 +7267,7 @@
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
     </row>
-    <row r="103" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>113</v>
       </c>
@@ -7297,7 +7315,7 @@
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
     </row>
-    <row r="104" spans="1:28" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>79</v>
       </c>
@@ -7345,7 +7363,7 @@
       <c r="AA104" s="2"/>
       <c r="AB104" s="2"/>
     </row>
-    <row r="105" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>72</v>
       </c>
@@ -7393,7 +7411,7 @@
       <c r="AA105" s="2"/>
       <c r="AB105" s="2"/>
     </row>
-    <row r="106" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>275</v>
       </c>
@@ -7441,7 +7459,7 @@
       <c r="AA106" s="2"/>
       <c r="AB106" s="2"/>
     </row>
-    <row r="107" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>278</v>
       </c>
@@ -7489,12 +7507,12 @@
       <c r="AA107" s="2"/>
       <c r="AB107" s="2"/>
     </row>
-    <row r="108" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>280</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>367</v>
+        <v>244</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>73</v>
@@ -7537,12 +7555,12 @@
       <c r="AA108" s="2"/>
       <c r="AB108" s="2"/>
     </row>
-    <row r="109" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>367</v>
+        <v>244</v>
       </c>
       <c r="C109" s="18" t="s">
         <v>73</v>
@@ -7585,7 +7603,7 @@
       <c r="AA109" s="2"/>
       <c r="AB109" s="2"/>
     </row>
-    <row r="110" spans="1:28" s="1" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>76</v>
       </c>
@@ -7633,12 +7651,12 @@
       <c r="AA110" s="2"/>
       <c r="AB110" s="2"/>
     </row>
-    <row r="111" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>367</v>
+        <v>244</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>114</v>
@@ -7681,7 +7699,7 @@
       <c r="AA111" s="2"/>
       <c r="AB111" s="2"/>
     </row>
-    <row r="112" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>286</v>
       </c>
@@ -7729,12 +7747,12 @@
       <c r="AA112" s="2"/>
       <c r="AB112" s="2"/>
     </row>
-    <row r="113" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>291</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>367</v>
+        <v>244</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>288</v>
@@ -7777,7 +7795,7 @@
       <c r="AA113" s="2"/>
       <c r="AB113" s="2"/>
     </row>
-    <row r="114" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>293</v>
       </c>
@@ -7825,7 +7843,7 @@
       <c r="AA114" s="2"/>
       <c r="AB114" s="2"/>
     </row>
-    <row r="115" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="11" t="s">
         <v>110</v>
       </c>
@@ -7873,7 +7891,7 @@
       <c r="AA115" s="2"/>
       <c r="AB115" s="2"/>
     </row>
-    <row r="116" spans="1:28" s="1" customFormat="1" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:28" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="11" t="s">
         <v>109</v>
       </c>
@@ -7921,7 +7939,7 @@
       <c r="AA116" s="2"/>
       <c r="AB116" s="2"/>
     </row>
-    <row r="117" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>151</v>
       </c>
@@ -7969,7 +7987,7 @@
       <c r="AA117" s="2"/>
       <c r="AB117" s="2"/>
     </row>
-    <row r="118" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>154</v>
       </c>
@@ -8017,7 +8035,7 @@
       <c r="AA118" s="2"/>
       <c r="AB118" s="2"/>
     </row>
-    <row r="119" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>269</v>
       </c>
@@ -8065,7 +8083,7 @@
       <c r="AA119" s="2"/>
       <c r="AB119" s="2"/>
     </row>
-    <row r="120" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>267</v>
       </c>
@@ -8113,7 +8131,7 @@
       <c r="AA120" s="2"/>
       <c r="AB120" s="2"/>
     </row>
-    <row r="121" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>265</v>
       </c>
@@ -8161,7 +8179,7 @@
       <c r="AA121" s="2"/>
       <c r="AB121" s="2"/>
     </row>
-    <row r="122" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>332</v>
       </c>
@@ -8209,7 +8227,7 @@
       <c r="AA122" s="2"/>
       <c r="AB122" s="2"/>
     </row>
-    <row r="123" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>156</v>
       </c>
@@ -8257,7 +8275,7 @@
       <c r="AA123" s="2"/>
       <c r="AB123" s="2"/>
     </row>
-    <row r="124" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:28" s="1" customFormat="1" ht="288" x14ac:dyDescent="0.3">
       <c r="A124" s="11" t="s">
         <v>179</v>
       </c>
@@ -8305,7 +8323,7 @@
       <c r="AA124" s="2"/>
       <c r="AB124" s="2"/>
     </row>
-    <row r="125" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A125" s="11" t="s">
         <v>181</v>
       </c>
@@ -8357,7 +8375,7 @@
       <c r="AA125" s="2"/>
       <c r="AB125" s="2"/>
     </row>
-    <row r="126" spans="1:28" s="1" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:28" s="1" customFormat="1" ht="288" x14ac:dyDescent="0.3">
       <c r="A126" s="11" t="s">
         <v>182</v>
       </c>
@@ -8415,7 +8433,7 @@
       <c r="AA126" s="2"/>
       <c r="AB126" s="2"/>
     </row>
-    <row r="127" spans="1:28" s="1" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:28" s="1" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="22" t="s">
         <v>226</v>
       </c>
@@ -8467,7 +8485,7 @@
       <c r="AA127" s="2"/>
       <c r="AB127" s="2"/>
     </row>
-    <row r="128" spans="1:28" s="1" customFormat="1" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="11" t="s">
         <v>228</v>
       </c>
@@ -8515,7 +8533,7 @@
       <c r="AA128" s="2"/>
       <c r="AB128" s="2"/>
     </row>
-    <row r="129" spans="1:28" s="1" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:28" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A129" s="11" t="s">
         <v>235</v>
       </c>
@@ -8567,7 +8585,7 @@
       <c r="AA129" s="2"/>
       <c r="AB129" s="2"/>
     </row>
-    <row r="130" spans="1:28" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>350</v>
       </c>
@@ -8596,7 +8614,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="131" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>352</v>
       </c>
@@ -8625,7 +8643,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="132" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>354</v>
       </c>
@@ -8654,7 +8672,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="133" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>356</v>
       </c>
@@ -8683,7 +8701,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="134" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>358</v>
       </c>
@@ -8712,7 +8730,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="135" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:28" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>360</v>
       </c>
@@ -8741,7 +8759,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="136" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>362</v>
       </c>
@@ -8770,7 +8788,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="137" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>364</v>
       </c>
@@ -8799,12 +8817,12 @@
         <v>370</v>
       </c>
     </row>
-    <row r="138" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>365</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>367</v>
+        <v>244</v>
       </c>
       <c r="C138" s="6" t="s">
         <v>114</v>
@@ -8828,7 +8846,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="139" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:28" ht="144" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>366</v>
       </c>
@@ -8857,7 +8875,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="140" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:28" s="1" customFormat="1" ht="182.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>233</v>
       </c>
@@ -8903,14 +8921,37 @@
       <c r="AA140" s="2"/>
       <c r="AB140" s="2"/>
     </row>
+    <row r="141" spans="1:28" ht="144" x14ac:dyDescent="0.3">
+      <c r="A141" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="D141" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E141" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F141" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G141" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="H141" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="I141" s="19" t="s">
+        <v>374</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I140" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I141" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Test Script with Portal Option
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/TestScript-admin.xlsx
+++ b/Web/coyni/resources/TestScript-admin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Coyni 2.3\2023\042523_Web_2.3\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Coyni 2.3\2023\042523_Web_2.3_1\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6FD3D7-9F50-49EA-BF40-D74956FFC8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B6628B-4BCF-44B0-B50E-BA1F78AACBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$135</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="415">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -2413,6 +2413,9 @@
 -preason,
 -ptoastTitle,
 -ptoastWithdrawMessage</t>
+  </si>
+  <si>
+    <t>Portal</t>
   </si>
 </sst>
 </file>
@@ -2557,7 +2560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2635,6 +2638,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2917,9 +2921,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A151" sqref="A151"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H143" sqref="H143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2931,16 +2935,17 @@
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
-    <col min="9" max="9" width="43.140625" customWidth="1"/>
-    <col min="10" max="10" width="38.85546875" customWidth="1"/>
-    <col min="11" max="11" width="30.28515625" customWidth="1"/>
-    <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" customWidth="1"/>
-    <col min="14" max="14" width="25.5703125" customWidth="1"/>
+    <col min="8" max="8" width="36" customWidth="1"/>
+    <col min="9" max="9" width="47.42578125" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" customWidth="1"/>
+    <col min="11" max="11" width="38.85546875" customWidth="1"/>
+    <col min="12" max="12" width="30.28515625" customWidth="1"/>
+    <col min="13" max="13" width="26" customWidth="1"/>
+    <col min="14" max="14" width="26.42578125" customWidth="1"/>
+    <col min="15" max="15" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2963,18 +2968,21 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:29" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2996,16 +3004,16 @@
       <c r="G2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
-      <c r="O2" s="2"/>
+      <c r="O2" s="9"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -3019,8 +3027,9 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
-    </row>
-    <row r="3" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC2" s="2"/>
+    </row>
+    <row r="3" spans="1:29" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>307</v>
       </c>
@@ -3042,16 +3051,16 @@
       <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
-      <c r="O3" s="2"/>
+      <c r="O3" s="9"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -3065,8 +3074,9 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
-    </row>
-    <row r="4" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC3" s="2"/>
+    </row>
+    <row r="4" spans="1:29" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>225</v>
       </c>
@@ -3088,16 +3098,16 @@
       <c r="G4" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="27"/>
+      <c r="I4" s="29" t="s">
         <v>323</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="9"/>
+      <c r="J4" s="30"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="2"/>
+      <c r="O4" s="9"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
@@ -3111,8 +3121,9 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
-    </row>
-    <row r="5" spans="1:28" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC4" s="2"/>
+    </row>
+    <row r="5" spans="1:29" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -3134,16 +3145,16 @@
       <c r="G5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="2"/>
+      <c r="O5" s="9"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -3157,8 +3168,9 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
-    </row>
-    <row r="6" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC5" s="2"/>
+    </row>
+    <row r="6" spans="1:29" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
@@ -3180,16 +3192,16 @@
       <c r="G6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="2"/>
+      <c r="O6" s="9"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
@@ -3203,8 +3215,9 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
-    </row>
-    <row r="7" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC6" s="2"/>
+    </row>
+    <row r="7" spans="1:29" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>138</v>
       </c>
@@ -3226,16 +3239,16 @@
       <c r="G7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="2"/>
+      <c r="O7" s="9"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -3249,8 +3262,9 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
-    </row>
-    <row r="8" spans="1:28" ht="240" x14ac:dyDescent="0.25">
+      <c r="AC7" s="2"/>
+    </row>
+    <row r="8" spans="1:29" ht="240" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -3272,16 +3286,16 @@
       <c r="G8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="2"/>
+      <c r="O8" s="9"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -3295,8 +3309,9 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
-    </row>
-    <row r="9" spans="1:28" ht="210.75" x14ac:dyDescent="0.3">
+      <c r="AC8" s="2"/>
+    </row>
+    <row r="9" spans="1:29" ht="210.75" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>26</v>
       </c>
@@ -3318,16 +3333,16 @@
       <c r="G9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="6"/>
+      <c r="I9" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="2"/>
+      <c r="O9" s="9"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -3341,8 +3356,9 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
-    </row>
-    <row r="10" spans="1:28" ht="210" x14ac:dyDescent="0.25">
+      <c r="AC9" s="2"/>
+    </row>
+    <row r="10" spans="1:29" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>27</v>
       </c>
@@ -3364,16 +3380,16 @@
       <c r="G10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="27"/>
+      <c r="I10" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="2"/>
+      <c r="O10" s="9"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -3387,8 +3403,9 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
-    </row>
-    <row r="11" spans="1:28" ht="180" x14ac:dyDescent="0.25">
+      <c r="AC10" s="2"/>
+    </row>
+    <row r="11" spans="1:29" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>325</v>
       </c>
@@ -3410,16 +3427,16 @@
       <c r="G11" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="27"/>
+      <c r="I11" s="29" t="s">
         <v>326</v>
       </c>
-      <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="2"/>
+      <c r="O11" s="9"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -3433,8 +3450,9 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
-    </row>
-    <row r="12" spans="1:28" ht="120" x14ac:dyDescent="0.25">
+      <c r="AC11" s="2"/>
+    </row>
+    <row r="12" spans="1:29" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -3456,16 +3474,16 @@
       <c r="G12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="6"/>
+      <c r="I12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
-      <c r="O12" s="2"/>
+      <c r="O12" s="9"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -3479,8 +3497,9 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
-    </row>
-    <row r="13" spans="1:28" ht="255" x14ac:dyDescent="0.25">
+      <c r="AC12" s="2"/>
+    </row>
+    <row r="13" spans="1:29" ht="255" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -3502,16 +3521,16 @@
       <c r="G13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="6"/>
+      <c r="I13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
-      <c r="O13" s="2"/>
+      <c r="O13" s="9"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -3525,8 +3544,9 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
-    </row>
-    <row r="14" spans="1:28" ht="225" x14ac:dyDescent="0.25">
+      <c r="AC13" s="2"/>
+    </row>
+    <row r="14" spans="1:29" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -3548,16 +3568,16 @@
       <c r="G14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="6"/>
+      <c r="I14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="2"/>
+      <c r="O14" s="9"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -3571,8 +3591,9 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
-    </row>
-    <row r="15" spans="1:28" ht="210" x14ac:dyDescent="0.25">
+      <c r="AC14" s="2"/>
+    </row>
+    <row r="15" spans="1:29" ht="210" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -3594,16 +3615,16 @@
       <c r="G15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="6"/>
+      <c r="I15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
-      <c r="O15" s="2"/>
+      <c r="O15" s="9"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -3617,8 +3638,9 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
-    </row>
-    <row r="16" spans="1:28" ht="240" x14ac:dyDescent="0.25">
+      <c r="AC15" s="2"/>
+    </row>
+    <row r="16" spans="1:29" ht="240" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>327</v>
       </c>
@@ -3640,16 +3662,16 @@
       <c r="G16" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="27"/>
+      <c r="I16" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="2"/>
+      <c r="O16" s="9"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -3663,8 +3685,9 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
-    </row>
-    <row r="17" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="AC16" s="2"/>
+    </row>
+    <row r="17" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -3686,16 +3709,16 @@
       <c r="G17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="6"/>
+      <c r="I17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="2"/>
+      <c r="O17" s="9"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -3709,8 +3732,9 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
-    </row>
-    <row r="18" spans="1:28" ht="195" x14ac:dyDescent="0.25">
+      <c r="AC17" s="2"/>
+    </row>
+    <row r="18" spans="1:29" ht="195" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -3732,16 +3756,16 @@
       <c r="G18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="6"/>
+      <c r="I18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="2"/>
+      <c r="O18" s="9"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -3755,8 +3779,9 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
-    </row>
-    <row r="19" spans="1:28" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC18" s="2"/>
+    </row>
+    <row r="19" spans="1:29" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>219</v>
       </c>
@@ -3778,18 +3803,18 @@
       <c r="G19" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="14"/>
+      <c r="I19" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="J19" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="2"/>
+      <c r="O19" s="9"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -3803,8 +3828,9 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
-    </row>
-    <row r="20" spans="1:28" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="AC19" s="2"/>
+    </row>
+    <row r="20" spans="1:29" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>127</v>
       </c>
@@ -3826,18 +3852,18 @@
       <c r="G20" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="14"/>
+      <c r="I20" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="J20" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="2"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="9"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -3851,8 +3877,9 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
-    </row>
-    <row r="21" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+      <c r="AC20" s="2"/>
+    </row>
+    <row r="21" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>128</v>
       </c>
@@ -3874,18 +3901,18 @@
       <c r="G21" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="14"/>
+      <c r="I21" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="J21" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="2"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="9"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
@@ -3899,8 +3926,9 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
-    </row>
-    <row r="22" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+      <c r="AC21" s="2"/>
+    </row>
+    <row r="22" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>130</v>
       </c>
@@ -3922,18 +3950,18 @@
       <c r="G22" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="14"/>
+      <c r="I22" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="J22" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="2"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="9"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
@@ -3947,8 +3975,9 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
-    </row>
-    <row r="23" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+      <c r="AC22" s="2"/>
+    </row>
+    <row r="23" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>147</v>
       </c>
@@ -3970,18 +3999,18 @@
       <c r="G23" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="14"/>
+      <c r="I23" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="J23" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="2"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="9"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
@@ -3995,8 +4024,9 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
-    </row>
-    <row r="24" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+      <c r="AC23" s="2"/>
+    </row>
+    <row r="24" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
@@ -4018,18 +4048,18 @@
       <c r="G24" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="6"/>
+      <c r="I24" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="J24" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="2"/>
+      <c r="O24" s="9"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
@@ -4043,8 +4073,9 @@
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
-    </row>
-    <row r="25" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+      <c r="AC24" s="2"/>
+    </row>
+    <row r="25" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
@@ -4066,18 +4097,18 @@
       <c r="G25" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="6"/>
+      <c r="I25" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="9"/>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
-      <c r="O25" s="2"/>
+      <c r="O25" s="9"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
@@ -4091,8 +4122,9 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
-    </row>
-    <row r="26" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC25" s="2"/>
+    </row>
+    <row r="26" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
@@ -4114,18 +4146,18 @@
       <c r="G26" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="8"/>
+      <c r="I26" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="J26" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J26" s="9"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
-      <c r="O26" s="2"/>
+      <c r="O26" s="9"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
@@ -4139,8 +4171,9 @@
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
-    </row>
-    <row r="27" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC26" s="2"/>
+    </row>
+    <row r="27" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
         <v>318</v>
       </c>
@@ -4162,18 +4195,18 @@
       <c r="G27" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="8"/>
+      <c r="I27" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="J27" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
-      <c r="O27" s="2"/>
+      <c r="O27" s="9"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
@@ -4187,8 +4220,9 @@
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
-    </row>
-    <row r="28" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC27" s="2"/>
+    </row>
+    <row r="28" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>320</v>
       </c>
@@ -4210,18 +4244,18 @@
       <c r="G28" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="8"/>
+      <c r="I28" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="J28" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
-      <c r="O28" s="2"/>
+      <c r="O28" s="9"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
@@ -4235,8 +4269,9 @@
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
-    </row>
-    <row r="29" spans="1:28" ht="270" x14ac:dyDescent="0.25">
+      <c r="AC28" s="2"/>
+    </row>
+    <row r="29" spans="1:29" ht="270" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>209</v>
       </c>
@@ -4258,18 +4293,18 @@
       <c r="G29" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="6"/>
+      <c r="I29" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="J29" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
-      <c r="O29" s="2"/>
+      <c r="O29" s="9"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
@@ -4283,8 +4318,9 @@
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
-    </row>
-    <row r="30" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC29" s="2"/>
+    </row>
+    <row r="30" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>210</v>
       </c>
@@ -4306,18 +4342,18 @@
       <c r="G30" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="6"/>
+      <c r="I30" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="J30" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
-      <c r="O30" s="2"/>
+      <c r="O30" s="9"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
@@ -4331,8 +4367,9 @@
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
-    </row>
-    <row r="31" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC30" s="2"/>
+    </row>
+    <row r="31" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>211</v>
       </c>
@@ -4354,18 +4391,18 @@
       <c r="G31" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H31" s="6"/>
+      <c r="I31" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I31" s="8" t="s">
+      <c r="J31" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
-      <c r="O31" s="2"/>
+      <c r="O31" s="9"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
@@ -4379,8 +4416,9 @@
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
-    </row>
-    <row r="32" spans="1:28" ht="285" x14ac:dyDescent="0.25">
+      <c r="AC31" s="2"/>
+    </row>
+    <row r="32" spans="1:29" ht="285" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>212</v>
       </c>
@@ -4402,18 +4440,18 @@
       <c r="G32" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="6"/>
+      <c r="I32" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="J32" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
-      <c r="O32" s="2"/>
+      <c r="O32" s="9"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
@@ -4427,8 +4465,9 @@
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
-    </row>
-    <row r="33" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC32" s="2"/>
+    </row>
+    <row r="33" spans="1:29" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>143</v>
       </c>
@@ -4450,19 +4489,20 @@
       <c r="G33" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="6"/>
+      <c r="I33" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I33" s="19" t="s">
+      <c r="J33" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="J33" s="9"/>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
-    </row>
-    <row r="34" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="O33" s="9"/>
+    </row>
+    <row r="34" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
@@ -4484,18 +4524,18 @@
       <c r="G34" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="6"/>
+      <c r="I34" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I34" s="20" t="s">
+      <c r="J34" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
-      <c r="O34" s="2"/>
+      <c r="O34" s="9"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
@@ -4509,8 +4549,9 @@
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
-    </row>
-    <row r="35" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="AC34" s="2"/>
+    </row>
+    <row r="35" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>300</v>
       </c>
@@ -4532,18 +4573,18 @@
       <c r="G35" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="6"/>
+      <c r="I35" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I35" s="20" t="s">
+      <c r="J35" s="20" t="s">
         <v>301</v>
       </c>
-      <c r="J35" s="9"/>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="9"/>
-      <c r="O35" s="2"/>
+      <c r="O35" s="9"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
@@ -4557,8 +4598,9 @@
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
-    </row>
-    <row r="36" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="AC35" s="2"/>
+    </row>
+    <row r="36" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>298</v>
       </c>
@@ -4580,18 +4622,18 @@
       <c r="G36" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H36" s="6"/>
+      <c r="I36" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I36" s="20" t="s">
+      <c r="J36" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="J36" s="9"/>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
-      <c r="O36" s="2"/>
+      <c r="O36" s="9"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
@@ -4605,8 +4647,9 @@
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
-    </row>
-    <row r="37" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC36" s="2"/>
+    </row>
+    <row r="37" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>97</v>
       </c>
@@ -4628,18 +4671,18 @@
       <c r="G37" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H37" s="6"/>
+      <c r="I37" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="J37" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
-      <c r="O37" s="2"/>
+      <c r="O37" s="9"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
@@ -4653,8 +4696,9 @@
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
-    </row>
-    <row r="38" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC37" s="2"/>
+    </row>
+    <row r="38" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>99</v>
       </c>
@@ -4676,18 +4720,18 @@
       <c r="G38" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="H38" s="6"/>
+      <c r="I38" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="J38" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
-      <c r="O38" s="2"/>
+      <c r="O38" s="9"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
@@ -4701,8 +4745,9 @@
       <c r="Z38" s="2"/>
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
-    </row>
-    <row r="39" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC38" s="2"/>
+    </row>
+    <row r="39" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>101</v>
       </c>
@@ -4724,18 +4769,18 @@
       <c r="G39" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H39" s="6"/>
+      <c r="I39" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="J39" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="J39" s="9"/>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
-      <c r="O39" s="2"/>
+      <c r="O39" s="9"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
@@ -4749,8 +4794,9 @@
       <c r="Z39" s="2"/>
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
-    </row>
-    <row r="40" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC39" s="2"/>
+    </row>
+    <row r="40" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>103</v>
       </c>
@@ -4772,18 +4818,18 @@
       <c r="G40" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H40" s="8" t="s">
+      <c r="H40" s="6"/>
+      <c r="I40" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I40" s="8" t="s">
+      <c r="J40" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="J40" s="9"/>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
-      <c r="O40" s="2"/>
+      <c r="O40" s="9"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
@@ -4797,8 +4843,9 @@
       <c r="Z40" s="2"/>
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
-    </row>
-    <row r="41" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC40" s="2"/>
+    </row>
+    <row r="41" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>105</v>
       </c>
@@ -4820,18 +4867,18 @@
       <c r="G41" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H41" s="8" t="s">
+      <c r="H41" s="6"/>
+      <c r="I41" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="J41" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="J41" s="9"/>
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
       <c r="N41" s="9"/>
-      <c r="O41" s="2"/>
+      <c r="O41" s="9"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
@@ -4845,8 +4892,9 @@
       <c r="Z41" s="2"/>
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
-    </row>
-    <row r="42" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC41" s="2"/>
+    </row>
+    <row r="42" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>303</v>
       </c>
@@ -4868,18 +4916,18 @@
       <c r="G42" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="H42" s="6"/>
+      <c r="I42" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="J42" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="J42" s="9"/>
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
       <c r="M42" s="9"/>
       <c r="N42" s="9"/>
-      <c r="O42" s="2"/>
+      <c r="O42" s="9"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
@@ -4893,8 +4941,9 @@
       <c r="Z42" s="2"/>
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
-    </row>
-    <row r="43" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC42" s="2"/>
+    </row>
+    <row r="43" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
@@ -4916,18 +4965,18 @@
       <c r="G43" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H43" s="6"/>
+      <c r="I43" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="J43" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="J43" s="6"/>
-      <c r="K43" s="9"/>
+      <c r="K43" s="6"/>
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
-      <c r="O43" s="2"/>
+      <c r="O43" s="9"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
@@ -4941,8 +4990,9 @@
       <c r="Z43" s="2"/>
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
-    </row>
-    <row r="44" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC43" s="2"/>
+    </row>
+    <row r="44" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>167</v>
       </c>
@@ -4964,18 +5014,18 @@
       <c r="G44" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H44" s="6"/>
+      <c r="I44" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="J44" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="J44" s="6"/>
-      <c r="K44" s="9"/>
+      <c r="K44" s="6"/>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
-      <c r="O44" s="2"/>
+      <c r="O44" s="9"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
@@ -4989,8 +5039,9 @@
       <c r="Z44" s="2"/>
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
-    </row>
-    <row r="45" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC44" s="2"/>
+    </row>
+    <row r="45" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>46</v>
       </c>
@@ -5012,18 +5063,18 @@
       <c r="G45" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="H45" s="8" t="s">
+      <c r="H45" s="6"/>
+      <c r="I45" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="J45" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J45" s="6"/>
-      <c r="K45" s="9"/>
+      <c r="K45" s="6"/>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
-      <c r="O45" s="2"/>
+      <c r="O45" s="9"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
@@ -5037,8 +5088,9 @@
       <c r="Z45" s="2"/>
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
-    </row>
-    <row r="46" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC45" s="2"/>
+    </row>
+    <row r="46" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>48</v>
       </c>
@@ -5060,18 +5112,18 @@
       <c r="G46" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="H46" s="8" t="s">
+      <c r="H46" s="6"/>
+      <c r="I46" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I46" s="8" t="s">
+      <c r="J46" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J46" s="6"/>
-      <c r="K46" s="9"/>
+      <c r="K46" s="6"/>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
       <c r="N46" s="9"/>
-      <c r="O46" s="2"/>
+      <c r="O46" s="9"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
@@ -5085,8 +5137,9 @@
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
-    </row>
-    <row r="47" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC46" s="2"/>
+    </row>
+    <row r="47" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
@@ -5108,18 +5161,18 @@
       <c r="G47" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="H47" s="8" t="s">
+      <c r="H47" s="6"/>
+      <c r="I47" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I47" s="8" t="s">
+      <c r="J47" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="J47" s="6"/>
-      <c r="K47" s="9"/>
+      <c r="K47" s="6"/>
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
       <c r="N47" s="9"/>
-      <c r="O47" s="2"/>
+      <c r="O47" s="9"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
@@ -5133,8 +5186,9 @@
       <c r="Z47" s="2"/>
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
-    </row>
-    <row r="48" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC47" s="2"/>
+    </row>
+    <row r="48" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>52</v>
       </c>
@@ -5156,18 +5210,18 @@
       <c r="G48" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="H48" s="6"/>
+      <c r="I48" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="J48" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J48" s="6"/>
-      <c r="K48" s="9"/>
+      <c r="K48" s="6"/>
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
       <c r="N48" s="9"/>
-      <c r="O48" s="2"/>
+      <c r="O48" s="9"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
@@ -5181,8 +5235,9 @@
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
-    </row>
-    <row r="49" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC48" s="2"/>
+    </row>
+    <row r="49" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
@@ -5204,18 +5259,18 @@
       <c r="G49" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="H49" s="8" t="s">
+      <c r="H49" s="6"/>
+      <c r="I49" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I49" s="8" t="s">
+      <c r="J49" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="J49" s="6"/>
-      <c r="K49" s="9"/>
+      <c r="K49" s="6"/>
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
       <c r="N49" s="9"/>
-      <c r="O49" s="2"/>
+      <c r="O49" s="9"/>
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
@@ -5229,8 +5284,9 @@
       <c r="Z49" s="2"/>
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
-    </row>
-    <row r="50" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC49" s="2"/>
+    </row>
+    <row r="50" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
@@ -5252,18 +5308,18 @@
       <c r="G50" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="H50" s="8" t="s">
+      <c r="H50" s="6"/>
+      <c r="I50" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="J50" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="J50" s="6"/>
       <c r="K50" s="6"/>
-      <c r="L50" s="9"/>
+      <c r="L50" s="6"/>
       <c r="M50" s="9"/>
       <c r="N50" s="9"/>
-      <c r="O50" s="2"/>
+      <c r="O50" s="9"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
@@ -5277,8 +5333,9 @@
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
-    </row>
-    <row r="51" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC50" s="2"/>
+    </row>
+    <row r="51" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>58</v>
       </c>
@@ -5300,18 +5357,18 @@
       <c r="G51" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="H51" s="8" t="s">
+      <c r="H51" s="6"/>
+      <c r="I51" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I51" s="8" t="s">
+      <c r="J51" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="J51" s="6"/>
       <c r="K51" s="6"/>
-      <c r="L51" s="9"/>
+      <c r="L51" s="6"/>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
-      <c r="O51" s="2"/>
+      <c r="O51" s="9"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
@@ -5325,8 +5382,9 @@
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
-    </row>
-    <row r="52" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC51" s="2"/>
+    </row>
+    <row r="52" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>60</v>
       </c>
@@ -5348,18 +5406,18 @@
       <c r="G52" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="H52" s="6"/>
+      <c r="I52" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I52" s="8" t="s">
+      <c r="J52" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="J52" s="6"/>
       <c r="K52" s="6"/>
-      <c r="L52" s="9"/>
+      <c r="L52" s="6"/>
       <c r="M52" s="9"/>
       <c r="N52" s="9"/>
-      <c r="O52" s="2"/>
+      <c r="O52" s="9"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
@@ -5373,8 +5431,9 @@
       <c r="Z52" s="2"/>
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
-    </row>
-    <row r="53" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC52" s="2"/>
+    </row>
+    <row r="53" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>62</v>
       </c>
@@ -5396,18 +5455,18 @@
       <c r="G53" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="H53" s="8" t="s">
+      <c r="H53" s="6"/>
+      <c r="I53" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I53" s="8" t="s">
+      <c r="J53" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J53" s="6"/>
       <c r="K53" s="6"/>
-      <c r="L53" s="9"/>
+      <c r="L53" s="6"/>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
-      <c r="O53" s="2"/>
+      <c r="O53" s="9"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
@@ -5421,8 +5480,9 @@
       <c r="Z53" s="2"/>
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
-    </row>
-    <row r="54" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC53" s="2"/>
+    </row>
+    <row r="54" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>64</v>
       </c>
@@ -5444,18 +5504,18 @@
       <c r="G54" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="H54" s="8" t="s">
+      <c r="H54" s="6"/>
+      <c r="I54" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I54" s="8" t="s">
+      <c r="J54" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="J54" s="6"/>
       <c r="K54" s="6"/>
-      <c r="L54" s="9"/>
+      <c r="L54" s="6"/>
       <c r="M54" s="9"/>
       <c r="N54" s="9"/>
-      <c r="O54" s="2"/>
+      <c r="O54" s="9"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
@@ -5469,8 +5529,9 @@
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
-    </row>
-    <row r="55" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC54" s="2"/>
+    </row>
+    <row r="55" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>66</v>
       </c>
@@ -5492,18 +5553,18 @@
       <c r="G55" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="H55" s="8" t="s">
+      <c r="H55" s="6"/>
+      <c r="I55" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="J55" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="J55" s="6"/>
       <c r="K55" s="6"/>
-      <c r="L55" s="9"/>
+      <c r="L55" s="6"/>
       <c r="M55" s="9"/>
       <c r="N55" s="9"/>
-      <c r="O55" s="2"/>
+      <c r="O55" s="9"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
@@ -5517,8 +5578,9 @@
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
-    </row>
-    <row r="56" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC55" s="2"/>
+    </row>
+    <row r="56" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>68</v>
       </c>
@@ -5540,18 +5602,18 @@
       <c r="G56" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="H56" s="8" t="s">
+      <c r="H56" s="6"/>
+      <c r="I56" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I56" s="8" t="s">
+      <c r="J56" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="J56" s="6"/>
       <c r="K56" s="6"/>
-      <c r="L56" s="9"/>
+      <c r="L56" s="6"/>
       <c r="M56" s="9"/>
       <c r="N56" s="9"/>
-      <c r="O56" s="2"/>
+      <c r="O56" s="9"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
@@ -5565,8 +5627,9 @@
       <c r="Z56" s="2"/>
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
-    </row>
-    <row r="57" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC56" s="2"/>
+    </row>
+    <row r="57" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>133</v>
       </c>
@@ -5588,18 +5651,18 @@
       <c r="G57" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="H57" s="8" t="s">
+      <c r="H57" s="6"/>
+      <c r="I57" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I57" s="8" t="s">
+      <c r="J57" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="J57" s="6"/>
       <c r="K57" s="6"/>
-      <c r="L57" s="9"/>
+      <c r="L57" s="6"/>
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
-      <c r="O57" s="2"/>
+      <c r="O57" s="9"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
@@ -5613,8 +5676,9 @@
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
-    </row>
-    <row r="58" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC57" s="2"/>
+    </row>
+    <row r="58" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>70</v>
       </c>
@@ -5636,18 +5700,18 @@
       <c r="G58" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="H58" s="8" t="s">
+      <c r="H58" s="6"/>
+      <c r="I58" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I58" s="8" t="s">
+      <c r="J58" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="J58" s="6"/>
       <c r="K58" s="6"/>
-      <c r="L58" s="9"/>
+      <c r="L58" s="6"/>
       <c r="M58" s="9"/>
       <c r="N58" s="9"/>
-      <c r="O58" s="2"/>
+      <c r="O58" s="9"/>
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
@@ -5661,8 +5725,9 @@
       <c r="Z58" s="2"/>
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
-    </row>
-    <row r="59" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC58" s="2"/>
+    </row>
+    <row r="59" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>141</v>
       </c>
@@ -5684,18 +5749,18 @@
       <c r="G59" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="H59" s="8" t="s">
+      <c r="H59" s="6"/>
+      <c r="I59" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I59" s="19" t="s">
+      <c r="J59" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="J59" s="6"/>
       <c r="K59" s="6"/>
-      <c r="L59" s="9"/>
+      <c r="L59" s="6"/>
       <c r="M59" s="9"/>
       <c r="N59" s="9"/>
-      <c r="O59" s="2"/>
+      <c r="O59" s="9"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
@@ -5709,8 +5774,9 @@
       <c r="Z59" s="2"/>
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
-    </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC59" s="2"/>
+    </row>
+    <row r="60" spans="1:29" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>145</v>
       </c>
@@ -5732,18 +5798,18 @@
       <c r="G60" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="H60" s="8" t="s">
+      <c r="H60" s="6"/>
+      <c r="I60" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I60" s="19" t="s">
+      <c r="J60" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="J60" s="6"/>
       <c r="K60" s="6"/>
-      <c r="L60" s="9"/>
+      <c r="L60" s="6"/>
       <c r="M60" s="9"/>
       <c r="N60" s="9"/>
-      <c r="O60" s="2"/>
+      <c r="O60" s="9"/>
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
@@ -5757,8 +5823,9 @@
       <c r="Z60" s="2"/>
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
-    </row>
-    <row r="61" spans="1:28" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="AC60" s="2"/>
+    </row>
+    <row r="61" spans="1:29" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>117</v>
       </c>
@@ -5780,19 +5847,20 @@
       <c r="G61" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="H61" s="8" t="s">
+      <c r="H61" s="6"/>
+      <c r="I61" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I61" s="8" t="s">
+      <c r="J61" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="J61" s="9"/>
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
-    </row>
-    <row r="62" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="O61" s="9"/>
+    </row>
+    <row r="62" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>119</v>
       </c>
@@ -5814,18 +5882,18 @@
       <c r="G62" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="H62" s="8" t="s">
+      <c r="H62" s="6"/>
+      <c r="I62" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I62" s="21" t="s">
+      <c r="J62" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="J62" s="9"/>
       <c r="K62" s="9"/>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
       <c r="N62" s="9"/>
-      <c r="O62" s="2"/>
+      <c r="O62" s="9"/>
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
@@ -5839,8 +5907,9 @@
       <c r="Z62" s="2"/>
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
-    </row>
-    <row r="63" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="AC62" s="2"/>
+    </row>
+    <row r="63" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>120</v>
       </c>
@@ -5862,18 +5931,18 @@
       <c r="G63" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="H63" s="8" t="s">
+      <c r="H63" s="6"/>
+      <c r="I63" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I63" s="21" t="s">
+      <c r="J63" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="J63" s="9"/>
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
-      <c r="O63" s="2"/>
+      <c r="O63" s="9"/>
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
@@ -5887,8 +5956,9 @@
       <c r="Z63" s="2"/>
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
-    </row>
-    <row r="64" spans="1:28" ht="214.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC63" s="2"/>
+    </row>
+    <row r="64" spans="1:29" ht="214.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>304</v>
       </c>
@@ -5910,18 +5980,18 @@
       <c r="G64" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="H64" s="8" t="s">
+      <c r="H64" s="6"/>
+      <c r="I64" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I64" s="21" t="s">
+      <c r="J64" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="J64" s="9"/>
       <c r="K64" s="9"/>
       <c r="L64" s="9"/>
       <c r="M64" s="9"/>
       <c r="N64" s="9"/>
-      <c r="O64" s="2"/>
+      <c r="O64" s="9"/>
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
@@ -5935,8 +6005,9 @@
       <c r="Z64" s="2"/>
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
-    </row>
-    <row r="65" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="AC64" s="2"/>
+    </row>
+    <row r="65" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>122</v>
       </c>
@@ -5958,18 +6029,18 @@
       <c r="G65" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="H65" s="8" t="s">
+      <c r="H65" s="6"/>
+      <c r="I65" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I65" s="21" t="s">
+      <c r="J65" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="J65" s="9"/>
       <c r="K65" s="9"/>
       <c r="L65" s="9"/>
       <c r="M65" s="9"/>
       <c r="N65" s="9"/>
-      <c r="O65" s="2"/>
+      <c r="O65" s="9"/>
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
@@ -5983,8 +6054,9 @@
       <c r="Z65" s="2"/>
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
-    </row>
-    <row r="66" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="AC65" s="2"/>
+    </row>
+    <row r="66" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>125</v>
       </c>
@@ -6006,18 +6078,18 @@
       <c r="G66" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="H66" s="8" t="s">
+      <c r="H66" s="6"/>
+      <c r="I66" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I66" s="21" t="s">
+      <c r="J66" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="J66" s="9"/>
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
       <c r="M66" s="9"/>
       <c r="N66" s="9"/>
-      <c r="O66" s="2"/>
+      <c r="O66" s="9"/>
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
@@ -6031,8 +6103,9 @@
       <c r="Z66" s="2"/>
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
-    </row>
-    <row r="67" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC66" s="2"/>
+    </row>
+    <row r="67" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>171</v>
       </c>
@@ -6054,18 +6127,18 @@
       <c r="G67" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H67" s="8" t="s">
+      <c r="H67" s="6"/>
+      <c r="I67" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I67" s="21" t="s">
+      <c r="J67" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="J67" s="9"/>
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
-      <c r="O67" s="2"/>
+      <c r="O67" s="9"/>
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
@@ -6079,8 +6152,9 @@
       <c r="Z67" s="2"/>
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
-    </row>
-    <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC67" s="2"/>
+    </row>
+    <row r="68" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>172</v>
       </c>
@@ -6102,18 +6176,18 @@
       <c r="G68" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H68" s="8" t="s">
+      <c r="H68" s="6"/>
+      <c r="I68" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I68" s="21" t="s">
+      <c r="J68" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="J68" s="9"/>
       <c r="K68" s="9"/>
       <c r="L68" s="9"/>
       <c r="M68" s="9"/>
       <c r="N68" s="9"/>
-      <c r="O68" s="2"/>
+      <c r="O68" s="9"/>
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
@@ -6127,8 +6201,9 @@
       <c r="Z68" s="2"/>
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
-    </row>
-    <row r="69" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC68" s="2"/>
+    </row>
+    <row r="69" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>170</v>
       </c>
@@ -6150,18 +6225,18 @@
       <c r="G69" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H69" s="8" t="s">
+      <c r="H69" s="6"/>
+      <c r="I69" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I69" s="21" t="s">
+      <c r="J69" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="J69" s="9"/>
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
       <c r="N69" s="9"/>
-      <c r="O69" s="2"/>
+      <c r="O69" s="9"/>
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
       <c r="R69" s="2"/>
@@ -6175,8 +6250,9 @@
       <c r="Z69" s="2"/>
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
-    </row>
-    <row r="70" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC69" s="2"/>
+    </row>
+    <row r="70" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A70" s="23" t="s">
         <v>174</v>
       </c>
@@ -6198,18 +6274,18 @@
       <c r="G70" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H70" s="8" t="s">
+      <c r="H70" s="6"/>
+      <c r="I70" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I70" s="21" t="s">
+      <c r="J70" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="J70" s="9"/>
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
       <c r="N70" s="9"/>
-      <c r="O70" s="2"/>
+      <c r="O70" s="9"/>
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
       <c r="R70" s="2"/>
@@ -6223,8 +6299,9 @@
       <c r="Z70" s="2"/>
       <c r="AA70" s="2"/>
       <c r="AB70" s="2"/>
-    </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC70" s="2"/>
+    </row>
+    <row r="71" spans="1:29" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>175</v>
       </c>
@@ -6246,18 +6323,18 @@
       <c r="G71" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H71" s="8" t="s">
+      <c r="H71" s="6"/>
+      <c r="I71" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I71" s="21" t="s">
+      <c r="J71" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="J71" s="9"/>
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
       <c r="N71" s="9"/>
-      <c r="O71" s="2"/>
+      <c r="O71" s="9"/>
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
       <c r="R71" s="2"/>
@@ -6271,8 +6348,9 @@
       <c r="Z71" s="2"/>
       <c r="AA71" s="2"/>
       <c r="AB71" s="2"/>
-    </row>
-    <row r="72" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC71" s="2"/>
+    </row>
+    <row r="72" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>176</v>
       </c>
@@ -6294,18 +6372,18 @@
       <c r="G72" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H72" s="8" t="s">
+      <c r="H72" s="6"/>
+      <c r="I72" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I72" s="21" t="s">
+      <c r="J72" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="J72" s="9"/>
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
       <c r="M72" s="9"/>
       <c r="N72" s="9"/>
-      <c r="O72" s="2"/>
+      <c r="O72" s="9"/>
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
       <c r="R72" s="2"/>
@@ -6319,8 +6397,9 @@
       <c r="Z72" s="2"/>
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
-    </row>
-    <row r="73" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC72" s="2"/>
+    </row>
+    <row r="73" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>177</v>
       </c>
@@ -6342,18 +6421,18 @@
       <c r="G73" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H73" s="8" t="s">
+      <c r="H73" s="6"/>
+      <c r="I73" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I73" s="21" t="s">
+      <c r="J73" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="J73" s="9"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
       <c r="N73" s="9"/>
-      <c r="O73" s="2"/>
+      <c r="O73" s="9"/>
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
       <c r="R73" s="2"/>
@@ -6367,8 +6446,9 @@
       <c r="Z73" s="2"/>
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
-    </row>
-    <row r="74" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC73" s="2"/>
+    </row>
+    <row r="74" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>178</v>
       </c>
@@ -6390,18 +6470,18 @@
       <c r="G74" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H74" s="8" t="s">
+      <c r="H74" s="6"/>
+      <c r="I74" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I74" s="21" t="s">
+      <c r="J74" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="J74" s="9"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
       <c r="N74" s="9"/>
-      <c r="O74" s="2"/>
+      <c r="O74" s="9"/>
       <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
       <c r="R74" s="2"/>
@@ -6415,8 +6495,9 @@
       <c r="Z74" s="2"/>
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
-    </row>
-    <row r="75" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC74" s="2"/>
+    </row>
+    <row r="75" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>173</v>
       </c>
@@ -6438,18 +6519,18 @@
       <c r="G75" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H75" s="8" t="s">
+      <c r="H75" s="6"/>
+      <c r="I75" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I75" s="21" t="s">
+      <c r="J75" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="J75" s="9"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
       <c r="N75" s="9"/>
-      <c r="O75" s="2"/>
+      <c r="O75" s="9"/>
       <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
       <c r="R75" s="2"/>
@@ -6463,8 +6544,9 @@
       <c r="Z75" s="2"/>
       <c r="AA75" s="2"/>
       <c r="AB75" s="2"/>
-    </row>
-    <row r="76" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC75" s="2"/>
+    </row>
+    <row r="76" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>226</v>
       </c>
@@ -6486,14 +6568,15 @@
       <c r="G76" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H76" s="8" t="s">
+      <c r="H76" s="6"/>
+      <c r="I76" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I76" s="21" t="s">
+      <c r="J76" s="21" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>228</v>
       </c>
@@ -6515,14 +6598,15 @@
       <c r="G77" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H77" s="8" t="s">
+      <c r="H77" s="6"/>
+      <c r="I77" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I77" s="21" t="s">
+      <c r="J77" s="21" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>231</v>
       </c>
@@ -6544,14 +6628,15 @@
       <c r="G78" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H78" s="8" t="s">
+      <c r="H78" s="6"/>
+      <c r="I78" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I78" s="21" t="s">
+      <c r="J78" s="21" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>238</v>
       </c>
@@ -6573,14 +6658,15 @@
       <c r="G79" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H79" s="8" t="s">
+      <c r="H79" s="6"/>
+      <c r="I79" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I79" s="21" t="s">
+      <c r="J79" s="21" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>235</v>
       </c>
@@ -6602,14 +6688,15 @@
       <c r="G80" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H80" s="8" t="s">
+      <c r="H80" s="6"/>
+      <c r="I80" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I80" s="21" t="s">
+      <c r="J80" s="21" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>237</v>
       </c>
@@ -6631,14 +6718,15 @@
       <c r="G81" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H81" s="8" t="s">
+      <c r="H81" s="6"/>
+      <c r="I81" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I81" s="21" t="s">
+      <c r="J81" s="21" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>240</v>
       </c>
@@ -6660,14 +6748,15 @@
       <c r="G82" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H82" s="8" t="s">
+      <c r="H82" s="6"/>
+      <c r="I82" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I82" s="21" t="s">
+      <c r="J82" s="21" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>242</v>
       </c>
@@ -6689,14 +6778,15 @@
       <c r="G83" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H83" s="8" t="s">
+      <c r="H83" s="6"/>
+      <c r="I83" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I83" s="21" t="s">
+      <c r="J83" s="21" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>244</v>
       </c>
@@ -6718,14 +6808,15 @@
       <c r="G84" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H84" s="8" t="s">
+      <c r="H84" s="6"/>
+      <c r="I84" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I84" s="21" t="s">
+      <c r="J84" s="21" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>246</v>
       </c>
@@ -6747,14 +6838,15 @@
       <c r="G85" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H85" s="8" t="s">
+      <c r="H85" s="6"/>
+      <c r="I85" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I85" s="21" t="s">
+      <c r="J85" s="21" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="165" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:29" ht="165" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>254</v>
       </c>
@@ -6776,14 +6868,15 @@
       <c r="G86" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="H86" s="8" t="s">
+      <c r="H86" s="6"/>
+      <c r="I86" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I86" s="21" t="s">
+      <c r="J86" s="21" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:29" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>135</v>
       </c>
@@ -6805,18 +6898,18 @@
       <c r="G87" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H87" s="8" t="s">
+      <c r="H87" s="6"/>
+      <c r="I87" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I87" s="8" t="s">
+      <c r="J87" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="J87" s="6"/>
       <c r="K87" s="6"/>
-      <c r="L87" s="9"/>
+      <c r="L87" s="6"/>
       <c r="M87" s="9"/>
       <c r="N87" s="9"/>
-      <c r="O87" s="2"/>
+      <c r="O87" s="9"/>
       <c r="P87" s="2"/>
       <c r="Q87" s="2"/>
       <c r="R87" s="2"/>
@@ -6830,8 +6923,9 @@
       <c r="Z87" s="2"/>
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
-    </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="AC87" s="2"/>
+    </row>
+    <row r="88" spans="1:29" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>161</v>
       </c>
@@ -6853,18 +6947,18 @@
       <c r="G88" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H88" s="8" t="s">
+      <c r="H88" s="6"/>
+      <c r="I88" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I88" s="8" t="s">
+      <c r="J88" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="J88" s="8"/>
-      <c r="K88" s="9"/>
+      <c r="K88" s="8"/>
       <c r="L88" s="9"/>
       <c r="M88" s="9"/>
       <c r="N88" s="9"/>
-      <c r="O88" s="2"/>
+      <c r="O88" s="9"/>
       <c r="P88" s="2"/>
       <c r="Q88" s="2"/>
       <c r="R88" s="2"/>
@@ -6878,8 +6972,9 @@
       <c r="Z88" s="2"/>
       <c r="AA88" s="2"/>
       <c r="AB88" s="2"/>
-    </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="AC88" s="2"/>
+    </row>
+    <row r="89" spans="1:29" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>163</v>
       </c>
@@ -6901,18 +6996,18 @@
       <c r="G89" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H89" s="8" t="s">
+      <c r="H89" s="6"/>
+      <c r="I89" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I89" s="8" t="s">
+      <c r="J89" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="J89" s="8"/>
-      <c r="K89" s="9"/>
+      <c r="K89" s="8"/>
       <c r="L89" s="9"/>
       <c r="M89" s="9"/>
       <c r="N89" s="9"/>
-      <c r="O89" s="2"/>
+      <c r="O89" s="9"/>
       <c r="P89" s="2"/>
       <c r="Q89" s="2"/>
       <c r="R89" s="2"/>
@@ -6926,8 +7021,9 @@
       <c r="Z89" s="2"/>
       <c r="AA89" s="2"/>
       <c r="AB89" s="2"/>
-    </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC89" s="2"/>
+    </row>
+    <row r="90" spans="1:29" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>165</v>
       </c>
@@ -6949,20 +7045,20 @@
       <c r="G90" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H90" s="8" t="s">
+      <c r="H90" s="6"/>
+      <c r="I90" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I90" s="8" t="s">
+      <c r="J90" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="J90" s="20" t="s">
+      <c r="K90" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="K90" s="9"/>
       <c r="L90" s="9"/>
       <c r="M90" s="9"/>
       <c r="N90" s="9"/>
-      <c r="O90" s="2"/>
+      <c r="O90" s="9"/>
       <c r="P90" s="2"/>
       <c r="Q90" s="2"/>
       <c r="R90" s="2"/>
@@ -6976,8 +7072,9 @@
       <c r="Z90" s="2"/>
       <c r="AA90" s="2"/>
       <c r="AB90" s="2"/>
-    </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC90" s="2"/>
+    </row>
+    <row r="91" spans="1:29" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>330</v>
       </c>
@@ -6999,18 +7096,18 @@
       <c r="G91" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H91" s="8" t="s">
+      <c r="H91" s="6"/>
+      <c r="I91" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I91" s="20" t="s">
+      <c r="J91" s="20" t="s">
         <v>331</v>
       </c>
-      <c r="J91"/>
-      <c r="K91" s="9"/>
+      <c r="K91"/>
       <c r="L91" s="9"/>
       <c r="M91" s="9"/>
       <c r="N91" s="9"/>
-      <c r="O91" s="2"/>
+      <c r="O91" s="9"/>
       <c r="P91" s="2"/>
       <c r="Q91" s="2"/>
       <c r="R91" s="2"/>
@@ -7024,8 +7121,9 @@
       <c r="Z91" s="2"/>
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
-    </row>
-    <row r="92" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC91" s="2"/>
+    </row>
+    <row r="92" spans="1:29" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>81</v>
       </c>
@@ -7047,18 +7145,18 @@
       <c r="G92" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="H92" s="8" t="s">
+      <c r="H92" s="6"/>
+      <c r="I92" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I92" s="8" t="s">
+      <c r="J92" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="J92" s="6"/>
       <c r="K92" s="6"/>
       <c r="L92" s="6"/>
-      <c r="M92" s="9"/>
+      <c r="M92" s="6"/>
       <c r="N92" s="9"/>
-      <c r="O92" s="2"/>
+      <c r="O92" s="9"/>
       <c r="P92" s="2"/>
       <c r="Q92" s="2"/>
       <c r="R92" s="2"/>
@@ -7072,8 +7170,9 @@
       <c r="Z92" s="2"/>
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
-    </row>
-    <row r="93" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC92" s="2"/>
+    </row>
+    <row r="93" spans="1:29" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>84</v>
       </c>
@@ -7095,18 +7194,18 @@
       <c r="G93" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="H93" s="8" t="s">
+      <c r="H93" s="6"/>
+      <c r="I93" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I93" s="8" t="s">
+      <c r="J93" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="J93" s="6"/>
       <c r="K93" s="6"/>
       <c r="L93" s="6"/>
-      <c r="M93" s="9"/>
+      <c r="M93" s="6"/>
       <c r="N93" s="9"/>
-      <c r="O93" s="2"/>
+      <c r="O93" s="9"/>
       <c r="P93" s="2"/>
       <c r="Q93" s="2"/>
       <c r="R93" s="2"/>
@@ -7120,8 +7219,9 @@
       <c r="Z93" s="2"/>
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
-    </row>
-    <row r="94" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC93" s="2"/>
+    </row>
+    <row r="94" spans="1:29" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>86</v>
       </c>
@@ -7143,18 +7243,18 @@
       <c r="G94" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="H94" s="8" t="s">
+      <c r="H94" s="6"/>
+      <c r="I94" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I94" s="8" t="s">
+      <c r="J94" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J94" s="6"/>
       <c r="K94" s="6"/>
       <c r="L94" s="6"/>
-      <c r="M94" s="9"/>
+      <c r="M94" s="6"/>
       <c r="N94" s="9"/>
-      <c r="O94" s="2"/>
+      <c r="O94" s="9"/>
       <c r="P94" s="2"/>
       <c r="Q94" s="2"/>
       <c r="R94" s="2"/>
@@ -7168,8 +7268,9 @@
       <c r="Z94" s="2"/>
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
-    </row>
-    <row r="95" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC94" s="2"/>
+    </row>
+    <row r="95" spans="1:29" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>88</v>
       </c>
@@ -7191,18 +7292,18 @@
       <c r="G95" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="H95" s="8" t="s">
+      <c r="H95" s="6"/>
+      <c r="I95" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I95" s="8" t="s">
+      <c r="J95" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="J95" s="6"/>
       <c r="K95" s="6"/>
       <c r="L95" s="6"/>
-      <c r="M95" s="9"/>
+      <c r="M95" s="6"/>
       <c r="N95" s="9"/>
-      <c r="O95" s="2"/>
+      <c r="O95" s="9"/>
       <c r="P95" s="2"/>
       <c r="Q95" s="2"/>
       <c r="R95" s="2"/>
@@ -7216,8 +7317,9 @@
       <c r="Z95" s="2"/>
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
-    </row>
-    <row r="96" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC95" s="2"/>
+    </row>
+    <row r="96" spans="1:29" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>90</v>
       </c>
@@ -7239,18 +7341,18 @@
       <c r="G96" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="H96" s="8" t="s">
+      <c r="H96" s="6"/>
+      <c r="I96" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I96" s="8" t="s">
+      <c r="J96" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="J96" s="6"/>
       <c r="K96" s="6"/>
       <c r="L96" s="6"/>
-      <c r="M96" s="9"/>
+      <c r="M96" s="6"/>
       <c r="N96" s="9"/>
-      <c r="O96" s="2"/>
+      <c r="O96" s="9"/>
       <c r="P96" s="2"/>
       <c r="Q96" s="2"/>
       <c r="R96" s="2"/>
@@ -7264,8 +7366,9 @@
       <c r="Z96" s="2"/>
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
-    </row>
-    <row r="97" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC96" s="2"/>
+    </row>
+    <row r="97" spans="1:29" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A97" s="25" t="s">
         <v>256</v>
       </c>
@@ -7287,18 +7390,18 @@
       <c r="G97" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="H97" s="8" t="s">
+      <c r="H97" s="6"/>
+      <c r="I97" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I97" s="8" t="s">
+      <c r="J97" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="J97" s="6"/>
       <c r="K97" s="6"/>
       <c r="L97" s="6"/>
-      <c r="M97" s="9"/>
+      <c r="M97" s="6"/>
       <c r="N97" s="9"/>
-      <c r="O97" s="2"/>
+      <c r="O97" s="9"/>
       <c r="P97" s="2"/>
       <c r="Q97" s="2"/>
       <c r="R97" s="2"/>
@@ -7312,8 +7415,9 @@
       <c r="Z97" s="2"/>
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
-    </row>
-    <row r="98" spans="1:28" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="AC97" s="2"/>
+    </row>
+    <row r="98" spans="1:29" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>92</v>
       </c>
@@ -7335,18 +7439,18 @@
       <c r="G98" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="H98" s="8" t="s">
+      <c r="H98" s="6"/>
+      <c r="I98" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I98" s="8" t="s">
+      <c r="J98" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="J98" s="6"/>
       <c r="K98" s="6"/>
       <c r="L98" s="6"/>
-      <c r="M98" s="9"/>
+      <c r="M98" s="6"/>
       <c r="N98" s="9"/>
-      <c r="O98" s="2"/>
+      <c r="O98" s="9"/>
       <c r="P98" s="2"/>
       <c r="Q98" s="2"/>
       <c r="R98" s="2"/>
@@ -7360,8 +7464,9 @@
       <c r="Z98" s="2"/>
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
-    </row>
-    <row r="99" spans="1:28" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC98" s="2"/>
+    </row>
+    <row r="99" spans="1:29" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>197</v>
       </c>
@@ -7383,18 +7488,18 @@
       <c r="G99" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="H99" s="20" t="s">
+      <c r="H99" s="9"/>
+      <c r="I99" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="I99" s="20" t="s">
+      <c r="J99" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="J99" s="9"/>
       <c r="K99" s="9"/>
       <c r="L99" s="9"/>
       <c r="M99" s="9"/>
       <c r="N99" s="9"/>
-      <c r="O99" s="2"/>
+      <c r="O99" s="9"/>
       <c r="P99" s="2"/>
       <c r="Q99" s="2"/>
       <c r="R99" s="2"/>
@@ -7408,8 +7513,9 @@
       <c r="Z99" s="2"/>
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
-    </row>
-    <row r="100" spans="1:28" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC99" s="2"/>
+    </row>
+    <row r="100" spans="1:29" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>201</v>
       </c>
@@ -7431,18 +7537,18 @@
       <c r="G100" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="H100" s="20" t="s">
+      <c r="H100" s="9"/>
+      <c r="I100" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="I100" s="20" t="s">
+      <c r="J100" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="J100" s="9"/>
       <c r="K100" s="9"/>
       <c r="L100" s="9"/>
       <c r="M100" s="9"/>
       <c r="N100" s="9"/>
-      <c r="O100" s="2"/>
+      <c r="O100" s="9"/>
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
       <c r="R100" s="2"/>
@@ -7456,8 +7562,9 @@
       <c r="Z100" s="2"/>
       <c r="AA100" s="2"/>
       <c r="AB100" s="2"/>
-    </row>
-    <row r="101" spans="1:28" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC100" s="2"/>
+    </row>
+    <row r="101" spans="1:29" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>203</v>
       </c>
@@ -7479,18 +7586,18 @@
       <c r="G101" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="H101" s="20" t="s">
+      <c r="H101" s="9"/>
+      <c r="I101" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="I101" s="20" t="s">
+      <c r="J101" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="J101" s="9"/>
       <c r="K101" s="9"/>
       <c r="L101" s="9"/>
       <c r="M101" s="9"/>
       <c r="N101" s="9"/>
-      <c r="O101" s="2"/>
+      <c r="O101" s="9"/>
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
       <c r="R101" s="2"/>
@@ -7504,8 +7611,9 @@
       <c r="Z101" s="2"/>
       <c r="AA101" s="2"/>
       <c r="AB101" s="2"/>
-    </row>
-    <row r="102" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="AC101" s="2"/>
+    </row>
+    <row r="102" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>159</v>
       </c>
@@ -7527,18 +7635,18 @@
       <c r="G102" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="H102" s="8" t="s">
+      <c r="H102" s="6"/>
+      <c r="I102" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I102" s="8" t="s">
+      <c r="J102" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="J102" s="9"/>
       <c r="K102" s="9"/>
       <c r="L102" s="9"/>
       <c r="M102" s="9"/>
       <c r="N102" s="9"/>
-      <c r="O102" s="2"/>
+      <c r="O102" s="9"/>
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
       <c r="R102" s="2"/>
@@ -7552,8 +7660,9 @@
       <c r="Z102" s="2"/>
       <c r="AA102" s="2"/>
       <c r="AB102" s="2"/>
-    </row>
-    <row r="103" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="AC102" s="2"/>
+    </row>
+    <row r="103" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>113</v>
       </c>
@@ -7575,18 +7684,18 @@
       <c r="G103" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="H103" s="8" t="s">
+      <c r="H103" s="6"/>
+      <c r="I103" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I103" s="8" t="s">
+      <c r="J103" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="J103" s="9"/>
       <c r="K103" s="9"/>
       <c r="L103" s="9"/>
       <c r="M103" s="9"/>
       <c r="N103" s="9"/>
-      <c r="O103" s="2"/>
+      <c r="O103" s="9"/>
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
       <c r="R103" s="2"/>
@@ -7600,8 +7709,9 @@
       <c r="Z103" s="2"/>
       <c r="AA103" s="2"/>
       <c r="AB103" s="2"/>
-    </row>
-    <row r="104" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+      <c r="AC103" s="2"/>
+    </row>
+    <row r="104" spans="1:29" ht="150" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>79</v>
       </c>
@@ -7623,18 +7733,18 @@
       <c r="G104" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="H104" s="8" t="s">
+      <c r="H104" s="6"/>
+      <c r="I104" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="I104" s="8" t="s">
+      <c r="J104" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="J104" s="9"/>
       <c r="K104" s="9"/>
       <c r="L104" s="9"/>
       <c r="M104" s="9"/>
       <c r="N104" s="9"/>
-      <c r="O104" s="2"/>
+      <c r="O104" s="9"/>
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
       <c r="R104" s="2"/>
@@ -764